<commit_message>
f-test fix attempt in aat
</commit_message>
<xml_diff>
--- a/src/aat/resources/adv_bundling_functional_tests_ccd_def.xlsx
+++ b/src/aat/resources/adv_bundling_functional_tests_ccd_def.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pawel/workspace/rpa-em-ccd-orchestrator/src/aat/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49F901E8-7065-8344-9008-89EDC58CDE4F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4EC11BF-CD5C-0244-88C4-F7C3D378FEBB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="460" windowWidth="31940" windowHeight="14640" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="460" windowWidth="31940" windowHeight="14640" tabRatio="500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Change History" sheetId="1" r:id="rId1"/>
@@ -1144,9 +1144,6 @@
     <t>hasCoversheets</t>
   </si>
   <si>
-    <t>http://192.168.1.199:8080/api/new-bundle</t>
-  </si>
-  <si>
     <t>asyncStitchingComplete</t>
   </si>
   <si>
@@ -1166,6 +1163,9 @@
   </si>
   <si>
     <t>CCD_BUNDLE_MVP_v0.2</t>
+  </si>
+  <si>
+    <t>http://192.168.0.108:8080/api/new-bundle</t>
   </si>
 </sst>
 </file>
@@ -3019,14 +3019,14 @@
         <v>76</v>
       </c>
       <c r="D27" s="81" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E27" t="s">
         <v>58</v>
       </c>
       <c r="F27" s="81"/>
       <c r="G27" s="81" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="H27" s="91"/>
       <c r="I27" s="81"/>
@@ -3274,7 +3274,7 @@
       </c>
       <c r="B4" s="101"/>
       <c r="C4" s="11" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D4" s="40" t="s">
         <v>56</v>
@@ -3291,7 +3291,7 @@
         <v>42736</v>
       </c>
       <c r="C5" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D5" s="40" t="s">
         <v>59</v>
@@ -3308,7 +3308,7 @@
         <v>42736</v>
       </c>
       <c r="C6" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D6" s="40" t="s">
         <v>61</v>
@@ -3325,7 +3325,7 @@
         <v>42736</v>
       </c>
       <c r="C7" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D7" s="40" t="s">
         <v>63</v>
@@ -3440,7 +3440,7 @@
       </c>
       <c r="B4" s="101"/>
       <c r="C4" s="11" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D4" s="40" t="s">
         <v>56</v>
@@ -3457,7 +3457,7 @@
         <v>42736</v>
       </c>
       <c r="C5" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D5" s="40" t="s">
         <v>59</v>
@@ -3474,7 +3474,7 @@
         <v>42736</v>
       </c>
       <c r="C6" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D6" s="40" t="s">
         <v>61</v>
@@ -3491,7 +3491,7 @@
         <v>42736</v>
       </c>
       <c r="C7" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D7" s="40" t="s">
         <v>63</v>
@@ -3606,7 +3606,7 @@
       </c>
       <c r="B4" s="101"/>
       <c r="C4" s="11" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D4" s="40" t="s">
         <v>56</v>
@@ -3623,7 +3623,7 @@
         <v>42736</v>
       </c>
       <c r="C5" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D5" s="40" t="s">
         <v>59</v>
@@ -3640,7 +3640,7 @@
         <v>42736</v>
       </c>
       <c r="C6" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D6" s="40" t="s">
         <v>61</v>
@@ -3657,7 +3657,7 @@
         <v>42736</v>
       </c>
       <c r="C7" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D7" s="40" t="s">
         <v>63</v>
@@ -3758,7 +3758,7 @@
       </c>
       <c r="B4" s="101"/>
       <c r="C4" s="11" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D4" s="40" t="s">
         <v>56</v>
@@ -3775,7 +3775,7 @@
         <v>42736</v>
       </c>
       <c r="C5" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D5" s="40" t="s">
         <v>59</v>
@@ -3792,7 +3792,7 @@
         <v>42736</v>
       </c>
       <c r="C6" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D6" s="40" t="s">
         <v>61</v>
@@ -3809,7 +3809,7 @@
         <v>42736</v>
       </c>
       <c r="C7" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D7" s="40" t="s">
         <v>63</v>
@@ -3926,7 +3926,7 @@
         <v>24</v>
       </c>
       <c r="E4" s="114" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="F4" s="114" t="s">
         <v>113</v>
@@ -3944,7 +3944,7 @@
         <v>24</v>
       </c>
       <c r="E5" s="119" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="F5" s="119" t="s">
         <v>113</v>
@@ -3962,7 +3962,7 @@
         <v>24</v>
       </c>
       <c r="E6" s="119" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="F6" s="119" t="s">
         <v>113</v>
@@ -3980,7 +3980,7 @@
         <v>24</v>
       </c>
       <c r="E7" s="124" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="F7" s="124" t="s">
         <v>113</v>
@@ -3998,7 +3998,7 @@
         <v>24</v>
       </c>
       <c r="E8" s="124" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="F8" s="124" t="s">
         <v>113</v>
@@ -4093,7 +4093,7 @@
       </c>
       <c r="B4" s="126"/>
       <c r="C4" s="50" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D4" s="44" t="s">
         <v>328</v>
@@ -4207,7 +4207,7 @@
       </c>
       <c r="B4" s="87"/>
       <c r="C4" s="77" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D4" s="132" t="s">
         <v>56</v>
@@ -4225,7 +4225,7 @@
       </c>
       <c r="B5" s="93"/>
       <c r="C5" s="80" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D5" s="134" t="s">
         <v>59</v>
@@ -4243,7 +4243,7 @@
       </c>
       <c r="B6" s="93"/>
       <c r="C6" s="80" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D6" s="134" t="s">
         <v>61</v>
@@ -4261,7 +4261,7 @@
       </c>
       <c r="B7" s="93"/>
       <c r="C7" s="80" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D7" s="134" t="s">
         <v>63</v>
@@ -4279,7 +4279,7 @@
       </c>
       <c r="B8" s="93"/>
       <c r="C8" s="80" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D8" s="134" t="s">
         <v>65</v>
@@ -4297,7 +4297,7 @@
       </c>
       <c r="B9" s="93"/>
       <c r="C9" s="80" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D9" s="134" t="s">
         <v>68</v>
@@ -4315,7 +4315,7 @@
       </c>
       <c r="B10" s="93"/>
       <c r="C10" s="80" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D10" s="136" t="s">
         <v>72</v>
@@ -4333,7 +4333,7 @@
       </c>
       <c r="B11" s="93"/>
       <c r="C11" s="80" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D11" s="136" t="s">
         <v>77</v>
@@ -4351,7 +4351,7 @@
       </c>
       <c r="B12" s="93"/>
       <c r="C12" s="80" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D12" t="s">
         <v>80</v>
@@ -4465,7 +4465,7 @@
       </c>
       <c r="B4" s="139"/>
       <c r="C4" s="114" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D4" s="56" t="s">
         <v>141</v>
@@ -4483,7 +4483,7 @@
       </c>
       <c r="B5" s="142"/>
       <c r="C5" s="119" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D5" s="56" t="s">
         <v>145</v>
@@ -4501,7 +4501,7 @@
       </c>
       <c r="B6" s="142"/>
       <c r="C6" s="119" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D6" s="56" t="s">
         <v>149</v>
@@ -4519,7 +4519,7 @@
       </c>
       <c r="B7" s="142"/>
       <c r="C7" s="119" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D7" s="56" t="s">
         <v>152</v>
@@ -4537,7 +4537,7 @@
       </c>
       <c r="B8" s="142"/>
       <c r="C8" s="119" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D8" s="56" t="s">
         <v>159</v>
@@ -4555,7 +4555,7 @@
       </c>
       <c r="B9" s="142"/>
       <c r="C9" s="119" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D9" s="56" t="s">
         <v>155</v>
@@ -4573,7 +4573,7 @@
       </c>
       <c r="B10" s="142"/>
       <c r="C10" s="119" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D10" s="56" t="s">
         <v>163</v>
@@ -4591,7 +4591,7 @@
       </c>
       <c r="B11" s="142"/>
       <c r="C11" s="119" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D11" s="56" t="s">
         <v>170</v>
@@ -4609,10 +4609,10 @@
       </c>
       <c r="B12" s="142"/>
       <c r="C12" s="119" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D12" s="56" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="E12" s="143" t="s">
         <v>328</v>
@@ -4737,7 +4737,7 @@
       </c>
       <c r="B4" s="90"/>
       <c r="C4" s="124" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D4" s="124" t="s">
         <v>113</v>
@@ -4941,7 +4941,7 @@
       </c>
       <c r="B4" s="90"/>
       <c r="C4" s="124" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D4" s="124" t="s">
         <v>72</v>
@@ -4962,7 +4962,7 @@
       </c>
       <c r="B5" s="90"/>
       <c r="C5" s="124" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D5" s="124" t="s">
         <v>72</v>
@@ -4983,7 +4983,7 @@
       </c>
       <c r="B6" s="90"/>
       <c r="C6" s="124" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D6" s="124" t="s">
         <v>72</v>
@@ -5004,7 +5004,7 @@
       </c>
       <c r="B7" s="90"/>
       <c r="C7" s="124" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D7" s="124" t="s">
         <v>72</v>
@@ -5025,7 +5025,7 @@
       </c>
       <c r="B8" s="90"/>
       <c r="C8" s="124" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D8" s="124" t="s">
         <v>72</v>
@@ -5046,7 +5046,7 @@
       </c>
       <c r="B9" s="90"/>
       <c r="C9" s="124" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D9" s="124" t="s">
         <v>72</v>
@@ -5067,7 +5067,7 @@
       </c>
       <c r="B10" s="90"/>
       <c r="C10" s="124" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D10" s="124" t="s">
         <v>72</v>
@@ -5088,7 +5088,7 @@
       </c>
       <c r="B11" s="90"/>
       <c r="C11" s="124" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D11" s="124" t="s">
         <v>72</v>
@@ -5109,7 +5109,7 @@
       </c>
       <c r="B12" s="90"/>
       <c r="C12" s="124" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D12" s="124" t="s">
         <v>72</v>
@@ -5130,7 +5130,7 @@
       </c>
       <c r="B13" s="90"/>
       <c r="C13" s="124" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D13" s="124" t="s">
         <v>72</v>
@@ -5151,7 +5151,7 @@
       </c>
       <c r="B14" s="90"/>
       <c r="C14" s="124" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D14" s="124" t="s">
         <v>72</v>
@@ -5172,7 +5172,7 @@
       </c>
       <c r="B15" s="90"/>
       <c r="C15" s="124" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D15" s="124" t="s">
         <v>72</v>
@@ -5193,13 +5193,13 @@
       </c>
       <c r="B16" s="90"/>
       <c r="C16" s="124" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D16" s="124" t="s">
         <v>72</v>
       </c>
       <c r="E16" s="81" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="F16" s="146" t="s">
         <v>328</v>
@@ -5214,7 +5214,7 @@
       </c>
       <c r="B17" s="90"/>
       <c r="C17" s="124" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D17" s="124" t="s">
         <v>72</v>
@@ -5235,7 +5235,7 @@
       </c>
       <c r="B18" s="90"/>
       <c r="C18" s="124" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D18" s="124" t="s">
         <v>77</v>
@@ -5256,7 +5256,7 @@
       </c>
       <c r="B19" s="90"/>
       <c r="C19" s="124" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D19" s="124" t="s">
         <v>77</v>
@@ -5277,7 +5277,7 @@
       </c>
       <c r="B20" s="90"/>
       <c r="C20" s="124" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D20" s="124" t="s">
         <v>77</v>
@@ -5298,7 +5298,7 @@
       </c>
       <c r="B21" s="90"/>
       <c r="C21" s="124" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D21" s="124" t="s">
         <v>77</v>
@@ -5319,7 +5319,7 @@
       </c>
       <c r="B22" s="90"/>
       <c r="C22" s="124" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D22" s="124" t="s">
         <v>77</v>
@@ -5348,7 +5348,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:S4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
@@ -5463,13 +5463,13 @@
       </c>
       <c r="B4" s="19"/>
       <c r="C4" s="11" t="s">
+        <v>345</v>
+      </c>
+      <c r="D4" s="34" t="s">
         <v>346</v>
       </c>
-      <c r="D4" s="34" t="s">
+      <c r="E4" s="34" t="s">
         <v>347</v>
-      </c>
-      <c r="E4" s="34" t="s">
-        <v>348</v>
       </c>
       <c r="F4" s="21" t="s">
         <v>24</v>
@@ -5607,7 +5607,7 @@
       </c>
       <c r="B4" s="19"/>
       <c r="C4" s="11" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D4" s="40" t="s">
         <v>56</v>
@@ -5631,7 +5631,7 @@
       </c>
       <c r="B5" s="19"/>
       <c r="C5" s="11" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D5" s="40" t="s">
         <v>59</v>
@@ -5655,7 +5655,7 @@
       </c>
       <c r="B6" s="19"/>
       <c r="C6" s="11" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D6" s="40" t="s">
         <v>61</v>
@@ -5679,7 +5679,7 @@
       </c>
       <c r="B7" s="19"/>
       <c r="C7" s="11" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D7" s="40" t="s">
         <v>63</v>
@@ -5703,7 +5703,7 @@
       </c>
       <c r="B8" s="19"/>
       <c r="C8" s="11" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D8" s="40" t="s">
         <v>65</v>
@@ -5726,7 +5726,7 @@
         <v>42736</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D9" s="41" t="s">
         <v>68</v>
@@ -6360,7 +6360,7 @@
       </c>
       <c r="B10" s="19"/>
       <c r="C10" s="11" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D10" s="41" t="s">
         <v>72</v>
@@ -6388,7 +6388,7 @@
       </c>
       <c r="B11" s="19"/>
       <c r="C11" s="11" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D11" s="41" t="s">
         <v>77</v>
@@ -6414,7 +6414,7 @@
       </c>
       <c r="B12" s="19"/>
       <c r="C12" s="11" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D12" s="41" t="s">
         <v>80</v>
@@ -6568,7 +6568,7 @@
         <v>42736</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D4" s="42" t="s">
         <v>98</v>
@@ -6594,7 +6594,7 @@
         <v>42736</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D5" s="42" t="s">
         <v>98</v>
@@ -6620,7 +6620,7 @@
         <v>42736</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D6" s="42" t="s">
         <v>98</v>
@@ -6646,7 +6646,7 @@
         <v>42736</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D7" s="42" t="s">
         <v>98</v>
@@ -6673,7 +6673,7 @@
       </c>
       <c r="B8" s="42"/>
       <c r="C8" s="11" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D8" s="42" t="s">
         <v>98</v>
@@ -6700,7 +6700,7 @@
       </c>
       <c r="B9" s="42"/>
       <c r="C9" s="11" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D9" s="42" t="s">
         <v>98</v>
@@ -6727,7 +6727,7 @@
       </c>
       <c r="B10" s="42"/>
       <c r="C10" s="11" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D10" s="42" t="s">
         <v>98</v>
@@ -6753,7 +6753,7 @@
         <v>42736</v>
       </c>
       <c r="C11" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D11" t="s">
         <v>98</v>
@@ -6779,7 +6779,7 @@
         <v>42736</v>
       </c>
       <c r="C12" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D12" t="s">
         <v>98</v>
@@ -6917,7 +6917,7 @@
         <v>42736</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D4" s="50" t="s">
         <v>113</v>
@@ -6942,8 +6942,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:T14"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -7116,7 +7116,7 @@
         <v>10</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D4" s="56" t="s">
         <v>141</v>
@@ -7151,7 +7151,7 @@
       </c>
       <c r="B5" s="42"/>
       <c r="C5" s="11" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D5" s="56" t="s">
         <v>145</v>
@@ -7188,7 +7188,7 @@
       </c>
       <c r="B6" s="42"/>
       <c r="C6" s="11" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D6" s="56" t="s">
         <v>149</v>
@@ -7209,7 +7209,7 @@
         <v>113</v>
       </c>
       <c r="L6" s="154" t="s">
-        <v>341</v>
+        <v>348</v>
       </c>
       <c r="O6">
         <v>5</v>
@@ -7228,7 +7228,7 @@
       </c>
       <c r="B7" s="42"/>
       <c r="C7" s="11" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D7" s="56" t="s">
         <v>152</v>
@@ -7265,7 +7265,7 @@
       </c>
       <c r="B8" s="42"/>
       <c r="C8" s="11" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D8" s="56" t="s">
         <v>155</v>
@@ -7306,7 +7306,7 @@
       </c>
       <c r="B9" s="42"/>
       <c r="C9" s="11" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D9" s="56" t="s">
         <v>159</v>
@@ -7347,7 +7347,7 @@
       </c>
       <c r="B10" s="42"/>
       <c r="C10" s="11" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D10" s="56" t="s">
         <v>163</v>
@@ -7384,7 +7384,7 @@
       </c>
       <c r="B11" s="42"/>
       <c r="C11" s="11" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D11" s="56" t="s">
         <v>166</v>
@@ -7427,7 +7427,7 @@
       </c>
       <c r="B12" s="42"/>
       <c r="C12" s="11" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D12" s="56" t="s">
         <v>170</v>
@@ -7464,13 +7464,13 @@
       </c>
       <c r="B13" s="42"/>
       <c r="C13" s="11" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D13" s="56" t="s">
+        <v>341</v>
+      </c>
+      <c r="E13" s="57" t="s">
         <v>342</v>
-      </c>
-      <c r="E13" s="57" t="s">
-        <v>343</v>
       </c>
       <c r="F13" s="57" t="s">
         <v>172</v>
@@ -7662,7 +7662,7 @@
         <v>42736</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D4" s="63" t="s">
         <v>141</v>
@@ -7699,7 +7699,7 @@
         <v>42736</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D5" s="68" t="s">
         <v>141</v>
@@ -7736,7 +7736,7 @@
         <v>42736</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D6" s="68" t="s">
         <v>141</v>
@@ -7773,7 +7773,7 @@
         <v>42736</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D7" s="68" t="s">
         <v>141</v>
@@ -7810,7 +7810,7 @@
         <v>42736</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D8" s="70" t="s">
         <v>141</v>
@@ -7847,7 +7847,7 @@
         <v>42736</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D9" s="70" t="s">
         <v>141</v>
@@ -7884,7 +7884,7 @@
         <v>42736</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D10" s="63" t="s">
         <v>145</v>
@@ -7919,7 +7919,7 @@
         <v>42736</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D11" s="68" t="s">
         <v>145</v>
@@ -7954,7 +7954,7 @@
         <v>42736</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D12" s="68" t="s">
         <v>145</v>
@@ -7989,7 +7989,7 @@
         <v>42736</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D13" s="68" t="s">
         <v>145</v>
@@ -8024,7 +8024,7 @@
         <v>42736</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D14" s="70" t="s">
         <v>145</v>
@@ -8059,7 +8059,7 @@
         <v>42736</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D15" s="70" t="s">
         <v>145</v>
@@ -8094,7 +8094,7 @@
         <v>42736</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D16" s="70" t="s">
         <v>149</v>
@@ -8129,7 +8129,7 @@
         <v>42736</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D17" s="70" t="s">
         <v>152</v>
@@ -8164,7 +8164,7 @@
         <v>42736</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D18" s="70" t="s">
         <v>159</v>
@@ -8199,7 +8199,7 @@
         <v>42736</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D19" s="56" t="s">
         <v>155</v>
@@ -8234,7 +8234,7 @@
         <v>42736</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D20" s="56" t="s">
         <v>163</v>
@@ -8269,7 +8269,7 @@
         <v>42736</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D21" s="56" t="s">
         <v>170</v>

</xml_diff>

<commit_message>
EM-2142: Update CCD definition spreadsheet
</commit_message>
<xml_diff>
--- a/src/aat/resources/adv_bundling_functional_tests_ccd_def.xlsx
+++ b/src/aat/resources/adv_bundling_functional_tests_ccd_def.xlsx
@@ -881,7 +881,7 @@
     <t>bottomCenter</t>
   </si>
   <si>
-    <t>Bottom Center</t>
+    <t>Bottom Centre</t>
   </si>
   <si>
     <t>bottomRight</t>
@@ -1862,7 +1862,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="191">
+  <cellXfs count="190">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -2248,9 +2248,6 @@
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="14" fontId="0" borderId="25" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" borderId="19" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="0" borderId="26" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -4469,10 +4466,10 @@
       <c r="G29" t="s" s="86">
         <v>310</v>
       </c>
-      <c r="H29" s="129"/>
+      <c r="H29" s="85"/>
       <c r="I29" s="85"/>
       <c r="J29" s="85"/>
-      <c r="K29" t="s" s="130">
+      <c r="K29" t="s" s="129">
         <v>40</v>
       </c>
       <c r="L29" s="17"/>
@@ -4630,28 +4627,28 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="13" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="2" width="10.6719" style="131" customWidth="1"/>
-    <col min="3" max="3" width="20.3516" style="131" customWidth="1"/>
-    <col min="4" max="4" width="29.3516" style="131" customWidth="1"/>
-    <col min="5" max="10" width="10.6719" style="131" customWidth="1"/>
-    <col min="11" max="256" width="8.85156" style="131" customWidth="1"/>
+    <col min="1" max="2" width="10.6719" style="130" customWidth="1"/>
+    <col min="3" max="3" width="20.3516" style="130" customWidth="1"/>
+    <col min="4" max="4" width="29.3516" style="130" customWidth="1"/>
+    <col min="5" max="10" width="10.6719" style="130" customWidth="1"/>
+    <col min="11" max="256" width="8.85156" style="130" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="18" customHeight="1">
       <c r="A1" t="s" s="12">
         <v>321</v>
       </c>
-      <c r="B1" t="s" s="132">
+      <c r="B1" t="s" s="131">
         <v>11</v>
       </c>
-      <c r="C1" t="s" s="133">
+      <c r="C1" t="s" s="132">
         <v>12</v>
       </c>
-      <c r="D1" t="s" s="134">
+      <c r="D1" t="s" s="133">
         <v>13</v>
       </c>
-      <c r="E1" s="135"/>
-      <c r="F1" s="135"/>
+      <c r="E1" s="134"/>
+      <c r="F1" s="134"/>
       <c r="G1" s="17"/>
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
@@ -4676,10 +4673,10 @@
       <c r="F2" t="s" s="18">
         <v>324</v>
       </c>
-      <c r="G2" s="136"/>
-      <c r="H2" s="137"/>
-      <c r="I2" s="137"/>
-      <c r="J2" s="137"/>
+      <c r="G2" s="135"/>
+      <c r="H2" s="136"/>
+      <c r="I2" s="136"/>
+      <c r="J2" s="136"/>
     </row>
     <row r="3" ht="15" customHeight="1">
       <c r="A3" t="s" s="6">
@@ -4688,10 +4685,10 @@
       <c r="B3" t="s" s="6">
         <v>20</v>
       </c>
-      <c r="C3" t="s" s="138">
+      <c r="C3" t="s" s="137">
         <v>51</v>
       </c>
-      <c r="D3" t="s" s="138">
+      <c r="D3" t="s" s="137">
         <v>97</v>
       </c>
       <c r="E3" t="s" s="6">
@@ -4700,23 +4697,23 @@
       <c r="F3" t="s" s="6">
         <v>114</v>
       </c>
-      <c r="G3" s="139"/>
-      <c r="H3" s="140"/>
-      <c r="I3" s="140"/>
-      <c r="J3" s="140"/>
+      <c r="G3" s="138"/>
+      <c r="H3" s="139"/>
+      <c r="I3" s="139"/>
+      <c r="J3" s="139"/>
     </row>
     <row r="4" ht="15" customHeight="1">
       <c r="A4" s="24">
         <v>42736</v>
       </c>
-      <c r="B4" s="141"/>
+      <c r="B4" s="140"/>
       <c r="C4" t="s" s="37">
         <v>37</v>
       </c>
       <c r="D4" t="s" s="38">
         <v>59</v>
       </c>
-      <c r="E4" t="s" s="142">
+      <c r="E4" t="s" s="141">
         <v>325</v>
       </c>
       <c r="F4" s="96">
@@ -4846,8 +4843,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="13" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="16" width="10.6719" style="143" customWidth="1"/>
-    <col min="17" max="256" width="8.85156" style="143" customWidth="1"/>
+    <col min="1" max="16" width="10.6719" style="142" customWidth="1"/>
+    <col min="17" max="256" width="8.85156" style="142" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="18" customHeight="1">
@@ -4895,16 +4892,16 @@
       <c r="F2" t="s" s="18">
         <v>331</v>
       </c>
-      <c r="G2" s="136"/>
-      <c r="H2" s="137"/>
-      <c r="I2" s="137"/>
-      <c r="J2" s="137"/>
-      <c r="K2" s="137"/>
-      <c r="L2" s="137"/>
-      <c r="M2" s="137"/>
-      <c r="N2" s="137"/>
-      <c r="O2" s="137"/>
-      <c r="P2" s="137"/>
+      <c r="G2" s="135"/>
+      <c r="H2" s="136"/>
+      <c r="I2" s="136"/>
+      <c r="J2" s="136"/>
+      <c r="K2" s="136"/>
+      <c r="L2" s="136"/>
+      <c r="M2" s="136"/>
+      <c r="N2" s="136"/>
+      <c r="O2" s="136"/>
+      <c r="P2" s="136"/>
     </row>
     <row r="3" ht="15" customHeight="1">
       <c r="A3" t="s" s="6">
@@ -4913,10 +4910,10 @@
       <c r="B3" t="s" s="6">
         <v>20</v>
       </c>
-      <c r="C3" t="s" s="138">
+      <c r="C3" t="s" s="137">
         <v>51</v>
       </c>
-      <c r="D3" t="s" s="138">
+      <c r="D3" t="s" s="137">
         <v>97</v>
       </c>
       <c r="E3" t="s" s="6">
@@ -4925,29 +4922,29 @@
       <c r="F3" t="s" s="6">
         <v>114</v>
       </c>
-      <c r="G3" s="144"/>
-      <c r="H3" s="145"/>
-      <c r="I3" s="145"/>
-      <c r="J3" s="145"/>
-      <c r="K3" s="145"/>
-      <c r="L3" s="145"/>
-      <c r="M3" s="145"/>
-      <c r="N3" s="145"/>
-      <c r="O3" s="145"/>
-      <c r="P3" s="145"/>
+      <c r="G3" s="143"/>
+      <c r="H3" s="144"/>
+      <c r="I3" s="144"/>
+      <c r="J3" s="144"/>
+      <c r="K3" s="144"/>
+      <c r="L3" s="144"/>
+      <c r="M3" s="144"/>
+      <c r="N3" s="144"/>
+      <c r="O3" s="144"/>
+      <c r="P3" s="144"/>
     </row>
     <row r="4" ht="15" customHeight="1">
       <c r="A4" s="24">
         <v>42736</v>
       </c>
-      <c r="B4" s="141"/>
+      <c r="B4" s="140"/>
       <c r="C4" t="s" s="37">
         <v>37</v>
       </c>
       <c r="D4" t="s" s="38">
         <v>59</v>
       </c>
-      <c r="E4" t="s" s="142">
+      <c r="E4" t="s" s="141">
         <v>325</v>
       </c>
       <c r="F4" s="96">
@@ -5119,8 +5116,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="13" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="16" width="10.6719" style="146" customWidth="1"/>
-    <col min="17" max="256" width="8.85156" style="146" customWidth="1"/>
+    <col min="1" max="16" width="10.6719" style="145" customWidth="1"/>
+    <col min="17" max="256" width="8.85156" style="145" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="18" customHeight="1">
@@ -5168,16 +5165,16 @@
       <c r="F2" t="s" s="18">
         <v>331</v>
       </c>
-      <c r="G2" s="147"/>
-      <c r="H2" s="148"/>
-      <c r="I2" s="148"/>
-      <c r="J2" s="148"/>
-      <c r="K2" s="148"/>
-      <c r="L2" s="148"/>
-      <c r="M2" s="148"/>
-      <c r="N2" s="148"/>
-      <c r="O2" s="148"/>
-      <c r="P2" s="148"/>
+      <c r="G2" s="146"/>
+      <c r="H2" s="147"/>
+      <c r="I2" s="147"/>
+      <c r="J2" s="147"/>
+      <c r="K2" s="147"/>
+      <c r="L2" s="147"/>
+      <c r="M2" s="147"/>
+      <c r="N2" s="147"/>
+      <c r="O2" s="147"/>
+      <c r="P2" s="147"/>
     </row>
     <row r="3" ht="15" customHeight="1">
       <c r="A3" t="s" s="6">
@@ -5186,10 +5183,10 @@
       <c r="B3" t="s" s="6">
         <v>20</v>
       </c>
-      <c r="C3" t="s" s="138">
+      <c r="C3" t="s" s="137">
         <v>51</v>
       </c>
-      <c r="D3" t="s" s="138">
+      <c r="D3" t="s" s="137">
         <v>97</v>
       </c>
       <c r="E3" t="s" s="6">
@@ -5198,29 +5195,29 @@
       <c r="F3" t="s" s="6">
         <v>114</v>
       </c>
-      <c r="G3" s="144"/>
-      <c r="H3" s="145"/>
-      <c r="I3" s="145"/>
-      <c r="J3" s="145"/>
-      <c r="K3" s="145"/>
-      <c r="L3" s="145"/>
-      <c r="M3" s="145"/>
-      <c r="N3" s="145"/>
-      <c r="O3" s="145"/>
-      <c r="P3" s="145"/>
+      <c r="G3" s="143"/>
+      <c r="H3" s="144"/>
+      <c r="I3" s="144"/>
+      <c r="J3" s="144"/>
+      <c r="K3" s="144"/>
+      <c r="L3" s="144"/>
+      <c r="M3" s="144"/>
+      <c r="N3" s="144"/>
+      <c r="O3" s="144"/>
+      <c r="P3" s="144"/>
     </row>
     <row r="4" ht="15" customHeight="1">
       <c r="A4" s="24">
         <v>42736</v>
       </c>
-      <c r="B4" s="141"/>
+      <c r="B4" s="140"/>
       <c r="C4" t="s" s="37">
         <v>37</v>
       </c>
       <c r="D4" t="s" s="38">
         <v>59</v>
       </c>
-      <c r="E4" t="s" s="142">
+      <c r="E4" t="s" s="141">
         <v>325</v>
       </c>
       <c r="F4" s="96">
@@ -5392,25 +5389,25 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="13" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="10" width="10.6719" style="149" customWidth="1"/>
-    <col min="11" max="256" width="8.85156" style="149" customWidth="1"/>
+    <col min="1" max="10" width="10.6719" style="148" customWidth="1"/>
+    <col min="11" max="256" width="8.85156" style="148" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="19" customHeight="1">
-      <c r="A1" t="s" s="150">
+      <c r="A1" t="s" s="149">
         <v>333</v>
       </c>
-      <c r="B1" t="s" s="132">
+      <c r="B1" t="s" s="131">
         <v>11</v>
       </c>
-      <c r="C1" t="s" s="151">
+      <c r="C1" t="s" s="150">
         <v>12</v>
       </c>
-      <c r="D1" t="s" s="152">
+      <c r="D1" t="s" s="151">
         <v>13</v>
       </c>
-      <c r="E1" s="153"/>
-      <c r="F1" s="153"/>
+      <c r="E1" s="152"/>
+      <c r="F1" s="152"/>
       <c r="G1" s="17"/>
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
@@ -5435,10 +5432,10 @@
       <c r="F2" t="s" s="18">
         <v>324</v>
       </c>
-      <c r="G2" s="136"/>
-      <c r="H2" s="137"/>
-      <c r="I2" s="137"/>
-      <c r="J2" s="137"/>
+      <c r="G2" s="135"/>
+      <c r="H2" s="136"/>
+      <c r="I2" s="136"/>
+      <c r="J2" s="136"/>
     </row>
     <row r="3" ht="15" customHeight="1">
       <c r="A3" t="s" s="6">
@@ -5447,10 +5444,10 @@
       <c r="B3" t="s" s="6">
         <v>20</v>
       </c>
-      <c r="C3" t="s" s="138">
+      <c r="C3" t="s" s="137">
         <v>51</v>
       </c>
-      <c r="D3" t="s" s="138">
+      <c r="D3" t="s" s="137">
         <v>97</v>
       </c>
       <c r="E3" t="s" s="6">
@@ -5459,23 +5456,23 @@
       <c r="F3" t="s" s="6">
         <v>114</v>
       </c>
-      <c r="G3" s="139"/>
-      <c r="H3" s="140"/>
-      <c r="I3" s="140"/>
-      <c r="J3" s="140"/>
+      <c r="G3" s="138"/>
+      <c r="H3" s="139"/>
+      <c r="I3" s="139"/>
+      <c r="J3" s="139"/>
     </row>
     <row r="4" ht="15" customHeight="1">
       <c r="A4" s="24">
         <v>42736</v>
       </c>
-      <c r="B4" s="141"/>
+      <c r="B4" s="140"/>
       <c r="C4" t="s" s="37">
         <v>37</v>
       </c>
       <c r="D4" t="s" s="38">
         <v>59</v>
       </c>
-      <c r="E4" t="s" s="142">
+      <c r="E4" t="s" s="141">
         <v>325</v>
       </c>
       <c r="F4" s="96">
@@ -5605,8 +5602,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="13" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="16" width="10.6719" style="154" customWidth="1"/>
-    <col min="17" max="256" width="8.85156" style="154" customWidth="1"/>
+    <col min="1" max="16" width="10.6719" style="153" customWidth="1"/>
+    <col min="17" max="256" width="8.85156" style="153" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="18" customHeight="1">
@@ -5642,7 +5639,7 @@
       <c r="B2" t="s" s="18">
         <v>15</v>
       </c>
-      <c r="C2" s="155"/>
+      <c r="C2" s="154"/>
       <c r="D2" t="s" s="18">
         <v>335</v>
       </c>
@@ -5682,32 +5679,32 @@
       <c r="F3" t="s" s="30">
         <v>341</v>
       </c>
-      <c r="G3" s="156"/>
-      <c r="H3" s="157"/>
-      <c r="I3" s="157"/>
-      <c r="J3" s="157"/>
-      <c r="K3" s="157"/>
-      <c r="L3" s="157"/>
-      <c r="M3" s="157"/>
-      <c r="N3" s="157"/>
-      <c r="O3" s="157"/>
-      <c r="P3" s="157"/>
+      <c r="G3" s="155"/>
+      <c r="H3" s="156"/>
+      <c r="I3" s="156"/>
+      <c r="J3" s="156"/>
+      <c r="K3" s="156"/>
+      <c r="L3" s="156"/>
+      <c r="M3" s="156"/>
+      <c r="N3" s="156"/>
+      <c r="O3" s="156"/>
+      <c r="P3" s="156"/>
     </row>
     <row r="4" ht="13.65" customHeight="1">
       <c r="A4" s="123">
         <v>42736</v>
       </c>
       <c r="B4" s="114"/>
-      <c r="C4" t="s" s="158">
+      <c r="C4" t="s" s="157">
         <v>342</v>
       </c>
-      <c r="D4" t="s" s="159">
+      <c r="D4" t="s" s="158">
         <v>24</v>
       </c>
-      <c r="E4" t="s" s="160">
+      <c r="E4" t="s" s="159">
         <v>37</v>
       </c>
-      <c r="F4" t="s" s="160">
+      <c r="F4" t="s" s="159">
         <v>116</v>
       </c>
       <c r="G4" s="17"/>
@@ -5726,16 +5723,16 @@
         <v>42736</v>
       </c>
       <c r="B5" s="89"/>
-      <c r="C5" t="s" s="161">
+      <c r="C5" t="s" s="160">
         <v>343</v>
       </c>
-      <c r="D5" t="s" s="162">
+      <c r="D5" t="s" s="161">
         <v>24</v>
       </c>
-      <c r="E5" t="s" s="163">
+      <c r="E5" t="s" s="162">
         <v>37</v>
       </c>
-      <c r="F5" t="s" s="163">
+      <c r="F5" t="s" s="162">
         <v>116</v>
       </c>
       <c r="G5" s="17"/>
@@ -5754,16 +5751,16 @@
         <v>42736</v>
       </c>
       <c r="B6" s="89"/>
-      <c r="C6" t="s" s="161">
+      <c r="C6" t="s" s="160">
         <v>344</v>
       </c>
-      <c r="D6" t="s" s="162">
+      <c r="D6" t="s" s="161">
         <v>24</v>
       </c>
-      <c r="E6" t="s" s="163">
+      <c r="E6" t="s" s="162">
         <v>37</v>
       </c>
-      <c r="F6" t="s" s="163">
+      <c r="F6" t="s" s="162">
         <v>116</v>
       </c>
       <c r="G6" s="17"/>
@@ -5782,16 +5779,16 @@
         <v>42736</v>
       </c>
       <c r="B7" s="119"/>
-      <c r="C7" t="s" s="164">
+      <c r="C7" t="s" s="163">
         <v>345</v>
       </c>
-      <c r="D7" t="s" s="165">
+      <c r="D7" t="s" s="164">
         <v>24</v>
       </c>
-      <c r="E7" t="s" s="166">
+      <c r="E7" t="s" s="165">
         <v>37</v>
       </c>
-      <c r="F7" t="s" s="166">
+      <c r="F7" t="s" s="165">
         <v>116</v>
       </c>
       <c r="G7" s="17"/>
@@ -5809,8 +5806,8 @@
       <c r="A8" s="128">
         <v>42736</v>
       </c>
-      <c r="B8" s="167"/>
-      <c r="C8" t="s" s="168">
+      <c r="B8" s="166"/>
+      <c r="C8" t="s" s="167">
         <v>346</v>
       </c>
       <c r="D8" t="s" s="13">
@@ -5886,8 +5883,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="13" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="15" width="10.6719" style="169" customWidth="1"/>
-    <col min="16" max="256" width="8.85156" style="169" customWidth="1"/>
+    <col min="1" max="15" width="10.6719" style="168" customWidth="1"/>
+    <col min="16" max="256" width="8.85156" style="168" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="18" customHeight="1">
@@ -5931,16 +5928,16 @@
       <c r="E2" t="s" s="18">
         <v>350</v>
       </c>
-      <c r="F2" s="147"/>
-      <c r="G2" s="148"/>
-      <c r="H2" s="148"/>
-      <c r="I2" s="148"/>
-      <c r="J2" s="148"/>
-      <c r="K2" s="148"/>
-      <c r="L2" s="148"/>
-      <c r="M2" s="148"/>
-      <c r="N2" s="148"/>
-      <c r="O2" s="148"/>
+      <c r="F2" s="146"/>
+      <c r="G2" s="147"/>
+      <c r="H2" s="147"/>
+      <c r="I2" s="147"/>
+      <c r="J2" s="147"/>
+      <c r="K2" s="147"/>
+      <c r="L2" s="147"/>
+      <c r="M2" s="147"/>
+      <c r="N2" s="147"/>
+      <c r="O2" s="147"/>
     </row>
     <row r="3" ht="13.65" customHeight="1">
       <c r="A3" t="s" s="6">
@@ -5973,14 +5970,14 @@
       <c r="A4" s="128">
         <v>42736</v>
       </c>
-      <c r="B4" s="170"/>
+      <c r="B4" s="169"/>
       <c r="C4" t="s" s="70">
         <v>37</v>
       </c>
       <c r="D4" t="s" s="54">
         <v>353</v>
       </c>
-      <c r="E4" t="s" s="171">
+      <c r="E4" t="s" s="170">
         <v>352</v>
       </c>
       <c r="F4" s="17"/>
@@ -6113,11 +6110,11 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="13" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="3" width="10.6719" style="172" customWidth="1"/>
-    <col min="4" max="4" width="19.1719" style="172" customWidth="1"/>
-    <col min="5" max="5" width="31.1719" style="172" customWidth="1"/>
-    <col min="6" max="15" width="10.6719" style="172" customWidth="1"/>
-    <col min="16" max="256" width="8.85156" style="172" customWidth="1"/>
+    <col min="1" max="3" width="10.6719" style="171" customWidth="1"/>
+    <col min="4" max="4" width="19.1719" style="171" customWidth="1"/>
+    <col min="5" max="5" width="31.1719" style="171" customWidth="1"/>
+    <col min="6" max="15" width="10.6719" style="171" customWidth="1"/>
+    <col min="16" max="256" width="8.85156" style="171" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="18" customHeight="1">
@@ -6208,16 +6205,16 @@
         <v>42736</v>
       </c>
       <c r="B4" s="114"/>
-      <c r="C4" t="s" s="173">
+      <c r="C4" t="s" s="172">
         <v>37</v>
       </c>
       <c r="D4" t="s" s="38">
         <v>59</v>
       </c>
-      <c r="E4" t="s" s="174">
+      <c r="E4" t="s" s="173">
         <v>353</v>
       </c>
-      <c r="F4" t="s" s="171">
+      <c r="F4" t="s" s="170">
         <v>352</v>
       </c>
       <c r="G4" s="17"/>
@@ -6235,16 +6232,16 @@
         <v>42736</v>
       </c>
       <c r="B5" s="89"/>
-      <c r="C5" t="s" s="175">
+      <c r="C5" t="s" s="174">
         <v>37</v>
       </c>
       <c r="D5" t="s" s="43">
         <v>62</v>
       </c>
-      <c r="E5" t="s" s="176">
+      <c r="E5" t="s" s="175">
         <v>353</v>
       </c>
-      <c r="F5" t="s" s="171">
+      <c r="F5" t="s" s="170">
         <v>352</v>
       </c>
       <c r="G5" s="17"/>
@@ -6262,16 +6259,16 @@
         <v>42736</v>
       </c>
       <c r="B6" s="89"/>
-      <c r="C6" t="s" s="175">
+      <c r="C6" t="s" s="174">
         <v>37</v>
       </c>
       <c r="D6" t="s" s="43">
         <v>64</v>
       </c>
-      <c r="E6" t="s" s="176">
+      <c r="E6" t="s" s="175">
         <v>353</v>
       </c>
-      <c r="F6" t="s" s="171">
+      <c r="F6" t="s" s="170">
         <v>352</v>
       </c>
       <c r="G6" s="17"/>
@@ -6289,16 +6286,16 @@
         <v>42736</v>
       </c>
       <c r="B7" s="89"/>
-      <c r="C7" t="s" s="175">
+      <c r="C7" t="s" s="174">
         <v>37</v>
       </c>
       <c r="D7" t="s" s="43">
         <v>66</v>
       </c>
-      <c r="E7" t="s" s="176">
+      <c r="E7" t="s" s="175">
         <v>353</v>
       </c>
-      <c r="F7" t="s" s="171">
+      <c r="F7" t="s" s="170">
         <v>352</v>
       </c>
       <c r="G7" s="17"/>
@@ -6316,16 +6313,16 @@
         <v>42736</v>
       </c>
       <c r="B8" s="89"/>
-      <c r="C8" t="s" s="175">
+      <c r="C8" t="s" s="174">
         <v>37</v>
       </c>
       <c r="D8" t="s" s="43">
         <v>68</v>
       </c>
-      <c r="E8" t="s" s="176">
+      <c r="E8" t="s" s="175">
         <v>353</v>
       </c>
-      <c r="F8" t="s" s="171">
+      <c r="F8" t="s" s="170">
         <v>352</v>
       </c>
       <c r="G8" s="17"/>
@@ -6343,16 +6340,16 @@
         <v>42736</v>
       </c>
       <c r="B9" s="89"/>
-      <c r="C9" t="s" s="175">
+      <c r="C9" t="s" s="174">
         <v>37</v>
       </c>
       <c r="D9" t="s" s="43">
         <v>71</v>
       </c>
-      <c r="E9" t="s" s="176">
+      <c r="E9" t="s" s="175">
         <v>353</v>
       </c>
-      <c r="F9" t="s" s="171">
+      <c r="F9" t="s" s="170">
         <v>352</v>
       </c>
       <c r="G9" s="17"/>
@@ -6370,16 +6367,16 @@
         <v>42736</v>
       </c>
       <c r="B10" s="89"/>
-      <c r="C10" t="s" s="175">
+      <c r="C10" t="s" s="174">
         <v>37</v>
       </c>
       <c r="D10" t="s" s="47">
         <v>75</v>
       </c>
-      <c r="E10" t="s" s="176">
+      <c r="E10" t="s" s="175">
         <v>353</v>
       </c>
-      <c r="F10" t="s" s="171">
+      <c r="F10" t="s" s="170">
         <v>352</v>
       </c>
       <c r="G10" s="17"/>
@@ -6397,16 +6394,16 @@
         <v>42736</v>
       </c>
       <c r="B11" s="89"/>
-      <c r="C11" t="s" s="175">
+      <c r="C11" t="s" s="174">
         <v>37</v>
       </c>
       <c r="D11" t="s" s="47">
         <v>80</v>
       </c>
-      <c r="E11" t="s" s="176">
+      <c r="E11" t="s" s="175">
         <v>353</v>
       </c>
-      <c r="F11" t="s" s="171">
+      <c r="F11" t="s" s="170">
         <v>352</v>
       </c>
       <c r="G11" s="17"/>
@@ -6427,13 +6424,13 @@
       <c r="C12" t="s" s="116">
         <v>37</v>
       </c>
-      <c r="D12" t="s" s="177">
+      <c r="D12" t="s" s="176">
         <v>83</v>
       </c>
-      <c r="E12" t="s" s="178">
+      <c r="E12" t="s" s="177">
         <v>353</v>
       </c>
-      <c r="F12" t="s" s="171">
+      <c r="F12" t="s" s="170">
         <v>352</v>
       </c>
       <c r="G12" s="17"/>
@@ -6463,8 +6460,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="13" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="15" width="10.6719" style="179" customWidth="1"/>
-    <col min="16" max="256" width="8.85156" style="179" customWidth="1"/>
+    <col min="1" max="15" width="10.6719" style="178" customWidth="1"/>
+    <col min="16" max="256" width="8.85156" style="178" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="18" customHeight="1">
@@ -6528,13 +6525,13 @@
       <c r="B3" t="s" s="110">
         <v>20</v>
       </c>
-      <c r="C3" t="s" s="180">
+      <c r="C3" t="s" s="179">
         <v>51</v>
       </c>
-      <c r="D3" t="s" s="180">
+      <c r="D3" t="s" s="179">
         <v>191</v>
       </c>
-      <c r="E3" t="s" s="180">
+      <c r="E3" t="s" s="179">
         <v>351</v>
       </c>
       <c r="F3" t="s" s="110">
@@ -6551,20 +6548,20 @@
       <c r="O3" s="113"/>
     </row>
     <row r="4" ht="28" customHeight="1">
-      <c r="A4" s="181">
+      <c r="A4" s="180">
         <v>42736</v>
       </c>
       <c r="B4" s="78"/>
-      <c r="C4" t="s" s="160">
+      <c r="C4" t="s" s="159">
         <v>37</v>
       </c>
       <c r="D4" t="s" s="75">
         <v>144</v>
       </c>
-      <c r="E4" t="s" s="182">
+      <c r="E4" t="s" s="181">
         <v>353</v>
       </c>
-      <c r="F4" t="s" s="171">
+      <c r="F4" t="s" s="170">
         <v>352</v>
       </c>
       <c r="G4" s="17"/>
@@ -6578,20 +6575,20 @@
       <c r="O4" s="3"/>
     </row>
     <row r="5" ht="28" customHeight="1">
-      <c r="A5" s="183">
+      <c r="A5" s="182">
         <v>42736</v>
       </c>
       <c r="B5" s="83"/>
-      <c r="C5" t="s" s="163">
+      <c r="C5" t="s" s="162">
         <v>37</v>
       </c>
       <c r="D5" t="s" s="75">
         <v>148</v>
       </c>
-      <c r="E5" t="s" s="184">
+      <c r="E5" t="s" s="183">
         <v>353</v>
       </c>
-      <c r="F5" t="s" s="171">
+      <c r="F5" t="s" s="170">
         <v>352</v>
       </c>
       <c r="G5" s="17"/>
@@ -6605,20 +6602,20 @@
       <c r="O5" s="3"/>
     </row>
     <row r="6" ht="28" customHeight="1">
-      <c r="A6" s="183">
+      <c r="A6" s="182">
         <v>42736</v>
       </c>
       <c r="B6" s="83"/>
-      <c r="C6" t="s" s="163">
+      <c r="C6" t="s" s="162">
         <v>37</v>
       </c>
       <c r="D6" t="s" s="75">
         <v>152</v>
       </c>
-      <c r="E6" t="s" s="184">
+      <c r="E6" t="s" s="183">
         <v>353</v>
       </c>
-      <c r="F6" t="s" s="171">
+      <c r="F6" t="s" s="170">
         <v>352</v>
       </c>
       <c r="G6" s="17"/>
@@ -6632,20 +6629,20 @@
       <c r="O6" s="3"/>
     </row>
     <row r="7" ht="28" customHeight="1">
-      <c r="A7" s="183">
+      <c r="A7" s="182">
         <v>42736</v>
       </c>
       <c r="B7" s="83"/>
-      <c r="C7" t="s" s="163">
+      <c r="C7" t="s" s="162">
         <v>37</v>
       </c>
       <c r="D7" t="s" s="75">
         <v>156</v>
       </c>
-      <c r="E7" t="s" s="184">
+      <c r="E7" t="s" s="183">
         <v>353</v>
       </c>
-      <c r="F7" t="s" s="171">
+      <c r="F7" t="s" s="170">
         <v>352</v>
       </c>
       <c r="G7" s="17"/>
@@ -6659,20 +6656,20 @@
       <c r="O7" s="3"/>
     </row>
     <row r="8" ht="28" customHeight="1">
-      <c r="A8" s="183">
+      <c r="A8" s="182">
         <v>42736</v>
       </c>
       <c r="B8" s="83"/>
-      <c r="C8" t="s" s="163">
+      <c r="C8" t="s" s="162">
         <v>37</v>
       </c>
       <c r="D8" t="s" s="75">
         <v>163</v>
       </c>
-      <c r="E8" t="s" s="184">
+      <c r="E8" t="s" s="183">
         <v>353</v>
       </c>
-      <c r="F8" t="s" s="171">
+      <c r="F8" t="s" s="170">
         <v>352</v>
       </c>
       <c r="G8" s="17"/>
@@ -6686,20 +6683,20 @@
       <c r="O8" s="3"/>
     </row>
     <row r="9" ht="28" customHeight="1">
-      <c r="A9" s="183">
+      <c r="A9" s="182">
         <v>42736</v>
       </c>
       <c r="B9" s="83"/>
-      <c r="C9" t="s" s="163">
+      <c r="C9" t="s" s="162">
         <v>37</v>
       </c>
       <c r="D9" t="s" s="75">
         <v>159</v>
       </c>
-      <c r="E9" t="s" s="184">
+      <c r="E9" t="s" s="183">
         <v>353</v>
       </c>
-      <c r="F9" t="s" s="171">
+      <c r="F9" t="s" s="170">
         <v>352</v>
       </c>
       <c r="G9" s="17"/>
@@ -6713,20 +6710,20 @@
       <c r="O9" s="3"/>
     </row>
     <row r="10" ht="28" customHeight="1">
-      <c r="A10" s="183">
+      <c r="A10" s="182">
         <v>42736</v>
       </c>
       <c r="B10" s="83"/>
-      <c r="C10" t="s" s="163">
+      <c r="C10" t="s" s="162">
         <v>37</v>
       </c>
       <c r="D10" t="s" s="75">
         <v>167</v>
       </c>
-      <c r="E10" t="s" s="184">
+      <c r="E10" t="s" s="183">
         <v>353</v>
       </c>
-      <c r="F10" t="s" s="171">
+      <c r="F10" t="s" s="170">
         <v>352</v>
       </c>
       <c r="G10" s="17"/>
@@ -6740,20 +6737,20 @@
       <c r="O10" s="3"/>
     </row>
     <row r="11" ht="28" customHeight="1">
-      <c r="A11" s="183">
+      <c r="A11" s="182">
         <v>42736</v>
       </c>
       <c r="B11" s="83"/>
-      <c r="C11" t="s" s="163">
+      <c r="C11" t="s" s="162">
         <v>37</v>
       </c>
       <c r="D11" t="s" s="75">
         <v>174</v>
       </c>
-      <c r="E11" t="s" s="184">
+      <c r="E11" t="s" s="183">
         <v>353</v>
       </c>
-      <c r="F11" t="s" s="171">
+      <c r="F11" t="s" s="170">
         <v>352</v>
       </c>
       <c r="G11" s="17"/>
@@ -6767,20 +6764,20 @@
       <c r="O11" s="3"/>
     </row>
     <row r="12" ht="28" customHeight="1">
-      <c r="A12" s="183">
+      <c r="A12" s="182">
         <v>42736</v>
       </c>
       <c r="B12" s="83"/>
-      <c r="C12" t="s" s="163">
+      <c r="C12" t="s" s="162">
         <v>37</v>
       </c>
       <c r="D12" t="s" s="75">
         <v>177</v>
       </c>
-      <c r="E12" t="s" s="184">
+      <c r="E12" t="s" s="183">
         <v>353</v>
       </c>
-      <c r="F12" t="s" s="171">
+      <c r="F12" t="s" s="170">
         <v>352</v>
       </c>
       <c r="G12" s="17"/>
@@ -6794,12 +6791,12 @@
       <c r="O12" s="3"/>
     </row>
     <row r="13" ht="13.65" customHeight="1">
-      <c r="A13" s="185"/>
-      <c r="B13" s="186"/>
-      <c r="C13" s="186"/>
+      <c r="A13" s="184"/>
+      <c r="B13" s="185"/>
+      <c r="C13" s="185"/>
       <c r="D13" s="90"/>
-      <c r="E13" s="187"/>
-      <c r="F13" s="188"/>
+      <c r="E13" s="186"/>
+      <c r="F13" s="187"/>
       <c r="G13" s="17"/>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
@@ -6844,8 +6841,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="13" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="16" width="10.6719" style="189" customWidth="1"/>
-    <col min="17" max="256" width="8.85156" style="189" customWidth="1"/>
+    <col min="1" max="16" width="10.6719" style="188" customWidth="1"/>
+    <col min="17" max="256" width="8.85156" style="188" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="18" customHeight="1">
@@ -6911,13 +6908,13 @@
       <c r="B3" t="s" s="110">
         <v>20</v>
       </c>
-      <c r="C3" t="s" s="180">
+      <c r="C3" t="s" s="179">
         <v>51</v>
       </c>
-      <c r="D3" t="s" s="180">
+      <c r="D3" t="s" s="179">
         <v>361</v>
       </c>
-      <c r="E3" t="s" s="180">
+      <c r="E3" t="s" s="179">
         <v>351</v>
       </c>
       <c r="F3" t="s" s="110">
@@ -6938,7 +6935,7 @@
       <c r="A4" s="128">
         <v>42736</v>
       </c>
-      <c r="B4" s="167"/>
+      <c r="B4" s="166"/>
       <c r="C4" t="s" s="70">
         <v>37</v>
       </c>
@@ -6948,7 +6945,7 @@
       <c r="E4" t="s" s="54">
         <v>353</v>
       </c>
-      <c r="F4" t="s" s="171">
+      <c r="F4" t="s" s="170">
         <v>352</v>
       </c>
       <c r="G4" s="17"/>
@@ -7314,10 +7311,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="13" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="4" width="11.5" style="190" customWidth="1"/>
-    <col min="5" max="5" width="37.3516" style="190" customWidth="1"/>
-    <col min="6" max="7" width="11.5" style="190" customWidth="1"/>
-    <col min="8" max="256" width="8.85156" style="190" customWidth="1"/>
+    <col min="1" max="4" width="11.5" style="189" customWidth="1"/>
+    <col min="5" max="5" width="37.3516" style="189" customWidth="1"/>
+    <col min="6" max="7" width="11.5" style="189" customWidth="1"/>
+    <col min="8" max="256" width="8.85156" style="189" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="18" customHeight="1">
@@ -7338,8 +7335,8 @@
       <c r="G1" s="16"/>
     </row>
     <row r="2" ht="126" customHeight="1">
-      <c r="A2" s="155"/>
-      <c r="B2" s="155"/>
+      <c r="A2" s="154"/>
+      <c r="B2" s="154"/>
       <c r="C2" t="s" s="18">
         <v>355</v>
       </c>
@@ -7363,16 +7360,16 @@
       <c r="B3" t="s" s="110">
         <v>20</v>
       </c>
-      <c r="C3" t="s" s="180">
+      <c r="C3" t="s" s="179">
         <v>51</v>
       </c>
-      <c r="D3" t="s" s="180">
+      <c r="D3" t="s" s="179">
         <v>97</v>
       </c>
-      <c r="E3" t="s" s="180">
+      <c r="E3" t="s" s="179">
         <v>214</v>
       </c>
-      <c r="F3" t="s" s="180">
+      <c r="F3" t="s" s="179">
         <v>351</v>
       </c>
       <c r="G3" t="s" s="110">
@@ -7383,20 +7380,20 @@
       <c r="A4" s="128">
         <v>42736</v>
       </c>
-      <c r="B4" s="167"/>
+      <c r="B4" s="166"/>
       <c r="C4" t="s" s="70">
         <v>37</v>
       </c>
       <c r="D4" t="s" s="70">
         <v>75</v>
       </c>
-      <c r="E4" t="s" s="160">
+      <c r="E4" t="s" s="159">
         <v>285</v>
       </c>
       <c r="F4" t="s" s="54">
         <v>353</v>
       </c>
-      <c r="G4" t="s" s="171">
+      <c r="G4" t="s" s="170">
         <v>352</v>
       </c>
     </row>
@@ -7404,20 +7401,20 @@
       <c r="A5" s="128">
         <v>42736</v>
       </c>
-      <c r="B5" s="167"/>
+      <c r="B5" s="166"/>
       <c r="C5" t="s" s="70">
         <v>37</v>
       </c>
       <c r="D5" t="s" s="70">
         <v>75</v>
       </c>
-      <c r="E5" t="s" s="163">
+      <c r="E5" t="s" s="162">
         <v>287</v>
       </c>
       <c r="F5" t="s" s="54">
         <v>353</v>
       </c>
-      <c r="G5" t="s" s="171">
+      <c r="G5" t="s" s="170">
         <v>352</v>
       </c>
     </row>
@@ -7425,20 +7422,20 @@
       <c r="A6" s="128">
         <v>42736</v>
       </c>
-      <c r="B6" s="167"/>
+      <c r="B6" s="166"/>
       <c r="C6" t="s" s="70">
         <v>37</v>
       </c>
       <c r="D6" t="s" s="70">
         <v>75</v>
       </c>
-      <c r="E6" t="s" s="163">
+      <c r="E6" t="s" s="162">
         <v>273</v>
       </c>
       <c r="F6" t="s" s="54">
         <v>353</v>
       </c>
-      <c r="G6" t="s" s="171">
+      <c r="G6" t="s" s="170">
         <v>352</v>
       </c>
     </row>
@@ -7446,20 +7443,20 @@
       <c r="A7" s="128">
         <v>42736</v>
       </c>
-      <c r="B7" s="167"/>
+      <c r="B7" s="166"/>
       <c r="C7" t="s" s="70">
         <v>37</v>
       </c>
       <c r="D7" t="s" s="70">
         <v>75</v>
       </c>
-      <c r="E7" t="s" s="163">
+      <c r="E7" t="s" s="162">
         <v>289</v>
       </c>
       <c r="F7" t="s" s="54">
         <v>353</v>
       </c>
-      <c r="G7" t="s" s="171">
+      <c r="G7" t="s" s="170">
         <v>352</v>
       </c>
     </row>
@@ -7467,20 +7464,20 @@
       <c r="A8" s="128">
         <v>42736</v>
       </c>
-      <c r="B8" s="167"/>
+      <c r="B8" s="166"/>
       <c r="C8" t="s" s="70">
         <v>37</v>
       </c>
       <c r="D8" t="s" s="70">
         <v>75</v>
       </c>
-      <c r="E8" t="s" s="163">
+      <c r="E8" t="s" s="162">
         <v>292</v>
       </c>
       <c r="F8" t="s" s="54">
         <v>353</v>
       </c>
-      <c r="G8" t="s" s="171">
+      <c r="G8" t="s" s="170">
         <v>352</v>
       </c>
     </row>
@@ -7488,20 +7485,20 @@
       <c r="A9" s="128">
         <v>42736</v>
       </c>
-      <c r="B9" s="167"/>
+      <c r="B9" s="166"/>
       <c r="C9" t="s" s="70">
         <v>37</v>
       </c>
       <c r="D9" t="s" s="70">
         <v>75</v>
       </c>
-      <c r="E9" t="s" s="163">
+      <c r="E9" t="s" s="162">
         <v>279</v>
       </c>
       <c r="F9" t="s" s="54">
         <v>353</v>
       </c>
-      <c r="G9" t="s" s="171">
+      <c r="G9" t="s" s="170">
         <v>352</v>
       </c>
     </row>
@@ -7509,20 +7506,20 @@
       <c r="A10" s="128">
         <v>42736</v>
       </c>
-      <c r="B10" s="167"/>
+      <c r="B10" s="166"/>
       <c r="C10" t="s" s="70">
         <v>37</v>
       </c>
       <c r="D10" t="s" s="70">
         <v>75</v>
       </c>
-      <c r="E10" t="s" s="163">
+      <c r="E10" t="s" s="162">
         <v>283</v>
       </c>
       <c r="F10" t="s" s="54">
         <v>353</v>
       </c>
-      <c r="G10" t="s" s="171">
+      <c r="G10" t="s" s="170">
         <v>352</v>
       </c>
     </row>
@@ -7530,20 +7527,20 @@
       <c r="A11" s="128">
         <v>42736</v>
       </c>
-      <c r="B11" s="167"/>
+      <c r="B11" s="166"/>
       <c r="C11" t="s" s="70">
         <v>37</v>
       </c>
       <c r="D11" t="s" s="70">
         <v>75</v>
       </c>
-      <c r="E11" t="s" s="163">
+      <c r="E11" t="s" s="162">
         <v>296</v>
       </c>
       <c r="F11" t="s" s="54">
         <v>353</v>
       </c>
-      <c r="G11" t="s" s="171">
+      <c r="G11" t="s" s="170">
         <v>352</v>
       </c>
     </row>
@@ -7551,20 +7548,20 @@
       <c r="A12" s="128">
         <v>42736</v>
       </c>
-      <c r="B12" s="167"/>
+      <c r="B12" s="166"/>
       <c r="C12" t="s" s="70">
         <v>37</v>
       </c>
       <c r="D12" t="s" s="70">
         <v>75</v>
       </c>
-      <c r="E12" t="s" s="163">
+      <c r="E12" t="s" s="162">
         <v>298</v>
       </c>
       <c r="F12" t="s" s="54">
         <v>353</v>
       </c>
-      <c r="G12" t="s" s="171">
+      <c r="G12" t="s" s="170">
         <v>352</v>
       </c>
     </row>
@@ -7572,20 +7569,20 @@
       <c r="A13" s="128">
         <v>42736</v>
       </c>
-      <c r="B13" s="167"/>
+      <c r="B13" s="166"/>
       <c r="C13" t="s" s="70">
         <v>37</v>
       </c>
       <c r="D13" t="s" s="70">
         <v>75</v>
       </c>
-      <c r="E13" t="s" s="163">
+      <c r="E13" t="s" s="162">
         <v>300</v>
       </c>
       <c r="F13" t="s" s="54">
         <v>353</v>
       </c>
-      <c r="G13" t="s" s="171">
+      <c r="G13" t="s" s="170">
         <v>352</v>
       </c>
     </row>
@@ -7593,20 +7590,20 @@
       <c r="A14" s="128">
         <v>42736</v>
       </c>
-      <c r="B14" s="167"/>
+      <c r="B14" s="166"/>
       <c r="C14" t="s" s="70">
         <v>37</v>
       </c>
       <c r="D14" t="s" s="70">
         <v>75</v>
       </c>
-      <c r="E14" t="s" s="163">
+      <c r="E14" t="s" s="162">
         <v>304</v>
       </c>
       <c r="F14" t="s" s="54">
         <v>353</v>
       </c>
-      <c r="G14" t="s" s="171">
+      <c r="G14" t="s" s="170">
         <v>352</v>
       </c>
     </row>
@@ -7614,20 +7611,20 @@
       <c r="A15" s="128">
         <v>42736</v>
       </c>
-      <c r="B15" s="167"/>
+      <c r="B15" s="166"/>
       <c r="C15" t="s" s="70">
         <v>37</v>
       </c>
       <c r="D15" t="s" s="70">
         <v>75</v>
       </c>
-      <c r="E15" t="s" s="163">
+      <c r="E15" t="s" s="162">
         <v>302</v>
       </c>
       <c r="F15" t="s" s="54">
         <v>353</v>
       </c>
-      <c r="G15" t="s" s="171">
+      <c r="G15" t="s" s="170">
         <v>352</v>
       </c>
     </row>
@@ -7635,20 +7632,20 @@
       <c r="A16" s="128">
         <v>42736</v>
       </c>
-      <c r="B16" s="167"/>
+      <c r="B16" s="166"/>
       <c r="C16" t="s" s="70">
         <v>37</v>
       </c>
       <c r="D16" t="s" s="70">
         <v>75</v>
       </c>
-      <c r="E16" t="s" s="163">
+      <c r="E16" t="s" s="162">
         <v>306</v>
       </c>
       <c r="F16" t="s" s="54">
         <v>353</v>
       </c>
-      <c r="G16" t="s" s="171">
+      <c r="G16" t="s" s="170">
         <v>352</v>
       </c>
     </row>
@@ -7656,20 +7653,20 @@
       <c r="A17" s="128">
         <v>42736</v>
       </c>
-      <c r="B17" s="167"/>
+      <c r="B17" s="166"/>
       <c r="C17" t="s" s="70">
         <v>37</v>
       </c>
       <c r="D17" t="s" s="70">
         <v>75</v>
       </c>
-      <c r="E17" t="s" s="166">
+      <c r="E17" t="s" s="165">
         <v>308</v>
       </c>
       <c r="F17" t="s" s="54">
         <v>353</v>
       </c>
-      <c r="G17" t="s" s="171">
+      <c r="G17" t="s" s="170">
         <v>352</v>
       </c>
     </row>
@@ -7677,20 +7674,20 @@
       <c r="A18" s="128">
         <v>42736</v>
       </c>
-      <c r="B18" s="167"/>
+      <c r="B18" s="166"/>
       <c r="C18" t="s" s="70">
         <v>37</v>
       </c>
       <c r="D18" t="s" s="70">
         <v>80</v>
       </c>
-      <c r="E18" t="s" s="160">
+      <c r="E18" t="s" s="159">
         <v>311</v>
       </c>
       <c r="F18" t="s" s="54">
         <v>353</v>
       </c>
-      <c r="G18" t="s" s="171">
+      <c r="G18" t="s" s="170">
         <v>352</v>
       </c>
     </row>
@@ -7698,20 +7695,20 @@
       <c r="A19" s="128">
         <v>42736</v>
       </c>
-      <c r="B19" s="167"/>
+      <c r="B19" s="166"/>
       <c r="C19" t="s" s="70">
         <v>37</v>
       </c>
       <c r="D19" t="s" s="70">
         <v>80</v>
       </c>
-      <c r="E19" t="s" s="163">
+      <c r="E19" t="s" s="162">
         <v>313</v>
       </c>
       <c r="F19" t="s" s="54">
         <v>353</v>
       </c>
-      <c r="G19" t="s" s="171">
+      <c r="G19" t="s" s="170">
         <v>352</v>
       </c>
     </row>
@@ -7719,20 +7716,20 @@
       <c r="A20" s="128">
         <v>42736</v>
       </c>
-      <c r="B20" s="167"/>
+      <c r="B20" s="166"/>
       <c r="C20" t="s" s="70">
         <v>37</v>
       </c>
       <c r="D20" t="s" s="70">
         <v>80</v>
       </c>
-      <c r="E20" t="s" s="163">
+      <c r="E20" t="s" s="162">
         <v>315</v>
       </c>
       <c r="F20" t="s" s="54">
         <v>353</v>
       </c>
-      <c r="G20" t="s" s="171">
+      <c r="G20" t="s" s="170">
         <v>352</v>
       </c>
     </row>
@@ -7740,20 +7737,20 @@
       <c r="A21" s="128">
         <v>42736</v>
       </c>
-      <c r="B21" s="167"/>
+      <c r="B21" s="166"/>
       <c r="C21" t="s" s="70">
         <v>37</v>
       </c>
       <c r="D21" t="s" s="70">
         <v>80</v>
       </c>
-      <c r="E21" t="s" s="163">
+      <c r="E21" t="s" s="162">
         <v>316</v>
       </c>
       <c r="F21" t="s" s="54">
         <v>353</v>
       </c>
-      <c r="G21" t="s" s="171">
+      <c r="G21" t="s" s="170">
         <v>352</v>
       </c>
     </row>
@@ -7761,20 +7758,20 @@
       <c r="A22" s="128">
         <v>42736</v>
       </c>
-      <c r="B22" s="167"/>
+      <c r="B22" s="166"/>
       <c r="C22" t="s" s="70">
         <v>37</v>
       </c>
       <c r="D22" t="s" s="70">
         <v>80</v>
       </c>
-      <c r="E22" t="s" s="166">
+      <c r="E22" t="s" s="165">
         <v>319</v>
       </c>
       <c r="F22" t="s" s="54">
         <v>353</v>
       </c>
-      <c r="G22" t="s" s="171">
+      <c r="G22" t="s" s="170">
         <v>352</v>
       </c>
     </row>
@@ -12715,7 +12712,7 @@
     </row>
     <row r="4" ht="14" customHeight="1">
       <c r="A4" s="24">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B4" s="33"/>
       <c r="C4" t="s" s="69">
@@ -14639,9 +14636,9 @@
     <row r="25" ht="13.65" customHeight="1">
       <c r="A25" s="41"/>
       <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
+      <c r="C25" s="46"/>
+      <c r="D25" s="46"/>
+      <c r="E25" s="46"/>
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>

</xml_diff>

<commit_message>
EM-2142: Update CCD definition spreadsheet to include Jamils SSCS file
</commit_message>
<xml_diff>
--- a/src/aat/resources/adv_bundling_functional_tests_ccd_def.xlsx
+++ b/src/aat/resources/adv_bundling_functional_tests_ccd_def.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="365">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="367">
   <si>
     <t>Change History</t>
   </si>
@@ -843,6 +843,12 @@
   </si>
   <si>
     <t>Tests – Config uses an invalid documentSet property</t>
+  </si>
+  <si>
+    <t>sscs-demo-bundle.yaml</t>
+  </si>
+  <si>
+    <t>SSCS Demo Bundle</t>
   </si>
   <si>
     <t>paginationStyle</t>
@@ -1400,7 +1406,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="10"/>
+        <fgColor indexed="9"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
@@ -1439,28 +1445,28 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="hair">
         <color indexed="8"/>
@@ -1484,16 +1490,16 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="hair">
         <color indexed="8"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1502,26 +1508,26 @@
         <color indexed="8"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right/>
       <top style="hair">
         <color indexed="8"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1537,26 +1543,26 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="hair">
         <color indexed="8"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1570,26 +1576,26 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1598,13 +1604,13 @@
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="hair">
         <color indexed="8"/>
@@ -1613,7 +1619,7 @@
         <color indexed="8"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1622,13 +1628,13 @@
         <color indexed="8"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="hair">
         <color indexed="8"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1643,22 +1649,22 @@
         <color indexed="8"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="hair">
         <color indexed="8"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1670,19 +1676,19 @@
         <color indexed="8"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="hair">
         <color indexed="8"/>
@@ -1731,13 +1737,13 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="hair">
         <color indexed="8"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="hair">
         <color indexed="8"/>
@@ -1749,10 +1755,10 @@
         <color indexed="8"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="hair">
         <color indexed="8"/>
@@ -1764,7 +1770,7 @@
         <color indexed="8"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="hair">
         <color indexed="8"/>
@@ -1776,7 +1782,7 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="hair">
         <color indexed="8"/>
@@ -1797,7 +1803,7 @@
         <color indexed="8"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="hair">
         <color indexed="8"/>
@@ -1813,7 +1819,7 @@
         <color indexed="8"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1826,7 +1832,7 @@
         <color indexed="8"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1836,10 +1842,10 @@
       </left>
       <right/>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1849,10 +1855,10 @@
         <color indexed="8"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1869,61 +1875,61 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="59" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="59" fontId="0" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="6" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="7" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="8" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="9" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="9" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="10" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1935,13 +1941,13 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="60" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="60" fontId="0" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="6" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
@@ -1959,10 +1965,10 @@
     <xf numFmtId="49" fontId="4" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
@@ -1974,7 +1980,7 @@
     <xf numFmtId="49" fontId="10" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1983,13 +1989,13 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="14" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1998,10 +2004,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -2010,16 +2016,16 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="13" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="13" fillId="2" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="13" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
@@ -2031,31 +2037,31 @@
     <xf numFmtId="49" fontId="12" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="61" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="61" fontId="0" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="61" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="61" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -2070,16 +2076,16 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
@@ -2091,55 +2097,55 @@
     <xf numFmtId="49" fontId="0" fillId="5" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="16" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="14" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="14" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="18" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="14" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="14" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="19" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="19" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="6" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="17" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="14" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
@@ -2151,10 +2157,10 @@
     <xf numFmtId="49" fontId="0" fillId="3" borderId="20" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="5" borderId="21" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -2163,13 +2169,13 @@
     <xf numFmtId="49" fontId="0" fillId="3" borderId="21" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="5" borderId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -2187,85 +2193,85 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="4" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="10" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="10" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="4" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="4" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="14" fontId="0" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="23" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="24" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="24" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="23" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="23" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="14" fontId="0" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="14" fontId="0" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="14" fontId="0" borderId="24" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="24" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="16" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="16" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="14" fontId="0" borderId="25" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="25" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="26" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="26" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="17" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="17" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="18" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="18" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="19" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="19" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="20" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -2283,10 +2289,10 @@
     <xf numFmtId="0" fontId="20" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="20" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="14" fontId="20" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
@@ -2310,16 +2316,16 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="24" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="24" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="22" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="22" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="25" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="25" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="26" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
@@ -2334,64 +2340,64 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="16" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="16" fillId="2" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="6" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="16" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="16" fillId="2" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="6" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="16" borderId="27" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="16" fillId="2" borderId="27" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="6" borderId="27" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="27" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="27" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="27" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="26" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="16" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="16" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="6" borderId="26" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="26" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="28" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="28" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="29" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="30" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="30" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="31" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -2400,31 +2406,31 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="12" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="12" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="14" fontId="0" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" borderId="27" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="27" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="27" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="27" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
@@ -2450,8 +2456,8 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffaaaaaa"/>
-      <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffff3333"/>
       <rgbColor rgb="ffff0000"/>
       <rgbColor rgb="ffffc000"/>
@@ -2663,17 +2669,17 @@
         <a:solidFill>
           <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -2701,10 +2707,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -2952,12 +2958,12 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -3244,7 +3250,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -3272,10 +3278,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -3658,7 +3664,7 @@
   <sheetData>
     <row r="1" ht="18" customHeight="1">
       <c r="A1" t="s" s="12">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="B1" t="s" s="13">
         <v>11</v>
@@ -3687,10 +3693,10 @@
         <v>15</v>
       </c>
       <c r="C2" t="s" s="18">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D2" t="s" s="18">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="E2" t="s" s="18">
         <v>46</v>
@@ -3699,16 +3705,16 @@
         <v>47</v>
       </c>
       <c r="G2" t="s" s="18">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="H2" t="s" s="18">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="I2" t="s" s="18">
         <v>48</v>
       </c>
       <c r="J2" t="s" s="18">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="K2" t="s" s="18">
         <v>32</v>
@@ -3740,7 +3746,7 @@
         <v>55</v>
       </c>
       <c r="G3" t="s" s="6">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="H3" t="s" s="6">
         <v>99</v>
@@ -3767,17 +3773,17 @@
       </c>
       <c r="B4" s="114"/>
       <c r="C4" t="s" s="115">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="D4" t="s" s="8">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="E4" t="s" s="8">
         <v>61</v>
       </c>
       <c r="F4" s="33"/>
       <c r="G4" t="s" s="8">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="H4" s="33"/>
       <c r="I4" s="33"/>
@@ -3794,17 +3800,17 @@
       </c>
       <c r="B5" s="89"/>
       <c r="C5" t="s" s="116">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="D5" t="s" s="46">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="E5" t="s" s="46">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" t="s" s="46">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
@@ -3821,10 +3827,10 @@
       </c>
       <c r="B6" s="89"/>
       <c r="C6" t="s" s="116">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="D6" t="s" s="46">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="E6" t="s" s="46">
         <v>61</v>
@@ -3848,17 +3854,17 @@
       </c>
       <c r="B7" s="119"/>
       <c r="C7" t="s" s="120">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="D7" t="s" s="121">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="E7" t="s" s="121">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="F7" s="5"/>
       <c r="G7" t="s" s="121">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
@@ -3875,17 +3881,17 @@
       </c>
       <c r="B8" s="33"/>
       <c r="C8" t="s" s="8">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="D8" t="s" s="8">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="E8" t="s" s="8">
         <v>61</v>
       </c>
       <c r="F8" s="33"/>
       <c r="G8" t="s" s="8">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="H8" s="33"/>
       <c r="I8" s="33"/>
@@ -3902,19 +3908,19 @@
       </c>
       <c r="B9" s="3"/>
       <c r="C9" t="s" s="46">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="D9" t="s" s="46">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="E9" t="s" s="46">
         <v>78</v>
       </c>
       <c r="F9" t="s" s="46">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="G9" t="s" s="46">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
@@ -3931,17 +3937,17 @@
       </c>
       <c r="B10" s="5"/>
       <c r="C10" t="s" s="121">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="D10" t="s" s="121">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="E10" t="s" s="121">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="F10" s="5"/>
       <c r="G10" t="s" s="121">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
@@ -3958,17 +3964,17 @@
       </c>
       <c r="B11" s="33"/>
       <c r="C11" t="s" s="8">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="D11" t="s" s="8">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="E11" t="s" s="8">
         <v>61</v>
       </c>
       <c r="F11" s="33"/>
       <c r="G11" t="s" s="8">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="H11" s="33"/>
       <c r="I11" s="33"/>
@@ -3985,19 +3991,19 @@
       </c>
       <c r="B12" s="3"/>
       <c r="C12" t="s" s="46">
+        <v>283</v>
+      </c>
+      <c r="D12" t="s" s="46">
         <v>281</v>
-      </c>
-      <c r="D12" t="s" s="46">
-        <v>279</v>
       </c>
       <c r="E12" t="s" s="46">
         <v>78</v>
       </c>
       <c r="F12" t="s" s="46">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="G12" t="s" s="46">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
@@ -4014,19 +4020,19 @@
       </c>
       <c r="B13" s="3"/>
       <c r="C13" t="s" s="46">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="D13" t="s" s="46">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="E13" t="s" s="46">
         <v>78</v>
       </c>
       <c r="F13" t="s" s="46">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="G13" t="s" s="46">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
@@ -4043,17 +4049,17 @@
       </c>
       <c r="B14" s="5"/>
       <c r="C14" t="s" s="121">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="D14" t="s" s="121">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="E14" t="s" s="121">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="F14" s="5"/>
       <c r="G14" t="s" s="121">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
@@ -4073,14 +4079,14 @@
         <v>79</v>
       </c>
       <c r="D15" t="s" s="8">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="E15" t="s" s="8">
         <v>61</v>
       </c>
       <c r="F15" s="33"/>
       <c r="G15" t="s" s="8">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="H15" s="33"/>
       <c r="I15" s="33"/>
@@ -4100,14 +4106,14 @@
         <v>79</v>
       </c>
       <c r="D16" t="s" s="46">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="E16" t="s" s="46">
         <v>61</v>
       </c>
       <c r="F16" s="3"/>
       <c r="G16" t="s" s="46">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
@@ -4127,7 +4133,7 @@
         <v>79</v>
       </c>
       <c r="D17" t="s" s="46">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="E17" t="s" s="46">
         <v>70</v>
@@ -4154,14 +4160,14 @@
         <v>79</v>
       </c>
       <c r="D18" t="s" s="46">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="E18" t="s" s="46">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="F18" s="3"/>
       <c r="G18" t="s" s="46">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
@@ -4181,14 +4187,14 @@
         <v>79</v>
       </c>
       <c r="D19" t="s" s="46">
+        <v>294</v>
+      </c>
+      <c r="E19" t="s" s="46">
         <v>292</v>
-      </c>
-      <c r="E19" t="s" s="46">
-        <v>290</v>
       </c>
       <c r="F19" s="3"/>
       <c r="G19" t="s" s="46">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
@@ -4208,16 +4214,16 @@
         <v>79</v>
       </c>
       <c r="D20" t="s" s="46">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="E20" t="s" s="46">
         <v>78</v>
       </c>
       <c r="F20" t="s" s="46">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="G20" t="s" s="46">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
@@ -4237,16 +4243,16 @@
         <v>79</v>
       </c>
       <c r="D21" t="s" s="46">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="E21" t="s" s="46">
         <v>78</v>
       </c>
       <c r="F21" t="s" s="46">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="G21" t="s" s="46">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
@@ -4266,14 +4272,14 @@
         <v>79</v>
       </c>
       <c r="D22" t="s" s="46">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E22" t="s" s="46">
         <v>61</v>
       </c>
       <c r="F22" s="3"/>
       <c r="G22" t="s" s="46">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
@@ -4293,14 +4299,14 @@
         <v>79</v>
       </c>
       <c r="D23" t="s" s="46">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="E23" t="s" s="46">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="F23" s="3"/>
       <c r="G23" t="s" s="46">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="H23" s="126"/>
       <c r="I23" s="3"/>
@@ -4320,14 +4326,14 @@
         <v>79</v>
       </c>
       <c r="D24" t="s" s="46">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="E24" t="s" s="46">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="F24" s="3"/>
       <c r="G24" t="s" s="46">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="H24" s="126"/>
       <c r="I24" s="3"/>
@@ -4347,14 +4353,14 @@
         <v>79</v>
       </c>
       <c r="D25" t="s" s="46">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="E25" t="s" s="46">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="F25" s="3"/>
       <c r="G25" t="s" s="46">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="H25" s="126"/>
       <c r="I25" s="3"/>
@@ -4374,14 +4380,14 @@
         <v>79</v>
       </c>
       <c r="D26" t="s" s="46">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="E26" t="s" s="46">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="F26" s="3"/>
       <c r="G26" t="s" s="46">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="H26" s="126"/>
       <c r="I26" s="3"/>
@@ -4401,14 +4407,14 @@
         <v>79</v>
       </c>
       <c r="D27" t="s" s="46">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="E27" t="s" s="46">
         <v>61</v>
       </c>
       <c r="F27" s="3"/>
       <c r="G27" t="s" s="46">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="H27" s="126"/>
       <c r="I27" s="3"/>
@@ -4428,14 +4434,14 @@
         <v>79</v>
       </c>
       <c r="D28" t="s" s="121">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="E28" t="s" s="121">
         <v>61</v>
       </c>
       <c r="F28" s="5"/>
       <c r="G28" t="s" s="121">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="H28" s="127"/>
       <c r="I28" s="5"/>
@@ -4455,16 +4461,16 @@
         <v>79</v>
       </c>
       <c r="D29" t="s" s="86">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="E29" t="s" s="86">
         <v>73</v>
       </c>
       <c r="F29" t="s" s="86">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="G29" t="s" s="86">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="H29" s="85"/>
       <c r="I29" s="85"/>
@@ -4484,14 +4490,14 @@
         <v>82</v>
       </c>
       <c r="D30" t="s" s="8">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="E30" t="s" s="8">
         <v>61</v>
       </c>
       <c r="F30" s="33"/>
       <c r="G30" t="s" s="8">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="H30" s="33"/>
       <c r="I30" s="33"/>
@@ -4511,14 +4517,14 @@
         <v>82</v>
       </c>
       <c r="D31" t="s" s="46">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="E31" t="s" s="46">
         <v>61</v>
       </c>
       <c r="F31" s="3"/>
       <c r="G31" t="s" s="46">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="H31" s="3"/>
       <c r="I31" s="3"/>
@@ -4538,14 +4544,14 @@
         <v>82</v>
       </c>
       <c r="D32" t="s" s="46">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="E32" t="s" s="46">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="F32" s="3"/>
       <c r="G32" t="s" s="46">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="H32" s="3"/>
       <c r="I32" s="3"/>
@@ -4565,14 +4571,14 @@
         <v>82</v>
       </c>
       <c r="D33" t="s" s="46">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="E33" t="s" s="46">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="F33" s="3"/>
       <c r="G33" t="s" s="46">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="H33" s="3"/>
       <c r="I33" s="3"/>
@@ -4592,14 +4598,14 @@
         <v>82</v>
       </c>
       <c r="D34" t="s" s="121">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="E34" t="s" s="121">
         <v>61</v>
       </c>
       <c r="F34" s="5"/>
       <c r="G34" t="s" s="121">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="H34" s="5"/>
       <c r="I34" s="5"/>
@@ -4636,7 +4642,7 @@
   <sheetData>
     <row r="1" ht="18" customHeight="1">
       <c r="A1" t="s" s="12">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="B1" t="s" s="131">
         <v>11</v>
@@ -4665,13 +4671,13 @@
         <v>42</v>
       </c>
       <c r="D2" t="s" s="18">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="E2" t="s" s="18">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="F2" t="s" s="18">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="G2" s="135"/>
       <c r="H2" s="136"/>
@@ -4714,7 +4720,7 @@
         <v>59</v>
       </c>
       <c r="E4" t="s" s="141">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="F4" s="96">
         <v>1</v>
@@ -4736,7 +4742,7 @@
         <v>62</v>
       </c>
       <c r="E5" t="s" s="49">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="F5" s="100">
         <v>2</v>
@@ -4758,7 +4764,7 @@
         <v>64</v>
       </c>
       <c r="E6" t="s" s="49">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="F6" s="100">
         <v>3</v>
@@ -4849,7 +4855,7 @@
   <sheetData>
     <row r="1" ht="18" customHeight="1">
       <c r="A1" t="s" s="12">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="B1" t="s" s="13">
         <v>11</v>
@@ -4884,13 +4890,13 @@
         <v>42</v>
       </c>
       <c r="D2" t="s" s="18">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="E2" t="s" s="18">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="F2" t="s" s="18">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="G2" s="135"/>
       <c r="H2" s="136"/>
@@ -4945,7 +4951,7 @@
         <v>59</v>
       </c>
       <c r="E4" t="s" s="141">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="F4" s="96">
         <v>1</v>
@@ -4973,7 +4979,7 @@
         <v>62</v>
       </c>
       <c r="E5" t="s" s="49">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="F5" s="100">
         <v>2</v>
@@ -5001,7 +5007,7 @@
         <v>64</v>
       </c>
       <c r="E6" t="s" s="49">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="F6" s="100">
         <v>3</v>
@@ -5122,7 +5128,7 @@
   <sheetData>
     <row r="1" ht="18" customHeight="1">
       <c r="A1" t="s" s="12">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="B1" t="s" s="13">
         <v>11</v>
@@ -5157,13 +5163,13 @@
         <v>42</v>
       </c>
       <c r="D2" t="s" s="18">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="E2" t="s" s="18">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="F2" t="s" s="18">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="G2" s="146"/>
       <c r="H2" s="147"/>
@@ -5218,7 +5224,7 @@
         <v>59</v>
       </c>
       <c r="E4" t="s" s="141">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="F4" s="96">
         <v>1</v>
@@ -5246,7 +5252,7 @@
         <v>62</v>
       </c>
       <c r="E5" t="s" s="49">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="F5" s="100">
         <v>2</v>
@@ -5274,7 +5280,7 @@
         <v>64</v>
       </c>
       <c r="E6" t="s" s="49">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="F6" s="100">
         <v>3</v>
@@ -5395,7 +5401,7 @@
   <sheetData>
     <row r="1" ht="19" customHeight="1">
       <c r="A1" t="s" s="149">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="B1" t="s" s="131">
         <v>11</v>
@@ -5424,13 +5430,13 @@
         <v>42</v>
       </c>
       <c r="D2" t="s" s="18">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="E2" t="s" s="18">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="F2" t="s" s="18">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="G2" s="135"/>
       <c r="H2" s="136"/>
@@ -5473,7 +5479,7 @@
         <v>59</v>
       </c>
       <c r="E4" t="s" s="141">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="F4" s="96">
         <v>1</v>
@@ -5495,7 +5501,7 @@
         <v>62</v>
       </c>
       <c r="E5" t="s" s="49">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="F5" s="100">
         <v>2</v>
@@ -5517,7 +5523,7 @@
         <v>64</v>
       </c>
       <c r="E6" t="s" s="49">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="F6" s="100">
         <v>3</v>
@@ -5608,7 +5614,7 @@
   <sheetData>
     <row r="1" ht="18" customHeight="1">
       <c r="A1" t="s" s="12">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="B1" t="s" s="13">
         <v>11</v>
@@ -5641,13 +5647,13 @@
       </c>
       <c r="C2" s="154"/>
       <c r="D2" t="s" s="18">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="E2" t="s" s="18">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="F2" t="s" s="18">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="G2" s="17"/>
       <c r="H2" s="3"/>
@@ -5668,16 +5674,16 @@
         <v>20</v>
       </c>
       <c r="C3" t="s" s="21">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="D3" t="s" s="30">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="E3" t="s" s="30">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="F3" t="s" s="30">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="G3" s="155"/>
       <c r="H3" s="156"/>
@@ -5696,7 +5702,7 @@
       </c>
       <c r="B4" s="114"/>
       <c r="C4" t="s" s="157">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="D4" t="s" s="158">
         <v>24</v>
@@ -5724,7 +5730,7 @@
       </c>
       <c r="B5" s="89"/>
       <c r="C5" t="s" s="160">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="D5" t="s" s="161">
         <v>24</v>
@@ -5752,7 +5758,7 @@
       </c>
       <c r="B6" s="89"/>
       <c r="C6" t="s" s="160">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="D6" t="s" s="161">
         <v>24</v>
@@ -5780,7 +5786,7 @@
       </c>
       <c r="B7" s="119"/>
       <c r="C7" t="s" s="163">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="D7" t="s" s="164">
         <v>24</v>
@@ -5808,7 +5814,7 @@
       </c>
       <c r="B8" s="166"/>
       <c r="C8" t="s" s="167">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="D8" t="s" s="13">
         <v>24</v>
@@ -5889,7 +5895,7 @@
   <sheetData>
     <row r="1" ht="18" customHeight="1">
       <c r="A1" t="s" s="12">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="B1" t="s" s="13">
         <v>11</v>
@@ -5920,13 +5926,13 @@
         <v>15</v>
       </c>
       <c r="C2" t="s" s="18">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="D2" t="s" s="18">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="E2" t="s" s="18">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="F2" s="146"/>
       <c r="G2" s="147"/>
@@ -5950,10 +5956,10 @@
         <v>51</v>
       </c>
       <c r="D3" t="s" s="55">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="E3" t="s" s="6">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="F3" s="17"/>
       <c r="G3" s="3"/>
@@ -5975,10 +5981,10 @@
         <v>37</v>
       </c>
       <c r="D4" t="s" s="54">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="E4" t="s" s="170">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="F4" s="17"/>
       <c r="G4" s="3"/>
@@ -6119,7 +6125,7 @@
   <sheetData>
     <row r="1" ht="18" customHeight="1">
       <c r="A1" t="s" s="12">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="B1" t="s" s="13">
         <v>11</v>
@@ -6150,16 +6156,16 @@
         <v>15</v>
       </c>
       <c r="C2" t="s" s="18">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="D2" t="s" s="18">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="E2" t="s" s="18">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="F2" t="s" s="18">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="G2" s="19"/>
       <c r="H2" s="20"/>
@@ -6185,10 +6191,10 @@
         <v>97</v>
       </c>
       <c r="E3" t="s" s="55">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="F3" t="s" s="6">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="G3" s="22"/>
       <c r="H3" s="20"/>
@@ -6212,10 +6218,10 @@
         <v>59</v>
       </c>
       <c r="E4" t="s" s="173">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="F4" t="s" s="170">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="G4" s="17"/>
       <c r="H4" s="3"/>
@@ -6239,10 +6245,10 @@
         <v>62</v>
       </c>
       <c r="E5" t="s" s="175">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="F5" t="s" s="170">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="G5" s="17"/>
       <c r="H5" s="3"/>
@@ -6266,10 +6272,10 @@
         <v>64</v>
       </c>
       <c r="E6" t="s" s="175">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="F6" t="s" s="170">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="G6" s="17"/>
       <c r="H6" s="3"/>
@@ -6293,10 +6299,10 @@
         <v>66</v>
       </c>
       <c r="E7" t="s" s="175">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="F7" t="s" s="170">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="G7" s="17"/>
       <c r="H7" s="3"/>
@@ -6320,10 +6326,10 @@
         <v>68</v>
       </c>
       <c r="E8" t="s" s="175">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="F8" t="s" s="170">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="G8" s="17"/>
       <c r="H8" s="3"/>
@@ -6347,10 +6353,10 @@
         <v>71</v>
       </c>
       <c r="E9" t="s" s="175">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="F9" t="s" s="170">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="G9" s="17"/>
       <c r="H9" s="3"/>
@@ -6374,10 +6380,10 @@
         <v>75</v>
       </c>
       <c r="E10" t="s" s="175">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="F10" t="s" s="170">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="G10" s="17"/>
       <c r="H10" s="3"/>
@@ -6401,10 +6407,10 @@
         <v>80</v>
       </c>
       <c r="E11" t="s" s="175">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="F11" t="s" s="170">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="G11" s="17"/>
       <c r="H11" s="3"/>
@@ -6428,10 +6434,10 @@
         <v>83</v>
       </c>
       <c r="E12" t="s" s="177">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="F12" t="s" s="170">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="G12" s="17"/>
       <c r="H12" s="3"/>
@@ -6466,7 +6472,7 @@
   <sheetData>
     <row r="1" ht="18" customHeight="1">
       <c r="A1" t="s" s="12">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="B1" t="s" s="13">
         <v>11</v>
@@ -6497,16 +6503,16 @@
         <v>15</v>
       </c>
       <c r="C2" t="s" s="18">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="D2" t="s" s="18">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="E2" t="s" s="18">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="F2" t="s" s="18">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="G2" s="28"/>
       <c r="H2" s="29"/>
@@ -6532,10 +6538,10 @@
         <v>191</v>
       </c>
       <c r="E3" t="s" s="179">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="F3" t="s" s="110">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="G3" s="112"/>
       <c r="H3" s="29"/>
@@ -6559,10 +6565,10 @@
         <v>144</v>
       </c>
       <c r="E4" t="s" s="181">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="F4" t="s" s="170">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="G4" s="17"/>
       <c r="H4" s="3"/>
@@ -6586,10 +6592,10 @@
         <v>148</v>
       </c>
       <c r="E5" t="s" s="183">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="F5" t="s" s="170">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="G5" s="17"/>
       <c r="H5" s="3"/>
@@ -6613,10 +6619,10 @@
         <v>152</v>
       </c>
       <c r="E6" t="s" s="183">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="F6" t="s" s="170">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="G6" s="17"/>
       <c r="H6" s="3"/>
@@ -6640,10 +6646,10 @@
         <v>156</v>
       </c>
       <c r="E7" t="s" s="183">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="F7" t="s" s="170">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="G7" s="17"/>
       <c r="H7" s="3"/>
@@ -6667,10 +6673,10 @@
         <v>163</v>
       </c>
       <c r="E8" t="s" s="183">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="F8" t="s" s="170">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="G8" s="17"/>
       <c r="H8" s="3"/>
@@ -6694,10 +6700,10 @@
         <v>159</v>
       </c>
       <c r="E9" t="s" s="183">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="F9" t="s" s="170">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="G9" s="17"/>
       <c r="H9" s="3"/>
@@ -6721,10 +6727,10 @@
         <v>167</v>
       </c>
       <c r="E10" t="s" s="183">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="F10" t="s" s="170">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="G10" s="17"/>
       <c r="H10" s="3"/>
@@ -6748,10 +6754,10 @@
         <v>174</v>
       </c>
       <c r="E11" t="s" s="183">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="F11" t="s" s="170">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="G11" s="17"/>
       <c r="H11" s="3"/>
@@ -6775,10 +6781,10 @@
         <v>177</v>
       </c>
       <c r="E12" t="s" s="183">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="F12" t="s" s="170">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="G12" s="17"/>
       <c r="H12" s="3"/>
@@ -6847,7 +6853,7 @@
   <sheetData>
     <row r="1" ht="18" customHeight="1">
       <c r="A1" t="s" s="12">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="B1" t="s" s="13">
         <v>11</v>
@@ -6879,16 +6885,16 @@
         <v>15</v>
       </c>
       <c r="C2" t="s" s="18">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="D2" t="s" s="18">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="E2" t="s" s="18">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="F2" t="s" s="18">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="G2" s="28"/>
       <c r="H2" s="29"/>
@@ -6912,13 +6918,13 @@
         <v>51</v>
       </c>
       <c r="D3" t="s" s="179">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="E3" t="s" s="179">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="F3" t="s" s="110">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="G3" s="112"/>
       <c r="H3" s="113"/>
@@ -6943,10 +6949,10 @@
         <v>116</v>
       </c>
       <c r="E4" t="s" s="54">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="F4" t="s" s="170">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="G4" s="17"/>
       <c r="H4" s="3"/>
@@ -7319,7 +7325,7 @@
   <sheetData>
     <row r="1" ht="18" customHeight="1">
       <c r="A1" t="s" s="12">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="B1" t="s" s="13">
         <v>11</v>
@@ -7338,19 +7344,19 @@
       <c r="A2" s="154"/>
       <c r="B2" s="154"/>
       <c r="C2" t="s" s="18">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="D2" t="s" s="18">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="E2" t="s" s="18">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="F2" t="s" s="18">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="G2" t="s" s="18">
-        <v>350</v>
+        <v>352</v>
       </c>
     </row>
     <row r="3" ht="13.65" customHeight="1">
@@ -7370,10 +7376,10 @@
         <v>214</v>
       </c>
       <c r="F3" t="s" s="179">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="G3" t="s" s="110">
-        <v>352</v>
+        <v>354</v>
       </c>
     </row>
     <row r="4" ht="28" customHeight="1">
@@ -7388,13 +7394,13 @@
         <v>75</v>
       </c>
       <c r="E4" t="s" s="159">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="F4" t="s" s="54">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="G4" t="s" s="170">
-        <v>352</v>
+        <v>354</v>
       </c>
     </row>
     <row r="5" ht="28" customHeight="1">
@@ -7409,13 +7415,13 @@
         <v>75</v>
       </c>
       <c r="E5" t="s" s="162">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="F5" t="s" s="54">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="G5" t="s" s="170">
-        <v>352</v>
+        <v>354</v>
       </c>
     </row>
     <row r="6" ht="28" customHeight="1">
@@ -7430,13 +7436,13 @@
         <v>75</v>
       </c>
       <c r="E6" t="s" s="162">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="F6" t="s" s="54">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="G6" t="s" s="170">
-        <v>352</v>
+        <v>354</v>
       </c>
     </row>
     <row r="7" ht="28" customHeight="1">
@@ -7451,13 +7457,13 @@
         <v>75</v>
       </c>
       <c r="E7" t="s" s="162">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="F7" t="s" s="54">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="G7" t="s" s="170">
-        <v>352</v>
+        <v>354</v>
       </c>
     </row>
     <row r="8" ht="28" customHeight="1">
@@ -7472,13 +7478,13 @@
         <v>75</v>
       </c>
       <c r="E8" t="s" s="162">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="F8" t="s" s="54">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="G8" t="s" s="170">
-        <v>352</v>
+        <v>354</v>
       </c>
     </row>
     <row r="9" ht="28" customHeight="1">
@@ -7493,13 +7499,13 @@
         <v>75</v>
       </c>
       <c r="E9" t="s" s="162">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="F9" t="s" s="54">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="G9" t="s" s="170">
-        <v>352</v>
+        <v>354</v>
       </c>
     </row>
     <row r="10" ht="28" customHeight="1">
@@ -7514,13 +7520,13 @@
         <v>75</v>
       </c>
       <c r="E10" t="s" s="162">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="F10" t="s" s="54">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="G10" t="s" s="170">
-        <v>352</v>
+        <v>354</v>
       </c>
     </row>
     <row r="11" ht="28" customHeight="1">
@@ -7535,13 +7541,13 @@
         <v>75</v>
       </c>
       <c r="E11" t="s" s="162">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="F11" t="s" s="54">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="G11" t="s" s="170">
-        <v>352</v>
+        <v>354</v>
       </c>
     </row>
     <row r="12" ht="28" customHeight="1">
@@ -7556,13 +7562,13 @@
         <v>75</v>
       </c>
       <c r="E12" t="s" s="162">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="F12" t="s" s="54">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="G12" t="s" s="170">
-        <v>352</v>
+        <v>354</v>
       </c>
     </row>
     <row r="13" ht="28" customHeight="1">
@@ -7577,13 +7583,13 @@
         <v>75</v>
       </c>
       <c r="E13" t="s" s="162">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="F13" t="s" s="54">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="G13" t="s" s="170">
-        <v>352</v>
+        <v>354</v>
       </c>
     </row>
     <row r="14" ht="28" customHeight="1">
@@ -7598,13 +7604,13 @@
         <v>75</v>
       </c>
       <c r="E14" t="s" s="162">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="F14" t="s" s="54">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="G14" t="s" s="170">
-        <v>352</v>
+        <v>354</v>
       </c>
     </row>
     <row r="15" ht="28" customHeight="1">
@@ -7619,13 +7625,13 @@
         <v>75</v>
       </c>
       <c r="E15" t="s" s="162">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="F15" t="s" s="54">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="G15" t="s" s="170">
-        <v>352</v>
+        <v>354</v>
       </c>
     </row>
     <row r="16" ht="28" customHeight="1">
@@ -7640,13 +7646,13 @@
         <v>75</v>
       </c>
       <c r="E16" t="s" s="162">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="F16" t="s" s="54">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="G16" t="s" s="170">
-        <v>352</v>
+        <v>354</v>
       </c>
     </row>
     <row r="17" ht="28" customHeight="1">
@@ -7661,13 +7667,13 @@
         <v>75</v>
       </c>
       <c r="E17" t="s" s="165">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="F17" t="s" s="54">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="G17" t="s" s="170">
-        <v>352</v>
+        <v>354</v>
       </c>
     </row>
     <row r="18" ht="28" customHeight="1">
@@ -7682,13 +7688,13 @@
         <v>80</v>
       </c>
       <c r="E18" t="s" s="159">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="F18" t="s" s="54">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="G18" t="s" s="170">
-        <v>352</v>
+        <v>354</v>
       </c>
     </row>
     <row r="19" ht="28" customHeight="1">
@@ -7703,13 +7709,13 @@
         <v>80</v>
       </c>
       <c r="E19" t="s" s="162">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="F19" t="s" s="54">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="G19" t="s" s="170">
-        <v>352</v>
+        <v>354</v>
       </c>
     </row>
     <row r="20" ht="28" customHeight="1">
@@ -7724,13 +7730,13 @@
         <v>80</v>
       </c>
       <c r="E20" t="s" s="162">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="F20" t="s" s="54">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="G20" t="s" s="170">
-        <v>352</v>
+        <v>354</v>
       </c>
     </row>
     <row r="21" ht="28" customHeight="1">
@@ -7745,13 +7751,13 @@
         <v>80</v>
       </c>
       <c r="E21" t="s" s="162">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="F21" t="s" s="54">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="G21" t="s" s="170">
-        <v>352</v>
+        <v>354</v>
       </c>
     </row>
     <row r="22" ht="28" customHeight="1">
@@ -7766,13 +7772,13 @@
         <v>80</v>
       </c>
       <c r="E22" t="s" s="165">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="F22" t="s" s="54">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="G22" t="s" s="170">
-        <v>352</v>
+        <v>354</v>
       </c>
     </row>
   </sheetData>
@@ -12712,7 +12718,7 @@
     </row>
     <row r="4" ht="14" customHeight="1">
       <c r="A4" s="24">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B4" s="33"/>
       <c r="C4" t="s" s="69">
@@ -14039,7 +14045,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:N25"/>
+  <dimension ref="A1:N26"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -14469,15 +14475,15 @@
       <c r="A18" s="41">
         <v>42736</v>
       </c>
-      <c r="B18" s="3"/>
-      <c r="C18" t="s" s="8">
+      <c r="B18" s="89"/>
+      <c r="C18" t="s" s="70">
+        <v>74</v>
+      </c>
+      <c r="D18" t="s" s="116">
         <v>245</v>
       </c>
-      <c r="D18" t="s" s="46">
+      <c r="E18" t="s" s="46">
         <v>246</v>
-      </c>
-      <c r="E18" t="s" s="46">
-        <v>247</v>
       </c>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
@@ -14494,8 +14500,8 @@
         <v>42736</v>
       </c>
       <c r="B19" s="3"/>
-      <c r="C19" t="s" s="46">
-        <v>245</v>
+      <c r="C19" t="s" s="8">
+        <v>247</v>
       </c>
       <c r="D19" t="s" s="46">
         <v>248</v>
@@ -14519,7 +14525,7 @@
       </c>
       <c r="B20" s="3"/>
       <c r="C20" t="s" s="46">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="D20" t="s" s="46">
         <v>250</v>
@@ -14543,7 +14549,7 @@
       </c>
       <c r="B21" s="3"/>
       <c r="C21" t="s" s="46">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="D21" t="s" s="46">
         <v>252</v>
@@ -14567,7 +14573,7 @@
       </c>
       <c r="B22" s="3"/>
       <c r="C22" t="s" s="46">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="D22" t="s" s="46">
         <v>254</v>
@@ -14591,7 +14597,7 @@
       </c>
       <c r="B23" s="3"/>
       <c r="C23" t="s" s="46">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="D23" t="s" s="46">
         <v>256</v>
@@ -14615,7 +14621,7 @@
       </c>
       <c r="B24" s="3"/>
       <c r="C24" t="s" s="46">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="D24" t="s" s="46">
         <v>258</v>
@@ -14634,11 +14640,19 @@
       <c r="N24" s="3"/>
     </row>
     <row r="25" ht="13.65" customHeight="1">
-      <c r="A25" s="41"/>
+      <c r="A25" s="41">
+        <v>42736</v>
+      </c>
       <c r="B25" s="3"/>
-      <c r="C25" s="46"/>
-      <c r="D25" s="46"/>
-      <c r="E25" s="46"/>
+      <c r="C25" t="s" s="46">
+        <v>247</v>
+      </c>
+      <c r="D25" t="s" s="46">
+        <v>260</v>
+      </c>
+      <c r="E25" t="s" s="46">
+        <v>261</v>
+      </c>
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
@@ -14649,6 +14663,22 @@
       <c r="M25" s="3"/>
       <c r="N25" s="3"/>
     </row>
+    <row r="26" ht="13.65" customHeight="1">
+      <c r="A26" s="41"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="46"/>
+      <c r="D26" s="46"/>
+      <c r="E26" s="46"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="3"/>
+      <c r="L26" s="3"/>
+      <c r="M26" s="3"/>
+      <c r="N26" s="3"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511806" footer="0.511806"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>

<commit_message>
Updated spreadsheet with the values
</commit_message>
<xml_diff>
--- a/src/aat/resources/adv_bundling_functional_tests_ccd_def.xlsx
+++ b/src/aat/resources/adv_bundling_functional_tests_ccd_def.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pawel/workspace/rpa-em-ccd-orchestrator/src/aat/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yogeshhullatti/Documents/Solirius/rpa-em-ccd-orchestrator/src/aat/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4EC11BF-CD5C-0244-88C4-F7C3D378FEBB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72734D42-B78B-BC4F-B5A8-BBD7C8DA0DBF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="460" windowWidth="31940" windowHeight="14640" tabRatio="500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="460" windowWidth="31940" windowHeight="14640" tabRatio="500" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Change History" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
     <sheet name="AuthorisationCaseState" sheetId="19" r:id="rId19"/>
     <sheet name="AuthorisationComplexType" sheetId="20" r:id="rId20"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1124" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1130" uniqueCount="351">
   <si>
     <t>Change History</t>
   </si>
@@ -1166,6 +1166,12 @@
   </si>
   <si>
     <t>http://192.168.0.108:8080/api/new-bundle</t>
+  </si>
+  <si>
+    <t>pageNumberFormat</t>
+  </si>
+  <si>
+    <t>Page Number Format</t>
   </si>
 </sst>
 </file>
@@ -1439,7 +1445,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -1605,13 +1611,88 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="hair">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="hair">
+        <color indexed="8"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="hair">
+        <color indexed="8"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="hair">
+        <color indexed="8"/>
+      </right>
+      <top style="hair">
+        <color indexed="8"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="155">
+  <cellXfs count="161">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1887,6 +1968,12 @@
     </xf>
     <xf numFmtId="49" fontId="11" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Excel Built-in Explanatory Text" xfId="2" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
@@ -2329,10 +2416,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:M33"/>
+  <dimension ref="A1:M34"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2775,7 +2862,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A17" s="88">
         <v>42736</v>
       </c>
@@ -2795,7 +2882,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A18" s="88">
         <v>42736</v>
       </c>
@@ -2819,7 +2906,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A19" s="88">
         <v>42736</v>
       </c>
@@ -2843,7 +2930,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A20" s="88">
         <v>42736</v>
       </c>
@@ -2869,7 +2956,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A21" s="88">
         <v>42736</v>
       </c>
@@ -2895,7 +2982,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A22" s="88">
         <v>42736</v>
       </c>
@@ -2915,7 +3002,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A23" s="88">
         <v>42736</v>
       </c>
@@ -2939,7 +3026,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A24" s="88">
         <v>42736</v>
       </c>
@@ -2963,7 +3050,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A25" s="88">
         <v>42736</v>
       </c>
@@ -2987,7 +3074,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A26" s="88">
         <v>42736</v>
       </c>
@@ -3011,7 +3098,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A27" s="88">
         <v>42736</v>
       </c>
@@ -3035,7 +3122,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A28" s="89">
         <v>42736</v>
       </c>
@@ -3060,56 +3147,61 @@
         <v>37</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A29" s="86">
-        <v>42736</v>
-      </c>
-      <c r="B29" s="87"/>
-      <c r="C29" s="78" t="s">
+    <row r="29" spans="1:13" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A29" s="155">
+        <v>42736</v>
+      </c>
+      <c r="B29" s="156"/>
+      <c r="C29" s="157" t="s">
+        <v>76</v>
+      </c>
+      <c r="D29" s="157" t="s">
+        <v>349</v>
+      </c>
+      <c r="E29" s="90" t="s">
+        <v>58</v>
+      </c>
+      <c r="F29" s="157" t="s">
+        <v>349</v>
+      </c>
+      <c r="G29" s="157" t="s">
+        <v>350</v>
+      </c>
+      <c r="H29" s="156"/>
+      <c r="I29" s="156"/>
+      <c r="J29" s="156"/>
+      <c r="K29" s="158" t="s">
+        <v>37</v>
+      </c>
+      <c r="L29" s="159"/>
+      <c r="M29" s="160"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A30" s="86">
+        <v>42736</v>
+      </c>
+      <c r="B30" s="87"/>
+      <c r="C30" s="78" t="s">
         <v>79</v>
       </c>
-      <c r="D29" s="78" t="s">
+      <c r="D30" s="78" t="s">
         <v>286</v>
       </c>
-      <c r="E29" s="78" t="s">
+      <c r="E30" s="78" t="s">
         <v>58</v>
       </c>
-      <c r="F29" s="87"/>
-      <c r="G29" s="78" t="s">
+      <c r="F30" s="87"/>
+      <c r="G30" s="78" t="s">
         <v>287</v>
       </c>
-      <c r="H29" s="87"/>
-      <c r="I29" s="87"/>
-      <c r="J29" s="87"/>
-      <c r="K29" s="79" t="s">
+      <c r="H30" s="87"/>
+      <c r="I30" s="87"/>
+      <c r="J30" s="87"/>
+      <c r="K30" s="79" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A30" s="88">
-        <v>42736</v>
-      </c>
-      <c r="C30" s="81" t="s">
-        <v>79</v>
-      </c>
-      <c r="D30" s="81" t="s">
-        <v>288</v>
-      </c>
-      <c r="E30" s="81" t="s">
-        <v>58</v>
-      </c>
-      <c r="F30" s="93"/>
-      <c r="G30" s="81" t="s">
-        <v>289</v>
-      </c>
-      <c r="H30" s="93"/>
-      <c r="I30" s="93"/>
-      <c r="J30" s="93"/>
-      <c r="K30" s="82" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A31" s="88">
         <v>42736</v>
       </c>
@@ -3117,14 +3209,14 @@
         <v>79</v>
       </c>
       <c r="D31" s="81" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="E31" s="81" t="s">
-        <v>254</v>
+        <v>58</v>
       </c>
       <c r="F31" s="93"/>
       <c r="G31" s="81" t="s">
-        <v>254</v>
+        <v>289</v>
       </c>
       <c r="H31" s="93"/>
       <c r="I31" s="93"/>
@@ -3133,7 +3225,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A32" s="88">
         <v>42736</v>
       </c>
@@ -3141,14 +3233,14 @@
         <v>79</v>
       </c>
       <c r="D32" s="81" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E32" s="81" t="s">
-        <v>292</v>
+        <v>254</v>
       </c>
       <c r="F32" s="93"/>
       <c r="G32" s="81" t="s">
-        <v>293</v>
+        <v>254</v>
       </c>
       <c r="H32" s="93"/>
       <c r="I32" s="93"/>
@@ -3158,27 +3250,51 @@
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A33" s="89">
-        <v>42736</v>
-      </c>
-      <c r="B33" s="90"/>
-      <c r="C33" s="84" t="s">
+      <c r="A33" s="88">
+        <v>42736</v>
+      </c>
+      <c r="C33" s="81" t="s">
         <v>79</v>
       </c>
-      <c r="D33" s="84" t="s">
+      <c r="D33" s="81" t="s">
+        <v>291</v>
+      </c>
+      <c r="E33" s="81" t="s">
+        <v>292</v>
+      </c>
+      <c r="F33" s="93"/>
+      <c r="G33" s="81" t="s">
+        <v>293</v>
+      </c>
+      <c r="H33" s="93"/>
+      <c r="I33" s="93"/>
+      <c r="J33" s="93"/>
+      <c r="K33" s="82" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A34" s="89">
+        <v>42736</v>
+      </c>
+      <c r="B34" s="90"/>
+      <c r="C34" s="84" t="s">
+        <v>79</v>
+      </c>
+      <c r="D34" s="84" t="s">
         <v>294</v>
       </c>
-      <c r="E33" s="84" t="s">
+      <c r="E34" s="84" t="s">
         <v>58</v>
       </c>
-      <c r="F33" s="90"/>
-      <c r="G33" s="84" t="s">
+      <c r="F34" s="90"/>
+      <c r="G34" s="84" t="s">
         <v>295</v>
       </c>
-      <c r="H33" s="90"/>
-      <c r="I33" s="90"/>
-      <c r="J33" s="90"/>
-      <c r="K33" s="85" t="s">
+      <c r="H34" s="90"/>
+      <c r="I34" s="90"/>
+      <c r="J34" s="90"/>
+      <c r="K34" s="85" t="s">
         <v>37</v>
       </c>
     </row>
@@ -6942,7 +7058,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:T14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
adding sync stitch back
</commit_message>
<xml_diff>
--- a/src/aat/resources/adv_bundling_functional_tests_ccd_def.xlsx
+++ b/src/aat/resources/adv_bundling_functional_tests_ccd_def.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yogeshhullatti/Documents/Solirius/rpa-em-ccd-orchestrator/src/aat/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pawel/workspace/rpa-em-ccd-orchestrator/src/aat/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{724CC76A-868F-7B4B-BAD0-2ED3285E825F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B40003C7-B4B8-044F-82B5-86AE0CD1AB67}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33200" windowHeight="16320" firstSheet="11" activeTab="19" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33200" windowHeight="16320" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Change History" sheetId="1" r:id="rId1"/>
@@ -579,18 +579,6 @@
     <t>Submit bundle to be stitched</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="10"/>
-        <color indexed="20"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>http://em-ccd-orchestrator-aat.service.core-compute-aat.internal/api/stitch-ccd-bundles</t>
-    </r>
-  </si>
-  <si>
     <t>cloneBundle</t>
   </si>
   <si>
@@ -1201,6 +1189,9 @@
   <si>
     <t>The complex type element (field) ID (ListElement Id) should match the field attribute name used by the service team in creating the case MaxLength: 70</t>
   </si>
+  <si>
+    <t>http://em-ccd-orchestrator-aat.service.core-compute-aat.internal/api/async-stitch-ccd-bundles</t>
+  </si>
 </sst>
 </file>
 
@@ -1211,7 +1202,7 @@
     <numFmt numFmtId="165" formatCode="d/m/yy"/>
     <numFmt numFmtId="166" formatCode="d/m/yyyy"/>
   </numFmts>
-  <fonts count="26" x14ac:knownFonts="1">
+  <fonts count="27" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -1379,6 +1370,12 @@
       <color indexed="8"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="7">
@@ -2087,10 +2084,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="209">
+  <cellXfs count="210">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2420,8 +2418,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="25" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="26" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3714,7 +3714,7 @@
   <sheetData>
     <row r="1" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B1" s="13" t="s">
         <v>11</v>
@@ -3743,10 +3743,10 @@
         <v>15</v>
       </c>
       <c r="C2" s="18" t="s">
+        <v>245</v>
+      </c>
+      <c r="D2" s="18" t="s">
         <v>246</v>
-      </c>
-      <c r="D2" s="18" t="s">
-        <v>247</v>
       </c>
       <c r="E2" s="18" t="s">
         <v>46</v>
@@ -3755,16 +3755,16 @@
         <v>47</v>
       </c>
       <c r="G2" s="18" t="s">
+        <v>247</v>
+      </c>
+      <c r="H2" s="18" t="s">
         <v>248</v>
-      </c>
-      <c r="H2" s="18" t="s">
-        <v>249</v>
       </c>
       <c r="I2" s="18" t="s">
         <v>48</v>
       </c>
       <c r="J2" s="18" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="K2" s="18" t="s">
         <v>32</v>
@@ -3787,7 +3787,7 @@
         <v>21</v>
       </c>
       <c r="D3" s="21" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>54</v>
@@ -3796,7 +3796,7 @@
         <v>55</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="H3" s="6" t="s">
         <v>99</v>
@@ -3823,17 +3823,17 @@
       </c>
       <c r="B4" s="114"/>
       <c r="C4" s="115" t="s">
+        <v>251</v>
+      </c>
+      <c r="D4" s="8" t="s">
         <v>252</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>253</v>
       </c>
       <c r="E4" s="8" t="s">
         <v>61</v>
       </c>
       <c r="F4" s="33"/>
       <c r="G4" s="8" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="H4" s="33"/>
       <c r="I4" s="33"/>
@@ -3850,17 +3850,17 @@
       </c>
       <c r="B5" s="89"/>
       <c r="C5" s="116" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D5" s="46" t="s">
+        <v>254</v>
+      </c>
+      <c r="E5" s="46" t="s">
         <v>255</v>
-      </c>
-      <c r="E5" s="46" t="s">
-        <v>256</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="46" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
@@ -3877,10 +3877,10 @@
       </c>
       <c r="B6" s="89"/>
       <c r="C6" s="116" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D6" s="46" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E6" s="46" t="s">
         <v>61</v>
@@ -3904,17 +3904,17 @@
       </c>
       <c r="B7" s="119"/>
       <c r="C7" s="120" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D7" s="121" t="s">
+        <v>258</v>
+      </c>
+      <c r="E7" s="121" t="s">
         <v>259</v>
-      </c>
-      <c r="E7" s="121" t="s">
-        <v>260</v>
       </c>
       <c r="F7" s="5"/>
       <c r="G7" s="121" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
@@ -3931,17 +3931,17 @@
       </c>
       <c r="B8" s="33"/>
       <c r="C8" s="8" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E8" s="8" t="s">
         <v>61</v>
       </c>
       <c r="F8" s="33"/>
       <c r="G8" s="8" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="H8" s="33"/>
       <c r="I8" s="33"/>
@@ -3958,19 +3958,19 @@
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="46" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D9" s="46" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E9" s="46" t="s">
         <v>78</v>
       </c>
       <c r="F9" s="46" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="G9" s="46" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
@@ -3987,17 +3987,17 @@
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="121" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D10" s="121" t="s">
+        <v>254</v>
+      </c>
+      <c r="E10" s="121" t="s">
         <v>255</v>
-      </c>
-      <c r="E10" s="121" t="s">
-        <v>256</v>
       </c>
       <c r="F10" s="5"/>
       <c r="G10" s="121" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
@@ -4014,17 +4014,17 @@
       </c>
       <c r="B11" s="33"/>
       <c r="C11" s="8" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E11" s="8" t="s">
         <v>61</v>
       </c>
       <c r="F11" s="33"/>
       <c r="G11" s="8" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="H11" s="33"/>
       <c r="I11" s="33"/>
@@ -4041,19 +4041,19 @@
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="46" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D12" s="46" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E12" s="46" t="s">
         <v>78</v>
       </c>
       <c r="F12" s="46" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="G12" s="46" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
@@ -4070,19 +4070,19 @@
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="46" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D13" s="46" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E13" s="46" t="s">
         <v>78</v>
       </c>
       <c r="F13" s="46" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="G13" s="46" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
@@ -4099,17 +4099,17 @@
       </c>
       <c r="B14" s="5"/>
       <c r="C14" s="121" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D14" s="121" t="s">
+        <v>254</v>
+      </c>
+      <c r="E14" s="121" t="s">
         <v>255</v>
-      </c>
-      <c r="E14" s="121" t="s">
-        <v>256</v>
       </c>
       <c r="F14" s="5"/>
       <c r="G14" s="121" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
@@ -4129,14 +4129,14 @@
         <v>79</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E15" s="8" t="s">
         <v>61</v>
       </c>
       <c r="F15" s="33"/>
       <c r="G15" s="8" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="H15" s="33"/>
       <c r="I15" s="33"/>
@@ -4156,14 +4156,14 @@
         <v>79</v>
       </c>
       <c r="D16" s="46" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E16" s="46" t="s">
         <v>61</v>
       </c>
       <c r="F16" s="3"/>
       <c r="G16" s="46" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
@@ -4183,7 +4183,7 @@
         <v>79</v>
       </c>
       <c r="D17" s="46" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E17" s="46" t="s">
         <v>70</v>
@@ -4210,14 +4210,14 @@
         <v>79</v>
       </c>
       <c r="D18" s="46" t="s">
+        <v>273</v>
+      </c>
+      <c r="E18" s="46" t="s">
         <v>274</v>
-      </c>
-      <c r="E18" s="46" t="s">
-        <v>275</v>
       </c>
       <c r="F18" s="3"/>
       <c r="G18" s="46" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
@@ -4237,14 +4237,14 @@
         <v>79</v>
       </c>
       <c r="D19" s="46" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E19" s="46" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F19" s="3"/>
       <c r="G19" s="46" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
@@ -4264,16 +4264,16 @@
         <v>79</v>
       </c>
       <c r="D20" s="46" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E20" s="46" t="s">
         <v>78</v>
       </c>
       <c r="F20" s="46" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="G20" s="46" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
@@ -4293,16 +4293,16 @@
         <v>79</v>
       </c>
       <c r="D21" s="46" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E21" s="46" t="s">
         <v>78</v>
       </c>
       <c r="F21" s="46" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="G21" s="46" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
@@ -4322,14 +4322,14 @@
         <v>79</v>
       </c>
       <c r="D22" s="46" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E22" s="46" t="s">
         <v>61</v>
       </c>
       <c r="F22" s="3"/>
       <c r="G22" s="46" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
@@ -4349,14 +4349,14 @@
         <v>79</v>
       </c>
       <c r="D23" s="46" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E23" s="46" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F23" s="3"/>
       <c r="G23" s="46" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="H23" s="126"/>
       <c r="I23" s="3"/>
@@ -4376,14 +4376,14 @@
         <v>79</v>
       </c>
       <c r="D24" s="46" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E24" s="46" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F24" s="3"/>
       <c r="G24" s="46" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="H24" s="126"/>
       <c r="I24" s="3"/>
@@ -4403,14 +4403,14 @@
         <v>79</v>
       </c>
       <c r="D25" s="46" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E25" s="46" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F25" s="3"/>
       <c r="G25" s="46" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="H25" s="126"/>
       <c r="I25" s="3"/>
@@ -4430,14 +4430,14 @@
         <v>79</v>
       </c>
       <c r="D26" s="46" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E26" s="46" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F26" s="3"/>
       <c r="G26" s="46" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="H26" s="126"/>
       <c r="I26" s="3"/>
@@ -4457,14 +4457,14 @@
         <v>79</v>
       </c>
       <c r="D27" s="46" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E27" s="46" t="s">
         <v>61</v>
       </c>
       <c r="F27" s="3"/>
       <c r="G27" s="46" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="H27" s="126"/>
       <c r="I27" s="3"/>
@@ -4484,14 +4484,14 @@
         <v>79</v>
       </c>
       <c r="D28" s="129" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="E28" s="121" t="s">
         <v>61</v>
       </c>
       <c r="F28" s="128"/>
       <c r="G28" s="129" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="H28" s="130"/>
       <c r="I28" s="128"/>
@@ -4511,16 +4511,16 @@
         <v>79</v>
       </c>
       <c r="D29" s="136" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E29" s="137" t="s">
         <v>61</v>
       </c>
       <c r="F29" s="136" t="s">
+        <v>294</v>
+      </c>
+      <c r="G29" s="136" t="s">
         <v>295</v>
-      </c>
-      <c r="G29" s="136" t="s">
-        <v>296</v>
       </c>
       <c r="H29" s="135"/>
       <c r="I29" s="135"/>
@@ -4540,16 +4540,16 @@
         <v>79</v>
       </c>
       <c r="D30" s="143" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="E30" s="137" t="s">
         <v>61</v>
       </c>
       <c r="F30" s="143" t="s">
+        <v>296</v>
+      </c>
+      <c r="G30" s="143" t="s">
         <v>297</v>
-      </c>
-      <c r="G30" s="143" t="s">
-        <v>298</v>
       </c>
       <c r="H30" s="142"/>
       <c r="I30" s="142"/>
@@ -4569,14 +4569,14 @@
         <v>82</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="E31" s="8" t="s">
         <v>61</v>
       </c>
       <c r="F31" s="33"/>
       <c r="G31" s="8" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="H31" s="33"/>
       <c r="I31" s="33"/>
@@ -4596,14 +4596,14 @@
         <v>82</v>
       </c>
       <c r="D32" s="46" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E32" s="46" t="s">
         <v>61</v>
       </c>
       <c r="F32" s="3"/>
       <c r="G32" s="46" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="H32" s="3"/>
       <c r="I32" s="3"/>
@@ -4623,14 +4623,14 @@
         <v>82</v>
       </c>
       <c r="D33" s="46" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E33" s="46" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F33" s="3"/>
       <c r="G33" s="46" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="H33" s="3"/>
       <c r="I33" s="3"/>
@@ -4650,14 +4650,14 @@
         <v>82</v>
       </c>
       <c r="D34" s="46" t="s">
+        <v>303</v>
+      </c>
+      <c r="E34" s="46" t="s">
         <v>304</v>
-      </c>
-      <c r="E34" s="46" t="s">
-        <v>305</v>
       </c>
       <c r="F34" s="3"/>
       <c r="G34" s="46" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="H34" s="3"/>
       <c r="I34" s="3"/>
@@ -4677,14 +4677,14 @@
         <v>82</v>
       </c>
       <c r="D35" s="121" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E35" s="121" t="s">
         <v>61</v>
       </c>
       <c r="F35" s="5"/>
       <c r="G35" s="121" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="H35" s="5"/>
       <c r="I35" s="5"/>
@@ -4721,7 +4721,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B1" s="148" t="s">
         <v>11</v>
@@ -4750,13 +4750,13 @@
         <v>42</v>
       </c>
       <c r="D2" s="18" t="s">
+        <v>309</v>
+      </c>
+      <c r="E2" s="18" t="s">
         <v>310</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="F2" s="18" t="s">
         <v>311</v>
-      </c>
-      <c r="F2" s="18" t="s">
-        <v>312</v>
       </c>
       <c r="G2" s="152"/>
       <c r="H2" s="153"/>
@@ -4799,7 +4799,7 @@
         <v>59</v>
       </c>
       <c r="E4" s="158" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="F4" s="96">
         <v>1</v>
@@ -4821,7 +4821,7 @@
         <v>62</v>
       </c>
       <c r="E5" s="49" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="F5" s="100">
         <v>2</v>
@@ -4843,7 +4843,7 @@
         <v>64</v>
       </c>
       <c r="E6" s="49" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="F6" s="100">
         <v>3</v>
@@ -4934,7 +4934,7 @@
   <sheetData>
     <row r="1" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B1" s="13" t="s">
         <v>11</v>
@@ -4969,13 +4969,13 @@
         <v>42</v>
       </c>
       <c r="D2" s="18" t="s">
+        <v>316</v>
+      </c>
+      <c r="E2" s="18" t="s">
         <v>317</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="F2" s="18" t="s">
         <v>318</v>
-      </c>
-      <c r="F2" s="18" t="s">
-        <v>319</v>
       </c>
       <c r="G2" s="152"/>
       <c r="H2" s="153"/>
@@ -5030,7 +5030,7 @@
         <v>59</v>
       </c>
       <c r="E4" s="158" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="F4" s="96">
         <v>1</v>
@@ -5058,7 +5058,7 @@
         <v>62</v>
       </c>
       <c r="E5" s="49" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="F5" s="100">
         <v>2</v>
@@ -5086,7 +5086,7 @@
         <v>64</v>
       </c>
       <c r="E6" s="49" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="F6" s="100">
         <v>3</v>
@@ -5207,7 +5207,7 @@
   <sheetData>
     <row r="1" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B1" s="13" t="s">
         <v>11</v>
@@ -5242,13 +5242,13 @@
         <v>42</v>
       </c>
       <c r="D2" s="18" t="s">
+        <v>316</v>
+      </c>
+      <c r="E2" s="18" t="s">
         <v>317</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="F2" s="18" t="s">
         <v>318</v>
-      </c>
-      <c r="F2" s="18" t="s">
-        <v>319</v>
       </c>
       <c r="G2" s="163"/>
       <c r="H2" s="164"/>
@@ -5303,7 +5303,7 @@
         <v>59</v>
       </c>
       <c r="E4" s="158" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="F4" s="96">
         <v>1</v>
@@ -5331,7 +5331,7 @@
         <v>62</v>
       </c>
       <c r="E5" s="49" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="F5" s="100">
         <v>2</v>
@@ -5359,7 +5359,7 @@
         <v>64</v>
       </c>
       <c r="E6" s="49" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="F6" s="100">
         <v>3</v>
@@ -5480,7 +5480,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="166" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B1" s="148" t="s">
         <v>11</v>
@@ -5509,13 +5509,13 @@
         <v>42</v>
       </c>
       <c r="D2" s="18" t="s">
+        <v>309</v>
+      </c>
+      <c r="E2" s="18" t="s">
         <v>310</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="F2" s="18" t="s">
         <v>311</v>
-      </c>
-      <c r="F2" s="18" t="s">
-        <v>312</v>
       </c>
       <c r="G2" s="152"/>
       <c r="H2" s="153"/>
@@ -5558,7 +5558,7 @@
         <v>59</v>
       </c>
       <c r="E4" s="158" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="F4" s="96">
         <v>1</v>
@@ -5580,7 +5580,7 @@
         <v>62</v>
       </c>
       <c r="E5" s="49" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="F5" s="100">
         <v>2</v>
@@ -5602,7 +5602,7 @@
         <v>64</v>
       </c>
       <c r="E6" s="49" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="F6" s="100">
         <v>3</v>
@@ -5693,7 +5693,7 @@
   <sheetData>
     <row r="1" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B1" s="13" t="s">
         <v>11</v>
@@ -5726,13 +5726,13 @@
       </c>
       <c r="C2" s="171"/>
       <c r="D2" s="18" t="s">
+        <v>322</v>
+      </c>
+      <c r="E2" s="18" t="s">
         <v>323</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="F2" s="18" t="s">
         <v>324</v>
-      </c>
-      <c r="F2" s="18" t="s">
-        <v>325</v>
       </c>
       <c r="G2" s="17"/>
       <c r="H2" s="3"/>
@@ -5753,16 +5753,16 @@
         <v>20</v>
       </c>
       <c r="C3" s="21" t="s">
+        <v>325</v>
+      </c>
+      <c r="D3" s="30" t="s">
         <v>326</v>
       </c>
-      <c r="D3" s="30" t="s">
+      <c r="E3" s="30" t="s">
         <v>327</v>
       </c>
-      <c r="E3" s="30" t="s">
+      <c r="F3" s="30" t="s">
         <v>328</v>
-      </c>
-      <c r="F3" s="30" t="s">
-        <v>329</v>
       </c>
       <c r="G3" s="172"/>
       <c r="H3" s="173"/>
@@ -5781,7 +5781,7 @@
       </c>
       <c r="B4" s="114"/>
       <c r="C4" s="174" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D4" s="175" t="s">
         <v>24</v>
@@ -5809,7 +5809,7 @@
       </c>
       <c r="B5" s="89"/>
       <c r="C5" s="177" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D5" s="178" t="s">
         <v>24</v>
@@ -5837,7 +5837,7 @@
       </c>
       <c r="B6" s="89"/>
       <c r="C6" s="177" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D6" s="178" t="s">
         <v>24</v>
@@ -5865,7 +5865,7 @@
       </c>
       <c r="B7" s="119"/>
       <c r="C7" s="180" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D7" s="181" t="s">
         <v>24</v>
@@ -5893,7 +5893,7 @@
       </c>
       <c r="B8" s="184"/>
       <c r="C8" s="185" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D8" s="13" t="s">
         <v>24</v>
@@ -5974,7 +5974,7 @@
   <sheetData>
     <row r="1" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B1" s="13" t="s">
         <v>11</v>
@@ -6005,13 +6005,13 @@
         <v>15</v>
       </c>
       <c r="C2" s="18" t="s">
+        <v>335</v>
+      </c>
+      <c r="D2" s="18" t="s">
         <v>336</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="E2" s="18" t="s">
         <v>337</v>
-      </c>
-      <c r="E2" s="18" t="s">
-        <v>338</v>
       </c>
       <c r="F2" s="163"/>
       <c r="G2" s="164"/>
@@ -6035,10 +6035,10 @@
         <v>51</v>
       </c>
       <c r="D3" s="55" t="s">
+        <v>338</v>
+      </c>
+      <c r="E3" s="6" t="s">
         <v>339</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>340</v>
       </c>
       <c r="F3" s="17"/>
       <c r="G3" s="3"/>
@@ -6060,10 +6060,10 @@
         <v>37</v>
       </c>
       <c r="D4" s="54" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E4" s="188" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="F4" s="17"/>
       <c r="G4" s="3"/>
@@ -6204,7 +6204,7 @@
   <sheetData>
     <row r="1" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B1" s="13" t="s">
         <v>11</v>
@@ -6235,16 +6235,16 @@
         <v>15</v>
       </c>
       <c r="C2" s="18" t="s">
+        <v>342</v>
+      </c>
+      <c r="D2" s="18" t="s">
         <v>343</v>
       </c>
-      <c r="D2" s="18" t="s">
-        <v>344</v>
-      </c>
       <c r="E2" s="18" t="s">
+        <v>336</v>
+      </c>
+      <c r="F2" s="18" t="s">
         <v>337</v>
-      </c>
-      <c r="F2" s="18" t="s">
-        <v>338</v>
       </c>
       <c r="G2" s="19"/>
       <c r="H2" s="20"/>
@@ -6270,10 +6270,10 @@
         <v>97</v>
       </c>
       <c r="E3" s="55" t="s">
+        <v>338</v>
+      </c>
+      <c r="F3" s="6" t="s">
         <v>339</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>340</v>
       </c>
       <c r="G3" s="22"/>
       <c r="H3" s="20"/>
@@ -6297,10 +6297,10 @@
         <v>59</v>
       </c>
       <c r="E4" s="191" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="F4" s="188" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G4" s="17"/>
       <c r="H4" s="3"/>
@@ -6324,10 +6324,10 @@
         <v>62</v>
       </c>
       <c r="E5" s="193" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="F5" s="188" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G5" s="17"/>
       <c r="H5" s="3"/>
@@ -6351,10 +6351,10 @@
         <v>64</v>
       </c>
       <c r="E6" s="193" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="F6" s="188" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G6" s="17"/>
       <c r="H6" s="3"/>
@@ -6378,10 +6378,10 @@
         <v>66</v>
       </c>
       <c r="E7" s="193" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="F7" s="188" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G7" s="17"/>
       <c r="H7" s="3"/>
@@ -6405,10 +6405,10 @@
         <v>68</v>
       </c>
       <c r="E8" s="193" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="F8" s="188" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G8" s="17"/>
       <c r="H8" s="3"/>
@@ -6432,10 +6432,10 @@
         <v>71</v>
       </c>
       <c r="E9" s="193" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="F9" s="188" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G9" s="17"/>
       <c r="H9" s="3"/>
@@ -6459,10 +6459,10 @@
         <v>75</v>
       </c>
       <c r="E10" s="193" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="F10" s="188" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G10" s="17"/>
       <c r="H10" s="3"/>
@@ -6486,10 +6486,10 @@
         <v>80</v>
       </c>
       <c r="E11" s="193" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="F11" s="188" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G11" s="17"/>
       <c r="H11" s="3"/>
@@ -6513,10 +6513,10 @@
         <v>83</v>
       </c>
       <c r="E12" s="195" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="F12" s="188" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G12" s="17"/>
       <c r="H12" s="3"/>
@@ -6551,7 +6551,7 @@
   <sheetData>
     <row r="1" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B1" s="13" t="s">
         <v>11</v>
@@ -6582,16 +6582,16 @@
         <v>15</v>
       </c>
       <c r="C2" s="18" t="s">
+        <v>335</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>345</v>
+      </c>
+      <c r="E2" s="18" t="s">
         <v>336</v>
       </c>
-      <c r="D2" s="18" t="s">
-        <v>346</v>
-      </c>
-      <c r="E2" s="18" t="s">
+      <c r="F2" s="18" t="s">
         <v>337</v>
-      </c>
-      <c r="F2" s="18" t="s">
-        <v>338</v>
       </c>
       <c r="G2" s="28"/>
       <c r="H2" s="29"/>
@@ -6614,13 +6614,13 @@
         <v>51</v>
       </c>
       <c r="D3" s="197" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E3" s="197" t="s">
+        <v>338</v>
+      </c>
+      <c r="F3" s="110" t="s">
         <v>339</v>
-      </c>
-      <c r="F3" s="110" t="s">
-        <v>340</v>
       </c>
       <c r="G3" s="112"/>
       <c r="H3" s="29"/>
@@ -6644,10 +6644,10 @@
         <v>144</v>
       </c>
       <c r="E4" s="199" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="F4" s="188" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G4" s="17"/>
       <c r="H4" s="3"/>
@@ -6671,10 +6671,10 @@
         <v>148</v>
       </c>
       <c r="E5" s="201" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="F5" s="188" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G5" s="17"/>
       <c r="H5" s="3"/>
@@ -6698,10 +6698,10 @@
         <v>152</v>
       </c>
       <c r="E6" s="201" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="F6" s="188" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G6" s="17"/>
       <c r="H6" s="3"/>
@@ -6725,10 +6725,10 @@
         <v>156</v>
       </c>
       <c r="E7" s="201" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="F7" s="188" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G7" s="17"/>
       <c r="H7" s="3"/>
@@ -6749,13 +6749,13 @@
         <v>37</v>
       </c>
       <c r="D8" s="75" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E8" s="201" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="F8" s="188" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G8" s="17"/>
       <c r="H8" s="3"/>
@@ -6779,10 +6779,10 @@
         <v>159</v>
       </c>
       <c r="E9" s="201" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="F9" s="188" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G9" s="17"/>
       <c r="H9" s="3"/>
@@ -6803,13 +6803,13 @@
         <v>37</v>
       </c>
       <c r="D10" s="75" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E10" s="201" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="F10" s="188" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G10" s="17"/>
       <c r="H10" s="3"/>
@@ -6830,13 +6830,13 @@
         <v>37</v>
       </c>
       <c r="D11" s="75" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E11" s="201" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="F11" s="188" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G11" s="17"/>
       <c r="H11" s="3"/>
@@ -6857,13 +6857,13 @@
         <v>37</v>
       </c>
       <c r="D12" s="75" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E12" s="201" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="F12" s="188" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G12" s="17"/>
       <c r="H12" s="3"/>
@@ -6932,7 +6932,7 @@
   <sheetData>
     <row r="1" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B1" s="13" t="s">
         <v>11</v>
@@ -6964,16 +6964,16 @@
         <v>15</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="E2" s="18" t="s">
+        <v>336</v>
+      </c>
+      <c r="F2" s="18" t="s">
         <v>337</v>
-      </c>
-      <c r="F2" s="18" t="s">
-        <v>338</v>
       </c>
       <c r="G2" s="28"/>
       <c r="H2" s="29"/>
@@ -6997,13 +6997,13 @@
         <v>51</v>
       </c>
       <c r="D3" s="197" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E3" s="197" t="s">
+        <v>338</v>
+      </c>
+      <c r="F3" s="110" t="s">
         <v>339</v>
-      </c>
-      <c r="F3" s="110" t="s">
-        <v>340</v>
       </c>
       <c r="G3" s="112"/>
       <c r="H3" s="113"/>
@@ -7028,10 +7028,10 @@
         <v>116</v>
       </c>
       <c r="E4" s="54" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="F4" s="188" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G4" s="17"/>
       <c r="H4" s="3"/>
@@ -7392,7 +7392,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:IV24"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
@@ -7410,7 +7410,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B1" s="13" t="s">
         <v>11</v>
@@ -7429,19 +7429,19 @@
       <c r="A2" s="171"/>
       <c r="B2" s="171"/>
       <c r="C2" s="18" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D2" s="18" t="s">
+        <v>350</v>
+      </c>
+      <c r="E2" s="18" t="s">
         <v>351</v>
       </c>
-      <c r="E2" s="18" t="s">
-        <v>352</v>
-      </c>
       <c r="F2" s="18" t="s">
+        <v>336</v>
+      </c>
+      <c r="G2" s="18" t="s">
         <v>337</v>
-      </c>
-      <c r="G2" s="18" t="s">
-        <v>338</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -7458,13 +7458,13 @@
         <v>97</v>
       </c>
       <c r="E3" s="197" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F3" s="197" t="s">
+        <v>338</v>
+      </c>
+      <c r="G3" s="110" t="s">
         <v>339</v>
-      </c>
-      <c r="G3" s="110" t="s">
-        <v>340</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="28" customHeight="1" x14ac:dyDescent="0.15">
@@ -7479,13 +7479,13 @@
         <v>75</v>
       </c>
       <c r="E4" s="176" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="F4" s="54" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G4" s="188" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="28" customHeight="1" x14ac:dyDescent="0.15">
@@ -7500,13 +7500,13 @@
         <v>75</v>
       </c>
       <c r="E5" s="179" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="F5" s="54" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G5" s="188" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="28" customHeight="1" x14ac:dyDescent="0.15">
@@ -7521,13 +7521,13 @@
         <v>75</v>
       </c>
       <c r="E6" s="179" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F6" s="54" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G6" s="188" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="28" customHeight="1" x14ac:dyDescent="0.15">
@@ -7542,13 +7542,13 @@
         <v>75</v>
       </c>
       <c r="E7" s="179" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="F7" s="54" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G7" s="188" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="28" customHeight="1" x14ac:dyDescent="0.15">
@@ -7563,13 +7563,13 @@
         <v>75</v>
       </c>
       <c r="E8" s="179" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F8" s="54" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G8" s="188" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="28" customHeight="1" x14ac:dyDescent="0.15">
@@ -7584,13 +7584,13 @@
         <v>75</v>
       </c>
       <c r="E9" s="179" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F9" s="54" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G9" s="188" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="28" customHeight="1" x14ac:dyDescent="0.15">
@@ -7605,13 +7605,13 @@
         <v>75</v>
       </c>
       <c r="E10" s="179" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="F10" s="54" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G10" s="188" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="28" customHeight="1" x14ac:dyDescent="0.15">
@@ -7626,13 +7626,13 @@
         <v>75</v>
       </c>
       <c r="E11" s="179" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F11" s="54" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G11" s="188" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="28" customHeight="1" x14ac:dyDescent="0.15">
@@ -7647,13 +7647,13 @@
         <v>75</v>
       </c>
       <c r="E12" s="179" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F12" s="54" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G12" s="188" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="28" customHeight="1" x14ac:dyDescent="0.15">
@@ -7668,13 +7668,13 @@
         <v>75</v>
       </c>
       <c r="E13" s="179" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="F13" s="54" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G13" s="188" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="28" customHeight="1" x14ac:dyDescent="0.15">
@@ -7689,13 +7689,13 @@
         <v>75</v>
       </c>
       <c r="E14" s="179" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="F14" s="54" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G14" s="188" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="28" customHeight="1" x14ac:dyDescent="0.15">
@@ -7710,13 +7710,13 @@
         <v>75</v>
       </c>
       <c r="E15" s="179" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="F15" s="54" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G15" s="188" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="28" customHeight="1" x14ac:dyDescent="0.15">
@@ -7731,13 +7731,13 @@
         <v>75</v>
       </c>
       <c r="E16" s="208" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="F16" s="54" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G16" s="188" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="28" customHeight="1" x14ac:dyDescent="0.15">
@@ -7752,13 +7752,13 @@
         <v>75</v>
       </c>
       <c r="E17" s="208" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="F17" s="54" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G17" s="188" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="28" customHeight="1" x14ac:dyDescent="0.15">
@@ -7773,13 +7773,13 @@
         <v>75</v>
       </c>
       <c r="E18" s="179" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="F18" s="54" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G18" s="188" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="28" customHeight="1" x14ac:dyDescent="0.15">
@@ -7794,13 +7794,13 @@
         <v>75</v>
       </c>
       <c r="E19" s="182" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F19" s="54" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G19" s="188" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="28" customHeight="1" x14ac:dyDescent="0.15">
@@ -7815,13 +7815,13 @@
         <v>80</v>
       </c>
       <c r="E20" s="176" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="F20" s="54" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G20" s="188" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="28" customHeight="1" x14ac:dyDescent="0.15">
@@ -7836,13 +7836,13 @@
         <v>80</v>
       </c>
       <c r="E21" s="179" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="F21" s="54" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G21" s="188" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="28" customHeight="1" x14ac:dyDescent="0.15">
@@ -7857,13 +7857,13 @@
         <v>80</v>
       </c>
       <c r="E22" s="179" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="F22" s="54" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G22" s="188" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="28" customHeight="1" x14ac:dyDescent="0.15">
@@ -7878,13 +7878,13 @@
         <v>80</v>
       </c>
       <c r="E23" s="179" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F23" s="54" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G23" s="188" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="28" customHeight="1" x14ac:dyDescent="0.15">
@@ -7899,13 +7899,13 @@
         <v>80</v>
       </c>
       <c r="E24" s="182" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="F24" s="54" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G24" s="188" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
   </sheetData>
@@ -12675,7 +12675,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:IV14"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -13041,8 +13043,8 @@
       </c>
       <c r="J8" s="77"/>
       <c r="K8" s="83"/>
-      <c r="L8" s="70" t="s">
-        <v>162</v>
+      <c r="L8" s="209" t="s">
+        <v>352</v>
       </c>
       <c r="M8" s="17"/>
       <c r="N8" s="33"/>
@@ -13068,13 +13070,13 @@
         <v>37</v>
       </c>
       <c r="D9" s="75" t="s">
+        <v>162</v>
+      </c>
+      <c r="E9" s="70" t="s">
         <v>163</v>
       </c>
-      <c r="E9" s="70" t="s">
+      <c r="F9" s="70" t="s">
         <v>164</v>
-      </c>
-      <c r="F9" s="70" t="s">
-        <v>165</v>
       </c>
       <c r="G9" s="82">
         <v>6</v>
@@ -13088,7 +13090,7 @@
       <c r="J9" s="77"/>
       <c r="K9" s="83"/>
       <c r="L9" s="70" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="M9" s="17"/>
       <c r="N9" s="5"/>
@@ -13114,13 +13116,13 @@
         <v>37</v>
       </c>
       <c r="D10" s="75" t="s">
+        <v>166</v>
+      </c>
+      <c r="E10" s="70" t="s">
         <v>167</v>
       </c>
-      <c r="E10" s="70" t="s">
+      <c r="F10" s="70" t="s">
         <v>168</v>
-      </c>
-      <c r="F10" s="70" t="s">
-        <v>169</v>
       </c>
       <c r="G10" s="82">
         <v>7</v>
@@ -13156,13 +13158,13 @@
         <v>37</v>
       </c>
       <c r="D11" s="75" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E11" s="70" t="s">
         <v>160</v>
       </c>
       <c r="F11" s="70" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G11" s="82">
         <v>5</v>
@@ -13174,11 +13176,11 @@
         <v>116</v>
       </c>
       <c r="J11" s="88" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="K11" s="83"/>
       <c r="L11" s="70" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="M11" s="17"/>
       <c r="N11" s="85"/>
@@ -13204,13 +13206,13 @@
         <v>37</v>
       </c>
       <c r="D12" s="75" t="s">
+        <v>173</v>
+      </c>
+      <c r="E12" s="70" t="s">
         <v>174</v>
       </c>
-      <c r="E12" s="70" t="s">
+      <c r="F12" s="70" t="s">
         <v>175</v>
-      </c>
-      <c r="F12" s="70" t="s">
-        <v>176</v>
       </c>
       <c r="G12" s="82">
         <v>8</v>
@@ -13246,13 +13248,13 @@
         <v>37</v>
       </c>
       <c r="D13" s="75" t="s">
+        <v>176</v>
+      </c>
+      <c r="E13" s="70" t="s">
         <v>177</v>
       </c>
-      <c r="E13" s="70" t="s">
-        <v>178</v>
-      </c>
       <c r="F13" s="70" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G13" s="82">
         <v>9</v>
@@ -13332,7 +13334,7 @@
   <sheetData>
     <row r="1" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B1" s="13" t="s">
         <v>11</v>
@@ -13366,40 +13368,40 @@
         <v>42</v>
       </c>
       <c r="D2" s="18" t="s">
+        <v>179</v>
+      </c>
+      <c r="E2" s="18" t="s">
         <v>180</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="F2" s="18" t="s">
         <v>181</v>
       </c>
-      <c r="F2" s="18" t="s">
+      <c r="G2" s="18" t="s">
         <v>182</v>
       </c>
-      <c r="G2" s="18" t="s">
+      <c r="H2" s="18" t="s">
         <v>183</v>
       </c>
-      <c r="H2" s="18" t="s">
+      <c r="I2" s="18" t="s">
         <v>184</v>
       </c>
-      <c r="I2" s="18" t="s">
+      <c r="J2" s="18" t="s">
         <v>185</v>
       </c>
-      <c r="J2" s="18" t="s">
+      <c r="K2" s="18" t="s">
         <v>186</v>
       </c>
-      <c r="K2" s="18" t="s">
+      <c r="L2" s="18" t="s">
         <v>187</v>
       </c>
-      <c r="L2" s="18" t="s">
+      <c r="M2" s="18" t="s">
         <v>188</v>
       </c>
-      <c r="M2" s="18" t="s">
+      <c r="N2" s="18" t="s">
         <v>189</v>
       </c>
-      <c r="N2" s="18" t="s">
-        <v>190</v>
-      </c>
       <c r="O2" s="18" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -13413,40 +13415,40 @@
         <v>51</v>
       </c>
       <c r="D3" s="55" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E3" s="55" t="s">
         <v>97</v>
       </c>
       <c r="F3" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="G3" s="6" t="s">
         <v>192</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="H3" s="21" t="s">
         <v>193</v>
       </c>
-      <c r="H3" s="21" t="s">
+      <c r="I3" s="6" t="s">
         <v>194</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="J3" s="6" t="s">
         <v>195</v>
       </c>
-      <c r="J3" s="6" t="s">
+      <c r="K3" s="6" t="s">
         <v>196</v>
-      </c>
-      <c r="K3" s="6" t="s">
-        <v>197</v>
       </c>
       <c r="L3" s="6" t="s">
         <v>99</v>
       </c>
       <c r="M3" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="N3" s="6" t="s">
         <v>198</v>
       </c>
-      <c r="N3" s="6" t="s">
+      <c r="O3" s="6" t="s">
         <v>199</v>
-      </c>
-      <c r="O3" s="6" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -13467,7 +13469,7 @@
         <v>1</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H4" s="96">
         <v>1</v>
@@ -13506,7 +13508,7 @@
         <v>2</v>
       </c>
       <c r="G5" s="46" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H5" s="100">
         <v>1</v>
@@ -13545,7 +13547,7 @@
         <v>3</v>
       </c>
       <c r="G6" s="46" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H6" s="100">
         <v>1</v>
@@ -13584,7 +13586,7 @@
         <v>4</v>
       </c>
       <c r="G7" s="46" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H7" s="100">
         <v>1</v>
@@ -13623,7 +13625,7 @@
         <v>5</v>
       </c>
       <c r="G8" s="46" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H8" s="100">
         <v>1</v>
@@ -13662,13 +13664,13 @@
         <v>6</v>
       </c>
       <c r="G9" s="46" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H9" s="100">
         <v>1</v>
       </c>
       <c r="I9" s="101" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="J9" s="100">
         <v>1</v>
@@ -13701,13 +13703,13 @@
         <v>1</v>
       </c>
       <c r="G10" s="46" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H10" s="100">
         <v>1</v>
       </c>
       <c r="I10" s="101" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="J10" s="100">
         <v>1</v>
@@ -13738,13 +13740,13 @@
         <v>2</v>
       </c>
       <c r="G11" s="46" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H11" s="100">
         <v>1</v>
       </c>
       <c r="I11" s="101" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="J11" s="100">
         <v>1</v>
@@ -13775,13 +13777,13 @@
         <v>3</v>
       </c>
       <c r="G12" s="46" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H12" s="100">
         <v>1</v>
       </c>
       <c r="I12" s="101" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="J12" s="100">
         <v>1</v>
@@ -13812,13 +13814,13 @@
         <v>4</v>
       </c>
       <c r="G13" s="46" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H13" s="100">
         <v>1</v>
       </c>
       <c r="I13" s="101" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="J13" s="100">
         <v>1</v>
@@ -13849,13 +13851,13 @@
         <v>5</v>
       </c>
       <c r="G14" s="46" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H14" s="100">
         <v>1</v>
       </c>
       <c r="I14" s="101" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="J14" s="100">
         <v>1</v>
@@ -13886,13 +13888,13 @@
         <v>6</v>
       </c>
       <c r="G15" s="46" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H15" s="100">
         <v>1</v>
       </c>
       <c r="I15" s="101" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="J15" s="100">
         <v>1</v>
@@ -13923,13 +13925,13 @@
         <v>1</v>
       </c>
       <c r="G16" s="46" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H16" s="100">
         <v>1</v>
       </c>
       <c r="I16" s="101" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="J16" s="100">
         <v>1</v>
@@ -13960,13 +13962,13 @@
         <v>1</v>
       </c>
       <c r="G17" s="46" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H17" s="100">
         <v>1</v>
       </c>
       <c r="I17" s="101" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="J17" s="100">
         <v>1</v>
@@ -13988,7 +13990,7 @@
         <v>37</v>
       </c>
       <c r="D18" s="75" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E18" s="106" t="s">
         <v>75</v>
@@ -13997,13 +13999,13 @@
         <v>1</v>
       </c>
       <c r="G18" s="46" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H18" s="100">
         <v>1</v>
       </c>
       <c r="I18" s="101" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J18" s="100">
         <v>1</v>
@@ -14034,13 +14036,13 @@
         <v>1</v>
       </c>
       <c r="G19" s="46" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H19" s="100">
         <v>1</v>
       </c>
       <c r="I19" s="101" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="J19" s="100">
         <v>1</v>
@@ -14062,7 +14064,7 @@
         <v>37</v>
       </c>
       <c r="D20" s="75" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E20" s="106" t="s">
         <v>80</v>
@@ -14071,13 +14073,13 @@
         <v>1</v>
       </c>
       <c r="G20" s="46" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H20" s="100">
         <v>1</v>
       </c>
       <c r="I20" s="101" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="J20" s="100">
         <v>1</v>
@@ -14099,7 +14101,7 @@
         <v>37</v>
       </c>
       <c r="D21" s="75" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E21" s="106" t="s">
         <v>83</v>
@@ -14108,13 +14110,13 @@
         <v>1</v>
       </c>
       <c r="G21" s="46" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H21" s="100">
         <v>1</v>
       </c>
       <c r="I21" s="101" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="J21" s="100">
         <v>1</v>
@@ -14188,7 +14190,7 @@
   <sheetData>
     <row r="1" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B1" s="13" t="s">
         <v>11</v>
@@ -14218,13 +14220,13 @@
         <v>15</v>
       </c>
       <c r="C2" s="18" t="s">
+        <v>210</v>
+      </c>
+      <c r="D2" s="18" t="s">
         <v>211</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="E2" s="18" t="s">
         <v>212</v>
-      </c>
-      <c r="E2" s="18" t="s">
-        <v>213</v>
       </c>
       <c r="F2" s="28"/>
       <c r="G2" s="29"/>
@@ -14247,10 +14249,10 @@
         <v>21</v>
       </c>
       <c r="D3" s="111" t="s">
+        <v>213</v>
+      </c>
+      <c r="E3" s="110" t="s">
         <v>214</v>
-      </c>
-      <c r="E3" s="110" t="s">
-        <v>215</v>
       </c>
       <c r="F3" s="112"/>
       <c r="G3" s="113"/>
@@ -14268,13 +14270,13 @@
       </c>
       <c r="B4" s="114"/>
       <c r="C4" s="70" t="s">
+        <v>215</v>
+      </c>
+      <c r="D4" s="70" t="s">
         <v>216</v>
       </c>
-      <c r="D4" s="70" t="s">
+      <c r="E4" s="70" t="s">
         <v>217</v>
-      </c>
-      <c r="E4" s="70" t="s">
-        <v>218</v>
       </c>
       <c r="F4" s="17"/>
       <c r="G4" s="3"/>
@@ -14295,10 +14297,10 @@
         <v>74</v>
       </c>
       <c r="D5" s="70" t="s">
+        <v>218</v>
+      </c>
+      <c r="E5" s="70" t="s">
         <v>219</v>
-      </c>
-      <c r="E5" s="70" t="s">
-        <v>220</v>
       </c>
       <c r="F5" s="17"/>
       <c r="G5" s="3"/>
@@ -14319,10 +14321,10 @@
         <v>74</v>
       </c>
       <c r="D6" s="115" t="s">
+        <v>220</v>
+      </c>
+      <c r="E6" s="8" t="s">
         <v>221</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>222</v>
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
@@ -14343,10 +14345,10 @@
         <v>74</v>
       </c>
       <c r="D7" s="116" t="s">
+        <v>222</v>
+      </c>
+      <c r="E7" s="46" t="s">
         <v>223</v>
-      </c>
-      <c r="E7" s="46" t="s">
-        <v>224</v>
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
@@ -14367,10 +14369,10 @@
         <v>74</v>
       </c>
       <c r="D8" s="116" t="s">
+        <v>224</v>
+      </c>
+      <c r="E8" s="46" t="s">
         <v>225</v>
-      </c>
-      <c r="E8" s="46" t="s">
-        <v>226</v>
       </c>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
@@ -14391,10 +14393,10 @@
         <v>74</v>
       </c>
       <c r="D9" s="116" t="s">
+        <v>226</v>
+      </c>
+      <c r="E9" s="46" t="s">
         <v>227</v>
-      </c>
-      <c r="E9" s="46" t="s">
-        <v>228</v>
       </c>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
@@ -14415,10 +14417,10 @@
         <v>74</v>
       </c>
       <c r="D10" s="116" t="s">
+        <v>228</v>
+      </c>
+      <c r="E10" s="46" t="s">
         <v>229</v>
-      </c>
-      <c r="E10" s="46" t="s">
-        <v>230</v>
       </c>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
@@ -14439,10 +14441,10 @@
         <v>74</v>
       </c>
       <c r="D11" s="116" t="s">
+        <v>230</v>
+      </c>
+      <c r="E11" s="46" t="s">
         <v>231</v>
-      </c>
-      <c r="E11" s="46" t="s">
-        <v>232</v>
       </c>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
@@ -14463,10 +14465,10 @@
         <v>74</v>
       </c>
       <c r="D12" s="116" t="s">
+        <v>232</v>
+      </c>
+      <c r="E12" s="46" t="s">
         <v>233</v>
-      </c>
-      <c r="E12" s="46" t="s">
-        <v>234</v>
       </c>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
@@ -14487,10 +14489,10 @@
         <v>74</v>
       </c>
       <c r="D13" s="116" t="s">
+        <v>234</v>
+      </c>
+      <c r="E13" s="46" t="s">
         <v>235</v>
-      </c>
-      <c r="E13" s="46" t="s">
-        <v>236</v>
       </c>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
@@ -14511,10 +14513,10 @@
         <v>74</v>
       </c>
       <c r="D14" s="116" t="s">
+        <v>236</v>
+      </c>
+      <c r="E14" s="46" t="s">
         <v>237</v>
-      </c>
-      <c r="E14" s="46" t="s">
-        <v>238</v>
       </c>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
@@ -14535,10 +14537,10 @@
         <v>74</v>
       </c>
       <c r="D15" s="116" t="s">
+        <v>238</v>
+      </c>
+      <c r="E15" s="46" t="s">
         <v>239</v>
-      </c>
-      <c r="E15" s="46" t="s">
-        <v>240</v>
       </c>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
@@ -14559,10 +14561,10 @@
         <v>74</v>
       </c>
       <c r="D16" s="116" t="s">
+        <v>240</v>
+      </c>
+      <c r="E16" s="46" t="s">
         <v>241</v>
-      </c>
-      <c r="E16" s="46" t="s">
-        <v>242</v>
       </c>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
@@ -14583,10 +14585,10 @@
         <v>74</v>
       </c>
       <c r="D17" s="116" t="s">
+        <v>242</v>
+      </c>
+      <c r="E17" s="46" t="s">
         <v>243</v>
-      </c>
-      <c r="E17" s="46" t="s">
-        <v>244</v>
       </c>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>

</xml_diff>

<commit_message>
Adding dynamic data for cover page
</commit_message>
<xml_diff>
--- a/src/aat/resources/adv_bundling_functional_tests_ccd_def.xlsx
+++ b/src/aat/resources/adv_bundling_functional_tests_ccd_def.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Change History" sheetId="1" state="visible" r:id="rId2"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1283" uniqueCount="383">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1283" uniqueCount="382">
   <si>
     <t xml:space="preserve">Change History</t>
   </si>
@@ -247,7 +247,7 @@
     <t xml:space="preserve">Text</t>
   </si>
   <si>
-    <t xml:space="preserve">`</t>
+    <t xml:space="preserve">caseOwner</t>
   </si>
   <si>
     <t xml:space="preserve">Case owner</t>
@@ -402,9 +402,6 @@
   </si>
   <si>
     <t xml:space="preserve">Case Overiew</t>
-  </si>
-  <si>
-    <t xml:space="preserve">caseOwner</t>
   </si>
   <si>
     <t xml:space="preserve">CaseBundles</t>
@@ -2229,7 +2226,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="1" style="1" width="10.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="1" style="1" width="10.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="256" min="6" style="1" width="8.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="257" style="0" width="8.83"/>
   </cols>
@@ -2350,21 +2347,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="32.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="37.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="10.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="10.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="19.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="30.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="9.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="9" style="1" width="10.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="9" style="1" width="10.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="255" min="14" style="1" width="8.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="256" style="0" width="8.83"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="10" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>11</v>
@@ -2635,10 +2632,10 @@
         <v>15</v>
       </c>
       <c r="C2" s="14" t="s">
+        <v>275</v>
+      </c>
+      <c r="D2" s="14" t="s">
         <v>276</v>
-      </c>
-      <c r="D2" s="14" t="s">
-        <v>277</v>
       </c>
       <c r="E2" s="14" t="s">
         <v>46</v>
@@ -2647,16 +2644,16 @@
         <v>47</v>
       </c>
       <c r="G2" s="14" t="s">
+        <v>277</v>
+      </c>
+      <c r="H2" s="14" t="s">
         <v>278</v>
-      </c>
-      <c r="H2" s="14" t="s">
-        <v>279</v>
       </c>
       <c r="I2" s="14" t="s">
         <v>48</v>
       </c>
       <c r="J2" s="14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="K2" s="14" t="s">
         <v>32</v>
@@ -2921,7 +2918,7 @@
         <v>21</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>54</v>
@@ -2930,7 +2927,7 @@
         <v>55</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="H3" s="6" t="s">
         <v>108</v>
@@ -3199,17 +3196,17 @@
       </c>
       <c r="B4" s="72"/>
       <c r="C4" s="73" t="s">
+        <v>281</v>
+      </c>
+      <c r="D4" s="8" t="s">
         <v>282</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>283</v>
       </c>
       <c r="E4" s="8" t="s">
         <v>62</v>
       </c>
       <c r="F4" s="24"/>
       <c r="G4" s="8" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="H4" s="24"/>
       <c r="I4" s="24"/>
@@ -3468,17 +3465,17 @@
       </c>
       <c r="B5" s="60"/>
       <c r="C5" s="74" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D5" s="34" t="s">
+        <v>284</v>
+      </c>
+      <c r="E5" s="34" t="s">
         <v>285</v>
-      </c>
-      <c r="E5" s="34" t="s">
-        <v>286</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="34" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
@@ -3737,10 +3734,10 @@
       </c>
       <c r="B6" s="60"/>
       <c r="C6" s="74" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D6" s="34" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="E6" s="34" t="s">
         <v>62</v>
@@ -4006,17 +4003,17 @@
       </c>
       <c r="B7" s="83"/>
       <c r="C7" s="84" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D7" s="85" t="s">
+        <v>288</v>
+      </c>
+      <c r="E7" s="85" t="s">
         <v>289</v>
-      </c>
-      <c r="E7" s="85" t="s">
-        <v>290</v>
       </c>
       <c r="F7" s="5"/>
       <c r="G7" s="85" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
@@ -4275,17 +4272,17 @@
       </c>
       <c r="B8" s="24"/>
       <c r="C8" s="8" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E8" s="8" t="s">
         <v>62</v>
       </c>
       <c r="F8" s="24"/>
       <c r="G8" s="8" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="H8" s="24"/>
       <c r="I8" s="24"/>
@@ -4544,19 +4541,19 @@
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="34" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D9" s="34" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E9" s="34" t="s">
         <v>79</v>
       </c>
       <c r="F9" s="34" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="G9" s="34" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
@@ -4815,17 +4812,17 @@
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="85" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D10" s="85" t="s">
+        <v>284</v>
+      </c>
+      <c r="E10" s="85" t="s">
         <v>285</v>
-      </c>
-      <c r="E10" s="85" t="s">
-        <v>286</v>
       </c>
       <c r="F10" s="5"/>
       <c r="G10" s="85" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
@@ -5084,17 +5081,17 @@
       </c>
       <c r="B11" s="24"/>
       <c r="C11" s="8" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E11" s="8" t="s">
         <v>62</v>
       </c>
       <c r="F11" s="24"/>
       <c r="G11" s="8" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="H11" s="24"/>
       <c r="I11" s="24"/>
@@ -5353,19 +5350,19 @@
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="34" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D12" s="34" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E12" s="34" t="s">
         <v>79</v>
       </c>
       <c r="F12" s="34" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="G12" s="34" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
@@ -5624,19 +5621,19 @@
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="34" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D13" s="34" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E13" s="34" t="s">
         <v>79</v>
       </c>
       <c r="F13" s="34" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="G13" s="34" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
@@ -5895,17 +5892,17 @@
       </c>
       <c r="B14" s="5"/>
       <c r="C14" s="85" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D14" s="85" t="s">
+        <v>284</v>
+      </c>
+      <c r="E14" s="85" t="s">
         <v>285</v>
-      </c>
-      <c r="E14" s="85" t="s">
-        <v>286</v>
       </c>
       <c r="F14" s="5"/>
       <c r="G14" s="85" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
@@ -6167,14 +6164,14 @@
         <v>80</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E15" s="8" t="s">
         <v>62</v>
       </c>
       <c r="F15" s="24"/>
       <c r="G15" s="8" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="H15" s="24"/>
       <c r="I15" s="24"/>
@@ -6436,14 +6433,14 @@
         <v>80</v>
       </c>
       <c r="D16" s="34" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="E16" s="34" t="s">
         <v>62</v>
       </c>
       <c r="F16" s="3"/>
       <c r="G16" s="34" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
@@ -6705,7 +6702,7 @@
         <v>80</v>
       </c>
       <c r="D17" s="34" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="E17" s="34" t="s">
         <v>71</v>
@@ -6974,14 +6971,14 @@
         <v>80</v>
       </c>
       <c r="D18" s="34" t="s">
+        <v>303</v>
+      </c>
+      <c r="E18" s="34" t="s">
         <v>304</v>
-      </c>
-      <c r="E18" s="34" t="s">
-        <v>305</v>
       </c>
       <c r="F18" s="3"/>
       <c r="G18" s="34" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
@@ -7243,14 +7240,14 @@
         <v>80</v>
       </c>
       <c r="D19" s="34" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E19" s="34" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="F19" s="3"/>
       <c r="G19" s="34" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
@@ -7512,16 +7509,16 @@
         <v>80</v>
       </c>
       <c r="D20" s="34" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E20" s="34" t="s">
         <v>79</v>
       </c>
       <c r="F20" s="34" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="G20" s="34" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
@@ -7783,16 +7780,16 @@
         <v>80</v>
       </c>
       <c r="D21" s="34" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E21" s="34" t="s">
         <v>79</v>
       </c>
       <c r="F21" s="34" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="G21" s="34" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
@@ -8054,14 +8051,14 @@
         <v>80</v>
       </c>
       <c r="D22" s="34" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E22" s="34" t="s">
         <v>62</v>
       </c>
       <c r="F22" s="3"/>
       <c r="G22" s="34" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
@@ -8323,14 +8320,14 @@
         <v>80</v>
       </c>
       <c r="D23" s="34" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="E23" s="34" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="F23" s="3"/>
       <c r="G23" s="34" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
@@ -8592,14 +8589,14 @@
         <v>80</v>
       </c>
       <c r="D24" s="34" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="E24" s="34" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="F24" s="3"/>
       <c r="G24" s="34" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H24" s="3"/>
       <c r="I24" s="3"/>
@@ -8861,14 +8858,14 @@
         <v>80</v>
       </c>
       <c r="D25" s="34" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E25" s="34" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="F25" s="3"/>
       <c r="G25" s="34" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="H25" s="3"/>
       <c r="I25" s="3"/>
@@ -9130,14 +9127,14 @@
         <v>80</v>
       </c>
       <c r="D26" s="34" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E26" s="34" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="F26" s="3"/>
       <c r="G26" s="34" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="H26" s="3"/>
       <c r="I26" s="3"/>
@@ -9399,14 +9396,14 @@
         <v>80</v>
       </c>
       <c r="D27" s="34" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E27" s="34" t="s">
         <v>62</v>
       </c>
       <c r="F27" s="3"/>
       <c r="G27" s="34" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="H27" s="3"/>
       <c r="I27" s="3"/>
@@ -9668,14 +9665,14 @@
         <v>80</v>
       </c>
       <c r="D28" s="85" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E28" s="85" t="s">
         <v>62</v>
       </c>
       <c r="F28" s="5"/>
       <c r="G28" s="85" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="H28" s="5"/>
       <c r="I28" s="5"/>
@@ -9937,16 +9934,16 @@
         <v>80</v>
       </c>
       <c r="D29" s="75" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E29" s="75" t="s">
         <v>74</v>
       </c>
       <c r="F29" s="75" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="G29" s="75" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="H29" s="57"/>
       <c r="I29" s="57"/>
@@ -10208,14 +10205,14 @@
         <v>80</v>
       </c>
       <c r="D30" s="75" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E30" s="75" t="s">
         <v>62</v>
       </c>
       <c r="F30" s="58"/>
       <c r="G30" s="75" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="H30" s="57"/>
       <c r="I30" s="57"/>
@@ -10477,16 +10474,16 @@
         <v>80</v>
       </c>
       <c r="D31" s="75" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E31" s="75" t="s">
         <v>74</v>
       </c>
       <c r="F31" s="75" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G31" s="75" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="H31" s="57"/>
       <c r="I31" s="57"/>
@@ -10748,14 +10745,14 @@
         <v>83</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E32" s="8" t="s">
         <v>62</v>
       </c>
       <c r="F32" s="24"/>
       <c r="G32" s="8" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="H32" s="24"/>
       <c r="I32" s="24"/>
@@ -11017,14 +11014,14 @@
         <v>83</v>
       </c>
       <c r="D33" s="34" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E33" s="34" t="s">
         <v>62</v>
       </c>
       <c r="F33" s="3"/>
       <c r="G33" s="34" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="H33" s="3"/>
       <c r="I33" s="3"/>
@@ -11286,14 +11283,14 @@
         <v>83</v>
       </c>
       <c r="D34" s="34" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E34" s="34" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="F34" s="3"/>
       <c r="G34" s="34" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="H34" s="3"/>
       <c r="I34" s="3"/>
@@ -11555,14 +11552,14 @@
         <v>83</v>
       </c>
       <c r="D35" s="34" t="s">
+        <v>333</v>
+      </c>
+      <c r="E35" s="34" t="s">
         <v>334</v>
-      </c>
-      <c r="E35" s="34" t="s">
-        <v>335</v>
       </c>
       <c r="F35" s="3"/>
       <c r="G35" s="34" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="H35" s="3"/>
       <c r="I35" s="3"/>
@@ -11824,14 +11821,14 @@
         <v>83</v>
       </c>
       <c r="D36" s="85" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E36" s="85" t="s">
         <v>62</v>
       </c>
       <c r="F36" s="5"/>
       <c r="G36" s="85" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="H36" s="5"/>
       <c r="I36" s="5"/>
@@ -12108,17 +12105,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="20.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="29.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="5" style="1" width="10.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="29.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="5" style="1" width="10.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="256" min="11" style="1" width="8.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="257" style="0" width="8.83"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="10" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B1" s="95" t="s">
         <v>11</v>
@@ -12147,13 +12144,13 @@
         <v>42</v>
       </c>
       <c r="D2" s="14" t="s">
+        <v>339</v>
+      </c>
+      <c r="E2" s="14" t="s">
         <v>340</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="F2" s="14" t="s">
         <v>341</v>
-      </c>
-      <c r="F2" s="14" t="s">
-        <v>342</v>
       </c>
       <c r="G2" s="98"/>
       <c r="H2" s="99"/>
@@ -12177,7 +12174,7 @@
         <v>52</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G3" s="101"/>
       <c r="H3" s="102"/>
@@ -12196,7 +12193,7 @@
         <v>60</v>
       </c>
       <c r="E4" s="104" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="F4" s="51" t="n">
         <v>1</v>
@@ -12215,10 +12212,10 @@
         <v>59</v>
       </c>
       <c r="D5" s="31" t="s">
-        <v>113</v>
+        <v>63</v>
       </c>
       <c r="E5" s="35" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="F5" s="4" t="n">
         <v>2</v>
@@ -12240,7 +12237,7 @@
         <v>65</v>
       </c>
       <c r="E6" s="35" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="F6" s="4" t="n">
         <v>3</v>
@@ -12332,14 +12329,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="1" style="1" width="10.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="1" style="1" width="10.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="256" min="17" style="1" width="8.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="257" style="0" width="8.83"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="10" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>11</v>
@@ -12374,13 +12371,13 @@
         <v>42</v>
       </c>
       <c r="D2" s="14" t="s">
+        <v>346</v>
+      </c>
+      <c r="E2" s="14" t="s">
         <v>347</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="F2" s="14" t="s">
         <v>348</v>
-      </c>
-      <c r="F2" s="14" t="s">
-        <v>349</v>
       </c>
       <c r="G2" s="98"/>
       <c r="H2" s="99"/>
@@ -12410,7 +12407,7 @@
         <v>52</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G3" s="106"/>
       <c r="H3" s="107"/>
@@ -12435,7 +12432,7 @@
         <v>60</v>
       </c>
       <c r="E4" s="104" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="F4" s="51" t="n">
         <v>1</v>
@@ -12460,10 +12457,10 @@
         <v>59</v>
       </c>
       <c r="D5" s="31" t="s">
-        <v>113</v>
+        <v>63</v>
       </c>
       <c r="E5" s="35" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="F5" s="4" t="n">
         <v>2</v>
@@ -12491,7 +12488,7 @@
         <v>65</v>
       </c>
       <c r="E6" s="35" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="F6" s="4" t="n">
         <v>3</v>
@@ -12613,14 +12610,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="1" style="1" width="10.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="1" style="1" width="10.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="256" min="17" style="1" width="8.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="257" style="0" width="8.83"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="10" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>11</v>
@@ -12655,13 +12652,13 @@
         <v>42</v>
       </c>
       <c r="D2" s="14" t="s">
+        <v>346</v>
+      </c>
+      <c r="E2" s="14" t="s">
         <v>347</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="F2" s="14" t="s">
         <v>348</v>
-      </c>
-      <c r="F2" s="14" t="s">
-        <v>349</v>
       </c>
       <c r="G2" s="108"/>
       <c r="H2" s="109"/>
@@ -12691,7 +12688,7 @@
         <v>52</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G3" s="106"/>
       <c r="H3" s="107"/>
@@ -12716,7 +12713,7 @@
         <v>60</v>
       </c>
       <c r="E4" s="104" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="F4" s="51" t="n">
         <v>1</v>
@@ -12741,10 +12738,10 @@
         <v>59</v>
       </c>
       <c r="D5" s="31" t="s">
-        <v>113</v>
+        <v>63</v>
       </c>
       <c r="E5" s="35" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="F5" s="4" t="n">
         <v>2</v>
@@ -12772,7 +12769,7 @@
         <v>65</v>
       </c>
       <c r="E6" s="35" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="F6" s="4" t="n">
         <v>3</v>
@@ -12894,14 +12891,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="1" style="1" width="10.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="1" style="1" width="10.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="256" min="11" style="1" width="8.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="257" style="0" width="8.83"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="110" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B1" s="95" t="s">
         <v>11</v>
@@ -12930,13 +12927,13 @@
         <v>42</v>
       </c>
       <c r="D2" s="14" t="s">
+        <v>339</v>
+      </c>
+      <c r="E2" s="14" t="s">
         <v>340</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="F2" s="14" t="s">
         <v>341</v>
-      </c>
-      <c r="F2" s="14" t="s">
-        <v>342</v>
       </c>
       <c r="G2" s="98"/>
       <c r="H2" s="99"/>
@@ -12960,7 +12957,7 @@
         <v>52</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G3" s="101"/>
       <c r="H3" s="102"/>
@@ -12979,7 +12976,7 @@
         <v>60</v>
       </c>
       <c r="E4" s="104" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="F4" s="51" t="n">
         <v>1</v>
@@ -12998,10 +12995,10 @@
         <v>59</v>
       </c>
       <c r="D5" s="31" t="s">
-        <v>113</v>
+        <v>63</v>
       </c>
       <c r="E5" s="35" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="F5" s="4" t="n">
         <v>2</v>
@@ -13023,7 +13020,7 @@
         <v>65</v>
       </c>
       <c r="E6" s="35" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="F6" s="4" t="n">
         <v>3</v>
@@ -13115,14 +13112,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="1" style="1" width="10.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="1" style="1" width="10.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="256" min="17" style="1" width="8.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="257" style="0" width="8.83"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>11</v>
@@ -13155,13 +13152,13 @@
       </c>
       <c r="C2" s="111"/>
       <c r="D2" s="14" t="s">
+        <v>352</v>
+      </c>
+      <c r="E2" s="14" t="s">
         <v>353</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="F2" s="14" t="s">
         <v>354</v>
-      </c>
-      <c r="F2" s="14" t="s">
-        <v>355</v>
       </c>
       <c r="G2" s="13"/>
       <c r="H2" s="3"/>
@@ -13182,16 +13179,16 @@
         <v>20</v>
       </c>
       <c r="C3" s="6" t="s">
+        <v>355</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>356</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="E3" s="6" t="s">
         <v>357</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="F3" s="6" t="s">
         <v>358</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>359</v>
       </c>
       <c r="G3" s="112"/>
       <c r="H3" s="113"/>
@@ -13210,7 +13207,7 @@
       </c>
       <c r="B4" s="72"/>
       <c r="C4" s="114" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="D4" s="114" t="s">
         <v>24</v>
@@ -13219,7 +13216,7 @@
         <v>59</v>
       </c>
       <c r="F4" s="114" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G4" s="13"/>
       <c r="H4" s="3"/>
@@ -13238,7 +13235,7 @@
       </c>
       <c r="B5" s="60"/>
       <c r="C5" s="115" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="D5" s="115" t="s">
         <v>24</v>
@@ -13247,7 +13244,7 @@
         <v>59</v>
       </c>
       <c r="F5" s="115" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G5" s="13"/>
       <c r="H5" s="3"/>
@@ -13266,7 +13263,7 @@
       </c>
       <c r="B6" s="60"/>
       <c r="C6" s="115" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D6" s="115" t="s">
         <v>24</v>
@@ -13275,7 +13272,7 @@
         <v>59</v>
       </c>
       <c r="F6" s="115" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G6" s="13"/>
       <c r="H6" s="3"/>
@@ -13294,7 +13291,7 @@
       </c>
       <c r="B7" s="83"/>
       <c r="C7" s="116" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D7" s="116" t="s">
         <v>24</v>
@@ -13303,7 +13300,7 @@
         <v>59</v>
       </c>
       <c r="F7" s="116" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G7" s="13"/>
       <c r="H7" s="3"/>
@@ -13322,7 +13319,7 @@
       </c>
       <c r="B8" s="117"/>
       <c r="C8" s="11" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="D8" s="11" t="s">
         <v>24</v>
@@ -13331,7 +13328,7 @@
         <v>59</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G8" s="13"/>
       <c r="H8" s="3"/>
@@ -13404,14 +13401,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="1" style="1" width="10.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="1" style="1" width="10.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="256" min="16" style="1" width="8.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="257" style="0" width="8.83"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="10" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>11</v>
@@ -13442,13 +13439,13 @@
         <v>15</v>
       </c>
       <c r="C2" s="14" t="s">
+        <v>365</v>
+      </c>
+      <c r="D2" s="14" t="s">
         <v>366</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="E2" s="14" t="s">
         <v>367</v>
-      </c>
-      <c r="E2" s="14" t="s">
-        <v>368</v>
       </c>
       <c r="F2" s="108"/>
       <c r="G2" s="109"/>
@@ -13472,10 +13469,10 @@
         <v>51</v>
       </c>
       <c r="D3" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="E3" s="6" t="s">
         <v>369</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>370</v>
       </c>
       <c r="F3" s="13"/>
       <c r="G3" s="3"/>
@@ -13497,10 +13494,10 @@
         <v>59</v>
       </c>
       <c r="D4" s="38" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="E4" s="118" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="F4" s="13"/>
       <c r="G4" s="3"/>
@@ -13639,17 +13636,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="1" width="10.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="1" width="10.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="19.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="31.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="6" style="1" width="10.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="31.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="6" style="1" width="10.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="256" min="16" style="1" width="8.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="257" style="0" width="8.83"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="10" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>11</v>
@@ -13680,16 +13677,16 @@
         <v>15</v>
       </c>
       <c r="C2" s="14" t="s">
+        <v>372</v>
+      </c>
+      <c r="D2" s="14" t="s">
         <v>373</v>
       </c>
-      <c r="D2" s="14" t="s">
-        <v>374</v>
-      </c>
       <c r="E2" s="14" t="s">
+        <v>366</v>
+      </c>
+      <c r="F2" s="14" t="s">
         <v>367</v>
-      </c>
-      <c r="F2" s="14" t="s">
-        <v>368</v>
       </c>
       <c r="G2" s="15"/>
       <c r="H2" s="16"/>
@@ -13715,10 +13712,10 @@
         <v>106</v>
       </c>
       <c r="E3" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="F3" s="6" t="s">
         <v>369</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>370</v>
       </c>
       <c r="G3" s="17"/>
       <c r="H3" s="16"/>
@@ -13742,10 +13739,10 @@
         <v>60</v>
       </c>
       <c r="E4" s="120" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="F4" s="118" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="G4" s="13"/>
       <c r="H4" s="3"/>
@@ -13766,13 +13763,13 @@
         <v>59</v>
       </c>
       <c r="D5" s="31" t="s">
-        <v>113</v>
+        <v>63</v>
       </c>
       <c r="E5" s="122" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="F5" s="118" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="G5" s="13"/>
       <c r="H5" s="3"/>
@@ -13796,10 +13793,10 @@
         <v>65</v>
       </c>
       <c r="E6" s="122" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="F6" s="118" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="G6" s="13"/>
       <c r="H6" s="3"/>
@@ -13823,10 +13820,10 @@
         <v>67</v>
       </c>
       <c r="E7" s="122" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="F7" s="118" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="G7" s="13"/>
       <c r="H7" s="3"/>
@@ -13850,10 +13847,10 @@
         <v>69</v>
       </c>
       <c r="E8" s="122" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="F8" s="118" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="G8" s="13"/>
       <c r="H8" s="3"/>
@@ -13877,10 +13874,10 @@
         <v>72</v>
       </c>
       <c r="E9" s="122" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="F9" s="118" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="G9" s="13"/>
       <c r="H9" s="3"/>
@@ -13904,10 +13901,10 @@
         <v>76</v>
       </c>
       <c r="E10" s="122" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="F10" s="118" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="G10" s="13"/>
       <c r="H10" s="3"/>
@@ -13931,10 +13928,10 @@
         <v>81</v>
       </c>
       <c r="E11" s="122" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="F11" s="118" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="G11" s="13"/>
       <c r="H11" s="3"/>
@@ -13958,10 +13955,10 @@
         <v>84</v>
       </c>
       <c r="E12" s="124" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="F12" s="118" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="G12" s="13"/>
       <c r="H12" s="3"/>
@@ -13985,10 +13982,10 @@
         <v>85</v>
       </c>
       <c r="E13" s="122" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="F13" s="118" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="G13" s="13"/>
       <c r="H13" s="3"/>
@@ -14012,10 +14009,10 @@
         <v>87</v>
       </c>
       <c r="E14" s="122" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="F14" s="118" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="G14" s="13"/>
       <c r="H14" s="3"/>
@@ -14039,10 +14036,10 @@
         <v>89</v>
       </c>
       <c r="E15" s="122" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="F15" s="118" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="G15" s="13"/>
       <c r="H15" s="3"/>
@@ -14066,10 +14063,10 @@
         <v>91</v>
       </c>
       <c r="E16" s="122" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="F16" s="118" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="G16" s="13"/>
       <c r="H16" s="3"/>
@@ -14105,14 +14102,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="1" style="1" width="10.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="1" style="1" width="10.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="256" min="16" style="1" width="8.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="257" style="0" width="8.83"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="10" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>11</v>
@@ -14143,16 +14140,16 @@
         <v>15</v>
       </c>
       <c r="C2" s="14" t="s">
+        <v>365</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>375</v>
+      </c>
+      <c r="E2" s="14" t="s">
         <v>366</v>
       </c>
-      <c r="D2" s="14" t="s">
-        <v>376</v>
-      </c>
-      <c r="E2" s="14" t="s">
+      <c r="F2" s="14" t="s">
         <v>367</v>
-      </c>
-      <c r="F2" s="14" t="s">
-        <v>368</v>
       </c>
       <c r="G2" s="21"/>
       <c r="H2" s="22"/>
@@ -14175,13 +14172,13 @@
         <v>51</v>
       </c>
       <c r="D3" s="69" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E3" s="69" t="s">
+        <v>368</v>
+      </c>
+      <c r="F3" s="69" t="s">
         <v>369</v>
-      </c>
-      <c r="F3" s="69" t="s">
-        <v>370</v>
       </c>
       <c r="G3" s="70"/>
       <c r="H3" s="22"/>
@@ -14202,13 +14199,13 @@
         <v>59</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E4" s="126" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="F4" s="118" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="G4" s="13"/>
       <c r="H4" s="3"/>
@@ -14229,13 +14226,13 @@
         <v>59</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E5" s="128" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="F5" s="118" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="G5" s="13"/>
       <c r="H5" s="3"/>
@@ -14256,13 +14253,13 @@
         <v>59</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E6" s="128" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="F6" s="118" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="G6" s="13"/>
       <c r="H6" s="3"/>
@@ -14283,13 +14280,13 @@
         <v>59</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E7" s="128" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="F7" s="118" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="G7" s="13"/>
       <c r="H7" s="3"/>
@@ -14310,13 +14307,13 @@
         <v>59</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E8" s="128" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="F8" s="118" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="G8" s="13"/>
       <c r="H8" s="3"/>
@@ -14337,13 +14334,13 @@
         <v>59</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E9" s="128" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="F9" s="118" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="G9" s="13"/>
       <c r="H9" s="3"/>
@@ -14364,13 +14361,13 @@
         <v>59</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E10" s="128" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="F10" s="118" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="G10" s="13"/>
       <c r="H10" s="3"/>
@@ -14391,13 +14388,13 @@
         <v>59</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E11" s="128" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="F11" s="118" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="G11" s="13"/>
       <c r="H11" s="3"/>
@@ -14418,13 +14415,13 @@
         <v>59</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E12" s="128" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="F12" s="118" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="G12" s="13"/>
       <c r="H12" s="3"/>
@@ -14494,14 +14491,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="1" style="1" width="10.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="1" style="1" width="10.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="256" min="17" style="1" width="8.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="257" style="0" width="8.83"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="10" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>11</v>
@@ -14533,16 +14530,16 @@
         <v>15</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="E2" s="14" t="s">
+        <v>366</v>
+      </c>
+      <c r="F2" s="14" t="s">
         <v>367</v>
-      </c>
-      <c r="F2" s="14" t="s">
-        <v>368</v>
       </c>
       <c r="G2" s="21"/>
       <c r="H2" s="22"/>
@@ -14566,13 +14563,13 @@
         <v>51</v>
       </c>
       <c r="D3" s="69" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="E3" s="69" t="s">
+        <v>368</v>
+      </c>
+      <c r="F3" s="69" t="s">
         <v>369</v>
-      </c>
-      <c r="F3" s="69" t="s">
-        <v>370</v>
       </c>
       <c r="G3" s="70"/>
       <c r="H3" s="71"/>
@@ -14594,13 +14591,13 @@
         <v>59</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E4" s="38" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="F4" s="118" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="G4" s="13"/>
       <c r="H4" s="3"/>
@@ -14745,7 +14742,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="1" style="1" width="10.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="1" style="1" width="10.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="256" min="16" style="1" width="8.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="257" style="0" width="8.83"/>
   </cols>
@@ -14982,10 +14979,10 @@
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="33.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="30.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="30.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="15.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="10.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="10.66"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="11.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="256" min="8" style="1" width="8.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="257" style="0" width="8.83"/>
@@ -14993,7 +14990,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="10" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>11</v>
@@ -15012,19 +15009,19 @@
       <c r="A2" s="111"/>
       <c r="B2" s="111"/>
       <c r="C2" s="14" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D2" s="14" t="s">
+        <v>380</v>
+      </c>
+      <c r="E2" s="14" t="s">
         <v>381</v>
       </c>
-      <c r="E2" s="14" t="s">
-        <v>382</v>
-      </c>
       <c r="F2" s="14" t="s">
+        <v>366</v>
+      </c>
+      <c r="G2" s="14" t="s">
         <v>367</v>
-      </c>
-      <c r="G2" s="14" t="s">
-        <v>368</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15041,13 +15038,13 @@
         <v>106</v>
       </c>
       <c r="E3" s="69" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F3" s="69" t="s">
+        <v>368</v>
+      </c>
+      <c r="G3" s="69" t="s">
         <v>369</v>
-      </c>
-      <c r="G3" s="69" t="s">
-        <v>370</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15062,13 +15059,13 @@
         <v>76</v>
       </c>
       <c r="E4" s="114" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="F4" s="38" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="G4" s="118" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15083,13 +15080,13 @@
         <v>76</v>
       </c>
       <c r="E5" s="115" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="F5" s="38" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="G5" s="118" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15104,13 +15101,13 @@
         <v>76</v>
       </c>
       <c r="E6" s="115" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F6" s="38" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="G6" s="118" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15125,13 +15122,13 @@
         <v>76</v>
       </c>
       <c r="E7" s="115" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F7" s="38" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="G7" s="118" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15146,13 +15143,13 @@
         <v>76</v>
       </c>
       <c r="E8" s="115" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="F8" s="38" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="G8" s="118" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15167,13 +15164,13 @@
         <v>76</v>
       </c>
       <c r="E9" s="115" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="F9" s="38" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="G9" s="118" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15188,13 +15185,13 @@
         <v>76</v>
       </c>
       <c r="E10" s="115" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="F10" s="38" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="G10" s="118" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15209,13 +15206,13 @@
         <v>76</v>
       </c>
       <c r="E11" s="115" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F11" s="38" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="G11" s="118" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15230,13 +15227,13 @@
         <v>76</v>
       </c>
       <c r="E12" s="115" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="F12" s="38" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="G12" s="118" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15251,13 +15248,13 @@
         <v>76</v>
       </c>
       <c r="E13" s="115" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="F13" s="38" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="G13" s="118" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15272,13 +15269,13 @@
         <v>76</v>
       </c>
       <c r="E14" s="115" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="F14" s="38" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="G14" s="118" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15293,13 +15290,13 @@
         <v>76</v>
       </c>
       <c r="E15" s="115" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="F15" s="38" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="G15" s="118" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15314,13 +15311,13 @@
         <v>76</v>
       </c>
       <c r="E16" s="115" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F16" s="38" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="G16" s="118" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15335,13 +15332,13 @@
         <v>76</v>
       </c>
       <c r="E17" s="115" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F17" s="38" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="G17" s="118" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15356,13 +15353,13 @@
         <v>76</v>
       </c>
       <c r="E18" s="115" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F18" s="38" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="G18" s="118" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15377,13 +15374,13 @@
         <v>76</v>
       </c>
       <c r="E19" s="115" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="F19" s="38" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="G19" s="118" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15398,13 +15395,13 @@
         <v>76</v>
       </c>
       <c r="E20" s="116" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="F20" s="38" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="G20" s="118" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15419,13 +15416,13 @@
         <v>81</v>
       </c>
       <c r="E21" s="114" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="F21" s="38" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="G21" s="118" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15440,13 +15437,13 @@
         <v>81</v>
       </c>
       <c r="E22" s="115" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="F22" s="38" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="G22" s="118" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15461,13 +15458,13 @@
         <v>81</v>
       </c>
       <c r="E23" s="115" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="F23" s="38" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="G23" s="118" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15482,13 +15479,13 @@
         <v>81</v>
       </c>
       <c r="E24" s="115" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F24" s="38" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="G24" s="118" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15503,13 +15500,13 @@
         <v>81</v>
       </c>
       <c r="E25" s="116" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="F25" s="38" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="G25" s="118" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
   </sheetData>
@@ -15530,15 +15527,15 @@
   </sheetPr>
   <dimension ref="A1:S10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="10.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="4" style="1" width="10.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="4" style="1" width="10.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="256" min="20" style="1" width="8.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="257" style="0" width="8.83"/>
   </cols>
@@ -15827,19 +15824,19 @@
   </sheetPr>
   <dimension ref="A1:IU16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E28" activeCellId="0" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="29.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="29.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="34.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="18.17"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="6" min="6" style="1" width="8.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="13.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="255" min="8" style="1" width="10.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="255" min="8" style="1" width="10.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="256" style="0" width="8.83"/>
   </cols>
   <sheetData>
@@ -20199,13 +20196,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="1" style="1" width="10.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="1" style="1" width="10.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="23.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="26.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="24.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="31.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="18.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="1" width="10.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="18.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="1" width="10.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="256" min="12" style="1" width="8.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="257" style="0" width="8.83"/>
   </cols>
@@ -20351,7 +20348,7 @@
         <v>1</v>
       </c>
       <c r="H5" s="31" t="s">
-        <v>113</v>
+        <v>63</v>
       </c>
       <c r="I5" s="44" t="n">
         <v>2</v>
@@ -20487,10 +20484,10 @@
         <v>110</v>
       </c>
       <c r="E10" s="30" t="s">
+        <v>113</v>
+      </c>
+      <c r="F10" s="31" t="s">
         <v>114</v>
-      </c>
-      <c r="F10" s="31" t="s">
-        <v>115</v>
       </c>
       <c r="G10" s="43" t="n">
         <v>4</v>
@@ -20516,7 +20513,7 @@
         <v>110</v>
       </c>
       <c r="E11" s="30" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F11" s="31" t="s">
         <v>82</v>
@@ -20548,7 +20545,7 @@
         <v>84</v>
       </c>
       <c r="F12" s="31" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G12" s="43" t="n">
         <v>5</v>
@@ -20702,14 +20699,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="1" style="1" width="10.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="1" style="1" width="10.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="256" min="18" style="1" width="8.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="257" style="0" width="8.83"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>11</v>
@@ -20745,19 +20742,19 @@
         <v>42</v>
       </c>
       <c r="D2" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="E2" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="F2" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="G2" s="14" t="s">
         <v>121</v>
       </c>
-      <c r="G2" s="14" t="s">
+      <c r="H2" s="14" t="s">
         <v>122</v>
-      </c>
-      <c r="H2" s="14" t="s">
-        <v>123</v>
       </c>
       <c r="I2" s="15"/>
       <c r="J2" s="16"/>
@@ -20789,10 +20786,10 @@
         <v>23</v>
       </c>
       <c r="G3" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="H3" s="6" t="s">
         <v>124</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>125</v>
       </c>
       <c r="I3" s="13"/>
       <c r="J3" s="3"/>
@@ -20813,13 +20810,13 @@
         <v>59</v>
       </c>
       <c r="D4" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="E4" s="11" t="s">
         <v>126</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="F4" s="11" t="s">
         <v>127</v>
-      </c>
-      <c r="F4" s="11" t="s">
-        <v>128</v>
       </c>
       <c r="G4" s="46" t="n">
         <v>1</v>
@@ -20973,20 +20970,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="1" width="10.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="1" width="10.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="21.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="20.18"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="6" min="6" style="1" width="8.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="7" style="1" width="10.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="7" style="1" width="10.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="23.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="11" style="1" width="10.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="11" style="1" width="10.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="256" min="21" style="1" width="8.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="257" style="0" width="8.83"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>11</v>
@@ -21025,55 +21022,55 @@
         <v>42</v>
       </c>
       <c r="D2" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="E2" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="F2" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="G2" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="G2" s="14" t="s">
+      <c r="H2" s="14" t="s">
         <v>133</v>
       </c>
-      <c r="H2" s="14" t="s">
+      <c r="I2" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="I2" s="14" t="s">
+      <c r="J2" s="14" t="s">
         <v>135</v>
       </c>
-      <c r="J2" s="14" t="s">
+      <c r="K2" s="14" t="s">
         <v>136</v>
       </c>
-      <c r="K2" s="14" t="s">
-        <v>137</v>
-      </c>
       <c r="L2" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="M2" s="14" t="s">
         <v>136</v>
       </c>
-      <c r="M2" s="14" t="s">
-        <v>137</v>
-      </c>
       <c r="N2" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="O2" s="14" t="s">
         <v>136</v>
-      </c>
-      <c r="O2" s="14" t="s">
-        <v>137</v>
       </c>
       <c r="P2" s="14" t="s">
         <v>32</v>
       </c>
       <c r="Q2" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="R2" s="14" t="s">
         <v>138</v>
       </c>
-      <c r="R2" s="14" t="s">
+      <c r="S2" s="14" t="s">
         <v>139</v>
       </c>
-      <c r="S2" s="14" t="s">
+      <c r="T2" s="14" t="s">
         <v>140</v>
-      </c>
-      <c r="T2" s="14" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="56" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -21096,46 +21093,46 @@
         <v>23</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H3" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="I3" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="J3" s="23" t="s">
         <v>143</v>
       </c>
-      <c r="J3" s="23" t="s">
+      <c r="K3" s="23" t="s">
         <v>144</v>
       </c>
-      <c r="K3" s="23" t="s">
+      <c r="L3" s="23" t="s">
         <v>145</v>
       </c>
-      <c r="L3" s="23" t="s">
+      <c r="M3" s="23" t="s">
         <v>146</v>
       </c>
-      <c r="M3" s="23" t="s">
+      <c r="N3" s="23" t="s">
         <v>147</v>
       </c>
-      <c r="N3" s="23" t="s">
+      <c r="O3" s="23" t="s">
         <v>148</v>
-      </c>
-      <c r="O3" s="23" t="s">
-        <v>149</v>
       </c>
       <c r="P3" s="6" t="s">
         <v>36</v>
       </c>
       <c r="Q3" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="R3" s="6" t="s">
         <v>150</v>
       </c>
-      <c r="R3" s="6" t="s">
+      <c r="S3" s="6" t="s">
         <v>151</v>
       </c>
-      <c r="S3" s="6" t="s">
+      <c r="T3" s="6" t="s">
         <v>152</v>
-      </c>
-      <c r="T3" s="6" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -21147,20 +21144,20 @@
         <v>59</v>
       </c>
       <c r="D4" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="E4" s="11" t="s">
         <v>154</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="F4" s="11" t="s">
         <v>155</v>
-      </c>
-      <c r="F4" s="11" t="s">
-        <v>156</v>
       </c>
       <c r="G4" s="49" t="n">
         <v>1</v>
       </c>
       <c r="H4" s="24"/>
       <c r="I4" s="45" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J4" s="12"/>
       <c r="K4" s="50"/>
@@ -21173,7 +21170,7 @@
       </c>
       <c r="Q4" s="51"/>
       <c r="R4" s="52" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="S4" s="24"/>
       <c r="T4" s="24"/>
@@ -21187,22 +21184,22 @@
         <v>59</v>
       </c>
       <c r="D5" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="E5" s="11" t="s">
         <v>158</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="F5" s="11" t="s">
         <v>159</v>
-      </c>
-      <c r="F5" s="11" t="s">
-        <v>160</v>
       </c>
       <c r="G5" s="54" t="n">
         <v>2</v>
       </c>
       <c r="H5" s="34" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I5" s="53" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J5" s="12"/>
       <c r="K5" s="55"/>
@@ -21215,7 +21212,7 @@
       </c>
       <c r="Q5" s="4"/>
       <c r="R5" s="56" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="S5" s="3"/>
       <c r="T5" s="3"/>
@@ -21229,27 +21226,27 @@
         <v>59</v>
       </c>
       <c r="D6" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="E6" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="F6" s="11" t="s">
         <v>163</v>
-      </c>
-      <c r="F6" s="11" t="s">
-        <v>164</v>
       </c>
       <c r="G6" s="54" t="n">
         <v>3</v>
       </c>
       <c r="H6" s="34" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I6" s="34" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J6" s="57"/>
       <c r="K6" s="3"/>
       <c r="L6" s="58" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="M6" s="3"/>
       <c r="N6" s="57"/>
@@ -21261,7 +21258,7 @@
       </c>
       <c r="Q6" s="4"/>
       <c r="R6" s="56" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="S6" s="3"/>
       <c r="T6" s="3"/>
@@ -21275,22 +21272,22 @@
         <v>59</v>
       </c>
       <c r="D7" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="E7" s="11" t="s">
         <v>166</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="F7" s="11" t="s">
         <v>167</v>
-      </c>
-      <c r="F7" s="11" t="s">
-        <v>168</v>
       </c>
       <c r="G7" s="54" t="n">
         <v>4</v>
       </c>
       <c r="H7" s="34" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I7" s="53" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J7" s="12"/>
       <c r="K7" s="55"/>
@@ -21303,7 +21300,7 @@
       </c>
       <c r="Q7" s="4"/>
       <c r="R7" s="56" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="S7" s="3"/>
       <c r="T7" s="3"/>
@@ -21317,27 +21314,27 @@
         <v>59</v>
       </c>
       <c r="D8" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="E8" s="11" t="s">
         <v>169</v>
       </c>
-      <c r="E8" s="11" t="s">
+      <c r="F8" s="11" t="s">
         <v>170</v>
-      </c>
-      <c r="F8" s="11" t="s">
-        <v>171</v>
       </c>
       <c r="G8" s="54" t="n">
         <v>5</v>
       </c>
       <c r="H8" s="34" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I8" s="53" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J8" s="12"/>
       <c r="K8" s="55"/>
       <c r="L8" s="59" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="M8" s="13"/>
       <c r="N8" s="24"/>
@@ -21349,7 +21346,7 @@
       </c>
       <c r="Q8" s="4"/>
       <c r="R8" s="56" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="S8" s="3"/>
       <c r="T8" s="3"/>
@@ -21363,27 +21360,27 @@
         <v>59</v>
       </c>
       <c r="D9" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="E9" s="11" t="s">
         <v>173</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="F9" s="11" t="s">
         <v>174</v>
-      </c>
-      <c r="F9" s="11" t="s">
-        <v>175</v>
       </c>
       <c r="G9" s="54" t="n">
         <v>6</v>
       </c>
       <c r="H9" s="34" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I9" s="53" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J9" s="12"/>
       <c r="K9" s="55"/>
       <c r="L9" s="59" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="M9" s="13"/>
       <c r="N9" s="5"/>
@@ -21395,7 +21392,7 @@
       </c>
       <c r="Q9" s="4"/>
       <c r="R9" s="56" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="S9" s="3"/>
       <c r="T9" s="3"/>
@@ -21409,22 +21406,22 @@
         <v>59</v>
       </c>
       <c r="D10" s="11" t="s">
+        <v>176</v>
+      </c>
+      <c r="E10" s="11" t="s">
         <v>177</v>
       </c>
-      <c r="E10" s="11" t="s">
+      <c r="F10" s="11" t="s">
         <v>178</v>
-      </c>
-      <c r="F10" s="11" t="s">
-        <v>179</v>
       </c>
       <c r="G10" s="54" t="n">
         <v>7</v>
       </c>
       <c r="H10" s="34" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I10" s="53" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J10" s="12"/>
       <c r="K10" s="55"/>
@@ -21437,7 +21434,7 @@
       </c>
       <c r="Q10" s="4"/>
       <c r="R10" s="56" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="S10" s="3"/>
       <c r="T10" s="3"/>
@@ -21451,29 +21448,29 @@
         <v>59</v>
       </c>
       <c r="D11" s="11" t="s">
+        <v>179</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>169</v>
+      </c>
+      <c r="F11" s="11" t="s">
         <v>180</v>
-      </c>
-      <c r="E11" s="11" t="s">
-        <v>170</v>
-      </c>
-      <c r="F11" s="11" t="s">
-        <v>181</v>
       </c>
       <c r="G11" s="54" t="n">
         <v>5</v>
       </c>
       <c r="H11" s="34" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I11" s="53" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J11" s="11" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="K11" s="55"/>
       <c r="L11" s="11" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="M11" s="13"/>
       <c r="N11" s="57"/>
@@ -21485,7 +21482,7 @@
       </c>
       <c r="Q11" s="4"/>
       <c r="R11" s="56" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="S11" s="3"/>
       <c r="T11" s="3"/>
@@ -21499,22 +21496,22 @@
         <v>59</v>
       </c>
       <c r="D12" s="11" t="s">
+        <v>183</v>
+      </c>
+      <c r="E12" s="11" t="s">
         <v>184</v>
       </c>
-      <c r="E12" s="11" t="s">
+      <c r="F12" s="11" t="s">
         <v>185</v>
-      </c>
-      <c r="F12" s="11" t="s">
-        <v>186</v>
       </c>
       <c r="G12" s="54" t="n">
         <v>8</v>
       </c>
       <c r="H12" s="34" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I12" s="53" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J12" s="12"/>
       <c r="K12" s="55"/>
@@ -21527,7 +21524,7 @@
       </c>
       <c r="Q12" s="4"/>
       <c r="R12" s="56" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="S12" s="3"/>
       <c r="T12" s="3"/>
@@ -21541,22 +21538,22 @@
         <v>59</v>
       </c>
       <c r="D13" s="11" t="s">
+        <v>186</v>
+      </c>
+      <c r="E13" s="11" t="s">
         <v>187</v>
       </c>
-      <c r="E13" s="11" t="s">
-        <v>188</v>
-      </c>
       <c r="F13" s="11" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G13" s="54" t="n">
         <v>9</v>
       </c>
       <c r="H13" s="34" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I13" s="53" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J13" s="12"/>
       <c r="K13" s="55"/>
@@ -21569,7 +21566,7 @@
       </c>
       <c r="Q13" s="4"/>
       <c r="R13" s="56" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="S13" s="3"/>
       <c r="T13" s="3"/>
@@ -21625,17 +21622,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="1" width="10.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="27.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="1" width="10.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="27.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="38.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="6" style="1" width="10.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="6" style="1" width="10.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="256" min="16" style="1" width="8.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="257" style="0" width="8.83"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="10" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>11</v>
@@ -21669,40 +21666,40 @@
         <v>42</v>
       </c>
       <c r="D2" s="14" t="s">
+        <v>189</v>
+      </c>
+      <c r="E2" s="14" t="s">
         <v>190</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="F2" s="14" t="s">
         <v>191</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="G2" s="14" t="s">
         <v>192</v>
       </c>
-      <c r="G2" s="14" t="s">
+      <c r="H2" s="14" t="s">
         <v>193</v>
       </c>
-      <c r="H2" s="14" t="s">
+      <c r="I2" s="14" t="s">
         <v>194</v>
       </c>
-      <c r="I2" s="14" t="s">
+      <c r="J2" s="14" t="s">
         <v>195</v>
       </c>
-      <c r="J2" s="14" t="s">
+      <c r="K2" s="14" t="s">
         <v>196</v>
       </c>
-      <c r="K2" s="14" t="s">
+      <c r="L2" s="14" t="s">
         <v>197</v>
       </c>
-      <c r="L2" s="14" t="s">
+      <c r="M2" s="14" t="s">
         <v>198</v>
       </c>
-      <c r="M2" s="14" t="s">
+      <c r="N2" s="14" t="s">
         <v>199</v>
       </c>
-      <c r="N2" s="14" t="s">
-        <v>200</v>
-      </c>
       <c r="O2" s="14" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -21716,40 +21713,40 @@
         <v>51</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>106</v>
       </c>
       <c r="F3" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="G3" s="6" t="s">
         <v>202</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="H3" s="6" t="s">
         <v>203</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="I3" s="6" t="s">
         <v>204</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="J3" s="6" t="s">
         <v>205</v>
       </c>
-      <c r="J3" s="6" t="s">
+      <c r="K3" s="6" t="s">
         <v>206</v>
-      </c>
-      <c r="K3" s="6" t="s">
-        <v>207</v>
       </c>
       <c r="L3" s="6" t="s">
         <v>108</v>
       </c>
       <c r="M3" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="N3" s="6" t="s">
         <v>208</v>
       </c>
-      <c r="N3" s="6" t="s">
+      <c r="O3" s="6" t="s">
         <v>209</v>
-      </c>
-      <c r="O3" s="6" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -21761,7 +21758,7 @@
         <v>59</v>
       </c>
       <c r="D4" s="62" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E4" s="62" t="s">
         <v>60</v>
@@ -21770,13 +21767,13 @@
         <v>1</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H4" s="51" t="n">
         <v>1</v>
       </c>
       <c r="I4" s="63" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J4" s="51" t="n">
         <v>1</v>
@@ -21787,7 +21784,7 @@
       <c r="L4" s="24"/>
       <c r="M4" s="24"/>
       <c r="N4" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="O4" s="24"/>
     </row>
@@ -21800,22 +21797,22 @@
         <v>59</v>
       </c>
       <c r="D5" s="64" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E5" s="64" t="s">
-        <v>113</v>
+        <v>63</v>
       </c>
       <c r="F5" s="54" t="n">
         <v>2</v>
       </c>
       <c r="G5" s="34" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H5" s="4" t="n">
         <v>1</v>
       </c>
       <c r="I5" s="65" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J5" s="4" t="n">
         <v>1</v>
@@ -21826,7 +21823,7 @@
       <c r="L5" s="3"/>
       <c r="M5" s="3"/>
       <c r="N5" s="66" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="O5" s="3"/>
     </row>
@@ -21839,7 +21836,7 @@
         <v>59</v>
       </c>
       <c r="D6" s="64" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E6" s="64" t="s">
         <v>65</v>
@@ -21848,13 +21845,13 @@
         <v>3</v>
       </c>
       <c r="G6" s="34" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H6" s="4" t="n">
         <v>1</v>
       </c>
       <c r="I6" s="65" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J6" s="4" t="n">
         <v>1</v>
@@ -21865,7 +21862,7 @@
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
       <c r="N6" s="66" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="O6" s="3"/>
     </row>
@@ -21878,7 +21875,7 @@
         <v>59</v>
       </c>
       <c r="D7" s="64" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E7" s="64" t="s">
         <v>67</v>
@@ -21887,13 +21884,13 @@
         <v>4</v>
       </c>
       <c r="G7" s="34" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H7" s="4" t="n">
         <v>1</v>
       </c>
       <c r="I7" s="65" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J7" s="4" t="n">
         <v>1</v>
@@ -21904,7 +21901,7 @@
       <c r="L7" s="3"/>
       <c r="M7" s="3"/>
       <c r="N7" s="66" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="O7" s="3"/>
     </row>
@@ -21917,7 +21914,7 @@
         <v>59</v>
       </c>
       <c r="D8" s="67" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E8" s="67" t="s">
         <v>69</v>
@@ -21926,13 +21923,13 @@
         <v>5</v>
       </c>
       <c r="G8" s="34" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H8" s="4" t="n">
         <v>1</v>
       </c>
       <c r="I8" s="65" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J8" s="4" t="n">
         <v>1</v>
@@ -21943,7 +21940,7 @@
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
       <c r="N8" s="66" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="O8" s="3"/>
     </row>
@@ -21956,7 +21953,7 @@
         <v>59</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E9" s="11" t="s">
         <v>72</v>
@@ -21965,13 +21962,13 @@
         <v>6</v>
       </c>
       <c r="G9" s="34" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H9" s="4" t="n">
         <v>1</v>
       </c>
       <c r="I9" s="65" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="J9" s="4" t="n">
         <v>1</v>
@@ -21982,7 +21979,7 @@
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>
       <c r="N9" s="66" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="O9" s="3"/>
     </row>
@@ -21995,7 +21992,7 @@
         <v>59</v>
       </c>
       <c r="D10" s="62" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E10" s="62" t="s">
         <v>85</v>
@@ -22004,13 +22001,13 @@
         <v>7</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H10" s="51" t="n">
         <v>1</v>
       </c>
       <c r="I10" s="63" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J10" s="51" t="n">
         <v>1</v>
@@ -22021,7 +22018,7 @@
       <c r="L10" s="24"/>
       <c r="M10" s="24"/>
       <c r="N10" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="O10" s="24"/>
     </row>
@@ -22034,7 +22031,7 @@
         <v>59</v>
       </c>
       <c r="D11" s="62" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E11" s="62" t="s">
         <v>87</v>
@@ -22043,13 +22040,13 @@
         <v>8</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H11" s="51" t="n">
         <v>1</v>
       </c>
       <c r="I11" s="63" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J11" s="51" t="n">
         <v>1</v>
@@ -22060,7 +22057,7 @@
       <c r="L11" s="24"/>
       <c r="M11" s="24"/>
       <c r="N11" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="O11" s="24"/>
     </row>
@@ -22073,7 +22070,7 @@
         <v>59</v>
       </c>
       <c r="D12" s="62" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E12" s="62" t="s">
         <v>89</v>
@@ -22082,13 +22079,13 @@
         <v>9</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H12" s="51" t="n">
         <v>1</v>
       </c>
       <c r="I12" s="63" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J12" s="51" t="n">
         <v>1</v>
@@ -22099,7 +22096,7 @@
       <c r="L12" s="24"/>
       <c r="M12" s="24"/>
       <c r="N12" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="O12" s="24"/>
     </row>
@@ -22112,7 +22109,7 @@
         <v>59</v>
       </c>
       <c r="D13" s="62" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E13" s="62" t="s">
         <v>91</v>
@@ -22121,13 +22118,13 @@
         <v>10</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H13" s="51" t="n">
         <v>1</v>
       </c>
       <c r="I13" s="63" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J13" s="51" t="n">
         <v>1</v>
@@ -22138,7 +22135,7 @@
       <c r="L13" s="24"/>
       <c r="M13" s="24"/>
       <c r="N13" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="O13" s="24"/>
     </row>
@@ -22151,7 +22148,7 @@
         <v>59</v>
       </c>
       <c r="D14" s="62" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E14" s="62" t="s">
         <v>60</v>
@@ -22160,13 +22157,13 @@
         <v>1</v>
       </c>
       <c r="G14" s="34" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H14" s="4" t="n">
         <v>1</v>
       </c>
       <c r="I14" s="65" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="J14" s="4" t="n">
         <v>1</v>
@@ -22188,22 +22185,22 @@
         <v>59</v>
       </c>
       <c r="D15" s="64" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E15" s="64" t="s">
-        <v>113</v>
+        <v>63</v>
       </c>
       <c r="F15" s="54" t="n">
         <v>2</v>
       </c>
       <c r="G15" s="34" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H15" s="4" t="n">
         <v>1</v>
       </c>
       <c r="I15" s="65" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="J15" s="4" t="n">
         <v>1</v>
@@ -22225,7 +22222,7 @@
         <v>59</v>
       </c>
       <c r="D16" s="64" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E16" s="64" t="s">
         <v>65</v>
@@ -22234,13 +22231,13 @@
         <v>3</v>
       </c>
       <c r="G16" s="34" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H16" s="4" t="n">
         <v>1</v>
       </c>
       <c r="I16" s="65" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="J16" s="4" t="n">
         <v>1</v>
@@ -22262,7 +22259,7 @@
         <v>59</v>
       </c>
       <c r="D17" s="64" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E17" s="64" t="s">
         <v>67</v>
@@ -22271,13 +22268,13 @@
         <v>4</v>
       </c>
       <c r="G17" s="34" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H17" s="4" t="n">
         <v>1</v>
       </c>
       <c r="I17" s="65" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="J17" s="4" t="n">
         <v>1</v>
@@ -22299,7 +22296,7 @@
         <v>59</v>
       </c>
       <c r="D18" s="67" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E18" s="67" t="s">
         <v>69</v>
@@ -22308,13 +22305,13 @@
         <v>5</v>
       </c>
       <c r="G18" s="34" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H18" s="4" t="n">
         <v>1</v>
       </c>
       <c r="I18" s="65" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="J18" s="4" t="n">
         <v>1</v>
@@ -22336,7 +22333,7 @@
         <v>59</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E19" s="11" t="s">
         <v>72</v>
@@ -22345,13 +22342,13 @@
         <v>6</v>
       </c>
       <c r="G19" s="34" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H19" s="4" t="n">
         <v>1</v>
       </c>
       <c r="I19" s="65" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="J19" s="4" t="n">
         <v>1</v>
@@ -22373,7 +22370,7 @@
         <v>59</v>
       </c>
       <c r="D20" s="62" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E20" s="62" t="s">
         <v>85</v>
@@ -22382,13 +22379,13 @@
         <v>7</v>
       </c>
       <c r="G20" s="34" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H20" s="4" t="n">
         <v>1</v>
       </c>
       <c r="I20" s="65" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="J20" s="4" t="n">
         <v>1</v>
@@ -22410,7 +22407,7 @@
         <v>59</v>
       </c>
       <c r="D21" s="62" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E21" s="62" t="s">
         <v>87</v>
@@ -22419,13 +22416,13 @@
         <v>8</v>
       </c>
       <c r="G21" s="34" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H21" s="4" t="n">
         <v>1</v>
       </c>
       <c r="I21" s="65" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="J21" s="4" t="n">
         <v>1</v>
@@ -22447,7 +22444,7 @@
         <v>59</v>
       </c>
       <c r="D22" s="62" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E22" s="62" t="s">
         <v>89</v>
@@ -22456,13 +22453,13 @@
         <v>9</v>
       </c>
       <c r="G22" s="34" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H22" s="4" t="n">
         <v>1</v>
       </c>
       <c r="I22" s="65" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="J22" s="4" t="n">
         <v>1</v>
@@ -22484,7 +22481,7 @@
         <v>59</v>
       </c>
       <c r="D23" s="62" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E23" s="62" t="s">
         <v>91</v>
@@ -22493,13 +22490,13 @@
         <v>10</v>
       </c>
       <c r="G23" s="34" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H23" s="4" t="n">
         <v>1</v>
       </c>
       <c r="I23" s="65" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="J23" s="4" t="n">
         <v>1</v>
@@ -22521,7 +22518,7 @@
         <v>59</v>
       </c>
       <c r="D24" s="11" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E24" s="11" t="s">
         <v>76</v>
@@ -22530,13 +22527,13 @@
         <v>1</v>
       </c>
       <c r="G24" s="34" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H24" s="4" t="n">
         <v>1</v>
       </c>
       <c r="I24" s="65" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J24" s="4" t="n">
         <v>1</v>
@@ -22558,7 +22555,7 @@
         <v>59</v>
       </c>
       <c r="D25" s="11" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E25" s="11" t="s">
         <v>76</v>
@@ -22567,13 +22564,13 @@
         <v>1</v>
       </c>
       <c r="G25" s="34" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H25" s="4" t="n">
         <v>1</v>
       </c>
       <c r="I25" s="65" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="J25" s="4" t="n">
         <v>1</v>
@@ -22595,7 +22592,7 @@
         <v>59</v>
       </c>
       <c r="D26" s="11" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E26" s="11" t="s">
         <v>76</v>
@@ -22604,13 +22601,13 @@
         <v>1</v>
       </c>
       <c r="G26" s="34" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H26" s="4" t="n">
         <v>1</v>
       </c>
       <c r="I26" s="65" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="J26" s="4" t="n">
         <v>1</v>
@@ -22632,7 +22629,7 @@
         <v>59</v>
       </c>
       <c r="D27" s="11" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E27" s="11" t="s">
         <v>76</v>
@@ -22641,13 +22638,13 @@
         <v>1</v>
       </c>
       <c r="G27" s="34" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H27" s="4" t="n">
         <v>1</v>
       </c>
       <c r="I27" s="65" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="J27" s="4" t="n">
         <v>1</v>
@@ -22669,7 +22666,7 @@
         <v>59</v>
       </c>
       <c r="D28" s="11" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E28" s="11" t="s">
         <v>81</v>
@@ -22678,13 +22675,13 @@
         <v>1</v>
       </c>
       <c r="G28" s="34" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H28" s="4" t="n">
         <v>1</v>
       </c>
       <c r="I28" s="65" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="J28" s="4" t="n">
         <v>1</v>
@@ -22706,7 +22703,7 @@
         <v>59</v>
       </c>
       <c r="D29" s="11" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E29" s="11" t="s">
         <v>84</v>
@@ -22715,13 +22712,13 @@
         <v>1</v>
       </c>
       <c r="G29" s="34" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H29" s="4" t="n">
         <v>1</v>
       </c>
       <c r="I29" s="65" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J29" s="4" t="n">
         <v>1</v>
@@ -22792,18 +22789,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="23.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="33.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="33.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="44.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="6" style="1" width="10.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="6" style="1" width="10.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="256" min="15" style="1" width="8.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="257" style="0" width="8.83"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="10" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>11</v>
@@ -22833,13 +22830,13 @@
         <v>15</v>
       </c>
       <c r="C2" s="14" t="s">
+        <v>220</v>
+      </c>
+      <c r="D2" s="14" t="s">
         <v>221</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="E2" s="14" t="s">
         <v>222</v>
-      </c>
-      <c r="E2" s="14" t="s">
-        <v>223</v>
       </c>
       <c r="F2" s="21"/>
       <c r="G2" s="22"/>
@@ -22862,10 +22859,10 @@
         <v>21</v>
       </c>
       <c r="D3" s="69" t="s">
+        <v>223</v>
+      </c>
+      <c r="E3" s="69" t="s">
         <v>224</v>
-      </c>
-      <c r="E3" s="69" t="s">
-        <v>225</v>
       </c>
       <c r="F3" s="70"/>
       <c r="G3" s="71"/>
@@ -22883,13 +22880,13 @@
       </c>
       <c r="B4" s="72"/>
       <c r="C4" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="D4" s="11" t="s">
         <v>226</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="E4" s="11" t="s">
         <v>227</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>228</v>
       </c>
       <c r="F4" s="13"/>
       <c r="G4" s="3"/>
@@ -22910,10 +22907,10 @@
         <v>75</v>
       </c>
       <c r="D5" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="E5" s="11" t="s">
         <v>229</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>230</v>
       </c>
       <c r="F5" s="13"/>
       <c r="G5" s="3"/>
@@ -22934,10 +22931,10 @@
         <v>75</v>
       </c>
       <c r="D6" s="73" t="s">
+        <v>230</v>
+      </c>
+      <c r="E6" s="8" t="s">
         <v>231</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>232</v>
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
@@ -22958,10 +22955,10 @@
         <v>75</v>
       </c>
       <c r="D7" s="74" t="s">
+        <v>232</v>
+      </c>
+      <c r="E7" s="34" t="s">
         <v>233</v>
-      </c>
-      <c r="E7" s="34" t="s">
-        <v>234</v>
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
@@ -22982,10 +22979,10 @@
         <v>75</v>
       </c>
       <c r="D8" s="74" t="s">
+        <v>234</v>
+      </c>
+      <c r="E8" s="34" t="s">
         <v>235</v>
-      </c>
-      <c r="E8" s="34" t="s">
-        <v>236</v>
       </c>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
@@ -23006,10 +23003,10 @@
         <v>75</v>
       </c>
       <c r="D9" s="74" t="s">
+        <v>236</v>
+      </c>
+      <c r="E9" s="34" t="s">
         <v>237</v>
-      </c>
-      <c r="E9" s="34" t="s">
-        <v>238</v>
       </c>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
@@ -23030,10 +23027,10 @@
         <v>75</v>
       </c>
       <c r="D10" s="74" t="s">
+        <v>238</v>
+      </c>
+      <c r="E10" s="34" t="s">
         <v>239</v>
-      </c>
-      <c r="E10" s="34" t="s">
-        <v>240</v>
       </c>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
@@ -23054,10 +23051,10 @@
         <v>75</v>
       </c>
       <c r="D11" s="74" t="s">
+        <v>240</v>
+      </c>
+      <c r="E11" s="34" t="s">
         <v>241</v>
-      </c>
-      <c r="E11" s="34" t="s">
-        <v>242</v>
       </c>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
@@ -23078,10 +23075,10 @@
         <v>75</v>
       </c>
       <c r="D12" s="74" t="s">
+        <v>242</v>
+      </c>
+      <c r="E12" s="34" t="s">
         <v>243</v>
-      </c>
-      <c r="E12" s="34" t="s">
-        <v>244</v>
       </c>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
@@ -23102,10 +23099,10 @@
         <v>75</v>
       </c>
       <c r="D13" s="74" t="s">
+        <v>244</v>
+      </c>
+      <c r="E13" s="34" t="s">
         <v>245</v>
-      </c>
-      <c r="E13" s="34" t="s">
-        <v>246</v>
       </c>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
@@ -23126,10 +23123,10 @@
         <v>75</v>
       </c>
       <c r="D14" s="74" t="s">
+        <v>246</v>
+      </c>
+      <c r="E14" s="34" t="s">
         <v>247</v>
-      </c>
-      <c r="E14" s="34" t="s">
-        <v>248</v>
       </c>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
@@ -23150,10 +23147,10 @@
         <v>75</v>
       </c>
       <c r="D15" s="74" t="s">
+        <v>248</v>
+      </c>
+      <c r="E15" s="34" t="s">
         <v>249</v>
-      </c>
-      <c r="E15" s="34" t="s">
-        <v>250</v>
       </c>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
@@ -23174,10 +23171,10 @@
         <v>75</v>
       </c>
       <c r="D16" s="74" t="s">
+        <v>250</v>
+      </c>
+      <c r="E16" s="34" t="s">
         <v>251</v>
-      </c>
-      <c r="E16" s="34" t="s">
-        <v>252</v>
       </c>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
@@ -23198,10 +23195,10 @@
         <v>75</v>
       </c>
       <c r="D17" s="74" t="s">
+        <v>252</v>
+      </c>
+      <c r="E17" s="34" t="s">
         <v>253</v>
-      </c>
-      <c r="E17" s="34" t="s">
-        <v>254</v>
       </c>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
@@ -23219,13 +23216,13 @@
       </c>
       <c r="B18" s="3"/>
       <c r="C18" s="75" t="s">
+        <v>254</v>
+      </c>
+      <c r="D18" s="34" t="s">
         <v>255</v>
       </c>
-      <c r="D18" s="34" t="s">
+      <c r="E18" s="34" t="s">
         <v>256</v>
-      </c>
-      <c r="E18" s="34" t="s">
-        <v>257</v>
       </c>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
@@ -23243,13 +23240,13 @@
       </c>
       <c r="B19" s="3"/>
       <c r="C19" s="75" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D19" s="34" t="s">
+        <v>257</v>
+      </c>
+      <c r="E19" s="34" t="s">
         <v>258</v>
-      </c>
-      <c r="E19" s="34" t="s">
-        <v>259</v>
       </c>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
@@ -23267,13 +23264,13 @@
       </c>
       <c r="B20" s="3"/>
       <c r="C20" s="75" t="s">
+        <v>259</v>
+      </c>
+      <c r="D20" s="34" t="s">
         <v>260</v>
       </c>
-      <c r="D20" s="34" t="s">
+      <c r="E20" s="34" t="s">
         <v>261</v>
-      </c>
-      <c r="E20" s="34" t="s">
-        <v>262</v>
       </c>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
@@ -23291,13 +23288,13 @@
       </c>
       <c r="B21" s="3"/>
       <c r="C21" s="75" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D21" s="34" t="s">
+        <v>262</v>
+      </c>
+      <c r="E21" s="34" t="s">
         <v>263</v>
-      </c>
-      <c r="E21" s="34" t="s">
-        <v>264</v>
       </c>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
@@ -23315,13 +23312,13 @@
       </c>
       <c r="B22" s="3"/>
       <c r="C22" s="75" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D22" s="34" t="s">
+        <v>264</v>
+      </c>
+      <c r="E22" s="34" t="s">
         <v>265</v>
-      </c>
-      <c r="E22" s="34" t="s">
-        <v>266</v>
       </c>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
@@ -23339,13 +23336,13 @@
       </c>
       <c r="B23" s="3"/>
       <c r="C23" s="75" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D23" s="34" t="s">
+        <v>266</v>
+      </c>
+      <c r="E23" s="34" t="s">
         <v>267</v>
-      </c>
-      <c r="E23" s="34" t="s">
-        <v>268</v>
       </c>
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
@@ -23363,13 +23360,13 @@
       </c>
       <c r="B24" s="3"/>
       <c r="C24" s="75" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D24" s="34" t="s">
+        <v>268</v>
+      </c>
+      <c r="E24" s="34" t="s">
         <v>269</v>
-      </c>
-      <c r="E24" s="34" t="s">
-        <v>270</v>
       </c>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
@@ -23387,13 +23384,13 @@
       </c>
       <c r="B25" s="3"/>
       <c r="C25" s="75" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D25" s="34" t="s">
+        <v>270</v>
+      </c>
+      <c r="E25" s="34" t="s">
         <v>271</v>
-      </c>
-      <c r="E25" s="34" t="s">
-        <v>272</v>
       </c>
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
@@ -23411,13 +23408,13 @@
       </c>
       <c r="B26" s="3"/>
       <c r="C26" s="75" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D26" s="34" t="s">
+        <v>272</v>
+      </c>
+      <c r="E26" s="34" t="s">
         <v>273</v>
-      </c>
-      <c r="E26" s="34" t="s">
-        <v>274</v>
       </c>
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>

</xml_diff>

<commit_message>
add sub sub folders to ccd definition file
</commit_message>
<xml_diff>
--- a/src/aat/resources/adv_bundling_functional_tests_ccd_def.xlsx
+++ b/src/aat/resources/adv_bundling_functional_tests_ccd_def.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="19"/>
   </bookViews>
   <sheets>
     <sheet name="Change History" sheetId="1" state="visible" r:id="rId2"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1259" uniqueCount="381">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1281" uniqueCount="382">
   <si>
     <t xml:space="preserve">Change History</t>
   </si>
@@ -971,28 +971,31 @@
     <t xml:space="preserve">Source Document</t>
   </si>
   <si>
+    <t xml:space="preserve">BundleSubfolder2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subfolder Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">documents</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Folder Documents</t>
+  </si>
+  <si>
     <t xml:space="preserve">BundleSubfolder</t>
   </si>
   <si>
-    <t xml:space="preserve">Subfolder Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">documents</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Folder Documents</t>
+    <t xml:space="preserve">folders</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subfolders</t>
   </si>
   <si>
     <t xml:space="preserve">BundleFolder</t>
   </si>
   <si>
     <t xml:space="preserve">Folder Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">folders</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Subfolders</t>
   </si>
   <si>
     <t xml:space="preserve">id</t>
@@ -2336,10 +2339,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:IU36"/>
+  <dimension ref="A1:IU40"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4537,7 +4540,7 @@
         <v>42736</v>
       </c>
       <c r="B9" s="3"/>
-      <c r="C9" s="34" t="s">
+      <c r="C9" s="8" t="s">
         <v>290</v>
       </c>
       <c r="D9" s="34" t="s">
@@ -4808,7 +4811,7 @@
         <v>42736</v>
       </c>
       <c r="B10" s="5"/>
-      <c r="C10" s="85" t="s">
+      <c r="C10" s="8" t="s">
         <v>290</v>
       </c>
       <c r="D10" s="85" t="s">
@@ -5088,7 +5091,7 @@
       </c>
       <c r="F11" s="24"/>
       <c r="G11" s="8" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="H11" s="24"/>
       <c r="I11" s="24"/>
@@ -5621,7 +5624,7 @@
         <v>294</v>
       </c>
       <c r="D13" s="34" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E13" s="34" t="s">
         <v>78</v>
@@ -5630,7 +5633,7 @@
         <v>290</v>
       </c>
       <c r="G13" s="34" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
@@ -6158,17 +6161,17 @@
       </c>
       <c r="B15" s="24"/>
       <c r="C15" s="8" t="s">
-        <v>79</v>
+        <v>297</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>298</v>
+        <v>281</v>
       </c>
       <c r="E15" s="8" t="s">
         <v>61</v>
       </c>
       <c r="F15" s="24"/>
       <c r="G15" s="8" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="H15" s="24"/>
       <c r="I15" s="24"/>
@@ -6427,17 +6430,19 @@
       </c>
       <c r="B16" s="3"/>
       <c r="C16" s="34" t="s">
-        <v>79</v>
+        <v>297</v>
       </c>
       <c r="D16" s="34" t="s">
-        <v>300</v>
+        <v>292</v>
       </c>
       <c r="E16" s="34" t="s">
-        <v>61</v>
-      </c>
-      <c r="F16" s="3"/>
+        <v>78</v>
+      </c>
+      <c r="F16" s="34" t="s">
+        <v>280</v>
+      </c>
       <c r="G16" s="34" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
@@ -6696,17 +6701,19 @@
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="34" t="s">
-        <v>79</v>
+        <v>297</v>
       </c>
       <c r="D17" s="34" t="s">
-        <v>286</v>
+        <v>295</v>
       </c>
       <c r="E17" s="34" t="s">
-        <v>70</v>
-      </c>
-      <c r="F17" s="3"/>
+        <v>78</v>
+      </c>
+      <c r="F17" s="34" t="s">
+        <v>294</v>
+      </c>
       <c r="G17" s="34" t="s">
-        <v>23</v>
+        <v>296</v>
       </c>
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
@@ -6960,27 +6967,27 @@
       <c r="IU17" s="80"/>
     </row>
     <row r="18" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="88" t="n">
+      <c r="A18" s="89" t="n">
         <v>42736</v>
       </c>
-      <c r="B18" s="3"/>
-      <c r="C18" s="34" t="s">
-        <v>79</v>
-      </c>
-      <c r="D18" s="34" t="s">
-        <v>302</v>
-      </c>
-      <c r="E18" s="34" t="s">
-        <v>303</v>
-      </c>
-      <c r="F18" s="3"/>
-      <c r="G18" s="34" t="s">
-        <v>304</v>
-      </c>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="53" t="s">
+      <c r="B18" s="5"/>
+      <c r="C18" s="85" t="s">
+        <v>297</v>
+      </c>
+      <c r="D18" s="85" t="s">
+        <v>283</v>
+      </c>
+      <c r="E18" s="85" t="s">
+        <v>284</v>
+      </c>
+      <c r="F18" s="5"/>
+      <c r="G18" s="85" t="s">
+        <v>285</v>
+      </c>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="86" t="s">
         <v>40</v>
       </c>
       <c r="L18" s="13"/>
@@ -7229,27 +7236,27 @@
       <c r="IU18" s="80"/>
     </row>
     <row r="19" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="88" t="n">
+      <c r="A19" s="87" t="n">
         <v>42736</v>
       </c>
-      <c r="B19" s="3"/>
-      <c r="C19" s="34" t="s">
+      <c r="B19" s="24"/>
+      <c r="C19" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="D19" s="34" t="s">
-        <v>305</v>
-      </c>
-      <c r="E19" s="34" t="s">
-        <v>303</v>
-      </c>
-      <c r="F19" s="3"/>
-      <c r="G19" s="34" t="s">
-        <v>306</v>
-      </c>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
-      <c r="K19" s="53" t="s">
+      <c r="D19" s="8" t="s">
+        <v>299</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="F19" s="24"/>
+      <c r="G19" s="8" t="s">
+        <v>300</v>
+      </c>
+      <c r="H19" s="24"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
+      <c r="K19" s="45" t="s">
         <v>40</v>
       </c>
       <c r="L19" s="13"/>
@@ -7506,16 +7513,14 @@
         <v>79</v>
       </c>
       <c r="D20" s="34" t="s">
-        <v>292</v>
+        <v>301</v>
       </c>
       <c r="E20" s="34" t="s">
-        <v>78</v>
-      </c>
-      <c r="F20" s="34" t="s">
-        <v>280</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="F20" s="3"/>
       <c r="G20" s="34" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
@@ -7777,16 +7782,14 @@
         <v>79</v>
       </c>
       <c r="D21" s="34" t="s">
-        <v>296</v>
+        <v>286</v>
       </c>
       <c r="E21" s="34" t="s">
-        <v>78</v>
-      </c>
-      <c r="F21" s="34" t="s">
-        <v>294</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="F21" s="3"/>
       <c r="G21" s="34" t="s">
-        <v>308</v>
+        <v>23</v>
       </c>
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
@@ -8048,14 +8051,14 @@
         <v>79</v>
       </c>
       <c r="D22" s="34" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
       <c r="E22" s="34" t="s">
-        <v>61</v>
+        <v>304</v>
       </c>
       <c r="F22" s="3"/>
       <c r="G22" s="34" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
@@ -8317,14 +8320,14 @@
         <v>79</v>
       </c>
       <c r="D23" s="34" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="E23" s="34" t="s">
-        <v>288</v>
+        <v>304</v>
       </c>
       <c r="F23" s="3"/>
       <c r="G23" s="34" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
@@ -8586,14 +8589,16 @@
         <v>79</v>
       </c>
       <c r="D24" s="34" t="s">
-        <v>313</v>
+        <v>292</v>
       </c>
       <c r="E24" s="34" t="s">
-        <v>303</v>
-      </c>
-      <c r="F24" s="3"/>
+        <v>78</v>
+      </c>
+      <c r="F24" s="34" t="s">
+        <v>280</v>
+      </c>
       <c r="G24" s="34" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="H24" s="3"/>
       <c r="I24" s="3"/>
@@ -8855,14 +8860,16 @@
         <v>79</v>
       </c>
       <c r="D25" s="34" t="s">
-        <v>315</v>
+        <v>295</v>
       </c>
       <c r="E25" s="34" t="s">
-        <v>303</v>
-      </c>
-      <c r="F25" s="3"/>
+        <v>78</v>
+      </c>
+      <c r="F25" s="34" t="s">
+        <v>297</v>
+      </c>
       <c r="G25" s="34" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="H25" s="3"/>
       <c r="I25" s="3"/>
@@ -9124,14 +9131,14 @@
         <v>79</v>
       </c>
       <c r="D26" s="34" t="s">
-        <v>317</v>
+        <v>310</v>
       </c>
       <c r="E26" s="34" t="s">
-        <v>303</v>
+        <v>61</v>
       </c>
       <c r="F26" s="3"/>
       <c r="G26" s="34" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
       <c r="H26" s="3"/>
       <c r="I26" s="3"/>
@@ -9393,14 +9400,14 @@
         <v>79</v>
       </c>
       <c r="D27" s="34" t="s">
-        <v>319</v>
+        <v>312</v>
       </c>
       <c r="E27" s="34" t="s">
-        <v>61</v>
+        <v>288</v>
       </c>
       <c r="F27" s="3"/>
       <c r="G27" s="34" t="s">
-        <v>320</v>
+        <v>313</v>
       </c>
       <c r="H27" s="3"/>
       <c r="I27" s="3"/>
@@ -9654,27 +9661,27 @@
       <c r="IU27" s="80"/>
     </row>
     <row r="28" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="89" t="n">
+      <c r="A28" s="88" t="n">
         <v>42736</v>
       </c>
-      <c r="B28" s="5"/>
-      <c r="C28" s="85" t="s">
+      <c r="B28" s="3"/>
+      <c r="C28" s="34" t="s">
         <v>79</v>
       </c>
-      <c r="D28" s="85" t="s">
-        <v>321</v>
-      </c>
-      <c r="E28" s="85" t="s">
-        <v>61</v>
-      </c>
-      <c r="F28" s="5"/>
-      <c r="G28" s="85" t="s">
-        <v>322</v>
-      </c>
-      <c r="H28" s="5"/>
-      <c r="I28" s="5"/>
-      <c r="J28" s="5"/>
-      <c r="K28" s="86" t="s">
+      <c r="D28" s="34" t="s">
+        <v>314</v>
+      </c>
+      <c r="E28" s="34" t="s">
+        <v>304</v>
+      </c>
+      <c r="F28" s="3"/>
+      <c r="G28" s="34" t="s">
+        <v>315</v>
+      </c>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
+      <c r="J28" s="3"/>
+      <c r="K28" s="53" t="s">
         <v>40</v>
       </c>
       <c r="L28" s="13"/>
@@ -9923,29 +9930,27 @@
       <c r="IU28" s="80"/>
     </row>
     <row r="29" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="90" t="n">
+      <c r="A29" s="88" t="n">
         <v>42736</v>
       </c>
-      <c r="B29" s="57"/>
-      <c r="C29" s="75" t="s">
+      <c r="B29" s="3"/>
+      <c r="C29" s="34" t="s">
         <v>79</v>
       </c>
-      <c r="D29" s="75" t="s">
-        <v>258</v>
-      </c>
-      <c r="E29" s="75" t="s">
-        <v>73</v>
-      </c>
-      <c r="F29" s="75" t="s">
-        <v>258</v>
-      </c>
-      <c r="G29" s="75" t="s">
-        <v>323</v>
-      </c>
-      <c r="H29" s="57"/>
-      <c r="I29" s="57"/>
-      <c r="J29" s="57"/>
-      <c r="K29" s="91" t="s">
+      <c r="D29" s="34" t="s">
+        <v>316</v>
+      </c>
+      <c r="E29" s="34" t="s">
+        <v>304</v>
+      </c>
+      <c r="F29" s="3"/>
+      <c r="G29" s="34" t="s">
+        <v>317</v>
+      </c>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
+      <c r="J29" s="3"/>
+      <c r="K29" s="53" t="s">
         <v>40</v>
       </c>
       <c r="L29" s="13"/>
@@ -10194,27 +10199,27 @@
       <c r="IU29" s="80"/>
     </row>
     <row r="30" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="90" t="n">
+      <c r="A30" s="88" t="n">
         <v>42736</v>
       </c>
-      <c r="B30" s="57"/>
-      <c r="C30" s="75" t="s">
+      <c r="B30" s="3"/>
+      <c r="C30" s="34" t="s">
         <v>79</v>
       </c>
-      <c r="D30" s="75" t="s">
-        <v>324</v>
-      </c>
-      <c r="E30" s="75" t="s">
-        <v>61</v>
-      </c>
-      <c r="F30" s="58"/>
-      <c r="G30" s="75" t="s">
-        <v>325</v>
-      </c>
-      <c r="H30" s="57"/>
-      <c r="I30" s="57"/>
-      <c r="J30" s="57"/>
-      <c r="K30" s="91" t="s">
+      <c r="D30" s="34" t="s">
+        <v>318</v>
+      </c>
+      <c r="E30" s="34" t="s">
+        <v>304</v>
+      </c>
+      <c r="F30" s="3"/>
+      <c r="G30" s="34" t="s">
+        <v>319</v>
+      </c>
+      <c r="H30" s="3"/>
+      <c r="I30" s="3"/>
+      <c r="J30" s="3"/>
+      <c r="K30" s="53" t="s">
         <v>40</v>
       </c>
       <c r="L30" s="13"/>
@@ -10463,29 +10468,27 @@
       <c r="IU30" s="80"/>
     </row>
     <row r="31" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="90" t="n">
+      <c r="A31" s="88" t="n">
         <v>42736</v>
       </c>
-      <c r="B31" s="57"/>
-      <c r="C31" s="75" t="s">
+      <c r="B31" s="3"/>
+      <c r="C31" s="34" t="s">
         <v>79</v>
       </c>
-      <c r="D31" s="75" t="s">
-        <v>253</v>
-      </c>
-      <c r="E31" s="75" t="s">
-        <v>73</v>
-      </c>
-      <c r="F31" s="75" t="s">
-        <v>253</v>
-      </c>
-      <c r="G31" s="75" t="s">
-        <v>326</v>
-      </c>
-      <c r="H31" s="57"/>
-      <c r="I31" s="57"/>
-      <c r="J31" s="57"/>
-      <c r="K31" s="91" t="s">
+      <c r="D31" s="34" t="s">
+        <v>320</v>
+      </c>
+      <c r="E31" s="34" t="s">
+        <v>61</v>
+      </c>
+      <c r="F31" s="3"/>
+      <c r="G31" s="34" t="s">
+        <v>321</v>
+      </c>
+      <c r="H31" s="3"/>
+      <c r="I31" s="3"/>
+      <c r="J31" s="3"/>
+      <c r="K31" s="53" t="s">
         <v>40</v>
       </c>
       <c r="L31" s="13"/>
@@ -10734,27 +10737,27 @@
       <c r="IU31" s="80"/>
     </row>
     <row r="32" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="87" t="n">
+      <c r="A32" s="89" t="n">
         <v>42736</v>
       </c>
-      <c r="B32" s="24"/>
-      <c r="C32" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="D32" s="8" t="s">
-        <v>327</v>
-      </c>
-      <c r="E32" s="8" t="s">
+      <c r="B32" s="5"/>
+      <c r="C32" s="85" t="s">
+        <v>79</v>
+      </c>
+      <c r="D32" s="85" t="s">
+        <v>322</v>
+      </c>
+      <c r="E32" s="85" t="s">
         <v>61</v>
       </c>
-      <c r="F32" s="24"/>
-      <c r="G32" s="8" t="s">
-        <v>328</v>
-      </c>
-      <c r="H32" s="24"/>
-      <c r="I32" s="24"/>
-      <c r="J32" s="24"/>
-      <c r="K32" s="45" t="s">
+      <c r="F32" s="5"/>
+      <c r="G32" s="85" t="s">
+        <v>323</v>
+      </c>
+      <c r="H32" s="5"/>
+      <c r="I32" s="5"/>
+      <c r="J32" s="5"/>
+      <c r="K32" s="86" t="s">
         <v>40</v>
       </c>
       <c r="L32" s="13"/>
@@ -11003,27 +11006,29 @@
       <c r="IU32" s="80"/>
     </row>
     <row r="33" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="88" t="n">
+      <c r="A33" s="90" t="n">
         <v>42736</v>
       </c>
-      <c r="B33" s="3"/>
-      <c r="C33" s="34" t="s">
-        <v>82</v>
-      </c>
-      <c r="D33" s="34" t="s">
-        <v>329</v>
-      </c>
-      <c r="E33" s="34" t="s">
-        <v>61</v>
-      </c>
-      <c r="F33" s="3"/>
-      <c r="G33" s="34" t="s">
-        <v>330</v>
-      </c>
-      <c r="H33" s="3"/>
-      <c r="I33" s="3"/>
-      <c r="J33" s="3"/>
-      <c r="K33" s="53" t="s">
+      <c r="B33" s="57"/>
+      <c r="C33" s="75" t="s">
+        <v>79</v>
+      </c>
+      <c r="D33" s="75" t="s">
+        <v>258</v>
+      </c>
+      <c r="E33" s="75" t="s">
+        <v>73</v>
+      </c>
+      <c r="F33" s="75" t="s">
+        <v>258</v>
+      </c>
+      <c r="G33" s="75" t="s">
+        <v>324</v>
+      </c>
+      <c r="H33" s="57"/>
+      <c r="I33" s="57"/>
+      <c r="J33" s="57"/>
+      <c r="K33" s="91" t="s">
         <v>40</v>
       </c>
       <c r="L33" s="13"/>
@@ -11272,27 +11277,27 @@
       <c r="IU33" s="80"/>
     </row>
     <row r="34" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="88" t="n">
+      <c r="A34" s="90" t="n">
         <v>42736</v>
       </c>
-      <c r="B34" s="3"/>
-      <c r="C34" s="34" t="s">
-        <v>82</v>
-      </c>
-      <c r="D34" s="34" t="s">
-        <v>331</v>
-      </c>
-      <c r="E34" s="34" t="s">
-        <v>288</v>
-      </c>
-      <c r="F34" s="3"/>
-      <c r="G34" s="34" t="s">
-        <v>288</v>
-      </c>
-      <c r="H34" s="3"/>
-      <c r="I34" s="3"/>
-      <c r="J34" s="3"/>
-      <c r="K34" s="53" t="s">
+      <c r="B34" s="57"/>
+      <c r="C34" s="75" t="s">
+        <v>79</v>
+      </c>
+      <c r="D34" s="75" t="s">
+        <v>325</v>
+      </c>
+      <c r="E34" s="75" t="s">
+        <v>61</v>
+      </c>
+      <c r="F34" s="58"/>
+      <c r="G34" s="75" t="s">
+        <v>326</v>
+      </c>
+      <c r="H34" s="57"/>
+      <c r="I34" s="57"/>
+      <c r="J34" s="57"/>
+      <c r="K34" s="91" t="s">
         <v>40</v>
       </c>
       <c r="L34" s="13"/>
@@ -11541,27 +11546,29 @@
       <c r="IU34" s="80"/>
     </row>
     <row r="35" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="88" t="n">
+      <c r="A35" s="90" t="n">
         <v>42736</v>
       </c>
-      <c r="B35" s="3"/>
-      <c r="C35" s="34" t="s">
-        <v>82</v>
-      </c>
-      <c r="D35" s="34" t="s">
-        <v>332</v>
-      </c>
-      <c r="E35" s="34" t="s">
-        <v>333</v>
-      </c>
-      <c r="F35" s="3"/>
-      <c r="G35" s="34" t="s">
-        <v>334</v>
-      </c>
-      <c r="H35" s="3"/>
-      <c r="I35" s="3"/>
-      <c r="J35" s="3"/>
-      <c r="K35" s="53" t="s">
+      <c r="B35" s="57"/>
+      <c r="C35" s="75" t="s">
+        <v>79</v>
+      </c>
+      <c r="D35" s="75" t="s">
+        <v>253</v>
+      </c>
+      <c r="E35" s="75" t="s">
+        <v>73</v>
+      </c>
+      <c r="F35" s="75" t="s">
+        <v>253</v>
+      </c>
+      <c r="G35" s="75" t="s">
+        <v>327</v>
+      </c>
+      <c r="H35" s="57"/>
+      <c r="I35" s="57"/>
+      <c r="J35" s="57"/>
+      <c r="K35" s="91" t="s">
         <v>40</v>
       </c>
       <c r="L35" s="13"/>
@@ -11810,273 +11817,1349 @@
       <c r="IU35" s="80"/>
     </row>
     <row r="36" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="89" t="n">
+      <c r="A36" s="87" t="n">
         <v>42736</v>
       </c>
-      <c r="B36" s="5"/>
-      <c r="C36" s="85" t="s">
+      <c r="B36" s="24"/>
+      <c r="C36" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="D36" s="85" t="s">
-        <v>335</v>
-      </c>
-      <c r="E36" s="85" t="s">
+      <c r="D36" s="8" t="s">
+        <v>328</v>
+      </c>
+      <c r="E36" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="F36" s="5"/>
-      <c r="G36" s="85" t="s">
-        <v>336</v>
-      </c>
-      <c r="H36" s="5"/>
-      <c r="I36" s="5"/>
-      <c r="J36" s="5"/>
-      <c r="K36" s="86" t="s">
+      <c r="F36" s="24"/>
+      <c r="G36" s="8" t="s">
+        <v>329</v>
+      </c>
+      <c r="H36" s="24"/>
+      <c r="I36" s="24"/>
+      <c r="J36" s="24"/>
+      <c r="K36" s="45" t="s">
         <v>40</v>
       </c>
       <c r="L36" s="13"/>
       <c r="M36" s="3"/>
-      <c r="N36" s="92"/>
-      <c r="O36" s="93"/>
-      <c r="P36" s="93"/>
-      <c r="Q36" s="93"/>
-      <c r="R36" s="93"/>
-      <c r="S36" s="93"/>
-      <c r="T36" s="93"/>
-      <c r="U36" s="93"/>
-      <c r="V36" s="93"/>
-      <c r="W36" s="93"/>
-      <c r="X36" s="93"/>
-      <c r="Y36" s="93"/>
-      <c r="Z36" s="93"/>
-      <c r="AA36" s="93"/>
-      <c r="AB36" s="93"/>
-      <c r="AC36" s="93"/>
-      <c r="AD36" s="93"/>
-      <c r="AE36" s="93"/>
-      <c r="AF36" s="93"/>
-      <c r="AG36" s="93"/>
-      <c r="AH36" s="93"/>
-      <c r="AI36" s="93"/>
-      <c r="AJ36" s="93"/>
-      <c r="AK36" s="93"/>
-      <c r="AL36" s="93"/>
-      <c r="AM36" s="93"/>
-      <c r="AN36" s="93"/>
-      <c r="AO36" s="93"/>
-      <c r="AP36" s="93"/>
-      <c r="AQ36" s="93"/>
-      <c r="AR36" s="93"/>
-      <c r="AS36" s="93"/>
-      <c r="AT36" s="93"/>
-      <c r="AU36" s="93"/>
-      <c r="AV36" s="93"/>
-      <c r="AW36" s="93"/>
-      <c r="AX36" s="93"/>
-      <c r="AY36" s="93"/>
-      <c r="AZ36" s="93"/>
-      <c r="BA36" s="93"/>
-      <c r="BB36" s="93"/>
-      <c r="BC36" s="93"/>
-      <c r="BD36" s="93"/>
-      <c r="BE36" s="93"/>
-      <c r="BF36" s="93"/>
-      <c r="BG36" s="93"/>
-      <c r="BH36" s="93"/>
-      <c r="BI36" s="93"/>
-      <c r="BJ36" s="93"/>
-      <c r="BK36" s="93"/>
-      <c r="BL36" s="93"/>
-      <c r="BM36" s="93"/>
-      <c r="BN36" s="93"/>
-      <c r="BO36" s="93"/>
-      <c r="BP36" s="93"/>
-      <c r="BQ36" s="93"/>
-      <c r="BR36" s="93"/>
-      <c r="BS36" s="93"/>
-      <c r="BT36" s="93"/>
-      <c r="BU36" s="93"/>
-      <c r="BV36" s="93"/>
-      <c r="BW36" s="93"/>
-      <c r="BX36" s="93"/>
-      <c r="BY36" s="93"/>
-      <c r="BZ36" s="93"/>
-      <c r="CA36" s="93"/>
-      <c r="CB36" s="93"/>
-      <c r="CC36" s="93"/>
-      <c r="CD36" s="93"/>
-      <c r="CE36" s="93"/>
-      <c r="CF36" s="93"/>
-      <c r="CG36" s="93"/>
-      <c r="CH36" s="93"/>
-      <c r="CI36" s="93"/>
-      <c r="CJ36" s="93"/>
-      <c r="CK36" s="93"/>
-      <c r="CL36" s="93"/>
-      <c r="CM36" s="93"/>
-      <c r="CN36" s="93"/>
-      <c r="CO36" s="93"/>
-      <c r="CP36" s="93"/>
-      <c r="CQ36" s="93"/>
-      <c r="CR36" s="93"/>
-      <c r="CS36" s="93"/>
-      <c r="CT36" s="93"/>
-      <c r="CU36" s="93"/>
-      <c r="CV36" s="93"/>
-      <c r="CW36" s="93"/>
-      <c r="CX36" s="93"/>
-      <c r="CY36" s="93"/>
-      <c r="CZ36" s="93"/>
-      <c r="DA36" s="93"/>
-      <c r="DB36" s="93"/>
-      <c r="DC36" s="93"/>
-      <c r="DD36" s="93"/>
-      <c r="DE36" s="93"/>
-      <c r="DF36" s="93"/>
-      <c r="DG36" s="93"/>
-      <c r="DH36" s="93"/>
-      <c r="DI36" s="93"/>
-      <c r="DJ36" s="93"/>
-      <c r="DK36" s="93"/>
-      <c r="DL36" s="93"/>
-      <c r="DM36" s="93"/>
-      <c r="DN36" s="93"/>
-      <c r="DO36" s="93"/>
-      <c r="DP36" s="93"/>
-      <c r="DQ36" s="93"/>
-      <c r="DR36" s="93"/>
-      <c r="DS36" s="93"/>
-      <c r="DT36" s="93"/>
-      <c r="DU36" s="93"/>
-      <c r="DV36" s="93"/>
-      <c r="DW36" s="93"/>
-      <c r="DX36" s="93"/>
-      <c r="DY36" s="93"/>
-      <c r="DZ36" s="93"/>
-      <c r="EA36" s="93"/>
-      <c r="EB36" s="93"/>
-      <c r="EC36" s="93"/>
-      <c r="ED36" s="93"/>
-      <c r="EE36" s="93"/>
-      <c r="EF36" s="93"/>
-      <c r="EG36" s="93"/>
-      <c r="EH36" s="93"/>
-      <c r="EI36" s="93"/>
-      <c r="EJ36" s="93"/>
-      <c r="EK36" s="93"/>
-      <c r="EL36" s="93"/>
-      <c r="EM36" s="93"/>
-      <c r="EN36" s="93"/>
-      <c r="EO36" s="93"/>
-      <c r="EP36" s="93"/>
-      <c r="EQ36" s="93"/>
-      <c r="ER36" s="93"/>
-      <c r="ES36" s="93"/>
-      <c r="ET36" s="93"/>
-      <c r="EU36" s="93"/>
-      <c r="EV36" s="93"/>
-      <c r="EW36" s="93"/>
-      <c r="EX36" s="93"/>
-      <c r="EY36" s="93"/>
-      <c r="EZ36" s="93"/>
-      <c r="FA36" s="93"/>
-      <c r="FB36" s="93"/>
-      <c r="FC36" s="93"/>
-      <c r="FD36" s="93"/>
-      <c r="FE36" s="93"/>
-      <c r="FF36" s="93"/>
-      <c r="FG36" s="93"/>
-      <c r="FH36" s="93"/>
-      <c r="FI36" s="93"/>
-      <c r="FJ36" s="93"/>
-      <c r="FK36" s="93"/>
-      <c r="FL36" s="93"/>
-      <c r="FM36" s="93"/>
-      <c r="FN36" s="93"/>
-      <c r="FO36" s="93"/>
-      <c r="FP36" s="93"/>
-      <c r="FQ36" s="93"/>
-      <c r="FR36" s="93"/>
-      <c r="FS36" s="93"/>
-      <c r="FT36" s="93"/>
-      <c r="FU36" s="93"/>
-      <c r="FV36" s="93"/>
-      <c r="FW36" s="93"/>
-      <c r="FX36" s="93"/>
-      <c r="FY36" s="93"/>
-      <c r="FZ36" s="93"/>
-      <c r="GA36" s="93"/>
-      <c r="GB36" s="93"/>
-      <c r="GC36" s="93"/>
-      <c r="GD36" s="93"/>
-      <c r="GE36" s="93"/>
-      <c r="GF36" s="93"/>
-      <c r="GG36" s="93"/>
-      <c r="GH36" s="93"/>
-      <c r="GI36" s="93"/>
-      <c r="GJ36" s="93"/>
-      <c r="GK36" s="93"/>
-      <c r="GL36" s="93"/>
-      <c r="GM36" s="93"/>
-      <c r="GN36" s="93"/>
-      <c r="GO36" s="93"/>
-      <c r="GP36" s="93"/>
-      <c r="GQ36" s="93"/>
-      <c r="GR36" s="93"/>
-      <c r="GS36" s="93"/>
-      <c r="GT36" s="93"/>
-      <c r="GU36" s="93"/>
-      <c r="GV36" s="93"/>
-      <c r="GW36" s="93"/>
-      <c r="GX36" s="93"/>
-      <c r="GY36" s="93"/>
-      <c r="GZ36" s="93"/>
-      <c r="HA36" s="93"/>
-      <c r="HB36" s="93"/>
-      <c r="HC36" s="93"/>
-      <c r="HD36" s="93"/>
-      <c r="HE36" s="93"/>
-      <c r="HF36" s="93"/>
-      <c r="HG36" s="93"/>
-      <c r="HH36" s="93"/>
-      <c r="HI36" s="93"/>
-      <c r="HJ36" s="93"/>
-      <c r="HK36" s="93"/>
-      <c r="HL36" s="93"/>
-      <c r="HM36" s="93"/>
-      <c r="HN36" s="93"/>
-      <c r="HO36" s="93"/>
-      <c r="HP36" s="93"/>
-      <c r="HQ36" s="93"/>
-      <c r="HR36" s="93"/>
-      <c r="HS36" s="93"/>
-      <c r="HT36" s="93"/>
-      <c r="HU36" s="93"/>
-      <c r="HV36" s="93"/>
-      <c r="HW36" s="93"/>
-      <c r="HX36" s="93"/>
-      <c r="HY36" s="93"/>
-      <c r="HZ36" s="93"/>
-      <c r="IA36" s="93"/>
-      <c r="IB36" s="93"/>
-      <c r="IC36" s="93"/>
-      <c r="ID36" s="93"/>
-      <c r="IE36" s="93"/>
-      <c r="IF36" s="93"/>
-      <c r="IG36" s="93"/>
-      <c r="IH36" s="93"/>
-      <c r="II36" s="93"/>
-      <c r="IJ36" s="93"/>
-      <c r="IK36" s="93"/>
-      <c r="IL36" s="93"/>
-      <c r="IM36" s="93"/>
-      <c r="IN36" s="93"/>
-      <c r="IO36" s="93"/>
-      <c r="IP36" s="93"/>
-      <c r="IQ36" s="93"/>
-      <c r="IR36" s="93"/>
-      <c r="IS36" s="93"/>
-      <c r="IT36" s="93"/>
-      <c r="IU36" s="94"/>
+      <c r="N36" s="81"/>
+      <c r="O36" s="32"/>
+      <c r="P36" s="32"/>
+      <c r="Q36" s="32"/>
+      <c r="R36" s="32"/>
+      <c r="S36" s="32"/>
+      <c r="T36" s="32"/>
+      <c r="U36" s="32"/>
+      <c r="V36" s="32"/>
+      <c r="W36" s="32"/>
+      <c r="X36" s="32"/>
+      <c r="Y36" s="32"/>
+      <c r="Z36" s="32"/>
+      <c r="AA36" s="32"/>
+      <c r="AB36" s="32"/>
+      <c r="AC36" s="32"/>
+      <c r="AD36" s="32"/>
+      <c r="AE36" s="32"/>
+      <c r="AF36" s="32"/>
+      <c r="AG36" s="32"/>
+      <c r="AH36" s="32"/>
+      <c r="AI36" s="32"/>
+      <c r="AJ36" s="32"/>
+      <c r="AK36" s="32"/>
+      <c r="AL36" s="32"/>
+      <c r="AM36" s="32"/>
+      <c r="AN36" s="32"/>
+      <c r="AO36" s="32"/>
+      <c r="AP36" s="32"/>
+      <c r="AQ36" s="32"/>
+      <c r="AR36" s="32"/>
+      <c r="AS36" s="32"/>
+      <c r="AT36" s="32"/>
+      <c r="AU36" s="32"/>
+      <c r="AV36" s="32"/>
+      <c r="AW36" s="32"/>
+      <c r="AX36" s="32"/>
+      <c r="AY36" s="32"/>
+      <c r="AZ36" s="32"/>
+      <c r="BA36" s="32"/>
+      <c r="BB36" s="32"/>
+      <c r="BC36" s="32"/>
+      <c r="BD36" s="32"/>
+      <c r="BE36" s="32"/>
+      <c r="BF36" s="32"/>
+      <c r="BG36" s="32"/>
+      <c r="BH36" s="32"/>
+      <c r="BI36" s="32"/>
+      <c r="BJ36" s="32"/>
+      <c r="BK36" s="32"/>
+      <c r="BL36" s="32"/>
+      <c r="BM36" s="32"/>
+      <c r="BN36" s="32"/>
+      <c r="BO36" s="32"/>
+      <c r="BP36" s="32"/>
+      <c r="BQ36" s="32"/>
+      <c r="BR36" s="32"/>
+      <c r="BS36" s="32"/>
+      <c r="BT36" s="32"/>
+      <c r="BU36" s="32"/>
+      <c r="BV36" s="32"/>
+      <c r="BW36" s="32"/>
+      <c r="BX36" s="32"/>
+      <c r="BY36" s="32"/>
+      <c r="BZ36" s="32"/>
+      <c r="CA36" s="32"/>
+      <c r="CB36" s="32"/>
+      <c r="CC36" s="32"/>
+      <c r="CD36" s="32"/>
+      <c r="CE36" s="32"/>
+      <c r="CF36" s="32"/>
+      <c r="CG36" s="32"/>
+      <c r="CH36" s="32"/>
+      <c r="CI36" s="32"/>
+      <c r="CJ36" s="32"/>
+      <c r="CK36" s="32"/>
+      <c r="CL36" s="32"/>
+      <c r="CM36" s="32"/>
+      <c r="CN36" s="32"/>
+      <c r="CO36" s="32"/>
+      <c r="CP36" s="32"/>
+      <c r="CQ36" s="32"/>
+      <c r="CR36" s="32"/>
+      <c r="CS36" s="32"/>
+      <c r="CT36" s="32"/>
+      <c r="CU36" s="32"/>
+      <c r="CV36" s="32"/>
+      <c r="CW36" s="32"/>
+      <c r="CX36" s="32"/>
+      <c r="CY36" s="32"/>
+      <c r="CZ36" s="32"/>
+      <c r="DA36" s="32"/>
+      <c r="DB36" s="32"/>
+      <c r="DC36" s="32"/>
+      <c r="DD36" s="32"/>
+      <c r="DE36" s="32"/>
+      <c r="DF36" s="32"/>
+      <c r="DG36" s="32"/>
+      <c r="DH36" s="32"/>
+      <c r="DI36" s="32"/>
+      <c r="DJ36" s="32"/>
+      <c r="DK36" s="32"/>
+      <c r="DL36" s="32"/>
+      <c r="DM36" s="32"/>
+      <c r="DN36" s="32"/>
+      <c r="DO36" s="32"/>
+      <c r="DP36" s="32"/>
+      <c r="DQ36" s="32"/>
+      <c r="DR36" s="32"/>
+      <c r="DS36" s="32"/>
+      <c r="DT36" s="32"/>
+      <c r="DU36" s="32"/>
+      <c r="DV36" s="32"/>
+      <c r="DW36" s="32"/>
+      <c r="DX36" s="32"/>
+      <c r="DY36" s="32"/>
+      <c r="DZ36" s="32"/>
+      <c r="EA36" s="32"/>
+      <c r="EB36" s="32"/>
+      <c r="EC36" s="32"/>
+      <c r="ED36" s="32"/>
+      <c r="EE36" s="32"/>
+      <c r="EF36" s="32"/>
+      <c r="EG36" s="32"/>
+      <c r="EH36" s="32"/>
+      <c r="EI36" s="32"/>
+      <c r="EJ36" s="32"/>
+      <c r="EK36" s="32"/>
+      <c r="EL36" s="32"/>
+      <c r="EM36" s="32"/>
+      <c r="EN36" s="32"/>
+      <c r="EO36" s="32"/>
+      <c r="EP36" s="32"/>
+      <c r="EQ36" s="32"/>
+      <c r="ER36" s="32"/>
+      <c r="ES36" s="32"/>
+      <c r="ET36" s="32"/>
+      <c r="EU36" s="32"/>
+      <c r="EV36" s="32"/>
+      <c r="EW36" s="32"/>
+      <c r="EX36" s="32"/>
+      <c r="EY36" s="32"/>
+      <c r="EZ36" s="32"/>
+      <c r="FA36" s="32"/>
+      <c r="FB36" s="32"/>
+      <c r="FC36" s="32"/>
+      <c r="FD36" s="32"/>
+      <c r="FE36" s="32"/>
+      <c r="FF36" s="32"/>
+      <c r="FG36" s="32"/>
+      <c r="FH36" s="32"/>
+      <c r="FI36" s="32"/>
+      <c r="FJ36" s="32"/>
+      <c r="FK36" s="32"/>
+      <c r="FL36" s="32"/>
+      <c r="FM36" s="32"/>
+      <c r="FN36" s="32"/>
+      <c r="FO36" s="32"/>
+      <c r="FP36" s="32"/>
+      <c r="FQ36" s="32"/>
+      <c r="FR36" s="32"/>
+      <c r="FS36" s="32"/>
+      <c r="FT36" s="32"/>
+      <c r="FU36" s="32"/>
+      <c r="FV36" s="32"/>
+      <c r="FW36" s="32"/>
+      <c r="FX36" s="32"/>
+      <c r="FY36" s="32"/>
+      <c r="FZ36" s="32"/>
+      <c r="GA36" s="32"/>
+      <c r="GB36" s="32"/>
+      <c r="GC36" s="32"/>
+      <c r="GD36" s="32"/>
+      <c r="GE36" s="32"/>
+      <c r="GF36" s="32"/>
+      <c r="GG36" s="32"/>
+      <c r="GH36" s="32"/>
+      <c r="GI36" s="32"/>
+      <c r="GJ36" s="32"/>
+      <c r="GK36" s="32"/>
+      <c r="GL36" s="32"/>
+      <c r="GM36" s="32"/>
+      <c r="GN36" s="32"/>
+      <c r="GO36" s="32"/>
+      <c r="GP36" s="32"/>
+      <c r="GQ36" s="32"/>
+      <c r="GR36" s="32"/>
+      <c r="GS36" s="32"/>
+      <c r="GT36" s="32"/>
+      <c r="GU36" s="32"/>
+      <c r="GV36" s="32"/>
+      <c r="GW36" s="32"/>
+      <c r="GX36" s="32"/>
+      <c r="GY36" s="32"/>
+      <c r="GZ36" s="32"/>
+      <c r="HA36" s="32"/>
+      <c r="HB36" s="32"/>
+      <c r="HC36" s="32"/>
+      <c r="HD36" s="32"/>
+      <c r="HE36" s="32"/>
+      <c r="HF36" s="32"/>
+      <c r="HG36" s="32"/>
+      <c r="HH36" s="32"/>
+      <c r="HI36" s="32"/>
+      <c r="HJ36" s="32"/>
+      <c r="HK36" s="32"/>
+      <c r="HL36" s="32"/>
+      <c r="HM36" s="32"/>
+      <c r="HN36" s="32"/>
+      <c r="HO36" s="32"/>
+      <c r="HP36" s="32"/>
+      <c r="HQ36" s="32"/>
+      <c r="HR36" s="32"/>
+      <c r="HS36" s="32"/>
+      <c r="HT36" s="32"/>
+      <c r="HU36" s="32"/>
+      <c r="HV36" s="32"/>
+      <c r="HW36" s="32"/>
+      <c r="HX36" s="32"/>
+      <c r="HY36" s="32"/>
+      <c r="HZ36" s="32"/>
+      <c r="IA36" s="32"/>
+      <c r="IB36" s="32"/>
+      <c r="IC36" s="32"/>
+      <c r="ID36" s="32"/>
+      <c r="IE36" s="32"/>
+      <c r="IF36" s="32"/>
+      <c r="IG36" s="32"/>
+      <c r="IH36" s="32"/>
+      <c r="II36" s="32"/>
+      <c r="IJ36" s="32"/>
+      <c r="IK36" s="32"/>
+      <c r="IL36" s="32"/>
+      <c r="IM36" s="32"/>
+      <c r="IN36" s="32"/>
+      <c r="IO36" s="32"/>
+      <c r="IP36" s="32"/>
+      <c r="IQ36" s="32"/>
+      <c r="IR36" s="32"/>
+      <c r="IS36" s="32"/>
+      <c r="IT36" s="32"/>
+      <c r="IU36" s="80"/>
+    </row>
+    <row r="37" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A37" s="88" t="n">
+        <v>42736</v>
+      </c>
+      <c r="B37" s="3"/>
+      <c r="C37" s="34" t="s">
+        <v>82</v>
+      </c>
+      <c r="D37" s="34" t="s">
+        <v>330</v>
+      </c>
+      <c r="E37" s="34" t="s">
+        <v>61</v>
+      </c>
+      <c r="F37" s="3"/>
+      <c r="G37" s="34" t="s">
+        <v>331</v>
+      </c>
+      <c r="H37" s="3"/>
+      <c r="I37" s="3"/>
+      <c r="J37" s="3"/>
+      <c r="K37" s="53" t="s">
+        <v>40</v>
+      </c>
+      <c r="L37" s="13"/>
+      <c r="M37" s="3"/>
+      <c r="N37" s="81"/>
+      <c r="O37" s="32"/>
+      <c r="P37" s="32"/>
+      <c r="Q37" s="32"/>
+      <c r="R37" s="32"/>
+      <c r="S37" s="32"/>
+      <c r="T37" s="32"/>
+      <c r="U37" s="32"/>
+      <c r="V37" s="32"/>
+      <c r="W37" s="32"/>
+      <c r="X37" s="32"/>
+      <c r="Y37" s="32"/>
+      <c r="Z37" s="32"/>
+      <c r="AA37" s="32"/>
+      <c r="AB37" s="32"/>
+      <c r="AC37" s="32"/>
+      <c r="AD37" s="32"/>
+      <c r="AE37" s="32"/>
+      <c r="AF37" s="32"/>
+      <c r="AG37" s="32"/>
+      <c r="AH37" s="32"/>
+      <c r="AI37" s="32"/>
+      <c r="AJ37" s="32"/>
+      <c r="AK37" s="32"/>
+      <c r="AL37" s="32"/>
+      <c r="AM37" s="32"/>
+      <c r="AN37" s="32"/>
+      <c r="AO37" s="32"/>
+      <c r="AP37" s="32"/>
+      <c r="AQ37" s="32"/>
+      <c r="AR37" s="32"/>
+      <c r="AS37" s="32"/>
+      <c r="AT37" s="32"/>
+      <c r="AU37" s="32"/>
+      <c r="AV37" s="32"/>
+      <c r="AW37" s="32"/>
+      <c r="AX37" s="32"/>
+      <c r="AY37" s="32"/>
+      <c r="AZ37" s="32"/>
+      <c r="BA37" s="32"/>
+      <c r="BB37" s="32"/>
+      <c r="BC37" s="32"/>
+      <c r="BD37" s="32"/>
+      <c r="BE37" s="32"/>
+      <c r="BF37" s="32"/>
+      <c r="BG37" s="32"/>
+      <c r="BH37" s="32"/>
+      <c r="BI37" s="32"/>
+      <c r="BJ37" s="32"/>
+      <c r="BK37" s="32"/>
+      <c r="BL37" s="32"/>
+      <c r="BM37" s="32"/>
+      <c r="BN37" s="32"/>
+      <c r="BO37" s="32"/>
+      <c r="BP37" s="32"/>
+      <c r="BQ37" s="32"/>
+      <c r="BR37" s="32"/>
+      <c r="BS37" s="32"/>
+      <c r="BT37" s="32"/>
+      <c r="BU37" s="32"/>
+      <c r="BV37" s="32"/>
+      <c r="BW37" s="32"/>
+      <c r="BX37" s="32"/>
+      <c r="BY37" s="32"/>
+      <c r="BZ37" s="32"/>
+      <c r="CA37" s="32"/>
+      <c r="CB37" s="32"/>
+      <c r="CC37" s="32"/>
+      <c r="CD37" s="32"/>
+      <c r="CE37" s="32"/>
+      <c r="CF37" s="32"/>
+      <c r="CG37" s="32"/>
+      <c r="CH37" s="32"/>
+      <c r="CI37" s="32"/>
+      <c r="CJ37" s="32"/>
+      <c r="CK37" s="32"/>
+      <c r="CL37" s="32"/>
+      <c r="CM37" s="32"/>
+      <c r="CN37" s="32"/>
+      <c r="CO37" s="32"/>
+      <c r="CP37" s="32"/>
+      <c r="CQ37" s="32"/>
+      <c r="CR37" s="32"/>
+      <c r="CS37" s="32"/>
+      <c r="CT37" s="32"/>
+      <c r="CU37" s="32"/>
+      <c r="CV37" s="32"/>
+      <c r="CW37" s="32"/>
+      <c r="CX37" s="32"/>
+      <c r="CY37" s="32"/>
+      <c r="CZ37" s="32"/>
+      <c r="DA37" s="32"/>
+      <c r="DB37" s="32"/>
+      <c r="DC37" s="32"/>
+      <c r="DD37" s="32"/>
+      <c r="DE37" s="32"/>
+      <c r="DF37" s="32"/>
+      <c r="DG37" s="32"/>
+      <c r="DH37" s="32"/>
+      <c r="DI37" s="32"/>
+      <c r="DJ37" s="32"/>
+      <c r="DK37" s="32"/>
+      <c r="DL37" s="32"/>
+      <c r="DM37" s="32"/>
+      <c r="DN37" s="32"/>
+      <c r="DO37" s="32"/>
+      <c r="DP37" s="32"/>
+      <c r="DQ37" s="32"/>
+      <c r="DR37" s="32"/>
+      <c r="DS37" s="32"/>
+      <c r="DT37" s="32"/>
+      <c r="DU37" s="32"/>
+      <c r="DV37" s="32"/>
+      <c r="DW37" s="32"/>
+      <c r="DX37" s="32"/>
+      <c r="DY37" s="32"/>
+      <c r="DZ37" s="32"/>
+      <c r="EA37" s="32"/>
+      <c r="EB37" s="32"/>
+      <c r="EC37" s="32"/>
+      <c r="ED37" s="32"/>
+      <c r="EE37" s="32"/>
+      <c r="EF37" s="32"/>
+      <c r="EG37" s="32"/>
+      <c r="EH37" s="32"/>
+      <c r="EI37" s="32"/>
+      <c r="EJ37" s="32"/>
+      <c r="EK37" s="32"/>
+      <c r="EL37" s="32"/>
+      <c r="EM37" s="32"/>
+      <c r="EN37" s="32"/>
+      <c r="EO37" s="32"/>
+      <c r="EP37" s="32"/>
+      <c r="EQ37" s="32"/>
+      <c r="ER37" s="32"/>
+      <c r="ES37" s="32"/>
+      <c r="ET37" s="32"/>
+      <c r="EU37" s="32"/>
+      <c r="EV37" s="32"/>
+      <c r="EW37" s="32"/>
+      <c r="EX37" s="32"/>
+      <c r="EY37" s="32"/>
+      <c r="EZ37" s="32"/>
+      <c r="FA37" s="32"/>
+      <c r="FB37" s="32"/>
+      <c r="FC37" s="32"/>
+      <c r="FD37" s="32"/>
+      <c r="FE37" s="32"/>
+      <c r="FF37" s="32"/>
+      <c r="FG37" s="32"/>
+      <c r="FH37" s="32"/>
+      <c r="FI37" s="32"/>
+      <c r="FJ37" s="32"/>
+      <c r="FK37" s="32"/>
+      <c r="FL37" s="32"/>
+      <c r="FM37" s="32"/>
+      <c r="FN37" s="32"/>
+      <c r="FO37" s="32"/>
+      <c r="FP37" s="32"/>
+      <c r="FQ37" s="32"/>
+      <c r="FR37" s="32"/>
+      <c r="FS37" s="32"/>
+      <c r="FT37" s="32"/>
+      <c r="FU37" s="32"/>
+      <c r="FV37" s="32"/>
+      <c r="FW37" s="32"/>
+      <c r="FX37" s="32"/>
+      <c r="FY37" s="32"/>
+      <c r="FZ37" s="32"/>
+      <c r="GA37" s="32"/>
+      <c r="GB37" s="32"/>
+      <c r="GC37" s="32"/>
+      <c r="GD37" s="32"/>
+      <c r="GE37" s="32"/>
+      <c r="GF37" s="32"/>
+      <c r="GG37" s="32"/>
+      <c r="GH37" s="32"/>
+      <c r="GI37" s="32"/>
+      <c r="GJ37" s="32"/>
+      <c r="GK37" s="32"/>
+      <c r="GL37" s="32"/>
+      <c r="GM37" s="32"/>
+      <c r="GN37" s="32"/>
+      <c r="GO37" s="32"/>
+      <c r="GP37" s="32"/>
+      <c r="GQ37" s="32"/>
+      <c r="GR37" s="32"/>
+      <c r="GS37" s="32"/>
+      <c r="GT37" s="32"/>
+      <c r="GU37" s="32"/>
+      <c r="GV37" s="32"/>
+      <c r="GW37" s="32"/>
+      <c r="GX37" s="32"/>
+      <c r="GY37" s="32"/>
+      <c r="GZ37" s="32"/>
+      <c r="HA37" s="32"/>
+      <c r="HB37" s="32"/>
+      <c r="HC37" s="32"/>
+      <c r="HD37" s="32"/>
+      <c r="HE37" s="32"/>
+      <c r="HF37" s="32"/>
+      <c r="HG37" s="32"/>
+      <c r="HH37" s="32"/>
+      <c r="HI37" s="32"/>
+      <c r="HJ37" s="32"/>
+      <c r="HK37" s="32"/>
+      <c r="HL37" s="32"/>
+      <c r="HM37" s="32"/>
+      <c r="HN37" s="32"/>
+      <c r="HO37" s="32"/>
+      <c r="HP37" s="32"/>
+      <c r="HQ37" s="32"/>
+      <c r="HR37" s="32"/>
+      <c r="HS37" s="32"/>
+      <c r="HT37" s="32"/>
+      <c r="HU37" s="32"/>
+      <c r="HV37" s="32"/>
+      <c r="HW37" s="32"/>
+      <c r="HX37" s="32"/>
+      <c r="HY37" s="32"/>
+      <c r="HZ37" s="32"/>
+      <c r="IA37" s="32"/>
+      <c r="IB37" s="32"/>
+      <c r="IC37" s="32"/>
+      <c r="ID37" s="32"/>
+      <c r="IE37" s="32"/>
+      <c r="IF37" s="32"/>
+      <c r="IG37" s="32"/>
+      <c r="IH37" s="32"/>
+      <c r="II37" s="32"/>
+      <c r="IJ37" s="32"/>
+      <c r="IK37" s="32"/>
+      <c r="IL37" s="32"/>
+      <c r="IM37" s="32"/>
+      <c r="IN37" s="32"/>
+      <c r="IO37" s="32"/>
+      <c r="IP37" s="32"/>
+      <c r="IQ37" s="32"/>
+      <c r="IR37" s="32"/>
+      <c r="IS37" s="32"/>
+      <c r="IT37" s="32"/>
+      <c r="IU37" s="80"/>
+    </row>
+    <row r="38" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A38" s="88" t="n">
+        <v>42736</v>
+      </c>
+      <c r="B38" s="3"/>
+      <c r="C38" s="34" t="s">
+        <v>82</v>
+      </c>
+      <c r="D38" s="34" t="s">
+        <v>332</v>
+      </c>
+      <c r="E38" s="34" t="s">
+        <v>288</v>
+      </c>
+      <c r="F38" s="3"/>
+      <c r="G38" s="34" t="s">
+        <v>288</v>
+      </c>
+      <c r="H38" s="3"/>
+      <c r="I38" s="3"/>
+      <c r="J38" s="3"/>
+      <c r="K38" s="53" t="s">
+        <v>40</v>
+      </c>
+      <c r="L38" s="13"/>
+      <c r="M38" s="3"/>
+      <c r="N38" s="81"/>
+      <c r="O38" s="32"/>
+      <c r="P38" s="32"/>
+      <c r="Q38" s="32"/>
+      <c r="R38" s="32"/>
+      <c r="S38" s="32"/>
+      <c r="T38" s="32"/>
+      <c r="U38" s="32"/>
+      <c r="V38" s="32"/>
+      <c r="W38" s="32"/>
+      <c r="X38" s="32"/>
+      <c r="Y38" s="32"/>
+      <c r="Z38" s="32"/>
+      <c r="AA38" s="32"/>
+      <c r="AB38" s="32"/>
+      <c r="AC38" s="32"/>
+      <c r="AD38" s="32"/>
+      <c r="AE38" s="32"/>
+      <c r="AF38" s="32"/>
+      <c r="AG38" s="32"/>
+      <c r="AH38" s="32"/>
+      <c r="AI38" s="32"/>
+      <c r="AJ38" s="32"/>
+      <c r="AK38" s="32"/>
+      <c r="AL38" s="32"/>
+      <c r="AM38" s="32"/>
+      <c r="AN38" s="32"/>
+      <c r="AO38" s="32"/>
+      <c r="AP38" s="32"/>
+      <c r="AQ38" s="32"/>
+      <c r="AR38" s="32"/>
+      <c r="AS38" s="32"/>
+      <c r="AT38" s="32"/>
+      <c r="AU38" s="32"/>
+      <c r="AV38" s="32"/>
+      <c r="AW38" s="32"/>
+      <c r="AX38" s="32"/>
+      <c r="AY38" s="32"/>
+      <c r="AZ38" s="32"/>
+      <c r="BA38" s="32"/>
+      <c r="BB38" s="32"/>
+      <c r="BC38" s="32"/>
+      <c r="BD38" s="32"/>
+      <c r="BE38" s="32"/>
+      <c r="BF38" s="32"/>
+      <c r="BG38" s="32"/>
+      <c r="BH38" s="32"/>
+      <c r="BI38" s="32"/>
+      <c r="BJ38" s="32"/>
+      <c r="BK38" s="32"/>
+      <c r="BL38" s="32"/>
+      <c r="BM38" s="32"/>
+      <c r="BN38" s="32"/>
+      <c r="BO38" s="32"/>
+      <c r="BP38" s="32"/>
+      <c r="BQ38" s="32"/>
+      <c r="BR38" s="32"/>
+      <c r="BS38" s="32"/>
+      <c r="BT38" s="32"/>
+      <c r="BU38" s="32"/>
+      <c r="BV38" s="32"/>
+      <c r="BW38" s="32"/>
+      <c r="BX38" s="32"/>
+      <c r="BY38" s="32"/>
+      <c r="BZ38" s="32"/>
+      <c r="CA38" s="32"/>
+      <c r="CB38" s="32"/>
+      <c r="CC38" s="32"/>
+      <c r="CD38" s="32"/>
+      <c r="CE38" s="32"/>
+      <c r="CF38" s="32"/>
+      <c r="CG38" s="32"/>
+      <c r="CH38" s="32"/>
+      <c r="CI38" s="32"/>
+      <c r="CJ38" s="32"/>
+      <c r="CK38" s="32"/>
+      <c r="CL38" s="32"/>
+      <c r="CM38" s="32"/>
+      <c r="CN38" s="32"/>
+      <c r="CO38" s="32"/>
+      <c r="CP38" s="32"/>
+      <c r="CQ38" s="32"/>
+      <c r="CR38" s="32"/>
+      <c r="CS38" s="32"/>
+      <c r="CT38" s="32"/>
+      <c r="CU38" s="32"/>
+      <c r="CV38" s="32"/>
+      <c r="CW38" s="32"/>
+      <c r="CX38" s="32"/>
+      <c r="CY38" s="32"/>
+      <c r="CZ38" s="32"/>
+      <c r="DA38" s="32"/>
+      <c r="DB38" s="32"/>
+      <c r="DC38" s="32"/>
+      <c r="DD38" s="32"/>
+      <c r="DE38" s="32"/>
+      <c r="DF38" s="32"/>
+      <c r="DG38" s="32"/>
+      <c r="DH38" s="32"/>
+      <c r="DI38" s="32"/>
+      <c r="DJ38" s="32"/>
+      <c r="DK38" s="32"/>
+      <c r="DL38" s="32"/>
+      <c r="DM38" s="32"/>
+      <c r="DN38" s="32"/>
+      <c r="DO38" s="32"/>
+      <c r="DP38" s="32"/>
+      <c r="DQ38" s="32"/>
+      <c r="DR38" s="32"/>
+      <c r="DS38" s="32"/>
+      <c r="DT38" s="32"/>
+      <c r="DU38" s="32"/>
+      <c r="DV38" s="32"/>
+      <c r="DW38" s="32"/>
+      <c r="DX38" s="32"/>
+      <c r="DY38" s="32"/>
+      <c r="DZ38" s="32"/>
+      <c r="EA38" s="32"/>
+      <c r="EB38" s="32"/>
+      <c r="EC38" s="32"/>
+      <c r="ED38" s="32"/>
+      <c r="EE38" s="32"/>
+      <c r="EF38" s="32"/>
+      <c r="EG38" s="32"/>
+      <c r="EH38" s="32"/>
+      <c r="EI38" s="32"/>
+      <c r="EJ38" s="32"/>
+      <c r="EK38" s="32"/>
+      <c r="EL38" s="32"/>
+      <c r="EM38" s="32"/>
+      <c r="EN38" s="32"/>
+      <c r="EO38" s="32"/>
+      <c r="EP38" s="32"/>
+      <c r="EQ38" s="32"/>
+      <c r="ER38" s="32"/>
+      <c r="ES38" s="32"/>
+      <c r="ET38" s="32"/>
+      <c r="EU38" s="32"/>
+      <c r="EV38" s="32"/>
+      <c r="EW38" s="32"/>
+      <c r="EX38" s="32"/>
+      <c r="EY38" s="32"/>
+      <c r="EZ38" s="32"/>
+      <c r="FA38" s="32"/>
+      <c r="FB38" s="32"/>
+      <c r="FC38" s="32"/>
+      <c r="FD38" s="32"/>
+      <c r="FE38" s="32"/>
+      <c r="FF38" s="32"/>
+      <c r="FG38" s="32"/>
+      <c r="FH38" s="32"/>
+      <c r="FI38" s="32"/>
+      <c r="FJ38" s="32"/>
+      <c r="FK38" s="32"/>
+      <c r="FL38" s="32"/>
+      <c r="FM38" s="32"/>
+      <c r="FN38" s="32"/>
+      <c r="FO38" s="32"/>
+      <c r="FP38" s="32"/>
+      <c r="FQ38" s="32"/>
+      <c r="FR38" s="32"/>
+      <c r="FS38" s="32"/>
+      <c r="FT38" s="32"/>
+      <c r="FU38" s="32"/>
+      <c r="FV38" s="32"/>
+      <c r="FW38" s="32"/>
+      <c r="FX38" s="32"/>
+      <c r="FY38" s="32"/>
+      <c r="FZ38" s="32"/>
+      <c r="GA38" s="32"/>
+      <c r="GB38" s="32"/>
+      <c r="GC38" s="32"/>
+      <c r="GD38" s="32"/>
+      <c r="GE38" s="32"/>
+      <c r="GF38" s="32"/>
+      <c r="GG38" s="32"/>
+      <c r="GH38" s="32"/>
+      <c r="GI38" s="32"/>
+      <c r="GJ38" s="32"/>
+      <c r="GK38" s="32"/>
+      <c r="GL38" s="32"/>
+      <c r="GM38" s="32"/>
+      <c r="GN38" s="32"/>
+      <c r="GO38" s="32"/>
+      <c r="GP38" s="32"/>
+      <c r="GQ38" s="32"/>
+      <c r="GR38" s="32"/>
+      <c r="GS38" s="32"/>
+      <c r="GT38" s="32"/>
+      <c r="GU38" s="32"/>
+      <c r="GV38" s="32"/>
+      <c r="GW38" s="32"/>
+      <c r="GX38" s="32"/>
+      <c r="GY38" s="32"/>
+      <c r="GZ38" s="32"/>
+      <c r="HA38" s="32"/>
+      <c r="HB38" s="32"/>
+      <c r="HC38" s="32"/>
+      <c r="HD38" s="32"/>
+      <c r="HE38" s="32"/>
+      <c r="HF38" s="32"/>
+      <c r="HG38" s="32"/>
+      <c r="HH38" s="32"/>
+      <c r="HI38" s="32"/>
+      <c r="HJ38" s="32"/>
+      <c r="HK38" s="32"/>
+      <c r="HL38" s="32"/>
+      <c r="HM38" s="32"/>
+      <c r="HN38" s="32"/>
+      <c r="HO38" s="32"/>
+      <c r="HP38" s="32"/>
+      <c r="HQ38" s="32"/>
+      <c r="HR38" s="32"/>
+      <c r="HS38" s="32"/>
+      <c r="HT38" s="32"/>
+      <c r="HU38" s="32"/>
+      <c r="HV38" s="32"/>
+      <c r="HW38" s="32"/>
+      <c r="HX38" s="32"/>
+      <c r="HY38" s="32"/>
+      <c r="HZ38" s="32"/>
+      <c r="IA38" s="32"/>
+      <c r="IB38" s="32"/>
+      <c r="IC38" s="32"/>
+      <c r="ID38" s="32"/>
+      <c r="IE38" s="32"/>
+      <c r="IF38" s="32"/>
+      <c r="IG38" s="32"/>
+      <c r="IH38" s="32"/>
+      <c r="II38" s="32"/>
+      <c r="IJ38" s="32"/>
+      <c r="IK38" s="32"/>
+      <c r="IL38" s="32"/>
+      <c r="IM38" s="32"/>
+      <c r="IN38" s="32"/>
+      <c r="IO38" s="32"/>
+      <c r="IP38" s="32"/>
+      <c r="IQ38" s="32"/>
+      <c r="IR38" s="32"/>
+      <c r="IS38" s="32"/>
+      <c r="IT38" s="32"/>
+      <c r="IU38" s="80"/>
+    </row>
+    <row r="39" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A39" s="88" t="n">
+        <v>42736</v>
+      </c>
+      <c r="B39" s="3"/>
+      <c r="C39" s="34" t="s">
+        <v>82</v>
+      </c>
+      <c r="D39" s="34" t="s">
+        <v>333</v>
+      </c>
+      <c r="E39" s="34" t="s">
+        <v>334</v>
+      </c>
+      <c r="F39" s="3"/>
+      <c r="G39" s="34" t="s">
+        <v>335</v>
+      </c>
+      <c r="H39" s="3"/>
+      <c r="I39" s="3"/>
+      <c r="J39" s="3"/>
+      <c r="K39" s="53" t="s">
+        <v>40</v>
+      </c>
+      <c r="L39" s="13"/>
+      <c r="M39" s="3"/>
+      <c r="N39" s="81"/>
+      <c r="O39" s="32"/>
+      <c r="P39" s="32"/>
+      <c r="Q39" s="32"/>
+      <c r="R39" s="32"/>
+      <c r="S39" s="32"/>
+      <c r="T39" s="32"/>
+      <c r="U39" s="32"/>
+      <c r="V39" s="32"/>
+      <c r="W39" s="32"/>
+      <c r="X39" s="32"/>
+      <c r="Y39" s="32"/>
+      <c r="Z39" s="32"/>
+      <c r="AA39" s="32"/>
+      <c r="AB39" s="32"/>
+      <c r="AC39" s="32"/>
+      <c r="AD39" s="32"/>
+      <c r="AE39" s="32"/>
+      <c r="AF39" s="32"/>
+      <c r="AG39" s="32"/>
+      <c r="AH39" s="32"/>
+      <c r="AI39" s="32"/>
+      <c r="AJ39" s="32"/>
+      <c r="AK39" s="32"/>
+      <c r="AL39" s="32"/>
+      <c r="AM39" s="32"/>
+      <c r="AN39" s="32"/>
+      <c r="AO39" s="32"/>
+      <c r="AP39" s="32"/>
+      <c r="AQ39" s="32"/>
+      <c r="AR39" s="32"/>
+      <c r="AS39" s="32"/>
+      <c r="AT39" s="32"/>
+      <c r="AU39" s="32"/>
+      <c r="AV39" s="32"/>
+      <c r="AW39" s="32"/>
+      <c r="AX39" s="32"/>
+      <c r="AY39" s="32"/>
+      <c r="AZ39" s="32"/>
+      <c r="BA39" s="32"/>
+      <c r="BB39" s="32"/>
+      <c r="BC39" s="32"/>
+      <c r="BD39" s="32"/>
+      <c r="BE39" s="32"/>
+      <c r="BF39" s="32"/>
+      <c r="BG39" s="32"/>
+      <c r="BH39" s="32"/>
+      <c r="BI39" s="32"/>
+      <c r="BJ39" s="32"/>
+      <c r="BK39" s="32"/>
+      <c r="BL39" s="32"/>
+      <c r="BM39" s="32"/>
+      <c r="BN39" s="32"/>
+      <c r="BO39" s="32"/>
+      <c r="BP39" s="32"/>
+      <c r="BQ39" s="32"/>
+      <c r="BR39" s="32"/>
+      <c r="BS39" s="32"/>
+      <c r="BT39" s="32"/>
+      <c r="BU39" s="32"/>
+      <c r="BV39" s="32"/>
+      <c r="BW39" s="32"/>
+      <c r="BX39" s="32"/>
+      <c r="BY39" s="32"/>
+      <c r="BZ39" s="32"/>
+      <c r="CA39" s="32"/>
+      <c r="CB39" s="32"/>
+      <c r="CC39" s="32"/>
+      <c r="CD39" s="32"/>
+      <c r="CE39" s="32"/>
+      <c r="CF39" s="32"/>
+      <c r="CG39" s="32"/>
+      <c r="CH39" s="32"/>
+      <c r="CI39" s="32"/>
+      <c r="CJ39" s="32"/>
+      <c r="CK39" s="32"/>
+      <c r="CL39" s="32"/>
+      <c r="CM39" s="32"/>
+      <c r="CN39" s="32"/>
+      <c r="CO39" s="32"/>
+      <c r="CP39" s="32"/>
+      <c r="CQ39" s="32"/>
+      <c r="CR39" s="32"/>
+      <c r="CS39" s="32"/>
+      <c r="CT39" s="32"/>
+      <c r="CU39" s="32"/>
+      <c r="CV39" s="32"/>
+      <c r="CW39" s="32"/>
+      <c r="CX39" s="32"/>
+      <c r="CY39" s="32"/>
+      <c r="CZ39" s="32"/>
+      <c r="DA39" s="32"/>
+      <c r="DB39" s="32"/>
+      <c r="DC39" s="32"/>
+      <c r="DD39" s="32"/>
+      <c r="DE39" s="32"/>
+      <c r="DF39" s="32"/>
+      <c r="DG39" s="32"/>
+      <c r="DH39" s="32"/>
+      <c r="DI39" s="32"/>
+      <c r="DJ39" s="32"/>
+      <c r="DK39" s="32"/>
+      <c r="DL39" s="32"/>
+      <c r="DM39" s="32"/>
+      <c r="DN39" s="32"/>
+      <c r="DO39" s="32"/>
+      <c r="DP39" s="32"/>
+      <c r="DQ39" s="32"/>
+      <c r="DR39" s="32"/>
+      <c r="DS39" s="32"/>
+      <c r="DT39" s="32"/>
+      <c r="DU39" s="32"/>
+      <c r="DV39" s="32"/>
+      <c r="DW39" s="32"/>
+      <c r="DX39" s="32"/>
+      <c r="DY39" s="32"/>
+      <c r="DZ39" s="32"/>
+      <c r="EA39" s="32"/>
+      <c r="EB39" s="32"/>
+      <c r="EC39" s="32"/>
+      <c r="ED39" s="32"/>
+      <c r="EE39" s="32"/>
+      <c r="EF39" s="32"/>
+      <c r="EG39" s="32"/>
+      <c r="EH39" s="32"/>
+      <c r="EI39" s="32"/>
+      <c r="EJ39" s="32"/>
+      <c r="EK39" s="32"/>
+      <c r="EL39" s="32"/>
+      <c r="EM39" s="32"/>
+      <c r="EN39" s="32"/>
+      <c r="EO39" s="32"/>
+      <c r="EP39" s="32"/>
+      <c r="EQ39" s="32"/>
+      <c r="ER39" s="32"/>
+      <c r="ES39" s="32"/>
+      <c r="ET39" s="32"/>
+      <c r="EU39" s="32"/>
+      <c r="EV39" s="32"/>
+      <c r="EW39" s="32"/>
+      <c r="EX39" s="32"/>
+      <c r="EY39" s="32"/>
+      <c r="EZ39" s="32"/>
+      <c r="FA39" s="32"/>
+      <c r="FB39" s="32"/>
+      <c r="FC39" s="32"/>
+      <c r="FD39" s="32"/>
+      <c r="FE39" s="32"/>
+      <c r="FF39" s="32"/>
+      <c r="FG39" s="32"/>
+      <c r="FH39" s="32"/>
+      <c r="FI39" s="32"/>
+      <c r="FJ39" s="32"/>
+      <c r="FK39" s="32"/>
+      <c r="FL39" s="32"/>
+      <c r="FM39" s="32"/>
+      <c r="FN39" s="32"/>
+      <c r="FO39" s="32"/>
+      <c r="FP39" s="32"/>
+      <c r="FQ39" s="32"/>
+      <c r="FR39" s="32"/>
+      <c r="FS39" s="32"/>
+      <c r="FT39" s="32"/>
+      <c r="FU39" s="32"/>
+      <c r="FV39" s="32"/>
+      <c r="FW39" s="32"/>
+      <c r="FX39" s="32"/>
+      <c r="FY39" s="32"/>
+      <c r="FZ39" s="32"/>
+      <c r="GA39" s="32"/>
+      <c r="GB39" s="32"/>
+      <c r="GC39" s="32"/>
+      <c r="GD39" s="32"/>
+      <c r="GE39" s="32"/>
+      <c r="GF39" s="32"/>
+      <c r="GG39" s="32"/>
+      <c r="GH39" s="32"/>
+      <c r="GI39" s="32"/>
+      <c r="GJ39" s="32"/>
+      <c r="GK39" s="32"/>
+      <c r="GL39" s="32"/>
+      <c r="GM39" s="32"/>
+      <c r="GN39" s="32"/>
+      <c r="GO39" s="32"/>
+      <c r="GP39" s="32"/>
+      <c r="GQ39" s="32"/>
+      <c r="GR39" s="32"/>
+      <c r="GS39" s="32"/>
+      <c r="GT39" s="32"/>
+      <c r="GU39" s="32"/>
+      <c r="GV39" s="32"/>
+      <c r="GW39" s="32"/>
+      <c r="GX39" s="32"/>
+      <c r="GY39" s="32"/>
+      <c r="GZ39" s="32"/>
+      <c r="HA39" s="32"/>
+      <c r="HB39" s="32"/>
+      <c r="HC39" s="32"/>
+      <c r="HD39" s="32"/>
+      <c r="HE39" s="32"/>
+      <c r="HF39" s="32"/>
+      <c r="HG39" s="32"/>
+      <c r="HH39" s="32"/>
+      <c r="HI39" s="32"/>
+      <c r="HJ39" s="32"/>
+      <c r="HK39" s="32"/>
+      <c r="HL39" s="32"/>
+      <c r="HM39" s="32"/>
+      <c r="HN39" s="32"/>
+      <c r="HO39" s="32"/>
+      <c r="HP39" s="32"/>
+      <c r="HQ39" s="32"/>
+      <c r="HR39" s="32"/>
+      <c r="HS39" s="32"/>
+      <c r="HT39" s="32"/>
+      <c r="HU39" s="32"/>
+      <c r="HV39" s="32"/>
+      <c r="HW39" s="32"/>
+      <c r="HX39" s="32"/>
+      <c r="HY39" s="32"/>
+      <c r="HZ39" s="32"/>
+      <c r="IA39" s="32"/>
+      <c r="IB39" s="32"/>
+      <c r="IC39" s="32"/>
+      <c r="ID39" s="32"/>
+      <c r="IE39" s="32"/>
+      <c r="IF39" s="32"/>
+      <c r="IG39" s="32"/>
+      <c r="IH39" s="32"/>
+      <c r="II39" s="32"/>
+      <c r="IJ39" s="32"/>
+      <c r="IK39" s="32"/>
+      <c r="IL39" s="32"/>
+      <c r="IM39" s="32"/>
+      <c r="IN39" s="32"/>
+      <c r="IO39" s="32"/>
+      <c r="IP39" s="32"/>
+      <c r="IQ39" s="32"/>
+      <c r="IR39" s="32"/>
+      <c r="IS39" s="32"/>
+      <c r="IT39" s="32"/>
+      <c r="IU39" s="80"/>
+    </row>
+    <row r="40" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A40" s="89" t="n">
+        <v>42736</v>
+      </c>
+      <c r="B40" s="5"/>
+      <c r="C40" s="85" t="s">
+        <v>82</v>
+      </c>
+      <c r="D40" s="85" t="s">
+        <v>336</v>
+      </c>
+      <c r="E40" s="85" t="s">
+        <v>61</v>
+      </c>
+      <c r="F40" s="5"/>
+      <c r="G40" s="85" t="s">
+        <v>337</v>
+      </c>
+      <c r="H40" s="5"/>
+      <c r="I40" s="5"/>
+      <c r="J40" s="5"/>
+      <c r="K40" s="86" t="s">
+        <v>40</v>
+      </c>
+      <c r="L40" s="13"/>
+      <c r="M40" s="3"/>
+      <c r="N40" s="92"/>
+      <c r="O40" s="93"/>
+      <c r="P40" s="93"/>
+      <c r="Q40" s="93"/>
+      <c r="R40" s="93"/>
+      <c r="S40" s="93"/>
+      <c r="T40" s="93"/>
+      <c r="U40" s="93"/>
+      <c r="V40" s="93"/>
+      <c r="W40" s="93"/>
+      <c r="X40" s="93"/>
+      <c r="Y40" s="93"/>
+      <c r="Z40" s="93"/>
+      <c r="AA40" s="93"/>
+      <c r="AB40" s="93"/>
+      <c r="AC40" s="93"/>
+      <c r="AD40" s="93"/>
+      <c r="AE40" s="93"/>
+      <c r="AF40" s="93"/>
+      <c r="AG40" s="93"/>
+      <c r="AH40" s="93"/>
+      <c r="AI40" s="93"/>
+      <c r="AJ40" s="93"/>
+      <c r="AK40" s="93"/>
+      <c r="AL40" s="93"/>
+      <c r="AM40" s="93"/>
+      <c r="AN40" s="93"/>
+      <c r="AO40" s="93"/>
+      <c r="AP40" s="93"/>
+      <c r="AQ40" s="93"/>
+      <c r="AR40" s="93"/>
+      <c r="AS40" s="93"/>
+      <c r="AT40" s="93"/>
+      <c r="AU40" s="93"/>
+      <c r="AV40" s="93"/>
+      <c r="AW40" s="93"/>
+      <c r="AX40" s="93"/>
+      <c r="AY40" s="93"/>
+      <c r="AZ40" s="93"/>
+      <c r="BA40" s="93"/>
+      <c r="BB40" s="93"/>
+      <c r="BC40" s="93"/>
+      <c r="BD40" s="93"/>
+      <c r="BE40" s="93"/>
+      <c r="BF40" s="93"/>
+      <c r="BG40" s="93"/>
+      <c r="BH40" s="93"/>
+      <c r="BI40" s="93"/>
+      <c r="BJ40" s="93"/>
+      <c r="BK40" s="93"/>
+      <c r="BL40" s="93"/>
+      <c r="BM40" s="93"/>
+      <c r="BN40" s="93"/>
+      <c r="BO40" s="93"/>
+      <c r="BP40" s="93"/>
+      <c r="BQ40" s="93"/>
+      <c r="BR40" s="93"/>
+      <c r="BS40" s="93"/>
+      <c r="BT40" s="93"/>
+      <c r="BU40" s="93"/>
+      <c r="BV40" s="93"/>
+      <c r="BW40" s="93"/>
+      <c r="BX40" s="93"/>
+      <c r="BY40" s="93"/>
+      <c r="BZ40" s="93"/>
+      <c r="CA40" s="93"/>
+      <c r="CB40" s="93"/>
+      <c r="CC40" s="93"/>
+      <c r="CD40" s="93"/>
+      <c r="CE40" s="93"/>
+      <c r="CF40" s="93"/>
+      <c r="CG40" s="93"/>
+      <c r="CH40" s="93"/>
+      <c r="CI40" s="93"/>
+      <c r="CJ40" s="93"/>
+      <c r="CK40" s="93"/>
+      <c r="CL40" s="93"/>
+      <c r="CM40" s="93"/>
+      <c r="CN40" s="93"/>
+      <c r="CO40" s="93"/>
+      <c r="CP40" s="93"/>
+      <c r="CQ40" s="93"/>
+      <c r="CR40" s="93"/>
+      <c r="CS40" s="93"/>
+      <c r="CT40" s="93"/>
+      <c r="CU40" s="93"/>
+      <c r="CV40" s="93"/>
+      <c r="CW40" s="93"/>
+      <c r="CX40" s="93"/>
+      <c r="CY40" s="93"/>
+      <c r="CZ40" s="93"/>
+      <c r="DA40" s="93"/>
+      <c r="DB40" s="93"/>
+      <c r="DC40" s="93"/>
+      <c r="DD40" s="93"/>
+      <c r="DE40" s="93"/>
+      <c r="DF40" s="93"/>
+      <c r="DG40" s="93"/>
+      <c r="DH40" s="93"/>
+      <c r="DI40" s="93"/>
+      <c r="DJ40" s="93"/>
+      <c r="DK40" s="93"/>
+      <c r="DL40" s="93"/>
+      <c r="DM40" s="93"/>
+      <c r="DN40" s="93"/>
+      <c r="DO40" s="93"/>
+      <c r="DP40" s="93"/>
+      <c r="DQ40" s="93"/>
+      <c r="DR40" s="93"/>
+      <c r="DS40" s="93"/>
+      <c r="DT40" s="93"/>
+      <c r="DU40" s="93"/>
+      <c r="DV40" s="93"/>
+      <c r="DW40" s="93"/>
+      <c r="DX40" s="93"/>
+      <c r="DY40" s="93"/>
+      <c r="DZ40" s="93"/>
+      <c r="EA40" s="93"/>
+      <c r="EB40" s="93"/>
+      <c r="EC40" s="93"/>
+      <c r="ED40" s="93"/>
+      <c r="EE40" s="93"/>
+      <c r="EF40" s="93"/>
+      <c r="EG40" s="93"/>
+      <c r="EH40" s="93"/>
+      <c r="EI40" s="93"/>
+      <c r="EJ40" s="93"/>
+      <c r="EK40" s="93"/>
+      <c r="EL40" s="93"/>
+      <c r="EM40" s="93"/>
+      <c r="EN40" s="93"/>
+      <c r="EO40" s="93"/>
+      <c r="EP40" s="93"/>
+      <c r="EQ40" s="93"/>
+      <c r="ER40" s="93"/>
+      <c r="ES40" s="93"/>
+      <c r="ET40" s="93"/>
+      <c r="EU40" s="93"/>
+      <c r="EV40" s="93"/>
+      <c r="EW40" s="93"/>
+      <c r="EX40" s="93"/>
+      <c r="EY40" s="93"/>
+      <c r="EZ40" s="93"/>
+      <c r="FA40" s="93"/>
+      <c r="FB40" s="93"/>
+      <c r="FC40" s="93"/>
+      <c r="FD40" s="93"/>
+      <c r="FE40" s="93"/>
+      <c r="FF40" s="93"/>
+      <c r="FG40" s="93"/>
+      <c r="FH40" s="93"/>
+      <c r="FI40" s="93"/>
+      <c r="FJ40" s="93"/>
+      <c r="FK40" s="93"/>
+      <c r="FL40" s="93"/>
+      <c r="FM40" s="93"/>
+      <c r="FN40" s="93"/>
+      <c r="FO40" s="93"/>
+      <c r="FP40" s="93"/>
+      <c r="FQ40" s="93"/>
+      <c r="FR40" s="93"/>
+      <c r="FS40" s="93"/>
+      <c r="FT40" s="93"/>
+      <c r="FU40" s="93"/>
+      <c r="FV40" s="93"/>
+      <c r="FW40" s="93"/>
+      <c r="FX40" s="93"/>
+      <c r="FY40" s="93"/>
+      <c r="FZ40" s="93"/>
+      <c r="GA40" s="93"/>
+      <c r="GB40" s="93"/>
+      <c r="GC40" s="93"/>
+      <c r="GD40" s="93"/>
+      <c r="GE40" s="93"/>
+      <c r="GF40" s="93"/>
+      <c r="GG40" s="93"/>
+      <c r="GH40" s="93"/>
+      <c r="GI40" s="93"/>
+      <c r="GJ40" s="93"/>
+      <c r="GK40" s="93"/>
+      <c r="GL40" s="93"/>
+      <c r="GM40" s="93"/>
+      <c r="GN40" s="93"/>
+      <c r="GO40" s="93"/>
+      <c r="GP40" s="93"/>
+      <c r="GQ40" s="93"/>
+      <c r="GR40" s="93"/>
+      <c r="GS40" s="93"/>
+      <c r="GT40" s="93"/>
+      <c r="GU40" s="93"/>
+      <c r="GV40" s="93"/>
+      <c r="GW40" s="93"/>
+      <c r="GX40" s="93"/>
+      <c r="GY40" s="93"/>
+      <c r="GZ40" s="93"/>
+      <c r="HA40" s="93"/>
+      <c r="HB40" s="93"/>
+      <c r="HC40" s="93"/>
+      <c r="HD40" s="93"/>
+      <c r="HE40" s="93"/>
+      <c r="HF40" s="93"/>
+      <c r="HG40" s="93"/>
+      <c r="HH40" s="93"/>
+      <c r="HI40" s="93"/>
+      <c r="HJ40" s="93"/>
+      <c r="HK40" s="93"/>
+      <c r="HL40" s="93"/>
+      <c r="HM40" s="93"/>
+      <c r="HN40" s="93"/>
+      <c r="HO40" s="93"/>
+      <c r="HP40" s="93"/>
+      <c r="HQ40" s="93"/>
+      <c r="HR40" s="93"/>
+      <c r="HS40" s="93"/>
+      <c r="HT40" s="93"/>
+      <c r="HU40" s="93"/>
+      <c r="HV40" s="93"/>
+      <c r="HW40" s="93"/>
+      <c r="HX40" s="93"/>
+      <c r="HY40" s="93"/>
+      <c r="HZ40" s="93"/>
+      <c r="IA40" s="93"/>
+      <c r="IB40" s="93"/>
+      <c r="IC40" s="93"/>
+      <c r="ID40" s="93"/>
+      <c r="IE40" s="93"/>
+      <c r="IF40" s="93"/>
+      <c r="IG40" s="93"/>
+      <c r="IH40" s="93"/>
+      <c r="II40" s="93"/>
+      <c r="IJ40" s="93"/>
+      <c r="IK40" s="93"/>
+      <c r="IL40" s="93"/>
+      <c r="IM40" s="93"/>
+      <c r="IN40" s="93"/>
+      <c r="IO40" s="93"/>
+      <c r="IP40" s="93"/>
+      <c r="IQ40" s="93"/>
+      <c r="IR40" s="93"/>
+      <c r="IS40" s="93"/>
+      <c r="IT40" s="93"/>
+      <c r="IU40" s="94"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -12112,7 +13195,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="10" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="B1" s="95" t="s">
         <v>11</v>
@@ -12141,13 +13224,13 @@
         <v>42</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="G2" s="98"/>
       <c r="H2" s="99"/>
@@ -12190,7 +13273,7 @@
         <v>59</v>
       </c>
       <c r="E4" s="104" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="F4" s="51" t="n">
         <v>1</v>
@@ -12212,7 +13295,7 @@
         <v>62</v>
       </c>
       <c r="E5" s="35" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="F5" s="4" t="n">
         <v>2</v>
@@ -12234,7 +13317,7 @@
         <v>64</v>
       </c>
       <c r="E6" s="35" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="F6" s="4" t="n">
         <v>3</v>
@@ -12333,7 +13416,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="10" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>11</v>
@@ -12368,13 +13451,13 @@
         <v>42</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="G2" s="98"/>
       <c r="H2" s="99"/>
@@ -12429,7 +13512,7 @@
         <v>59</v>
       </c>
       <c r="E4" s="104" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="F4" s="51" t="n">
         <v>1</v>
@@ -12457,7 +13540,7 @@
         <v>62</v>
       </c>
       <c r="E5" s="35" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="F5" s="4" t="n">
         <v>2</v>
@@ -12485,7 +13568,7 @@
         <v>64</v>
       </c>
       <c r="E6" s="35" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="F6" s="4" t="n">
         <v>3</v>
@@ -12614,7 +13697,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="10" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>11</v>
@@ -12649,13 +13732,13 @@
         <v>42</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="G2" s="108"/>
       <c r="H2" s="109"/>
@@ -12710,7 +13793,7 @@
         <v>59</v>
       </c>
       <c r="E4" s="104" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="F4" s="51" t="n">
         <v>1</v>
@@ -12738,7 +13821,7 @@
         <v>62</v>
       </c>
       <c r="E5" s="35" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="F5" s="4" t="n">
         <v>2</v>
@@ -12766,7 +13849,7 @@
         <v>64</v>
       </c>
       <c r="E6" s="35" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="F6" s="4" t="n">
         <v>3</v>
@@ -12895,7 +13978,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="19" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="110" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="B1" s="95" t="s">
         <v>11</v>
@@ -12924,13 +14007,13 @@
         <v>42</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="G2" s="98"/>
       <c r="H2" s="99"/>
@@ -12973,7 +14056,7 @@
         <v>59</v>
       </c>
       <c r="E4" s="104" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="F4" s="51" t="n">
         <v>1</v>
@@ -12995,7 +14078,7 @@
         <v>62</v>
       </c>
       <c r="E5" s="35" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="F5" s="4" t="n">
         <v>2</v>
@@ -13017,7 +14100,7 @@
         <v>64</v>
       </c>
       <c r="E6" s="35" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="F6" s="4" t="n">
         <v>3</v>
@@ -13116,7 +14199,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="10" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>11</v>
@@ -13149,13 +14232,13 @@
       </c>
       <c r="C2" s="111"/>
       <c r="D2" s="14" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="G2" s="13"/>
       <c r="H2" s="3"/>
@@ -13176,16 +14259,16 @@
         <v>20</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="G3" s="112"/>
       <c r="H3" s="113"/>
@@ -13204,7 +14287,7 @@
       </c>
       <c r="B4" s="72"/>
       <c r="C4" s="114" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="D4" s="114" t="s">
         <v>24</v>
@@ -13232,7 +14315,7 @@
       </c>
       <c r="B5" s="60"/>
       <c r="C5" s="115" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="D5" s="115" t="s">
         <v>24</v>
@@ -13260,7 +14343,7 @@
       </c>
       <c r="B6" s="60"/>
       <c r="C6" s="115" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="D6" s="115" t="s">
         <v>24</v>
@@ -13288,7 +14371,7 @@
       </c>
       <c r="B7" s="83"/>
       <c r="C7" s="116" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="D7" s="116" t="s">
         <v>24</v>
@@ -13316,7 +14399,7 @@
       </c>
       <c r="B8" s="117"/>
       <c r="C8" s="11" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="D8" s="11" t="s">
         <v>24</v>
@@ -13405,7 +14488,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="10" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>11</v>
@@ -13436,13 +14519,13 @@
         <v>15</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="F2" s="108"/>
       <c r="G2" s="109"/>
@@ -13466,10 +14549,10 @@
         <v>51</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="F3" s="13"/>
       <c r="G3" s="3"/>
@@ -13491,10 +14574,10 @@
         <v>37</v>
       </c>
       <c r="D4" s="38" t="s">
+        <v>370</v>
+      </c>
+      <c r="E4" s="118" t="s">
         <v>369</v>
-      </c>
-      <c r="E4" s="118" t="s">
-        <v>368</v>
       </c>
       <c r="F4" s="13"/>
       <c r="G4" s="3"/>
@@ -13643,7 +14726,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="10" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>11</v>
@@ -13674,16 +14757,16 @@
         <v>15</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="G2" s="15"/>
       <c r="H2" s="16"/>
@@ -13709,10 +14792,10 @@
         <v>105</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="G3" s="17"/>
       <c r="H3" s="16"/>
@@ -13736,10 +14819,10 @@
         <v>59</v>
       </c>
       <c r="E4" s="120" t="s">
+        <v>370</v>
+      </c>
+      <c r="F4" s="118" t="s">
         <v>369</v>
-      </c>
-      <c r="F4" s="118" t="s">
-        <v>368</v>
       </c>
       <c r="G4" s="13"/>
       <c r="H4" s="3"/>
@@ -13763,10 +14846,10 @@
         <v>62</v>
       </c>
       <c r="E5" s="122" t="s">
+        <v>370</v>
+      </c>
+      <c r="F5" s="118" t="s">
         <v>369</v>
-      </c>
-      <c r="F5" s="118" t="s">
-        <v>368</v>
       </c>
       <c r="G5" s="13"/>
       <c r="H5" s="3"/>
@@ -13790,10 +14873,10 @@
         <v>64</v>
       </c>
       <c r="E6" s="122" t="s">
+        <v>370</v>
+      </c>
+      <c r="F6" s="118" t="s">
         <v>369</v>
-      </c>
-      <c r="F6" s="118" t="s">
-        <v>368</v>
       </c>
       <c r="G6" s="13"/>
       <c r="H6" s="3"/>
@@ -13817,10 +14900,10 @@
         <v>66</v>
       </c>
       <c r="E7" s="122" t="s">
+        <v>370</v>
+      </c>
+      <c r="F7" s="118" t="s">
         <v>369</v>
-      </c>
-      <c r="F7" s="118" t="s">
-        <v>368</v>
       </c>
       <c r="G7" s="13"/>
       <c r="H7" s="3"/>
@@ -13844,10 +14927,10 @@
         <v>68</v>
       </c>
       <c r="E8" s="122" t="s">
+        <v>370</v>
+      </c>
+      <c r="F8" s="118" t="s">
         <v>369</v>
-      </c>
-      <c r="F8" s="118" t="s">
-        <v>368</v>
       </c>
       <c r="G8" s="13"/>
       <c r="H8" s="3"/>
@@ -13871,10 +14954,10 @@
         <v>71</v>
       </c>
       <c r="E9" s="122" t="s">
+        <v>370</v>
+      </c>
+      <c r="F9" s="118" t="s">
         <v>369</v>
-      </c>
-      <c r="F9" s="118" t="s">
-        <v>368</v>
       </c>
       <c r="G9" s="13"/>
       <c r="H9" s="3"/>
@@ -13898,10 +14981,10 @@
         <v>75</v>
       </c>
       <c r="E10" s="122" t="s">
+        <v>370</v>
+      </c>
+      <c r="F10" s="118" t="s">
         <v>369</v>
-      </c>
-      <c r="F10" s="118" t="s">
-        <v>368</v>
       </c>
       <c r="G10" s="13"/>
       <c r="H10" s="3"/>
@@ -13925,10 +15008,10 @@
         <v>80</v>
       </c>
       <c r="E11" s="122" t="s">
+        <v>370</v>
+      </c>
+      <c r="F11" s="118" t="s">
         <v>369</v>
-      </c>
-      <c r="F11" s="118" t="s">
-        <v>368</v>
       </c>
       <c r="G11" s="13"/>
       <c r="H11" s="3"/>
@@ -13952,10 +15035,10 @@
         <v>83</v>
       </c>
       <c r="E12" s="124" t="s">
+        <v>370</v>
+      </c>
+      <c r="F12" s="118" t="s">
         <v>369</v>
-      </c>
-      <c r="F12" s="118" t="s">
-        <v>368</v>
       </c>
       <c r="G12" s="13"/>
       <c r="H12" s="3"/>
@@ -13979,10 +15062,10 @@
         <v>84</v>
       </c>
       <c r="E13" s="122" t="s">
+        <v>370</v>
+      </c>
+      <c r="F13" s="118" t="s">
         <v>369</v>
-      </c>
-      <c r="F13" s="118" t="s">
-        <v>368</v>
       </c>
       <c r="G13" s="13"/>
       <c r="H13" s="3"/>
@@ -14006,10 +15089,10 @@
         <v>86</v>
       </c>
       <c r="E14" s="122" t="s">
+        <v>370</v>
+      </c>
+      <c r="F14" s="118" t="s">
         <v>369</v>
-      </c>
-      <c r="F14" s="118" t="s">
-        <v>368</v>
       </c>
       <c r="G14" s="13"/>
       <c r="H14" s="3"/>
@@ -14033,10 +15116,10 @@
         <v>88</v>
       </c>
       <c r="E15" s="122" t="s">
+        <v>370</v>
+      </c>
+      <c r="F15" s="118" t="s">
         <v>369</v>
-      </c>
-      <c r="F15" s="118" t="s">
-        <v>368</v>
       </c>
       <c r="G15" s="13"/>
       <c r="H15" s="3"/>
@@ -14060,10 +15143,10 @@
         <v>90</v>
       </c>
       <c r="E16" s="122" t="s">
+        <v>370</v>
+      </c>
+      <c r="F16" s="118" t="s">
         <v>369</v>
-      </c>
-      <c r="F16" s="118" t="s">
-        <v>368</v>
       </c>
       <c r="G16" s="13"/>
       <c r="H16" s="3"/>
@@ -14106,7 +15189,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="10" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>11</v>
@@ -14137,16 +15220,16 @@
         <v>15</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="G2" s="21"/>
       <c r="H2" s="22"/>
@@ -14172,10 +15255,10 @@
         <v>199</v>
       </c>
       <c r="E3" s="69" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="F3" s="69" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="G3" s="70"/>
       <c r="H3" s="22"/>
@@ -14199,10 +15282,10 @@
         <v>152</v>
       </c>
       <c r="E4" s="126" t="s">
+        <v>370</v>
+      </c>
+      <c r="F4" s="118" t="s">
         <v>369</v>
-      </c>
-      <c r="F4" s="118" t="s">
-        <v>368</v>
       </c>
       <c r="G4" s="13"/>
       <c r="H4" s="3"/>
@@ -14226,10 +15309,10 @@
         <v>156</v>
       </c>
       <c r="E5" s="128" t="s">
+        <v>370</v>
+      </c>
+      <c r="F5" s="118" t="s">
         <v>369</v>
-      </c>
-      <c r="F5" s="118" t="s">
-        <v>368</v>
       </c>
       <c r="G5" s="13"/>
       <c r="H5" s="3"/>
@@ -14253,10 +15336,10 @@
         <v>160</v>
       </c>
       <c r="E6" s="128" t="s">
+        <v>370</v>
+      </c>
+      <c r="F6" s="118" t="s">
         <v>369</v>
-      </c>
-      <c r="F6" s="118" t="s">
-        <v>368</v>
       </c>
       <c r="G6" s="13"/>
       <c r="H6" s="3"/>
@@ -14280,10 +15363,10 @@
         <v>164</v>
       </c>
       <c r="E7" s="128" t="s">
+        <v>370</v>
+      </c>
+      <c r="F7" s="118" t="s">
         <v>369</v>
-      </c>
-      <c r="F7" s="118" t="s">
-        <v>368</v>
       </c>
       <c r="G7" s="13"/>
       <c r="H7" s="3"/>
@@ -14307,10 +15390,10 @@
         <v>171</v>
       </c>
       <c r="E8" s="128" t="s">
+        <v>370</v>
+      </c>
+      <c r="F8" s="118" t="s">
         <v>369</v>
-      </c>
-      <c r="F8" s="118" t="s">
-        <v>368</v>
       </c>
       <c r="G8" s="13"/>
       <c r="H8" s="3"/>
@@ -14334,10 +15417,10 @@
         <v>167</v>
       </c>
       <c r="E9" s="128" t="s">
+        <v>370</v>
+      </c>
+      <c r="F9" s="118" t="s">
         <v>369</v>
-      </c>
-      <c r="F9" s="118" t="s">
-        <v>368</v>
       </c>
       <c r="G9" s="13"/>
       <c r="H9" s="3"/>
@@ -14361,10 +15444,10 @@
         <v>175</v>
       </c>
       <c r="E10" s="128" t="s">
+        <v>370</v>
+      </c>
+      <c r="F10" s="118" t="s">
         <v>369</v>
-      </c>
-      <c r="F10" s="118" t="s">
-        <v>368</v>
       </c>
       <c r="G10" s="13"/>
       <c r="H10" s="3"/>
@@ -14388,10 +15471,10 @@
         <v>182</v>
       </c>
       <c r="E11" s="128" t="s">
+        <v>370</v>
+      </c>
+      <c r="F11" s="118" t="s">
         <v>369</v>
-      </c>
-      <c r="F11" s="118" t="s">
-        <v>368</v>
       </c>
       <c r="G11" s="13"/>
       <c r="H11" s="3"/>
@@ -14415,10 +15498,10 @@
         <v>185</v>
       </c>
       <c r="E12" s="128" t="s">
+        <v>370</v>
+      </c>
+      <c r="F12" s="118" t="s">
         <v>369</v>
-      </c>
-      <c r="F12" s="118" t="s">
-        <v>368</v>
       </c>
       <c r="G12" s="13"/>
       <c r="H12" s="3"/>
@@ -14495,7 +15578,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="10" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>11</v>
@@ -14527,16 +15610,16 @@
         <v>15</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="G2" s="21"/>
       <c r="H2" s="22"/>
@@ -14560,13 +15643,13 @@
         <v>51</v>
       </c>
       <c r="D3" s="69" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="E3" s="69" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="F3" s="69" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="G3" s="70"/>
       <c r="H3" s="71"/>
@@ -14591,10 +15674,10 @@
         <v>124</v>
       </c>
       <c r="E4" s="38" t="s">
+        <v>370</v>
+      </c>
+      <c r="F4" s="118" t="s">
         <v>369</v>
-      </c>
-      <c r="F4" s="118" t="s">
-        <v>368</v>
       </c>
       <c r="G4" s="13"/>
       <c r="H4" s="3"/>
@@ -14968,7 +16051,7 @@
   </sheetPr>
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -14987,7 +16070,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="10" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>11</v>
@@ -15006,19 +16089,19 @@
       <c r="A2" s="111"/>
       <c r="B2" s="111"/>
       <c r="C2" s="14" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="G2" s="14" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15038,10 +16121,10 @@
         <v>222</v>
       </c>
       <c r="F3" s="69" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="G3" s="69" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15056,13 +16139,13 @@
         <v>75</v>
       </c>
       <c r="E4" s="114" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="F4" s="38" t="s">
+        <v>370</v>
+      </c>
+      <c r="G4" s="118" t="s">
         <v>369</v>
-      </c>
-      <c r="G4" s="118" t="s">
-        <v>368</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15077,13 +16160,13 @@
         <v>75</v>
       </c>
       <c r="E5" s="115" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="F5" s="38" t="s">
+        <v>370</v>
+      </c>
+      <c r="G5" s="118" t="s">
         <v>369</v>
-      </c>
-      <c r="G5" s="118" t="s">
-        <v>368</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15101,10 +16184,10 @@
         <v>286</v>
       </c>
       <c r="F6" s="38" t="s">
+        <v>370</v>
+      </c>
+      <c r="G6" s="118" t="s">
         <v>369</v>
-      </c>
-      <c r="G6" s="118" t="s">
-        <v>368</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15119,13 +16202,13 @@
         <v>75</v>
       </c>
       <c r="E7" s="115" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="F7" s="38" t="s">
+        <v>370</v>
+      </c>
+      <c r="G7" s="118" t="s">
         <v>369</v>
-      </c>
-      <c r="G7" s="118" t="s">
-        <v>368</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15140,13 +16223,13 @@
         <v>75</v>
       </c>
       <c r="E8" s="115" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="F8" s="38" t="s">
+        <v>370</v>
+      </c>
+      <c r="G8" s="118" t="s">
         <v>369</v>
-      </c>
-      <c r="G8" s="118" t="s">
-        <v>368</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15164,10 +16247,10 @@
         <v>292</v>
       </c>
       <c r="F9" s="38" t="s">
+        <v>370</v>
+      </c>
+      <c r="G9" s="118" t="s">
         <v>369</v>
-      </c>
-      <c r="G9" s="118" t="s">
-        <v>368</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15182,13 +16265,13 @@
         <v>75</v>
       </c>
       <c r="E10" s="115" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F10" s="38" t="s">
+        <v>370</v>
+      </c>
+      <c r="G10" s="118" t="s">
         <v>369</v>
-      </c>
-      <c r="G10" s="118" t="s">
-        <v>368</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15203,13 +16286,13 @@
         <v>75</v>
       </c>
       <c r="E11" s="115" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="F11" s="38" t="s">
+        <v>370</v>
+      </c>
+      <c r="G11" s="118" t="s">
         <v>369</v>
-      </c>
-      <c r="G11" s="118" t="s">
-        <v>368</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15224,13 +16307,13 @@
         <v>75</v>
       </c>
       <c r="E12" s="115" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="F12" s="38" t="s">
+        <v>370</v>
+      </c>
+      <c r="G12" s="118" t="s">
         <v>369</v>
-      </c>
-      <c r="G12" s="118" t="s">
-        <v>368</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15245,13 +16328,13 @@
         <v>75</v>
       </c>
       <c r="E13" s="115" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="F13" s="38" t="s">
+        <v>370</v>
+      </c>
+      <c r="G13" s="118" t="s">
         <v>369</v>
-      </c>
-      <c r="G13" s="118" t="s">
-        <v>368</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15266,13 +16349,13 @@
         <v>75</v>
       </c>
       <c r="E14" s="115" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="F14" s="38" t="s">
+        <v>370</v>
+      </c>
+      <c r="G14" s="118" t="s">
         <v>369</v>
-      </c>
-      <c r="G14" s="118" t="s">
-        <v>368</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15287,13 +16370,13 @@
         <v>75</v>
       </c>
       <c r="E15" s="115" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="F15" s="38" t="s">
+        <v>370</v>
+      </c>
+      <c r="G15" s="118" t="s">
         <v>369</v>
-      </c>
-      <c r="G15" s="118" t="s">
-        <v>368</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15311,10 +16394,10 @@
         <v>258</v>
       </c>
       <c r="F16" s="38" t="s">
+        <v>370</v>
+      </c>
+      <c r="G16" s="118" t="s">
         <v>369</v>
-      </c>
-      <c r="G16" s="118" t="s">
-        <v>368</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15332,10 +16415,10 @@
         <v>253</v>
       </c>
       <c r="F17" s="38" t="s">
+        <v>370</v>
+      </c>
+      <c r="G17" s="118" t="s">
         <v>369</v>
-      </c>
-      <c r="G17" s="118" t="s">
-        <v>368</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15350,13 +16433,13 @@
         <v>75</v>
       </c>
       <c r="E18" s="115" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="F18" s="38" t="s">
+        <v>370</v>
+      </c>
+      <c r="G18" s="118" t="s">
         <v>369</v>
-      </c>
-      <c r="G18" s="118" t="s">
-        <v>368</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15371,13 +16454,13 @@
         <v>75</v>
       </c>
       <c r="E19" s="115" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="F19" s="38" t="s">
+        <v>370</v>
+      </c>
+      <c r="G19" s="118" t="s">
         <v>369</v>
-      </c>
-      <c r="G19" s="118" t="s">
-        <v>368</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15392,13 +16475,13 @@
         <v>75</v>
       </c>
       <c r="E20" s="116" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="F20" s="38" t="s">
+        <v>370</v>
+      </c>
+      <c r="G20" s="118" t="s">
         <v>369</v>
-      </c>
-      <c r="G20" s="118" t="s">
-        <v>368</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15413,13 +16496,13 @@
         <v>80</v>
       </c>
       <c r="E21" s="114" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="F21" s="38" t="s">
+        <v>370</v>
+      </c>
+      <c r="G21" s="118" t="s">
         <v>369</v>
-      </c>
-      <c r="G21" s="118" t="s">
-        <v>368</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15434,13 +16517,13 @@
         <v>80</v>
       </c>
       <c r="E22" s="115" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="F22" s="38" t="s">
+        <v>370</v>
+      </c>
+      <c r="G22" s="118" t="s">
         <v>369</v>
-      </c>
-      <c r="G22" s="118" t="s">
-        <v>368</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15455,13 +16538,13 @@
         <v>80</v>
       </c>
       <c r="E23" s="115" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="F23" s="38" t="s">
+        <v>370</v>
+      </c>
+      <c r="G23" s="118" t="s">
         <v>369</v>
-      </c>
-      <c r="G23" s="118" t="s">
-        <v>368</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15476,13 +16559,13 @@
         <v>80</v>
       </c>
       <c r="E24" s="115" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="F24" s="38" t="s">
+        <v>370</v>
+      </c>
+      <c r="G24" s="118" t="s">
         <v>369</v>
-      </c>
-      <c r="G24" s="118" t="s">
-        <v>368</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15497,13 +16580,13 @@
         <v>80</v>
       </c>
       <c r="E25" s="116" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="F25" s="38" t="s">
+        <v>370</v>
+      </c>
+      <c r="G25" s="118" t="s">
         <v>369</v>
-      </c>
-      <c r="G25" s="118" t="s">
-        <v>368</v>
       </c>
     </row>
   </sheetData>
@@ -15821,7 +16904,7 @@
   </sheetPr>
   <dimension ref="A1:IU16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
bundle document sort order (#172)
* implement bundle sort order

* added f-test

* implement f-tests

* typo

* update ccd config
</commit_message>
<xml_diff>
--- a/src/aat/resources/adv_bundling_functional_tests_ccd_def.xlsx
+++ b/src/aat/resources/adv_bundling_functional_tests_ccd_def.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Change History" sheetId="1" state="visible" r:id="rId2"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1259" uniqueCount="381">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1265" uniqueCount="385">
   <si>
     <t xml:space="preserve">Change History</t>
   </si>
@@ -852,6 +852,18 @@
   </si>
   <si>
     <t xml:space="preserve">Tests – Config uses an invalid documentSet property</t>
+  </si>
+  <si>
+    <t xml:space="preserve">f-tests-12-sorting.yaml</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tests – Config sorts by date ascending</t>
+  </si>
+  <si>
+    <t xml:space="preserve">f-tests-13-sorting.yaml</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tests – Config sorts by date descending</t>
   </si>
   <si>
     <t xml:space="preserve">pageNumberFormat</t>
@@ -2200,12 +2212,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -2358,7 +2370,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="10" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>11</v>
@@ -2629,10 +2641,10 @@
         <v>15</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="E2" s="14" t="s">
         <v>46</v>
@@ -2641,16 +2653,16 @@
         <v>47</v>
       </c>
       <c r="G2" s="14" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="H2" s="14" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="I2" s="14" t="s">
         <v>48</v>
       </c>
       <c r="J2" s="14" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
       <c r="K2" s="14" t="s">
         <v>32</v>
@@ -2924,7 +2936,7 @@
         <v>55</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
       <c r="H3" s="6" t="s">
         <v>107</v>
@@ -3193,17 +3205,17 @@
       </c>
       <c r="B4" s="72"/>
       <c r="C4" s="73" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="E4" s="8" t="s">
         <v>61</v>
       </c>
       <c r="F4" s="24"/>
       <c r="G4" s="8" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
       <c r="H4" s="24"/>
       <c r="I4" s="24"/>
@@ -3462,17 +3474,17 @@
       </c>
       <c r="B5" s="60"/>
       <c r="C5" s="74" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="D5" s="34" t="s">
-        <v>283</v>
+        <v>287</v>
       </c>
       <c r="E5" s="34" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="34" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
@@ -3731,10 +3743,10 @@
       </c>
       <c r="B6" s="60"/>
       <c r="C6" s="74" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="D6" s="34" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
       <c r="E6" s="34" t="s">
         <v>61</v>
@@ -4000,17 +4012,17 @@
       </c>
       <c r="B7" s="83"/>
       <c r="C7" s="84" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="D7" s="85" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
       <c r="E7" s="85" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
       <c r="F7" s="5"/>
       <c r="G7" s="85" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
@@ -4269,17 +4281,17 @@
       </c>
       <c r="B8" s="24"/>
       <c r="C8" s="8" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="E8" s="8" t="s">
         <v>61</v>
       </c>
       <c r="F8" s="24"/>
       <c r="G8" s="8" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
       <c r="H8" s="24"/>
       <c r="I8" s="24"/>
@@ -4538,19 +4550,19 @@
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="34" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="D9" s="34" t="s">
-        <v>292</v>
+        <v>296</v>
       </c>
       <c r="E9" s="34" t="s">
         <v>78</v>
       </c>
       <c r="F9" s="34" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="G9" s="34" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
@@ -4809,17 +4821,17 @@
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="85" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="D10" s="85" t="s">
-        <v>283</v>
+        <v>287</v>
       </c>
       <c r="E10" s="85" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="F10" s="5"/>
       <c r="G10" s="85" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
@@ -5078,17 +5090,17 @@
       </c>
       <c r="B11" s="24"/>
       <c r="C11" s="8" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="E11" s="8" t="s">
         <v>61</v>
       </c>
       <c r="F11" s="24"/>
       <c r="G11" s="8" t="s">
-        <v>295</v>
+        <v>299</v>
       </c>
       <c r="H11" s="24"/>
       <c r="I11" s="24"/>
@@ -5347,19 +5359,19 @@
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="34" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="D12" s="34" t="s">
-        <v>292</v>
+        <v>296</v>
       </c>
       <c r="E12" s="34" t="s">
         <v>78</v>
       </c>
       <c r="F12" s="34" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="G12" s="34" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
@@ -5618,19 +5630,19 @@
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="34" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="D13" s="34" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
       <c r="E13" s="34" t="s">
         <v>78</v>
       </c>
       <c r="F13" s="34" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="G13" s="34" t="s">
-        <v>297</v>
+        <v>301</v>
       </c>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
@@ -5889,17 +5901,17 @@
       </c>
       <c r="B14" s="5"/>
       <c r="C14" s="85" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="D14" s="85" t="s">
-        <v>283</v>
+        <v>287</v>
       </c>
       <c r="E14" s="85" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="F14" s="5"/>
       <c r="G14" s="85" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
@@ -6161,14 +6173,14 @@
         <v>79</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>298</v>
+        <v>302</v>
       </c>
       <c r="E15" s="8" t="s">
         <v>61</v>
       </c>
       <c r="F15" s="24"/>
       <c r="G15" s="8" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
       <c r="H15" s="24"/>
       <c r="I15" s="24"/>
@@ -6430,14 +6442,14 @@
         <v>79</v>
       </c>
       <c r="D16" s="34" t="s">
-        <v>300</v>
+        <v>304</v>
       </c>
       <c r="E16" s="34" t="s">
         <v>61</v>
       </c>
       <c r="F16" s="3"/>
       <c r="G16" s="34" t="s">
-        <v>301</v>
+        <v>305</v>
       </c>
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
@@ -6699,7 +6711,7 @@
         <v>79</v>
       </c>
       <c r="D17" s="34" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
       <c r="E17" s="34" t="s">
         <v>70</v>
@@ -6968,14 +6980,14 @@
         <v>79</v>
       </c>
       <c r="D18" s="34" t="s">
-        <v>302</v>
+        <v>306</v>
       </c>
       <c r="E18" s="34" t="s">
-        <v>303</v>
+        <v>307</v>
       </c>
       <c r="F18" s="3"/>
       <c r="G18" s="34" t="s">
-        <v>304</v>
+        <v>308</v>
       </c>
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
@@ -7237,14 +7249,14 @@
         <v>79</v>
       </c>
       <c r="D19" s="34" t="s">
-        <v>305</v>
+        <v>309</v>
       </c>
       <c r="E19" s="34" t="s">
-        <v>303</v>
+        <v>307</v>
       </c>
       <c r="F19" s="3"/>
       <c r="G19" s="34" t="s">
-        <v>306</v>
+        <v>310</v>
       </c>
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
@@ -7506,16 +7518,16 @@
         <v>79</v>
       </c>
       <c r="D20" s="34" t="s">
-        <v>292</v>
+        <v>296</v>
       </c>
       <c r="E20" s="34" t="s">
         <v>78</v>
       </c>
       <c r="F20" s="34" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="G20" s="34" t="s">
-        <v>307</v>
+        <v>311</v>
       </c>
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
@@ -7777,16 +7789,16 @@
         <v>79</v>
       </c>
       <c r="D21" s="34" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
       <c r="E21" s="34" t="s">
         <v>78</v>
       </c>
       <c r="F21" s="34" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="G21" s="34" t="s">
-        <v>308</v>
+        <v>312</v>
       </c>
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
@@ -8048,14 +8060,14 @@
         <v>79</v>
       </c>
       <c r="D22" s="34" t="s">
-        <v>309</v>
+        <v>313</v>
       </c>
       <c r="E22" s="34" t="s">
         <v>61</v>
       </c>
       <c r="F22" s="3"/>
       <c r="G22" s="34" t="s">
-        <v>310</v>
+        <v>314</v>
       </c>
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
@@ -8317,14 +8329,14 @@
         <v>79</v>
       </c>
       <c r="D23" s="34" t="s">
-        <v>311</v>
+        <v>315</v>
       </c>
       <c r="E23" s="34" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
       <c r="F23" s="3"/>
       <c r="G23" s="34" t="s">
-        <v>312</v>
+        <v>316</v>
       </c>
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
@@ -8586,14 +8598,14 @@
         <v>79</v>
       </c>
       <c r="D24" s="34" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="E24" s="34" t="s">
-        <v>303</v>
+        <v>307</v>
       </c>
       <c r="F24" s="3"/>
       <c r="G24" s="34" t="s">
-        <v>314</v>
+        <v>318</v>
       </c>
       <c r="H24" s="3"/>
       <c r="I24" s="3"/>
@@ -8855,14 +8867,14 @@
         <v>79</v>
       </c>
       <c r="D25" s="34" t="s">
-        <v>315</v>
+        <v>319</v>
       </c>
       <c r="E25" s="34" t="s">
-        <v>303</v>
+        <v>307</v>
       </c>
       <c r="F25" s="3"/>
       <c r="G25" s="34" t="s">
-        <v>316</v>
+        <v>320</v>
       </c>
       <c r="H25" s="3"/>
       <c r="I25" s="3"/>
@@ -9124,14 +9136,14 @@
         <v>79</v>
       </c>
       <c r="D26" s="34" t="s">
-        <v>317</v>
+        <v>321</v>
       </c>
       <c r="E26" s="34" t="s">
-        <v>303</v>
+        <v>307</v>
       </c>
       <c r="F26" s="3"/>
       <c r="G26" s="34" t="s">
-        <v>318</v>
+        <v>322</v>
       </c>
       <c r="H26" s="3"/>
       <c r="I26" s="3"/>
@@ -9393,14 +9405,14 @@
         <v>79</v>
       </c>
       <c r="D27" s="34" t="s">
-        <v>319</v>
+        <v>323</v>
       </c>
       <c r="E27" s="34" t="s">
         <v>61</v>
       </c>
       <c r="F27" s="3"/>
       <c r="G27" s="34" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="H27" s="3"/>
       <c r="I27" s="3"/>
@@ -9662,14 +9674,14 @@
         <v>79</v>
       </c>
       <c r="D28" s="85" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="E28" s="85" t="s">
         <v>61</v>
       </c>
       <c r="F28" s="5"/>
       <c r="G28" s="85" t="s">
-        <v>322</v>
+        <v>326</v>
       </c>
       <c r="H28" s="5"/>
       <c r="I28" s="5"/>
@@ -9931,16 +9943,16 @@
         <v>79</v>
       </c>
       <c r="D29" s="75" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="E29" s="75" t="s">
         <v>73</v>
       </c>
       <c r="F29" s="75" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="G29" s="75" t="s">
-        <v>323</v>
+        <v>327</v>
       </c>
       <c r="H29" s="57"/>
       <c r="I29" s="57"/>
@@ -10202,14 +10214,14 @@
         <v>79</v>
       </c>
       <c r="D30" s="75" t="s">
-        <v>324</v>
+        <v>328</v>
       </c>
       <c r="E30" s="75" t="s">
         <v>61</v>
       </c>
       <c r="F30" s="58"/>
       <c r="G30" s="75" t="s">
-        <v>325</v>
+        <v>329</v>
       </c>
       <c r="H30" s="57"/>
       <c r="I30" s="57"/>
@@ -10471,16 +10483,16 @@
         <v>79</v>
       </c>
       <c r="D31" s="75" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="E31" s="75" t="s">
         <v>73</v>
       </c>
       <c r="F31" s="75" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="G31" s="75" t="s">
-        <v>326</v>
+        <v>330</v>
       </c>
       <c r="H31" s="57"/>
       <c r="I31" s="57"/>
@@ -10742,14 +10754,14 @@
         <v>82</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>327</v>
+        <v>331</v>
       </c>
       <c r="E32" s="8" t="s">
         <v>61</v>
       </c>
       <c r="F32" s="24"/>
       <c r="G32" s="8" t="s">
-        <v>328</v>
+        <v>332</v>
       </c>
       <c r="H32" s="24"/>
       <c r="I32" s="24"/>
@@ -11011,14 +11023,14 @@
         <v>82</v>
       </c>
       <c r="D33" s="34" t="s">
-        <v>329</v>
+        <v>333</v>
       </c>
       <c r="E33" s="34" t="s">
         <v>61</v>
       </c>
       <c r="F33" s="3"/>
       <c r="G33" s="34" t="s">
-        <v>330</v>
+        <v>334</v>
       </c>
       <c r="H33" s="3"/>
       <c r="I33" s="3"/>
@@ -11280,14 +11292,14 @@
         <v>82</v>
       </c>
       <c r="D34" s="34" t="s">
-        <v>331</v>
+        <v>335</v>
       </c>
       <c r="E34" s="34" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
       <c r="F34" s="3"/>
       <c r="G34" s="34" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
       <c r="H34" s="3"/>
       <c r="I34" s="3"/>
@@ -11549,14 +11561,14 @@
         <v>82</v>
       </c>
       <c r="D35" s="34" t="s">
-        <v>332</v>
+        <v>336</v>
       </c>
       <c r="E35" s="34" t="s">
-        <v>333</v>
+        <v>337</v>
       </c>
       <c r="F35" s="3"/>
       <c r="G35" s="34" t="s">
-        <v>334</v>
+        <v>338</v>
       </c>
       <c r="H35" s="3"/>
       <c r="I35" s="3"/>
@@ -11818,14 +11830,14 @@
         <v>82</v>
       </c>
       <c r="D36" s="85" t="s">
-        <v>335</v>
+        <v>339</v>
       </c>
       <c r="E36" s="85" t="s">
         <v>61</v>
       </c>
       <c r="F36" s="5"/>
       <c r="G36" s="85" t="s">
-        <v>336</v>
+        <v>340</v>
       </c>
       <c r="H36" s="5"/>
       <c r="I36" s="5"/>
@@ -12112,7 +12124,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="10" t="s">
-        <v>337</v>
+        <v>341</v>
       </c>
       <c r="B1" s="95" t="s">
         <v>11</v>
@@ -12141,13 +12153,13 @@
         <v>42</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>338</v>
+        <v>342</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>339</v>
+        <v>343</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>340</v>
+        <v>344</v>
       </c>
       <c r="G2" s="98"/>
       <c r="H2" s="99"/>
@@ -12190,7 +12202,7 @@
         <v>59</v>
       </c>
       <c r="E4" s="104" t="s">
-        <v>341</v>
+        <v>345</v>
       </c>
       <c r="F4" s="51" t="n">
         <v>1</v>
@@ -12212,7 +12224,7 @@
         <v>62</v>
       </c>
       <c r="E5" s="35" t="s">
-        <v>342</v>
+        <v>346</v>
       </c>
       <c r="F5" s="4" t="n">
         <v>2</v>
@@ -12234,7 +12246,7 @@
         <v>64</v>
       </c>
       <c r="E6" s="35" t="s">
-        <v>343</v>
+        <v>347</v>
       </c>
       <c r="F6" s="4" t="n">
         <v>3</v>
@@ -12333,7 +12345,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="10" t="s">
-        <v>344</v>
+        <v>348</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>11</v>
@@ -12368,13 +12380,13 @@
         <v>42</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>345</v>
+        <v>349</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>346</v>
+        <v>350</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>347</v>
+        <v>351</v>
       </c>
       <c r="G2" s="98"/>
       <c r="H2" s="99"/>
@@ -12429,7 +12441,7 @@
         <v>59</v>
       </c>
       <c r="E4" s="104" t="s">
-        <v>341</v>
+        <v>345</v>
       </c>
       <c r="F4" s="51" t="n">
         <v>1</v>
@@ -12457,7 +12469,7 @@
         <v>62</v>
       </c>
       <c r="E5" s="35" t="s">
-        <v>342</v>
+        <v>346</v>
       </c>
       <c r="F5" s="4" t="n">
         <v>2</v>
@@ -12485,7 +12497,7 @@
         <v>64</v>
       </c>
       <c r="E6" s="35" t="s">
-        <v>343</v>
+        <v>347</v>
       </c>
       <c r="F6" s="4" t="n">
         <v>3</v>
@@ -12614,7 +12626,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="10" t="s">
-        <v>348</v>
+        <v>352</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>11</v>
@@ -12649,13 +12661,13 @@
         <v>42</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>345</v>
+        <v>349</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>346</v>
+        <v>350</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>347</v>
+        <v>351</v>
       </c>
       <c r="G2" s="108"/>
       <c r="H2" s="109"/>
@@ -12710,7 +12722,7 @@
         <v>59</v>
       </c>
       <c r="E4" s="104" t="s">
-        <v>341</v>
+        <v>345</v>
       </c>
       <c r="F4" s="51" t="n">
         <v>1</v>
@@ -12738,7 +12750,7 @@
         <v>62</v>
       </c>
       <c r="E5" s="35" t="s">
-        <v>342</v>
+        <v>346</v>
       </c>
       <c r="F5" s="4" t="n">
         <v>2</v>
@@ -12766,7 +12778,7 @@
         <v>64</v>
       </c>
       <c r="E6" s="35" t="s">
-        <v>343</v>
+        <v>347</v>
       </c>
       <c r="F6" s="4" t="n">
         <v>3</v>
@@ -12895,7 +12907,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="19" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="110" t="s">
-        <v>349</v>
+        <v>353</v>
       </c>
       <c r="B1" s="95" t="s">
         <v>11</v>
@@ -12924,13 +12936,13 @@
         <v>42</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>338</v>
+        <v>342</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>339</v>
+        <v>343</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>340</v>
+        <v>344</v>
       </c>
       <c r="G2" s="98"/>
       <c r="H2" s="99"/>
@@ -12973,7 +12985,7 @@
         <v>59</v>
       </c>
       <c r="E4" s="104" t="s">
-        <v>341</v>
+        <v>345</v>
       </c>
       <c r="F4" s="51" t="n">
         <v>1</v>
@@ -12995,7 +13007,7 @@
         <v>62</v>
       </c>
       <c r="E5" s="35" t="s">
-        <v>342</v>
+        <v>346</v>
       </c>
       <c r="F5" s="4" t="n">
         <v>2</v>
@@ -13017,7 +13029,7 @@
         <v>64</v>
       </c>
       <c r="E6" s="35" t="s">
-        <v>343</v>
+        <v>347</v>
       </c>
       <c r="F6" s="4" t="n">
         <v>3</v>
@@ -13116,7 +13128,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="10" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>11</v>
@@ -13149,13 +13161,13 @@
       </c>
       <c r="C2" s="111"/>
       <c r="D2" s="14" t="s">
-        <v>351</v>
+        <v>355</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>352</v>
+        <v>356</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>353</v>
+        <v>357</v>
       </c>
       <c r="G2" s="13"/>
       <c r="H2" s="3"/>
@@ -13176,16 +13188,16 @@
         <v>20</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>354</v>
+        <v>358</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>355</v>
+        <v>359</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>356</v>
+        <v>360</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>357</v>
+        <v>361</v>
       </c>
       <c r="G3" s="112"/>
       <c r="H3" s="113"/>
@@ -13204,7 +13216,7 @@
       </c>
       <c r="B4" s="72"/>
       <c r="C4" s="114" t="s">
-        <v>358</v>
+        <v>362</v>
       </c>
       <c r="D4" s="114" t="s">
         <v>24</v>
@@ -13232,7 +13244,7 @@
       </c>
       <c r="B5" s="60"/>
       <c r="C5" s="115" t="s">
-        <v>359</v>
+        <v>363</v>
       </c>
       <c r="D5" s="115" t="s">
         <v>24</v>
@@ -13260,7 +13272,7 @@
       </c>
       <c r="B6" s="60"/>
       <c r="C6" s="115" t="s">
-        <v>360</v>
+        <v>364</v>
       </c>
       <c r="D6" s="115" t="s">
         <v>24</v>
@@ -13288,7 +13300,7 @@
       </c>
       <c r="B7" s="83"/>
       <c r="C7" s="116" t="s">
-        <v>361</v>
+        <v>365</v>
       </c>
       <c r="D7" s="116" t="s">
         <v>24</v>
@@ -13316,7 +13328,7 @@
       </c>
       <c r="B8" s="117"/>
       <c r="C8" s="11" t="s">
-        <v>362</v>
+        <v>366</v>
       </c>
       <c r="D8" s="11" t="s">
         <v>24</v>
@@ -13405,7 +13417,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="10" t="s">
-        <v>363</v>
+        <v>367</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>11</v>
@@ -13436,13 +13448,13 @@
         <v>15</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>364</v>
+        <v>368</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>365</v>
+        <v>369</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>366</v>
+        <v>370</v>
       </c>
       <c r="F2" s="108"/>
       <c r="G2" s="109"/>
@@ -13466,10 +13478,10 @@
         <v>51</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>367</v>
+        <v>371</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>368</v>
+        <v>372</v>
       </c>
       <c r="F3" s="13"/>
       <c r="G3" s="3"/>
@@ -13491,10 +13503,10 @@
         <v>37</v>
       </c>
       <c r="D4" s="38" t="s">
-        <v>369</v>
+        <v>373</v>
       </c>
       <c r="E4" s="118" t="s">
-        <v>368</v>
+        <v>372</v>
       </c>
       <c r="F4" s="13"/>
       <c r="G4" s="3"/>
@@ -13643,7 +13655,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="10" t="s">
-        <v>370</v>
+        <v>374</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>11</v>
@@ -13674,16 +13686,16 @@
         <v>15</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>371</v>
+        <v>375</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>372</v>
+        <v>376</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>365</v>
+        <v>369</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>366</v>
+        <v>370</v>
       </c>
       <c r="G2" s="15"/>
       <c r="H2" s="16"/>
@@ -13709,10 +13721,10 @@
         <v>105</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>367</v>
+        <v>371</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>368</v>
+        <v>372</v>
       </c>
       <c r="G3" s="17"/>
       <c r="H3" s="16"/>
@@ -13736,10 +13748,10 @@
         <v>59</v>
       </c>
       <c r="E4" s="120" t="s">
-        <v>369</v>
+        <v>373</v>
       </c>
       <c r="F4" s="118" t="s">
-        <v>368</v>
+        <v>372</v>
       </c>
       <c r="G4" s="13"/>
       <c r="H4" s="3"/>
@@ -13763,10 +13775,10 @@
         <v>62</v>
       </c>
       <c r="E5" s="122" t="s">
-        <v>369</v>
+        <v>373</v>
       </c>
       <c r="F5" s="118" t="s">
-        <v>368</v>
+        <v>372</v>
       </c>
       <c r="G5" s="13"/>
       <c r="H5" s="3"/>
@@ -13790,10 +13802,10 @@
         <v>64</v>
       </c>
       <c r="E6" s="122" t="s">
-        <v>369</v>
+        <v>373</v>
       </c>
       <c r="F6" s="118" t="s">
-        <v>368</v>
+        <v>372</v>
       </c>
       <c r="G6" s="13"/>
       <c r="H6" s="3"/>
@@ -13817,10 +13829,10 @@
         <v>66</v>
       </c>
       <c r="E7" s="122" t="s">
-        <v>369</v>
+        <v>373</v>
       </c>
       <c r="F7" s="118" t="s">
-        <v>368</v>
+        <v>372</v>
       </c>
       <c r="G7" s="13"/>
       <c r="H7" s="3"/>
@@ -13844,10 +13856,10 @@
         <v>68</v>
       </c>
       <c r="E8" s="122" t="s">
-        <v>369</v>
+        <v>373</v>
       </c>
       <c r="F8" s="118" t="s">
-        <v>368</v>
+        <v>372</v>
       </c>
       <c r="G8" s="13"/>
       <c r="H8" s="3"/>
@@ -13871,10 +13883,10 @@
         <v>71</v>
       </c>
       <c r="E9" s="122" t="s">
-        <v>369</v>
+        <v>373</v>
       </c>
       <c r="F9" s="118" t="s">
-        <v>368</v>
+        <v>372</v>
       </c>
       <c r="G9" s="13"/>
       <c r="H9" s="3"/>
@@ -13898,10 +13910,10 @@
         <v>75</v>
       </c>
       <c r="E10" s="122" t="s">
-        <v>369</v>
+        <v>373</v>
       </c>
       <c r="F10" s="118" t="s">
-        <v>368</v>
+        <v>372</v>
       </c>
       <c r="G10" s="13"/>
       <c r="H10" s="3"/>
@@ -13925,10 +13937,10 @@
         <v>80</v>
       </c>
       <c r="E11" s="122" t="s">
-        <v>369</v>
+        <v>373</v>
       </c>
       <c r="F11" s="118" t="s">
-        <v>368</v>
+        <v>372</v>
       </c>
       <c r="G11" s="13"/>
       <c r="H11" s="3"/>
@@ -13952,10 +13964,10 @@
         <v>83</v>
       </c>
       <c r="E12" s="124" t="s">
-        <v>369</v>
+        <v>373</v>
       </c>
       <c r="F12" s="118" t="s">
-        <v>368</v>
+        <v>372</v>
       </c>
       <c r="G12" s="13"/>
       <c r="H12" s="3"/>
@@ -13979,10 +13991,10 @@
         <v>84</v>
       </c>
       <c r="E13" s="122" t="s">
-        <v>369</v>
+        <v>373</v>
       </c>
       <c r="F13" s="118" t="s">
-        <v>368</v>
+        <v>372</v>
       </c>
       <c r="G13" s="13"/>
       <c r="H13" s="3"/>
@@ -14006,10 +14018,10 @@
         <v>86</v>
       </c>
       <c r="E14" s="122" t="s">
-        <v>369</v>
+        <v>373</v>
       </c>
       <c r="F14" s="118" t="s">
-        <v>368</v>
+        <v>372</v>
       </c>
       <c r="G14" s="13"/>
       <c r="H14" s="3"/>
@@ -14033,10 +14045,10 @@
         <v>88</v>
       </c>
       <c r="E15" s="122" t="s">
-        <v>369</v>
+        <v>373</v>
       </c>
       <c r="F15" s="118" t="s">
-        <v>368</v>
+        <v>372</v>
       </c>
       <c r="G15" s="13"/>
       <c r="H15" s="3"/>
@@ -14060,10 +14072,10 @@
         <v>90</v>
       </c>
       <c r="E16" s="122" t="s">
-        <v>369</v>
+        <v>373</v>
       </c>
       <c r="F16" s="118" t="s">
-        <v>368</v>
+        <v>372</v>
       </c>
       <c r="G16" s="13"/>
       <c r="H16" s="3"/>
@@ -14106,7 +14118,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="10" t="s">
-        <v>373</v>
+        <v>377</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>11</v>
@@ -14137,16 +14149,16 @@
         <v>15</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>364</v>
+        <v>368</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>374</v>
+        <v>378</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>365</v>
+        <v>369</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>366</v>
+        <v>370</v>
       </c>
       <c r="G2" s="21"/>
       <c r="H2" s="22"/>
@@ -14172,10 +14184,10 @@
         <v>199</v>
       </c>
       <c r="E3" s="69" t="s">
-        <v>367</v>
+        <v>371</v>
       </c>
       <c r="F3" s="69" t="s">
-        <v>368</v>
+        <v>372</v>
       </c>
       <c r="G3" s="70"/>
       <c r="H3" s="22"/>
@@ -14199,10 +14211,10 @@
         <v>152</v>
       </c>
       <c r="E4" s="126" t="s">
-        <v>369</v>
+        <v>373</v>
       </c>
       <c r="F4" s="118" t="s">
-        <v>368</v>
+        <v>372</v>
       </c>
       <c r="G4" s="13"/>
       <c r="H4" s="3"/>
@@ -14226,10 +14238,10 @@
         <v>156</v>
       </c>
       <c r="E5" s="128" t="s">
-        <v>369</v>
+        <v>373</v>
       </c>
       <c r="F5" s="118" t="s">
-        <v>368</v>
+        <v>372</v>
       </c>
       <c r="G5" s="13"/>
       <c r="H5" s="3"/>
@@ -14253,10 +14265,10 @@
         <v>160</v>
       </c>
       <c r="E6" s="128" t="s">
-        <v>369</v>
+        <v>373</v>
       </c>
       <c r="F6" s="118" t="s">
-        <v>368</v>
+        <v>372</v>
       </c>
       <c r="G6" s="13"/>
       <c r="H6" s="3"/>
@@ -14280,10 +14292,10 @@
         <v>164</v>
       </c>
       <c r="E7" s="128" t="s">
-        <v>369</v>
+        <v>373</v>
       </c>
       <c r="F7" s="118" t="s">
-        <v>368</v>
+        <v>372</v>
       </c>
       <c r="G7" s="13"/>
       <c r="H7" s="3"/>
@@ -14307,10 +14319,10 @@
         <v>171</v>
       </c>
       <c r="E8" s="128" t="s">
-        <v>369</v>
+        <v>373</v>
       </c>
       <c r="F8" s="118" t="s">
-        <v>368</v>
+        <v>372</v>
       </c>
       <c r="G8" s="13"/>
       <c r="H8" s="3"/>
@@ -14334,10 +14346,10 @@
         <v>167</v>
       </c>
       <c r="E9" s="128" t="s">
-        <v>369</v>
+        <v>373</v>
       </c>
       <c r="F9" s="118" t="s">
-        <v>368</v>
+        <v>372</v>
       </c>
       <c r="G9" s="13"/>
       <c r="H9" s="3"/>
@@ -14361,10 +14373,10 @@
         <v>175</v>
       </c>
       <c r="E10" s="128" t="s">
-        <v>369</v>
+        <v>373</v>
       </c>
       <c r="F10" s="118" t="s">
-        <v>368</v>
+        <v>372</v>
       </c>
       <c r="G10" s="13"/>
       <c r="H10" s="3"/>
@@ -14388,10 +14400,10 @@
         <v>182</v>
       </c>
       <c r="E11" s="128" t="s">
-        <v>369</v>
+        <v>373</v>
       </c>
       <c r="F11" s="118" t="s">
-        <v>368</v>
+        <v>372</v>
       </c>
       <c r="G11" s="13"/>
       <c r="H11" s="3"/>
@@ -14415,10 +14427,10 @@
         <v>185</v>
       </c>
       <c r="E12" s="128" t="s">
-        <v>369</v>
+        <v>373</v>
       </c>
       <c r="F12" s="118" t="s">
-        <v>368</v>
+        <v>372</v>
       </c>
       <c r="G12" s="13"/>
       <c r="H12" s="3"/>
@@ -14495,7 +14507,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="10" t="s">
-        <v>375</v>
+        <v>379</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>11</v>
@@ -14527,16 +14539,16 @@
         <v>15</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>371</v>
+        <v>375</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>376</v>
+        <v>380</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>365</v>
+        <v>369</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>366</v>
+        <v>370</v>
       </c>
       <c r="G2" s="21"/>
       <c r="H2" s="22"/>
@@ -14560,13 +14572,13 @@
         <v>51</v>
       </c>
       <c r="D3" s="69" t="s">
-        <v>377</v>
+        <v>381</v>
       </c>
       <c r="E3" s="69" t="s">
-        <v>367</v>
+        <v>371</v>
       </c>
       <c r="F3" s="69" t="s">
-        <v>368</v>
+        <v>372</v>
       </c>
       <c r="G3" s="70"/>
       <c r="H3" s="71"/>
@@ -14591,10 +14603,10 @@
         <v>124</v>
       </c>
       <c r="E4" s="38" t="s">
-        <v>369</v>
+        <v>373</v>
       </c>
       <c r="F4" s="118" t="s">
-        <v>368</v>
+        <v>372</v>
       </c>
       <c r="G4" s="13"/>
       <c r="H4" s="3"/>
@@ -14987,7 +14999,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="10" t="s">
-        <v>378</v>
+        <v>382</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>11</v>
@@ -15006,19 +15018,19 @@
       <c r="A2" s="111"/>
       <c r="B2" s="111"/>
       <c r="C2" s="14" t="s">
-        <v>371</v>
+        <v>375</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>379</v>
+        <v>383</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>380</v>
+        <v>384</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>365</v>
+        <v>369</v>
       </c>
       <c r="G2" s="14" t="s">
-        <v>366</v>
+        <v>370</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15038,10 +15050,10 @@
         <v>222</v>
       </c>
       <c r="F3" s="69" t="s">
-        <v>367</v>
+        <v>371</v>
       </c>
       <c r="G3" s="69" t="s">
-        <v>368</v>
+        <v>372</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15056,13 +15068,13 @@
         <v>75</v>
       </c>
       <c r="E4" s="114" t="s">
-        <v>298</v>
+        <v>302</v>
       </c>
       <c r="F4" s="38" t="s">
-        <v>369</v>
+        <v>373</v>
       </c>
       <c r="G4" s="118" t="s">
-        <v>368</v>
+        <v>372</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15077,13 +15089,13 @@
         <v>75</v>
       </c>
       <c r="E5" s="115" t="s">
-        <v>300</v>
+        <v>304</v>
       </c>
       <c r="F5" s="38" t="s">
-        <v>369</v>
+        <v>373</v>
       </c>
       <c r="G5" s="118" t="s">
-        <v>368</v>
+        <v>372</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15098,13 +15110,13 @@
         <v>75</v>
       </c>
       <c r="E6" s="115" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
       <c r="F6" s="38" t="s">
-        <v>369</v>
+        <v>373</v>
       </c>
       <c r="G6" s="118" t="s">
-        <v>368</v>
+        <v>372</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15119,13 +15131,13 @@
         <v>75</v>
       </c>
       <c r="E7" s="115" t="s">
-        <v>302</v>
+        <v>306</v>
       </c>
       <c r="F7" s="38" t="s">
-        <v>369</v>
+        <v>373</v>
       </c>
       <c r="G7" s="118" t="s">
-        <v>368</v>
+        <v>372</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15140,13 +15152,13 @@
         <v>75</v>
       </c>
       <c r="E8" s="115" t="s">
-        <v>305</v>
+        <v>309</v>
       </c>
       <c r="F8" s="38" t="s">
-        <v>369</v>
+        <v>373</v>
       </c>
       <c r="G8" s="118" t="s">
-        <v>368</v>
+        <v>372</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15161,13 +15173,13 @@
         <v>75</v>
       </c>
       <c r="E9" s="115" t="s">
-        <v>292</v>
+        <v>296</v>
       </c>
       <c r="F9" s="38" t="s">
-        <v>369</v>
+        <v>373</v>
       </c>
       <c r="G9" s="118" t="s">
-        <v>368</v>
+        <v>372</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15182,13 +15194,13 @@
         <v>75</v>
       </c>
       <c r="E10" s="115" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
       <c r="F10" s="38" t="s">
-        <v>369</v>
+        <v>373</v>
       </c>
       <c r="G10" s="118" t="s">
-        <v>368</v>
+        <v>372</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15203,13 +15215,13 @@
         <v>75</v>
       </c>
       <c r="E11" s="115" t="s">
-        <v>309</v>
+        <v>313</v>
       </c>
       <c r="F11" s="38" t="s">
-        <v>369</v>
+        <v>373</v>
       </c>
       <c r="G11" s="118" t="s">
-        <v>368</v>
+        <v>372</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15224,13 +15236,13 @@
         <v>75</v>
       </c>
       <c r="E12" s="115" t="s">
-        <v>311</v>
+        <v>315</v>
       </c>
       <c r="F12" s="38" t="s">
-        <v>369</v>
+        <v>373</v>
       </c>
       <c r="G12" s="118" t="s">
-        <v>368</v>
+        <v>372</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15245,13 +15257,13 @@
         <v>75</v>
       </c>
       <c r="E13" s="115" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="F13" s="38" t="s">
-        <v>369</v>
+        <v>373</v>
       </c>
       <c r="G13" s="118" t="s">
-        <v>368</v>
+        <v>372</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15266,13 +15278,13 @@
         <v>75</v>
       </c>
       <c r="E14" s="115" t="s">
-        <v>317</v>
+        <v>321</v>
       </c>
       <c r="F14" s="38" t="s">
-        <v>369</v>
+        <v>373</v>
       </c>
       <c r="G14" s="118" t="s">
-        <v>368</v>
+        <v>372</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15287,13 +15299,13 @@
         <v>75</v>
       </c>
       <c r="E15" s="115" t="s">
-        <v>315</v>
+        <v>319</v>
       </c>
       <c r="F15" s="38" t="s">
-        <v>369</v>
+        <v>373</v>
       </c>
       <c r="G15" s="118" t="s">
-        <v>368</v>
+        <v>372</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15308,13 +15320,13 @@
         <v>75</v>
       </c>
       <c r="E16" s="115" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="F16" s="38" t="s">
-        <v>369</v>
+        <v>373</v>
       </c>
       <c r="G16" s="118" t="s">
-        <v>368</v>
+        <v>372</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15329,13 +15341,13 @@
         <v>75</v>
       </c>
       <c r="E17" s="115" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="F17" s="38" t="s">
-        <v>369</v>
+        <v>373</v>
       </c>
       <c r="G17" s="118" t="s">
-        <v>368</v>
+        <v>372</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15350,13 +15362,13 @@
         <v>75</v>
       </c>
       <c r="E18" s="115" t="s">
-        <v>319</v>
+        <v>323</v>
       </c>
       <c r="F18" s="38" t="s">
-        <v>369</v>
+        <v>373</v>
       </c>
       <c r="G18" s="118" t="s">
-        <v>368</v>
+        <v>372</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15371,13 +15383,13 @@
         <v>75</v>
       </c>
       <c r="E19" s="115" t="s">
-        <v>324</v>
+        <v>328</v>
       </c>
       <c r="F19" s="38" t="s">
-        <v>369</v>
+        <v>373</v>
       </c>
       <c r="G19" s="118" t="s">
-        <v>368</v>
+        <v>372</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15392,13 +15404,13 @@
         <v>75</v>
       </c>
       <c r="E20" s="116" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="F20" s="38" t="s">
-        <v>369</v>
+        <v>373</v>
       </c>
       <c r="G20" s="118" t="s">
-        <v>368</v>
+        <v>372</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15413,13 +15425,13 @@
         <v>80</v>
       </c>
       <c r="E21" s="114" t="s">
-        <v>327</v>
+        <v>331</v>
       </c>
       <c r="F21" s="38" t="s">
-        <v>369</v>
+        <v>373</v>
       </c>
       <c r="G21" s="118" t="s">
-        <v>368</v>
+        <v>372</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15434,13 +15446,13 @@
         <v>80</v>
       </c>
       <c r="E22" s="115" t="s">
-        <v>329</v>
+        <v>333</v>
       </c>
       <c r="F22" s="38" t="s">
-        <v>369</v>
+        <v>373</v>
       </c>
       <c r="G22" s="118" t="s">
-        <v>368</v>
+        <v>372</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15455,13 +15467,13 @@
         <v>80</v>
       </c>
       <c r="E23" s="115" t="s">
-        <v>331</v>
+        <v>335</v>
       </c>
       <c r="F23" s="38" t="s">
-        <v>369</v>
+        <v>373</v>
       </c>
       <c r="G23" s="118" t="s">
-        <v>368</v>
+        <v>372</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15476,13 +15488,13 @@
         <v>80</v>
       </c>
       <c r="E24" s="115" t="s">
-        <v>332</v>
+        <v>336</v>
       </c>
       <c r="F24" s="38" t="s">
-        <v>369</v>
+        <v>373</v>
       </c>
       <c r="G24" s="118" t="s">
-        <v>368</v>
+        <v>372</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15497,13 +15509,13 @@
         <v>80</v>
       </c>
       <c r="E25" s="116" t="s">
-        <v>335</v>
+        <v>339</v>
       </c>
       <c r="F25" s="38" t="s">
-        <v>369</v>
+        <v>373</v>
       </c>
       <c r="G25" s="118" t="s">
-        <v>368</v>
+        <v>372</v>
       </c>
     </row>
   </sheetData>
@@ -15821,7 +15833,7 @@
   </sheetPr>
   <dimension ref="A1:IU16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -22626,10 +22638,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N26"/>
+  <dimension ref="A1:N28"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E20" activeCellId="0" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -23059,15 +23071,15 @@
       <c r="A18" s="29" t="n">
         <v>42736</v>
       </c>
-      <c r="B18" s="3"/>
-      <c r="C18" s="75" t="s">
+      <c r="B18" s="60"/>
+      <c r="C18" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="D18" s="74" t="s">
         <v>253</v>
       </c>
-      <c r="D18" s="34" t="s">
+      <c r="E18" s="34" t="s">
         <v>254</v>
-      </c>
-      <c r="E18" s="34" t="s">
-        <v>255</v>
       </c>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
@@ -23083,15 +23095,15 @@
       <c r="A19" s="29" t="n">
         <v>42736</v>
       </c>
-      <c r="B19" s="3"/>
-      <c r="C19" s="75" t="s">
-        <v>253</v>
-      </c>
-      <c r="D19" s="34" t="s">
+      <c r="B19" s="60"/>
+      <c r="C19" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="D19" s="74" t="s">
+        <v>255</v>
+      </c>
+      <c r="E19" s="34" t="s">
         <v>256</v>
-      </c>
-      <c r="E19" s="34" t="s">
-        <v>257</v>
       </c>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
@@ -23109,13 +23121,13 @@
       </c>
       <c r="B20" s="3"/>
       <c r="C20" s="75" t="s">
+        <v>257</v>
+      </c>
+      <c r="D20" s="34" t="s">
         <v>258</v>
       </c>
-      <c r="D20" s="34" t="s">
+      <c r="E20" s="34" t="s">
         <v>259</v>
-      </c>
-      <c r="E20" s="34" t="s">
-        <v>260</v>
       </c>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
@@ -23133,13 +23145,13 @@
       </c>
       <c r="B21" s="3"/>
       <c r="C21" s="75" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D21" s="34" t="s">
+        <v>260</v>
+      </c>
+      <c r="E21" s="34" t="s">
         <v>261</v>
-      </c>
-      <c r="E21" s="34" t="s">
-        <v>262</v>
       </c>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
@@ -23157,7 +23169,7 @@
       </c>
       <c r="B22" s="3"/>
       <c r="C22" s="75" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="D22" s="34" t="s">
         <v>263</v>
@@ -23181,7 +23193,7 @@
       </c>
       <c r="B23" s="3"/>
       <c r="C23" s="75" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="D23" s="34" t="s">
         <v>265</v>
@@ -23205,7 +23217,7 @@
       </c>
       <c r="B24" s="3"/>
       <c r="C24" s="75" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="D24" s="34" t="s">
         <v>267</v>
@@ -23229,7 +23241,7 @@
       </c>
       <c r="B25" s="3"/>
       <c r="C25" s="75" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="D25" s="34" t="s">
         <v>269</v>
@@ -23253,7 +23265,7 @@
       </c>
       <c r="B26" s="3"/>
       <c r="C26" s="75" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="D26" s="34" t="s">
         <v>271</v>
@@ -23270,6 +23282,54 @@
       <c r="L26" s="3"/>
       <c r="M26" s="3"/>
       <c r="N26" s="3"/>
+    </row>
+    <row r="27" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A27" s="29" t="n">
+        <v>42736</v>
+      </c>
+      <c r="B27" s="3"/>
+      <c r="C27" s="75" t="s">
+        <v>262</v>
+      </c>
+      <c r="D27" s="34" t="s">
+        <v>273</v>
+      </c>
+      <c r="E27" s="34" t="s">
+        <v>274</v>
+      </c>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3"/>
+      <c r="J27" s="3"/>
+      <c r="K27" s="3"/>
+      <c r="L27" s="3"/>
+      <c r="M27" s="3"/>
+      <c r="N27" s="3"/>
+    </row>
+    <row r="28" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A28" s="29" t="n">
+        <v>42736</v>
+      </c>
+      <c r="B28" s="3"/>
+      <c r="C28" s="75" t="s">
+        <v>262</v>
+      </c>
+      <c r="D28" s="34" t="s">
+        <v>275</v>
+      </c>
+      <c r="E28" s="34" t="s">
+        <v>276</v>
+      </c>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
+      <c r="J28" s="3"/>
+      <c r="K28" s="3"/>
+      <c r="L28" s="3"/>
+      <c r="M28" s="3"/>
+      <c r="N28" s="3"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
EM-1800 * Updated BundimgDTO & Mapper to contain the DocumentImage         * Removed the enabled field for DocumentImage         * enhanced testcases and yaml files
</commit_message>
<xml_diff>
--- a/src/aat/resources/adv_bundling_functional_tests_ccd_def.xlsx
+++ b/src/aat/resources/adv_bundling_functional_tests_ccd_def.xlsx
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1432" uniqueCount="424">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1427" uniqueCount="423">
   <si>
     <t xml:space="preserve">Change History</t>
   </si>
@@ -1061,15 +1061,6 @@
     <t xml:space="preserve">DocumentImage</t>
   </si>
   <si>
-    <t xml:space="preserve">enabled</t>
-  </si>
-  <si>
-    <t xml:space="preserve">YesOrNo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Configure image for stitched Pdf?</t>
-  </si>
-  <si>
     <t xml:space="preserve">imageRendering</t>
   </si>
   <si>
@@ -1113,6 +1104,9 @@
   </si>
   <si>
     <t xml:space="preserve">eligibleForStitching</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YesOrNo</t>
   </si>
   <si>
     <t xml:space="preserve">Is this the bundle you want to stitch?</t>
@@ -1191,6 +1185,9 @@
   </si>
   <si>
     <t xml:space="preserve">documentImage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Configure image for stitched Pdf?</t>
   </si>
   <si>
     <t xml:space="preserve">documentName</t>
@@ -2594,7 +2591,7 @@
   <dimension ref="A1:IU1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D29" activeCellId="0" sqref="D29"/>
+      <selection pane="topLeft" activeCell="A19" activeCellId="0" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7499,11 +7496,13 @@
         <v>320</v>
       </c>
       <c r="E19" s="41" t="s">
+        <v>73</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="G19" s="41" t="s">
         <v>321</v>
-      </c>
-      <c r="F19" s="5"/>
-      <c r="G19" s="41" t="s">
-        <v>322</v>
       </c>
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
@@ -7765,16 +7764,16 @@
         <v>319</v>
       </c>
       <c r="D20" s="41" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E20" s="41" t="s">
         <v>73</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>283</v>
+        <v>322</v>
       </c>
       <c r="G20" s="41" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
@@ -8036,16 +8035,14 @@
         <v>319</v>
       </c>
       <c r="D21" s="41" t="s">
+        <v>324</v>
+      </c>
+      <c r="E21" s="41" t="s">
+        <v>61</v>
+      </c>
+      <c r="F21" s="5"/>
+      <c r="G21" s="41" t="s">
         <v>325</v>
-      </c>
-      <c r="E21" s="41" t="s">
-        <v>73</v>
-      </c>
-      <c r="F21" s="5" t="s">
-        <v>325</v>
-      </c>
-      <c r="G21" s="41" t="s">
-        <v>326</v>
       </c>
       <c r="H21" s="5"/>
       <c r="I21" s="5"/>
@@ -8307,14 +8304,14 @@
         <v>319</v>
       </c>
       <c r="D22" s="41" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="E22" s="41" t="s">
-        <v>61</v>
+        <v>304</v>
       </c>
       <c r="F22" s="5"/>
       <c r="G22" s="41" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="H22" s="5"/>
       <c r="I22" s="5"/>
@@ -8576,14 +8573,14 @@
         <v>319</v>
       </c>
       <c r="D23" s="41" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E23" s="41" t="s">
         <v>304</v>
       </c>
       <c r="F23" s="5"/>
       <c r="G23" s="41" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="H23" s="5"/>
       <c r="I23" s="5"/>
@@ -8837,27 +8834,27 @@
       <c r="IU23" s="81"/>
     </row>
     <row r="24" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="105" t="n">
+      <c r="A24" s="103" t="n">
         <v>42736</v>
       </c>
-      <c r="B24" s="5"/>
-      <c r="C24" s="48" t="s">
-        <v>319</v>
-      </c>
-      <c r="D24" s="41" t="s">
+      <c r="B24" s="24"/>
+      <c r="C24" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>330</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="F24" s="24"/>
+      <c r="G24" s="8" t="s">
         <v>331</v>
       </c>
-      <c r="E24" s="41" t="s">
-        <v>304</v>
-      </c>
-      <c r="F24" s="5"/>
-      <c r="G24" s="41" t="s">
-        <v>332</v>
-      </c>
-      <c r="H24" s="5"/>
-      <c r="I24" s="5"/>
-      <c r="J24" s="5"/>
-      <c r="K24" s="102" t="s">
+      <c r="H24" s="24"/>
+      <c r="I24" s="24"/>
+      <c r="J24" s="24"/>
+      <c r="K24" s="61" t="s">
         <v>40</v>
       </c>
       <c r="L24" s="13"/>
@@ -9106,27 +9103,27 @@
       <c r="IU24" s="81"/>
     </row>
     <row r="25" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="103" t="n">
+      <c r="A25" s="104" t="n">
         <v>42736</v>
       </c>
-      <c r="B25" s="24"/>
-      <c r="C25" s="8" t="s">
+      <c r="B25" s="3"/>
+      <c r="C25" s="34" t="s">
         <v>79</v>
       </c>
-      <c r="D25" s="8" t="s">
+      <c r="D25" s="34" t="s">
+        <v>332</v>
+      </c>
+      <c r="E25" s="34" t="s">
+        <v>61</v>
+      </c>
+      <c r="F25" s="3"/>
+      <c r="G25" s="34" t="s">
         <v>333</v>
       </c>
-      <c r="E25" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="F25" s="24"/>
-      <c r="G25" s="8" t="s">
-        <v>334</v>
-      </c>
-      <c r="H25" s="24"/>
-      <c r="I25" s="24"/>
-      <c r="J25" s="24"/>
-      <c r="K25" s="61" t="s">
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="3"/>
+      <c r="K25" s="69" t="s">
         <v>40</v>
       </c>
       <c r="L25" s="13"/>
@@ -9383,14 +9380,14 @@
         <v>79</v>
       </c>
       <c r="D26" s="34" t="s">
-        <v>335</v>
+        <v>306</v>
       </c>
       <c r="E26" s="34" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="F26" s="3"/>
       <c r="G26" s="34" t="s">
-        <v>336</v>
+        <v>23</v>
       </c>
       <c r="H26" s="3"/>
       <c r="I26" s="3"/>
@@ -9652,14 +9649,14 @@
         <v>79</v>
       </c>
       <c r="D27" s="34" t="s">
-        <v>306</v>
+        <v>334</v>
       </c>
       <c r="E27" s="34" t="s">
-        <v>70</v>
+        <v>335</v>
       </c>
       <c r="F27" s="3"/>
       <c r="G27" s="34" t="s">
-        <v>23</v>
+        <v>336</v>
       </c>
       <c r="H27" s="3"/>
       <c r="I27" s="3"/>
@@ -9924,7 +9921,7 @@
         <v>337</v>
       </c>
       <c r="E28" s="34" t="s">
-        <v>321</v>
+        <v>335</v>
       </c>
       <c r="F28" s="3"/>
       <c r="G28" s="34" t="s">
@@ -10190,14 +10187,16 @@
         <v>79</v>
       </c>
       <c r="D29" s="34" t="s">
+        <v>312</v>
+      </c>
+      <c r="E29" s="34" t="s">
+        <v>78</v>
+      </c>
+      <c r="F29" s="34" t="s">
+        <v>300</v>
+      </c>
+      <c r="G29" s="34" t="s">
         <v>339</v>
-      </c>
-      <c r="E29" s="34" t="s">
-        <v>321</v>
-      </c>
-      <c r="F29" s="3"/>
-      <c r="G29" s="34" t="s">
-        <v>340</v>
       </c>
       <c r="H29" s="3"/>
       <c r="I29" s="3"/>
@@ -10459,16 +10458,16 @@
         <v>79</v>
       </c>
       <c r="D30" s="34" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="E30" s="34" t="s">
         <v>78</v>
       </c>
       <c r="F30" s="34" t="s">
-        <v>300</v>
+        <v>317</v>
       </c>
       <c r="G30" s="34" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="H30" s="3"/>
       <c r="I30" s="3"/>
@@ -10730,14 +10729,12 @@
         <v>79</v>
       </c>
       <c r="D31" s="34" t="s">
-        <v>315</v>
+        <v>341</v>
       </c>
       <c r="E31" s="34" t="s">
-        <v>78</v>
-      </c>
-      <c r="F31" s="34" t="s">
-        <v>317</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="F31" s="3"/>
       <c r="G31" s="34" t="s">
         <v>342</v>
       </c>
@@ -11004,7 +11001,7 @@
         <v>343</v>
       </c>
       <c r="E32" s="34" t="s">
-        <v>61</v>
+        <v>308</v>
       </c>
       <c r="F32" s="3"/>
       <c r="G32" s="34" t="s">
@@ -11273,7 +11270,7 @@
         <v>345</v>
       </c>
       <c r="E33" s="34" t="s">
-        <v>308</v>
+        <v>335</v>
       </c>
       <c r="F33" s="3"/>
       <c r="G33" s="34" t="s">
@@ -11542,7 +11539,7 @@
         <v>347</v>
       </c>
       <c r="E34" s="34" t="s">
-        <v>321</v>
+        <v>335</v>
       </c>
       <c r="F34" s="3"/>
       <c r="G34" s="34" t="s">
@@ -11811,7 +11808,7 @@
         <v>349</v>
       </c>
       <c r="E35" s="34" t="s">
-        <v>321</v>
+        <v>335</v>
       </c>
       <c r="F35" s="3"/>
       <c r="G35" s="34" t="s">
@@ -12080,7 +12077,7 @@
         <v>351</v>
       </c>
       <c r="E36" s="34" t="s">
-        <v>321</v>
+        <v>61</v>
       </c>
       <c r="F36" s="3"/>
       <c r="G36" s="34" t="s">
@@ -12338,27 +12335,27 @@
       <c r="IU36" s="81"/>
     </row>
     <row r="37" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="104" t="n">
+      <c r="A37" s="105" t="n">
         <v>42736</v>
       </c>
-      <c r="B37" s="3"/>
-      <c r="C37" s="34" t="s">
+      <c r="B37" s="5"/>
+      <c r="C37" s="41" t="s">
         <v>79</v>
       </c>
-      <c r="D37" s="34" t="s">
+      <c r="D37" s="41" t="s">
         <v>353</v>
       </c>
-      <c r="E37" s="34" t="s">
+      <c r="E37" s="41" t="s">
         <v>61</v>
       </c>
-      <c r="F37" s="3"/>
-      <c r="G37" s="34" t="s">
+      <c r="F37" s="5"/>
+      <c r="G37" s="41" t="s">
         <v>354</v>
       </c>
-      <c r="H37" s="3"/>
-      <c r="I37" s="3"/>
-      <c r="J37" s="3"/>
-      <c r="K37" s="69" t="s">
+      <c r="H37" s="5"/>
+      <c r="I37" s="5"/>
+      <c r="J37" s="5"/>
+      <c r="K37" s="102" t="s">
         <v>40</v>
       </c>
       <c r="L37" s="13"/>
@@ -12607,27 +12604,29 @@
       <c r="IU37" s="81"/>
     </row>
     <row r="38" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="105" t="n">
+      <c r="A38" s="106" t="n">
         <v>42736</v>
       </c>
-      <c r="B38" s="5"/>
-      <c r="C38" s="41" t="s">
+      <c r="B38" s="47"/>
+      <c r="C38" s="48" t="s">
         <v>79</v>
       </c>
-      <c r="D38" s="41" t="s">
+      <c r="D38" s="48" t="s">
+        <v>268</v>
+      </c>
+      <c r="E38" s="48" t="s">
+        <v>73</v>
+      </c>
+      <c r="F38" s="48" t="s">
+        <v>268</v>
+      </c>
+      <c r="G38" s="48" t="s">
         <v>355</v>
       </c>
-      <c r="E38" s="41" t="s">
-        <v>61</v>
-      </c>
-      <c r="F38" s="5"/>
-      <c r="G38" s="41" t="s">
-        <v>356</v>
-      </c>
-      <c r="H38" s="5"/>
-      <c r="I38" s="5"/>
-      <c r="J38" s="5"/>
-      <c r="K38" s="102" t="s">
+      <c r="H38" s="47"/>
+      <c r="I38" s="47"/>
+      <c r="J38" s="47"/>
+      <c r="K38" s="107" t="s">
         <v>40</v>
       </c>
       <c r="L38" s="13"/>
@@ -12884,14 +12883,12 @@
         <v>79</v>
       </c>
       <c r="D39" s="48" t="s">
-        <v>268</v>
+        <v>356</v>
       </c>
       <c r="E39" s="48" t="s">
-        <v>73</v>
-      </c>
-      <c r="F39" s="48" t="s">
-        <v>268</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="F39" s="48"/>
       <c r="G39" s="48" t="s">
         <v>357</v>
       </c>
@@ -13155,14 +13152,16 @@
         <v>79</v>
       </c>
       <c r="D40" s="48" t="s">
+        <v>263</v>
+      </c>
+      <c r="E40" s="48" t="s">
+        <v>73</v>
+      </c>
+      <c r="F40" s="48" t="s">
+        <v>263</v>
+      </c>
+      <c r="G40" s="48" t="s">
         <v>358</v>
-      </c>
-      <c r="E40" s="48" t="s">
-        <v>61</v>
-      </c>
-      <c r="F40" s="48"/>
-      <c r="G40" s="48" t="s">
-        <v>359</v>
       </c>
       <c r="H40" s="47"/>
       <c r="I40" s="47"/>
@@ -13424,14 +13423,12 @@
         <v>79</v>
       </c>
       <c r="D41" s="48" t="s">
-        <v>263</v>
+        <v>359</v>
       </c>
       <c r="E41" s="48" t="s">
-        <v>73</v>
-      </c>
-      <c r="F41" s="48" t="s">
-        <v>263</v>
-      </c>
+        <v>335</v>
+      </c>
+      <c r="F41" s="48"/>
       <c r="G41" s="48" t="s">
         <v>360</v>
       </c>
@@ -13698,9 +13695,11 @@
         <v>361</v>
       </c>
       <c r="E42" s="48" t="s">
-        <v>321</v>
-      </c>
-      <c r="F42" s="48"/>
+        <v>78</v>
+      </c>
+      <c r="F42" s="48" t="s">
+        <v>319</v>
+      </c>
       <c r="G42" s="48" t="s">
         <v>362</v>
       </c>
@@ -13956,29 +13955,27 @@
       <c r="IU42" s="81"/>
     </row>
     <row r="43" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A43" s="106" t="n">
+      <c r="A43" s="103" t="n">
         <v>42736</v>
       </c>
-      <c r="B43" s="47"/>
-      <c r="C43" s="48" t="s">
-        <v>79</v>
-      </c>
-      <c r="D43" s="48" t="s">
+      <c r="B43" s="24"/>
+      <c r="C43" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="D43" s="8" t="s">
         <v>363</v>
       </c>
-      <c r="E43" s="48" t="s">
-        <v>78</v>
-      </c>
-      <c r="F43" s="48" t="s">
-        <v>319</v>
-      </c>
-      <c r="G43" s="48" t="s">
-        <v>322</v>
-      </c>
-      <c r="H43" s="47"/>
-      <c r="I43" s="47"/>
-      <c r="J43" s="47"/>
-      <c r="K43" s="107" t="s">
+      <c r="E43" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="F43" s="24"/>
+      <c r="G43" s="8" t="s">
+        <v>364</v>
+      </c>
+      <c r="H43" s="24"/>
+      <c r="I43" s="24"/>
+      <c r="J43" s="24"/>
+      <c r="K43" s="61" t="s">
         <v>40</v>
       </c>
       <c r="L43" s="13"/>
@@ -14227,27 +14224,27 @@
       <c r="IU43" s="81"/>
     </row>
     <row r="44" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A44" s="103" t="n">
+      <c r="A44" s="104" t="n">
         <v>42736</v>
       </c>
-      <c r="B44" s="24"/>
-      <c r="C44" s="8" t="s">
+      <c r="B44" s="3"/>
+      <c r="C44" s="34" t="s">
         <v>82</v>
       </c>
-      <c r="D44" s="8" t="s">
-        <v>364</v>
-      </c>
-      <c r="E44" s="8" t="s">
+      <c r="D44" s="34" t="s">
+        <v>365</v>
+      </c>
+      <c r="E44" s="34" t="s">
         <v>61</v>
       </c>
-      <c r="F44" s="24"/>
-      <c r="G44" s="8" t="s">
-        <v>365</v>
-      </c>
-      <c r="H44" s="24"/>
-      <c r="I44" s="24"/>
-      <c r="J44" s="24"/>
-      <c r="K44" s="61" t="s">
+      <c r="F44" s="3"/>
+      <c r="G44" s="34" t="s">
+        <v>366</v>
+      </c>
+      <c r="H44" s="3"/>
+      <c r="I44" s="3"/>
+      <c r="J44" s="3"/>
+      <c r="K44" s="69" t="s">
         <v>40</v>
       </c>
       <c r="L44" s="13"/>
@@ -14504,14 +14501,14 @@
         <v>82</v>
       </c>
       <c r="D45" s="34" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="E45" s="34" t="s">
-        <v>61</v>
+        <v>308</v>
       </c>
       <c r="F45" s="3"/>
       <c r="G45" s="34" t="s">
-        <v>367</v>
+        <v>308</v>
       </c>
       <c r="H45" s="3"/>
       <c r="I45" s="3"/>
@@ -14776,11 +14773,11 @@
         <v>368</v>
       </c>
       <c r="E46" s="34" t="s">
-        <v>308</v>
+        <v>369</v>
       </c>
       <c r="F46" s="3"/>
       <c r="G46" s="34" t="s">
-        <v>308</v>
+        <v>370</v>
       </c>
       <c r="H46" s="3"/>
       <c r="I46" s="3"/>
@@ -15042,14 +15039,14 @@
         <v>82</v>
       </c>
       <c r="D47" s="34" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="E47" s="34" t="s">
-        <v>370</v>
+        <v>61</v>
       </c>
       <c r="F47" s="3"/>
       <c r="G47" s="34" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="H47" s="3"/>
       <c r="I47" s="3"/>
@@ -15059,251 +15056,251 @@
       </c>
       <c r="L47" s="13"/>
       <c r="M47" s="3"/>
-      <c r="N47" s="84"/>
-      <c r="O47" s="32"/>
-      <c r="P47" s="32"/>
-      <c r="Q47" s="32"/>
-      <c r="R47" s="32"/>
-      <c r="S47" s="32"/>
-      <c r="T47" s="32"/>
-      <c r="U47" s="32"/>
-      <c r="V47" s="32"/>
-      <c r="W47" s="32"/>
-      <c r="X47" s="32"/>
-      <c r="Y47" s="32"/>
-      <c r="Z47" s="32"/>
-      <c r="AA47" s="32"/>
-      <c r="AB47" s="32"/>
-      <c r="AC47" s="32"/>
-      <c r="AD47" s="32"/>
-      <c r="AE47" s="32"/>
-      <c r="AF47" s="32"/>
-      <c r="AG47" s="32"/>
-      <c r="AH47" s="32"/>
-      <c r="AI47" s="32"/>
-      <c r="AJ47" s="32"/>
-      <c r="AK47" s="32"/>
-      <c r="AL47" s="32"/>
-      <c r="AM47" s="32"/>
-      <c r="AN47" s="32"/>
-      <c r="AO47" s="32"/>
-      <c r="AP47" s="32"/>
-      <c r="AQ47" s="32"/>
-      <c r="AR47" s="32"/>
-      <c r="AS47" s="32"/>
-      <c r="AT47" s="32"/>
-      <c r="AU47" s="32"/>
-      <c r="AV47" s="32"/>
-      <c r="AW47" s="32"/>
-      <c r="AX47" s="32"/>
-      <c r="AY47" s="32"/>
-      <c r="AZ47" s="32"/>
-      <c r="BA47" s="32"/>
-      <c r="BB47" s="32"/>
-      <c r="BC47" s="32"/>
-      <c r="BD47" s="32"/>
-      <c r="BE47" s="32"/>
-      <c r="BF47" s="32"/>
-      <c r="BG47" s="32"/>
-      <c r="BH47" s="32"/>
-      <c r="BI47" s="32"/>
-      <c r="BJ47" s="32"/>
-      <c r="BK47" s="32"/>
-      <c r="BL47" s="32"/>
-      <c r="BM47" s="32"/>
-      <c r="BN47" s="32"/>
-      <c r="BO47" s="32"/>
-      <c r="BP47" s="32"/>
-      <c r="BQ47" s="32"/>
-      <c r="BR47" s="32"/>
-      <c r="BS47" s="32"/>
-      <c r="BT47" s="32"/>
-      <c r="BU47" s="32"/>
-      <c r="BV47" s="32"/>
-      <c r="BW47" s="32"/>
-      <c r="BX47" s="32"/>
-      <c r="BY47" s="32"/>
-      <c r="BZ47" s="32"/>
-      <c r="CA47" s="32"/>
-      <c r="CB47" s="32"/>
-      <c r="CC47" s="32"/>
-      <c r="CD47" s="32"/>
-      <c r="CE47" s="32"/>
-      <c r="CF47" s="32"/>
-      <c r="CG47" s="32"/>
-      <c r="CH47" s="32"/>
-      <c r="CI47" s="32"/>
-      <c r="CJ47" s="32"/>
-      <c r="CK47" s="32"/>
-      <c r="CL47" s="32"/>
-      <c r="CM47" s="32"/>
-      <c r="CN47" s="32"/>
-      <c r="CO47" s="32"/>
-      <c r="CP47" s="32"/>
-      <c r="CQ47" s="32"/>
-      <c r="CR47" s="32"/>
-      <c r="CS47" s="32"/>
-      <c r="CT47" s="32"/>
-      <c r="CU47" s="32"/>
-      <c r="CV47" s="32"/>
-      <c r="CW47" s="32"/>
-      <c r="CX47" s="32"/>
-      <c r="CY47" s="32"/>
-      <c r="CZ47" s="32"/>
-      <c r="DA47" s="32"/>
-      <c r="DB47" s="32"/>
-      <c r="DC47" s="32"/>
-      <c r="DD47" s="32"/>
-      <c r="DE47" s="32"/>
-      <c r="DF47" s="32"/>
-      <c r="DG47" s="32"/>
-      <c r="DH47" s="32"/>
-      <c r="DI47" s="32"/>
-      <c r="DJ47" s="32"/>
-      <c r="DK47" s="32"/>
-      <c r="DL47" s="32"/>
-      <c r="DM47" s="32"/>
-      <c r="DN47" s="32"/>
-      <c r="DO47" s="32"/>
-      <c r="DP47" s="32"/>
-      <c r="DQ47" s="32"/>
-      <c r="DR47" s="32"/>
-      <c r="DS47" s="32"/>
-      <c r="DT47" s="32"/>
-      <c r="DU47" s="32"/>
-      <c r="DV47" s="32"/>
-      <c r="DW47" s="32"/>
-      <c r="DX47" s="32"/>
-      <c r="DY47" s="32"/>
-      <c r="DZ47" s="32"/>
-      <c r="EA47" s="32"/>
-      <c r="EB47" s="32"/>
-      <c r="EC47" s="32"/>
-      <c r="ED47" s="32"/>
-      <c r="EE47" s="32"/>
-      <c r="EF47" s="32"/>
-      <c r="EG47" s="32"/>
-      <c r="EH47" s="32"/>
-      <c r="EI47" s="32"/>
-      <c r="EJ47" s="32"/>
-      <c r="EK47" s="32"/>
-      <c r="EL47" s="32"/>
-      <c r="EM47" s="32"/>
-      <c r="EN47" s="32"/>
-      <c r="EO47" s="32"/>
-      <c r="EP47" s="32"/>
-      <c r="EQ47" s="32"/>
-      <c r="ER47" s="32"/>
-      <c r="ES47" s="32"/>
-      <c r="ET47" s="32"/>
-      <c r="EU47" s="32"/>
-      <c r="EV47" s="32"/>
-      <c r="EW47" s="32"/>
-      <c r="EX47" s="32"/>
-      <c r="EY47" s="32"/>
-      <c r="EZ47" s="32"/>
-      <c r="FA47" s="32"/>
-      <c r="FB47" s="32"/>
-      <c r="FC47" s="32"/>
-      <c r="FD47" s="32"/>
-      <c r="FE47" s="32"/>
-      <c r="FF47" s="32"/>
-      <c r="FG47" s="32"/>
-      <c r="FH47" s="32"/>
-      <c r="FI47" s="32"/>
-      <c r="FJ47" s="32"/>
-      <c r="FK47" s="32"/>
-      <c r="FL47" s="32"/>
-      <c r="FM47" s="32"/>
-      <c r="FN47" s="32"/>
-      <c r="FO47" s="32"/>
-      <c r="FP47" s="32"/>
-      <c r="FQ47" s="32"/>
-      <c r="FR47" s="32"/>
-      <c r="FS47" s="32"/>
-      <c r="FT47" s="32"/>
-      <c r="FU47" s="32"/>
-      <c r="FV47" s="32"/>
-      <c r="FW47" s="32"/>
-      <c r="FX47" s="32"/>
-      <c r="FY47" s="32"/>
-      <c r="FZ47" s="32"/>
-      <c r="GA47" s="32"/>
-      <c r="GB47" s="32"/>
-      <c r="GC47" s="32"/>
-      <c r="GD47" s="32"/>
-      <c r="GE47" s="32"/>
-      <c r="GF47" s="32"/>
-      <c r="GG47" s="32"/>
-      <c r="GH47" s="32"/>
-      <c r="GI47" s="32"/>
-      <c r="GJ47" s="32"/>
-      <c r="GK47" s="32"/>
-      <c r="GL47" s="32"/>
-      <c r="GM47" s="32"/>
-      <c r="GN47" s="32"/>
-      <c r="GO47" s="32"/>
-      <c r="GP47" s="32"/>
-      <c r="GQ47" s="32"/>
-      <c r="GR47" s="32"/>
-      <c r="GS47" s="32"/>
-      <c r="GT47" s="32"/>
-      <c r="GU47" s="32"/>
-      <c r="GV47" s="32"/>
-      <c r="GW47" s="32"/>
-      <c r="GX47" s="32"/>
-      <c r="GY47" s="32"/>
-      <c r="GZ47" s="32"/>
-      <c r="HA47" s="32"/>
-      <c r="HB47" s="32"/>
-      <c r="HC47" s="32"/>
-      <c r="HD47" s="32"/>
-      <c r="HE47" s="32"/>
-      <c r="HF47" s="32"/>
-      <c r="HG47" s="32"/>
-      <c r="HH47" s="32"/>
-      <c r="HI47" s="32"/>
-      <c r="HJ47" s="32"/>
-      <c r="HK47" s="32"/>
-      <c r="HL47" s="32"/>
-      <c r="HM47" s="32"/>
-      <c r="HN47" s="32"/>
-      <c r="HO47" s="32"/>
-      <c r="HP47" s="32"/>
-      <c r="HQ47" s="32"/>
-      <c r="HR47" s="32"/>
-      <c r="HS47" s="32"/>
-      <c r="HT47" s="32"/>
-      <c r="HU47" s="32"/>
-      <c r="HV47" s="32"/>
-      <c r="HW47" s="32"/>
-      <c r="HX47" s="32"/>
-      <c r="HY47" s="32"/>
-      <c r="HZ47" s="32"/>
-      <c r="IA47" s="32"/>
-      <c r="IB47" s="32"/>
-      <c r="IC47" s="32"/>
-      <c r="ID47" s="32"/>
-      <c r="IE47" s="32"/>
-      <c r="IF47" s="32"/>
-      <c r="IG47" s="32"/>
-      <c r="IH47" s="32"/>
-      <c r="II47" s="32"/>
-      <c r="IJ47" s="32"/>
-      <c r="IK47" s="32"/>
-      <c r="IL47" s="32"/>
-      <c r="IM47" s="32"/>
-      <c r="IN47" s="32"/>
-      <c r="IO47" s="32"/>
-      <c r="IP47" s="32"/>
-      <c r="IQ47" s="32"/>
-      <c r="IR47" s="32"/>
-      <c r="IS47" s="32"/>
-      <c r="IT47" s="32"/>
-      <c r="IU47" s="81"/>
+      <c r="N47" s="90"/>
+      <c r="O47" s="91"/>
+      <c r="P47" s="91"/>
+      <c r="Q47" s="91"/>
+      <c r="R47" s="91"/>
+      <c r="S47" s="91"/>
+      <c r="T47" s="91"/>
+      <c r="U47" s="91"/>
+      <c r="V47" s="91"/>
+      <c r="W47" s="91"/>
+      <c r="X47" s="91"/>
+      <c r="Y47" s="91"/>
+      <c r="Z47" s="91"/>
+      <c r="AA47" s="91"/>
+      <c r="AB47" s="91"/>
+      <c r="AC47" s="91"/>
+      <c r="AD47" s="91"/>
+      <c r="AE47" s="91"/>
+      <c r="AF47" s="91"/>
+      <c r="AG47" s="91"/>
+      <c r="AH47" s="91"/>
+      <c r="AI47" s="91"/>
+      <c r="AJ47" s="91"/>
+      <c r="AK47" s="91"/>
+      <c r="AL47" s="91"/>
+      <c r="AM47" s="91"/>
+      <c r="AN47" s="91"/>
+      <c r="AO47" s="91"/>
+      <c r="AP47" s="91"/>
+      <c r="AQ47" s="91"/>
+      <c r="AR47" s="91"/>
+      <c r="AS47" s="91"/>
+      <c r="AT47" s="91"/>
+      <c r="AU47" s="91"/>
+      <c r="AV47" s="91"/>
+      <c r="AW47" s="91"/>
+      <c r="AX47" s="91"/>
+      <c r="AY47" s="91"/>
+      <c r="AZ47" s="91"/>
+      <c r="BA47" s="91"/>
+      <c r="BB47" s="91"/>
+      <c r="BC47" s="91"/>
+      <c r="BD47" s="91"/>
+      <c r="BE47" s="91"/>
+      <c r="BF47" s="91"/>
+      <c r="BG47" s="91"/>
+      <c r="BH47" s="91"/>
+      <c r="BI47" s="91"/>
+      <c r="BJ47" s="91"/>
+      <c r="BK47" s="91"/>
+      <c r="BL47" s="91"/>
+      <c r="BM47" s="91"/>
+      <c r="BN47" s="91"/>
+      <c r="BO47" s="91"/>
+      <c r="BP47" s="91"/>
+      <c r="BQ47" s="91"/>
+      <c r="BR47" s="91"/>
+      <c r="BS47" s="91"/>
+      <c r="BT47" s="91"/>
+      <c r="BU47" s="91"/>
+      <c r="BV47" s="91"/>
+      <c r="BW47" s="91"/>
+      <c r="BX47" s="91"/>
+      <c r="BY47" s="91"/>
+      <c r="BZ47" s="91"/>
+      <c r="CA47" s="91"/>
+      <c r="CB47" s="91"/>
+      <c r="CC47" s="91"/>
+      <c r="CD47" s="91"/>
+      <c r="CE47" s="91"/>
+      <c r="CF47" s="91"/>
+      <c r="CG47" s="91"/>
+      <c r="CH47" s="91"/>
+      <c r="CI47" s="91"/>
+      <c r="CJ47" s="91"/>
+      <c r="CK47" s="91"/>
+      <c r="CL47" s="91"/>
+      <c r="CM47" s="91"/>
+      <c r="CN47" s="91"/>
+      <c r="CO47" s="91"/>
+      <c r="CP47" s="91"/>
+      <c r="CQ47" s="91"/>
+      <c r="CR47" s="91"/>
+      <c r="CS47" s="91"/>
+      <c r="CT47" s="91"/>
+      <c r="CU47" s="91"/>
+      <c r="CV47" s="91"/>
+      <c r="CW47" s="91"/>
+      <c r="CX47" s="91"/>
+      <c r="CY47" s="91"/>
+      <c r="CZ47" s="91"/>
+      <c r="DA47" s="91"/>
+      <c r="DB47" s="91"/>
+      <c r="DC47" s="91"/>
+      <c r="DD47" s="91"/>
+      <c r="DE47" s="91"/>
+      <c r="DF47" s="91"/>
+      <c r="DG47" s="91"/>
+      <c r="DH47" s="91"/>
+      <c r="DI47" s="91"/>
+      <c r="DJ47" s="91"/>
+      <c r="DK47" s="91"/>
+      <c r="DL47" s="91"/>
+      <c r="DM47" s="91"/>
+      <c r="DN47" s="91"/>
+      <c r="DO47" s="91"/>
+      <c r="DP47" s="91"/>
+      <c r="DQ47" s="91"/>
+      <c r="DR47" s="91"/>
+      <c r="DS47" s="91"/>
+      <c r="DT47" s="91"/>
+      <c r="DU47" s="91"/>
+      <c r="DV47" s="91"/>
+      <c r="DW47" s="91"/>
+      <c r="DX47" s="91"/>
+      <c r="DY47" s="91"/>
+      <c r="DZ47" s="91"/>
+      <c r="EA47" s="91"/>
+      <c r="EB47" s="91"/>
+      <c r="EC47" s="91"/>
+      <c r="ED47" s="91"/>
+      <c r="EE47" s="91"/>
+      <c r="EF47" s="91"/>
+      <c r="EG47" s="91"/>
+      <c r="EH47" s="91"/>
+      <c r="EI47" s="91"/>
+      <c r="EJ47" s="91"/>
+      <c r="EK47" s="91"/>
+      <c r="EL47" s="91"/>
+      <c r="EM47" s="91"/>
+      <c r="EN47" s="91"/>
+      <c r="EO47" s="91"/>
+      <c r="EP47" s="91"/>
+      <c r="EQ47" s="91"/>
+      <c r="ER47" s="91"/>
+      <c r="ES47" s="91"/>
+      <c r="ET47" s="91"/>
+      <c r="EU47" s="91"/>
+      <c r="EV47" s="91"/>
+      <c r="EW47" s="91"/>
+      <c r="EX47" s="91"/>
+      <c r="EY47" s="91"/>
+      <c r="EZ47" s="91"/>
+      <c r="FA47" s="91"/>
+      <c r="FB47" s="91"/>
+      <c r="FC47" s="91"/>
+      <c r="FD47" s="91"/>
+      <c r="FE47" s="91"/>
+      <c r="FF47" s="91"/>
+      <c r="FG47" s="91"/>
+      <c r="FH47" s="91"/>
+      <c r="FI47" s="91"/>
+      <c r="FJ47" s="91"/>
+      <c r="FK47" s="91"/>
+      <c r="FL47" s="91"/>
+      <c r="FM47" s="91"/>
+      <c r="FN47" s="91"/>
+      <c r="FO47" s="91"/>
+      <c r="FP47" s="91"/>
+      <c r="FQ47" s="91"/>
+      <c r="FR47" s="91"/>
+      <c r="FS47" s="91"/>
+      <c r="FT47" s="91"/>
+      <c r="FU47" s="91"/>
+      <c r="FV47" s="91"/>
+      <c r="FW47" s="91"/>
+      <c r="FX47" s="91"/>
+      <c r="FY47" s="91"/>
+      <c r="FZ47" s="91"/>
+      <c r="GA47" s="91"/>
+      <c r="GB47" s="91"/>
+      <c r="GC47" s="91"/>
+      <c r="GD47" s="91"/>
+      <c r="GE47" s="91"/>
+      <c r="GF47" s="91"/>
+      <c r="GG47" s="91"/>
+      <c r="GH47" s="91"/>
+      <c r="GI47" s="91"/>
+      <c r="GJ47" s="91"/>
+      <c r="GK47" s="91"/>
+      <c r="GL47" s="91"/>
+      <c r="GM47" s="91"/>
+      <c r="GN47" s="91"/>
+      <c r="GO47" s="91"/>
+      <c r="GP47" s="91"/>
+      <c r="GQ47" s="91"/>
+      <c r="GR47" s="91"/>
+      <c r="GS47" s="91"/>
+      <c r="GT47" s="91"/>
+      <c r="GU47" s="91"/>
+      <c r="GV47" s="91"/>
+      <c r="GW47" s="91"/>
+      <c r="GX47" s="91"/>
+      <c r="GY47" s="91"/>
+      <c r="GZ47" s="91"/>
+      <c r="HA47" s="91"/>
+      <c r="HB47" s="91"/>
+      <c r="HC47" s="91"/>
+      <c r="HD47" s="91"/>
+      <c r="HE47" s="91"/>
+      <c r="HF47" s="91"/>
+      <c r="HG47" s="91"/>
+      <c r="HH47" s="91"/>
+      <c r="HI47" s="91"/>
+      <c r="HJ47" s="91"/>
+      <c r="HK47" s="91"/>
+      <c r="HL47" s="91"/>
+      <c r="HM47" s="91"/>
+      <c r="HN47" s="91"/>
+      <c r="HO47" s="91"/>
+      <c r="HP47" s="91"/>
+      <c r="HQ47" s="91"/>
+      <c r="HR47" s="91"/>
+      <c r="HS47" s="91"/>
+      <c r="HT47" s="91"/>
+      <c r="HU47" s="91"/>
+      <c r="HV47" s="91"/>
+      <c r="HW47" s="91"/>
+      <c r="HX47" s="91"/>
+      <c r="HY47" s="91"/>
+      <c r="HZ47" s="91"/>
+      <c r="IA47" s="91"/>
+      <c r="IB47" s="91"/>
+      <c r="IC47" s="91"/>
+      <c r="ID47" s="91"/>
+      <c r="IE47" s="91"/>
+      <c r="IF47" s="91"/>
+      <c r="IG47" s="91"/>
+      <c r="IH47" s="91"/>
+      <c r="II47" s="91"/>
+      <c r="IJ47" s="91"/>
+      <c r="IK47" s="91"/>
+      <c r="IL47" s="91"/>
+      <c r="IM47" s="91"/>
+      <c r="IN47" s="91"/>
+      <c r="IO47" s="91"/>
+      <c r="IP47" s="91"/>
+      <c r="IQ47" s="91"/>
+      <c r="IR47" s="91"/>
+      <c r="IS47" s="91"/>
+      <c r="IT47" s="91"/>
+      <c r="IU47" s="92"/>
     </row>
     <row r="48" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A48" s="104" t="n">
+      <c r="A48" s="29" t="n">
         <v>42736</v>
       </c>
       <c r="B48" s="3"/>
@@ -15311,265 +15308,265 @@
         <v>82</v>
       </c>
       <c r="D48" s="34" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="E48" s="34" t="s">
-        <v>61</v>
+        <v>369</v>
       </c>
       <c r="F48" s="3"/>
       <c r="G48" s="34" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="H48" s="3"/>
       <c r="I48" s="3"/>
       <c r="J48" s="3"/>
-      <c r="K48" s="69" t="s">
+      <c r="K48" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="L48" s="13"/>
+      <c r="L48" s="3"/>
       <c r="M48" s="3"/>
-      <c r="N48" s="90"/>
-      <c r="O48" s="91"/>
-      <c r="P48" s="91"/>
-      <c r="Q48" s="91"/>
-      <c r="R48" s="91"/>
-      <c r="S48" s="91"/>
-      <c r="T48" s="91"/>
-      <c r="U48" s="91"/>
-      <c r="V48" s="91"/>
-      <c r="W48" s="91"/>
-      <c r="X48" s="91"/>
-      <c r="Y48" s="91"/>
-      <c r="Z48" s="91"/>
-      <c r="AA48" s="91"/>
-      <c r="AB48" s="91"/>
-      <c r="AC48" s="91"/>
-      <c r="AD48" s="91"/>
-      <c r="AE48" s="91"/>
-      <c r="AF48" s="91"/>
-      <c r="AG48" s="91"/>
-      <c r="AH48" s="91"/>
-      <c r="AI48" s="91"/>
-      <c r="AJ48" s="91"/>
-      <c r="AK48" s="91"/>
-      <c r="AL48" s="91"/>
-      <c r="AM48" s="91"/>
-      <c r="AN48" s="91"/>
-      <c r="AO48" s="91"/>
-      <c r="AP48" s="91"/>
-      <c r="AQ48" s="91"/>
-      <c r="AR48" s="91"/>
-      <c r="AS48" s="91"/>
-      <c r="AT48" s="91"/>
-      <c r="AU48" s="91"/>
-      <c r="AV48" s="91"/>
-      <c r="AW48" s="91"/>
-      <c r="AX48" s="91"/>
-      <c r="AY48" s="91"/>
-      <c r="AZ48" s="91"/>
-      <c r="BA48" s="91"/>
-      <c r="BB48" s="91"/>
-      <c r="BC48" s="91"/>
-      <c r="BD48" s="91"/>
-      <c r="BE48" s="91"/>
-      <c r="BF48" s="91"/>
-      <c r="BG48" s="91"/>
-      <c r="BH48" s="91"/>
-      <c r="BI48" s="91"/>
-      <c r="BJ48" s="91"/>
-      <c r="BK48" s="91"/>
-      <c r="BL48" s="91"/>
-      <c r="BM48" s="91"/>
-      <c r="BN48" s="91"/>
-      <c r="BO48" s="91"/>
-      <c r="BP48" s="91"/>
-      <c r="BQ48" s="91"/>
-      <c r="BR48" s="91"/>
-      <c r="BS48" s="91"/>
-      <c r="BT48" s="91"/>
-      <c r="BU48" s="91"/>
-      <c r="BV48" s="91"/>
-      <c r="BW48" s="91"/>
-      <c r="BX48" s="91"/>
-      <c r="BY48" s="91"/>
-      <c r="BZ48" s="91"/>
-      <c r="CA48" s="91"/>
-      <c r="CB48" s="91"/>
-      <c r="CC48" s="91"/>
-      <c r="CD48" s="91"/>
-      <c r="CE48" s="91"/>
-      <c r="CF48" s="91"/>
-      <c r="CG48" s="91"/>
-      <c r="CH48" s="91"/>
-      <c r="CI48" s="91"/>
-      <c r="CJ48" s="91"/>
-      <c r="CK48" s="91"/>
-      <c r="CL48" s="91"/>
-      <c r="CM48" s="91"/>
-      <c r="CN48" s="91"/>
-      <c r="CO48" s="91"/>
-      <c r="CP48" s="91"/>
-      <c r="CQ48" s="91"/>
-      <c r="CR48" s="91"/>
-      <c r="CS48" s="91"/>
-      <c r="CT48" s="91"/>
-      <c r="CU48" s="91"/>
-      <c r="CV48" s="91"/>
-      <c r="CW48" s="91"/>
-      <c r="CX48" s="91"/>
-      <c r="CY48" s="91"/>
-      <c r="CZ48" s="91"/>
-      <c r="DA48" s="91"/>
-      <c r="DB48" s="91"/>
-      <c r="DC48" s="91"/>
-      <c r="DD48" s="91"/>
-      <c r="DE48" s="91"/>
-      <c r="DF48" s="91"/>
-      <c r="DG48" s="91"/>
-      <c r="DH48" s="91"/>
-      <c r="DI48" s="91"/>
-      <c r="DJ48" s="91"/>
-      <c r="DK48" s="91"/>
-      <c r="DL48" s="91"/>
-      <c r="DM48" s="91"/>
-      <c r="DN48" s="91"/>
-      <c r="DO48" s="91"/>
-      <c r="DP48" s="91"/>
-      <c r="DQ48" s="91"/>
-      <c r="DR48" s="91"/>
-      <c r="DS48" s="91"/>
-      <c r="DT48" s="91"/>
-      <c r="DU48" s="91"/>
-      <c r="DV48" s="91"/>
-      <c r="DW48" s="91"/>
-      <c r="DX48" s="91"/>
-      <c r="DY48" s="91"/>
-      <c r="DZ48" s="91"/>
-      <c r="EA48" s="91"/>
-      <c r="EB48" s="91"/>
-      <c r="EC48" s="91"/>
-      <c r="ED48" s="91"/>
-      <c r="EE48" s="91"/>
-      <c r="EF48" s="91"/>
-      <c r="EG48" s="91"/>
-      <c r="EH48" s="91"/>
-      <c r="EI48" s="91"/>
-      <c r="EJ48" s="91"/>
-      <c r="EK48" s="91"/>
-      <c r="EL48" s="91"/>
-      <c r="EM48" s="91"/>
-      <c r="EN48" s="91"/>
-      <c r="EO48" s="91"/>
-      <c r="EP48" s="91"/>
-      <c r="EQ48" s="91"/>
-      <c r="ER48" s="91"/>
-      <c r="ES48" s="91"/>
-      <c r="ET48" s="91"/>
-      <c r="EU48" s="91"/>
-      <c r="EV48" s="91"/>
-      <c r="EW48" s="91"/>
-      <c r="EX48" s="91"/>
-      <c r="EY48" s="91"/>
-      <c r="EZ48" s="91"/>
-      <c r="FA48" s="91"/>
-      <c r="FB48" s="91"/>
-      <c r="FC48" s="91"/>
-      <c r="FD48" s="91"/>
-      <c r="FE48" s="91"/>
-      <c r="FF48" s="91"/>
-      <c r="FG48" s="91"/>
-      <c r="FH48" s="91"/>
-      <c r="FI48" s="91"/>
-      <c r="FJ48" s="91"/>
-      <c r="FK48" s="91"/>
-      <c r="FL48" s="91"/>
-      <c r="FM48" s="91"/>
-      <c r="FN48" s="91"/>
-      <c r="FO48" s="91"/>
-      <c r="FP48" s="91"/>
-      <c r="FQ48" s="91"/>
-      <c r="FR48" s="91"/>
-      <c r="FS48" s="91"/>
-      <c r="FT48" s="91"/>
-      <c r="FU48" s="91"/>
-      <c r="FV48" s="91"/>
-      <c r="FW48" s="91"/>
-      <c r="FX48" s="91"/>
-      <c r="FY48" s="91"/>
-      <c r="FZ48" s="91"/>
-      <c r="GA48" s="91"/>
-      <c r="GB48" s="91"/>
-      <c r="GC48" s="91"/>
-      <c r="GD48" s="91"/>
-      <c r="GE48" s="91"/>
-      <c r="GF48" s="91"/>
-      <c r="GG48" s="91"/>
-      <c r="GH48" s="91"/>
-      <c r="GI48" s="91"/>
-      <c r="GJ48" s="91"/>
-      <c r="GK48" s="91"/>
-      <c r="GL48" s="91"/>
-      <c r="GM48" s="91"/>
-      <c r="GN48" s="91"/>
-      <c r="GO48" s="91"/>
-      <c r="GP48" s="91"/>
-      <c r="GQ48" s="91"/>
-      <c r="GR48" s="91"/>
-      <c r="GS48" s="91"/>
-      <c r="GT48" s="91"/>
-      <c r="GU48" s="91"/>
-      <c r="GV48" s="91"/>
-      <c r="GW48" s="91"/>
-      <c r="GX48" s="91"/>
-      <c r="GY48" s="91"/>
-      <c r="GZ48" s="91"/>
-      <c r="HA48" s="91"/>
-      <c r="HB48" s="91"/>
-      <c r="HC48" s="91"/>
-      <c r="HD48" s="91"/>
-      <c r="HE48" s="91"/>
-      <c r="HF48" s="91"/>
-      <c r="HG48" s="91"/>
-      <c r="HH48" s="91"/>
-      <c r="HI48" s="91"/>
-      <c r="HJ48" s="91"/>
-      <c r="HK48" s="91"/>
-      <c r="HL48" s="91"/>
-      <c r="HM48" s="91"/>
-      <c r="HN48" s="91"/>
-      <c r="HO48" s="91"/>
-      <c r="HP48" s="91"/>
-      <c r="HQ48" s="91"/>
-      <c r="HR48" s="91"/>
-      <c r="HS48" s="91"/>
-      <c r="HT48" s="91"/>
-      <c r="HU48" s="91"/>
-      <c r="HV48" s="91"/>
-      <c r="HW48" s="91"/>
-      <c r="HX48" s="91"/>
-      <c r="HY48" s="91"/>
-      <c r="HZ48" s="91"/>
-      <c r="IA48" s="91"/>
-      <c r="IB48" s="91"/>
-      <c r="IC48" s="91"/>
-      <c r="ID48" s="91"/>
-      <c r="IE48" s="91"/>
-      <c r="IF48" s="91"/>
-      <c r="IG48" s="91"/>
-      <c r="IH48" s="91"/>
-      <c r="II48" s="91"/>
-      <c r="IJ48" s="91"/>
-      <c r="IK48" s="91"/>
-      <c r="IL48" s="91"/>
-      <c r="IM48" s="91"/>
-      <c r="IN48" s="91"/>
-      <c r="IO48" s="91"/>
-      <c r="IP48" s="91"/>
-      <c r="IQ48" s="91"/>
-      <c r="IR48" s="91"/>
-      <c r="IS48" s="91"/>
-      <c r="IT48" s="91"/>
-      <c r="IU48" s="92"/>
+      <c r="N48" s="93"/>
+      <c r="O48" s="78"/>
+      <c r="P48" s="78"/>
+      <c r="Q48" s="78"/>
+      <c r="R48" s="78"/>
+      <c r="S48" s="78"/>
+      <c r="T48" s="78"/>
+      <c r="U48" s="78"/>
+      <c r="V48" s="78"/>
+      <c r="W48" s="78"/>
+      <c r="X48" s="78"/>
+      <c r="Y48" s="78"/>
+      <c r="Z48" s="78"/>
+      <c r="AA48" s="78"/>
+      <c r="AB48" s="78"/>
+      <c r="AC48" s="78"/>
+      <c r="AD48" s="78"/>
+      <c r="AE48" s="78"/>
+      <c r="AF48" s="78"/>
+      <c r="AG48" s="78"/>
+      <c r="AH48" s="78"/>
+      <c r="AI48" s="78"/>
+      <c r="AJ48" s="78"/>
+      <c r="AK48" s="78"/>
+      <c r="AL48" s="78"/>
+      <c r="AM48" s="78"/>
+      <c r="AN48" s="78"/>
+      <c r="AO48" s="78"/>
+      <c r="AP48" s="78"/>
+      <c r="AQ48" s="78"/>
+      <c r="AR48" s="78"/>
+      <c r="AS48" s="78"/>
+      <c r="AT48" s="78"/>
+      <c r="AU48" s="78"/>
+      <c r="AV48" s="78"/>
+      <c r="AW48" s="78"/>
+      <c r="AX48" s="78"/>
+      <c r="AY48" s="78"/>
+      <c r="AZ48" s="78"/>
+      <c r="BA48" s="78"/>
+      <c r="BB48" s="78"/>
+      <c r="BC48" s="78"/>
+      <c r="BD48" s="78"/>
+      <c r="BE48" s="78"/>
+      <c r="BF48" s="78"/>
+      <c r="BG48" s="78"/>
+      <c r="BH48" s="78"/>
+      <c r="BI48" s="78"/>
+      <c r="BJ48" s="78"/>
+      <c r="BK48" s="78"/>
+      <c r="BL48" s="78"/>
+      <c r="BM48" s="78"/>
+      <c r="BN48" s="78"/>
+      <c r="BO48" s="78"/>
+      <c r="BP48" s="78"/>
+      <c r="BQ48" s="78"/>
+      <c r="BR48" s="78"/>
+      <c r="BS48" s="78"/>
+      <c r="BT48" s="78"/>
+      <c r="BU48" s="78"/>
+      <c r="BV48" s="78"/>
+      <c r="BW48" s="78"/>
+      <c r="BX48" s="78"/>
+      <c r="BY48" s="78"/>
+      <c r="BZ48" s="78"/>
+      <c r="CA48" s="78"/>
+      <c r="CB48" s="78"/>
+      <c r="CC48" s="78"/>
+      <c r="CD48" s="78"/>
+      <c r="CE48" s="78"/>
+      <c r="CF48" s="78"/>
+      <c r="CG48" s="78"/>
+      <c r="CH48" s="78"/>
+      <c r="CI48" s="78"/>
+      <c r="CJ48" s="78"/>
+      <c r="CK48" s="78"/>
+      <c r="CL48" s="78"/>
+      <c r="CM48" s="78"/>
+      <c r="CN48" s="78"/>
+      <c r="CO48" s="78"/>
+      <c r="CP48" s="78"/>
+      <c r="CQ48" s="78"/>
+      <c r="CR48" s="78"/>
+      <c r="CS48" s="78"/>
+      <c r="CT48" s="78"/>
+      <c r="CU48" s="78"/>
+      <c r="CV48" s="78"/>
+      <c r="CW48" s="78"/>
+      <c r="CX48" s="78"/>
+      <c r="CY48" s="78"/>
+      <c r="CZ48" s="78"/>
+      <c r="DA48" s="78"/>
+      <c r="DB48" s="78"/>
+      <c r="DC48" s="78"/>
+      <c r="DD48" s="78"/>
+      <c r="DE48" s="78"/>
+      <c r="DF48" s="78"/>
+      <c r="DG48" s="78"/>
+      <c r="DH48" s="78"/>
+      <c r="DI48" s="78"/>
+      <c r="DJ48" s="78"/>
+      <c r="DK48" s="78"/>
+      <c r="DL48" s="78"/>
+      <c r="DM48" s="78"/>
+      <c r="DN48" s="78"/>
+      <c r="DO48" s="78"/>
+      <c r="DP48" s="78"/>
+      <c r="DQ48" s="78"/>
+      <c r="DR48" s="78"/>
+      <c r="DS48" s="78"/>
+      <c r="DT48" s="78"/>
+      <c r="DU48" s="78"/>
+      <c r="DV48" s="78"/>
+      <c r="DW48" s="78"/>
+      <c r="DX48" s="78"/>
+      <c r="DY48" s="78"/>
+      <c r="DZ48" s="78"/>
+      <c r="EA48" s="78"/>
+      <c r="EB48" s="78"/>
+      <c r="EC48" s="78"/>
+      <c r="ED48" s="78"/>
+      <c r="EE48" s="78"/>
+      <c r="EF48" s="78"/>
+      <c r="EG48" s="78"/>
+      <c r="EH48" s="78"/>
+      <c r="EI48" s="78"/>
+      <c r="EJ48" s="78"/>
+      <c r="EK48" s="78"/>
+      <c r="EL48" s="78"/>
+      <c r="EM48" s="78"/>
+      <c r="EN48" s="78"/>
+      <c r="EO48" s="78"/>
+      <c r="EP48" s="78"/>
+      <c r="EQ48" s="78"/>
+      <c r="ER48" s="78"/>
+      <c r="ES48" s="78"/>
+      <c r="ET48" s="78"/>
+      <c r="EU48" s="78"/>
+      <c r="EV48" s="78"/>
+      <c r="EW48" s="78"/>
+      <c r="EX48" s="78"/>
+      <c r="EY48" s="78"/>
+      <c r="EZ48" s="78"/>
+      <c r="FA48" s="78"/>
+      <c r="FB48" s="78"/>
+      <c r="FC48" s="78"/>
+      <c r="FD48" s="78"/>
+      <c r="FE48" s="78"/>
+      <c r="FF48" s="78"/>
+      <c r="FG48" s="78"/>
+      <c r="FH48" s="78"/>
+      <c r="FI48" s="78"/>
+      <c r="FJ48" s="78"/>
+      <c r="FK48" s="78"/>
+      <c r="FL48" s="78"/>
+      <c r="FM48" s="78"/>
+      <c r="FN48" s="78"/>
+      <c r="FO48" s="78"/>
+      <c r="FP48" s="78"/>
+      <c r="FQ48" s="78"/>
+      <c r="FR48" s="78"/>
+      <c r="FS48" s="78"/>
+      <c r="FT48" s="78"/>
+      <c r="FU48" s="78"/>
+      <c r="FV48" s="78"/>
+      <c r="FW48" s="78"/>
+      <c r="FX48" s="78"/>
+      <c r="FY48" s="78"/>
+      <c r="FZ48" s="78"/>
+      <c r="GA48" s="78"/>
+      <c r="GB48" s="78"/>
+      <c r="GC48" s="78"/>
+      <c r="GD48" s="78"/>
+      <c r="GE48" s="78"/>
+      <c r="GF48" s="78"/>
+      <c r="GG48" s="78"/>
+      <c r="GH48" s="78"/>
+      <c r="GI48" s="78"/>
+      <c r="GJ48" s="78"/>
+      <c r="GK48" s="78"/>
+      <c r="GL48" s="78"/>
+      <c r="GM48" s="78"/>
+      <c r="GN48" s="78"/>
+      <c r="GO48" s="78"/>
+      <c r="GP48" s="78"/>
+      <c r="GQ48" s="78"/>
+      <c r="GR48" s="78"/>
+      <c r="GS48" s="78"/>
+      <c r="GT48" s="78"/>
+      <c r="GU48" s="78"/>
+      <c r="GV48" s="78"/>
+      <c r="GW48" s="78"/>
+      <c r="GX48" s="78"/>
+      <c r="GY48" s="78"/>
+      <c r="GZ48" s="78"/>
+      <c r="HA48" s="78"/>
+      <c r="HB48" s="78"/>
+      <c r="HC48" s="78"/>
+      <c r="HD48" s="78"/>
+      <c r="HE48" s="78"/>
+      <c r="HF48" s="78"/>
+      <c r="HG48" s="78"/>
+      <c r="HH48" s="78"/>
+      <c r="HI48" s="78"/>
+      <c r="HJ48" s="78"/>
+      <c r="HK48" s="78"/>
+      <c r="HL48" s="78"/>
+      <c r="HM48" s="78"/>
+      <c r="HN48" s="78"/>
+      <c r="HO48" s="78"/>
+      <c r="HP48" s="78"/>
+      <c r="HQ48" s="78"/>
+      <c r="HR48" s="78"/>
+      <c r="HS48" s="78"/>
+      <c r="HT48" s="78"/>
+      <c r="HU48" s="78"/>
+      <c r="HV48" s="78"/>
+      <c r="HW48" s="78"/>
+      <c r="HX48" s="78"/>
+      <c r="HY48" s="78"/>
+      <c r="HZ48" s="78"/>
+      <c r="IA48" s="78"/>
+      <c r="IB48" s="78"/>
+      <c r="IC48" s="78"/>
+      <c r="ID48" s="78"/>
+      <c r="IE48" s="78"/>
+      <c r="IF48" s="78"/>
+      <c r="IG48" s="78"/>
+      <c r="IH48" s="78"/>
+      <c r="II48" s="78"/>
+      <c r="IJ48" s="78"/>
+      <c r="IK48" s="78"/>
+      <c r="IL48" s="78"/>
+      <c r="IM48" s="78"/>
+      <c r="IN48" s="78"/>
+      <c r="IO48" s="78"/>
+      <c r="IP48" s="78"/>
+      <c r="IQ48" s="78"/>
+      <c r="IR48" s="78"/>
+      <c r="IS48" s="78"/>
+      <c r="IT48" s="78"/>
+      <c r="IU48" s="79"/>
     </row>
     <row r="49" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="29" t="n">
@@ -15580,14 +15577,14 @@
         <v>82</v>
       </c>
       <c r="D49" s="34" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="E49" s="34" t="s">
-        <v>370</v>
+        <v>61</v>
       </c>
       <c r="F49" s="3"/>
       <c r="G49" s="34" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="H49" s="3"/>
       <c r="I49" s="3"/>
@@ -15597,248 +15594,248 @@
       </c>
       <c r="L49" s="3"/>
       <c r="M49" s="3"/>
-      <c r="N49" s="93"/>
-      <c r="O49" s="78"/>
-      <c r="P49" s="78"/>
-      <c r="Q49" s="78"/>
-      <c r="R49" s="78"/>
-      <c r="S49" s="78"/>
-      <c r="T49" s="78"/>
-      <c r="U49" s="78"/>
-      <c r="V49" s="78"/>
-      <c r="W49" s="78"/>
-      <c r="X49" s="78"/>
-      <c r="Y49" s="78"/>
-      <c r="Z49" s="78"/>
-      <c r="AA49" s="78"/>
-      <c r="AB49" s="78"/>
-      <c r="AC49" s="78"/>
-      <c r="AD49" s="78"/>
-      <c r="AE49" s="78"/>
-      <c r="AF49" s="78"/>
-      <c r="AG49" s="78"/>
-      <c r="AH49" s="78"/>
-      <c r="AI49" s="78"/>
-      <c r="AJ49" s="78"/>
-      <c r="AK49" s="78"/>
-      <c r="AL49" s="78"/>
-      <c r="AM49" s="78"/>
-      <c r="AN49" s="78"/>
-      <c r="AO49" s="78"/>
-      <c r="AP49" s="78"/>
-      <c r="AQ49" s="78"/>
-      <c r="AR49" s="78"/>
-      <c r="AS49" s="78"/>
-      <c r="AT49" s="78"/>
-      <c r="AU49" s="78"/>
-      <c r="AV49" s="78"/>
-      <c r="AW49" s="78"/>
-      <c r="AX49" s="78"/>
-      <c r="AY49" s="78"/>
-      <c r="AZ49" s="78"/>
-      <c r="BA49" s="78"/>
-      <c r="BB49" s="78"/>
-      <c r="BC49" s="78"/>
-      <c r="BD49" s="78"/>
-      <c r="BE49" s="78"/>
-      <c r="BF49" s="78"/>
-      <c r="BG49" s="78"/>
-      <c r="BH49" s="78"/>
-      <c r="BI49" s="78"/>
-      <c r="BJ49" s="78"/>
-      <c r="BK49" s="78"/>
-      <c r="BL49" s="78"/>
-      <c r="BM49" s="78"/>
-      <c r="BN49" s="78"/>
-      <c r="BO49" s="78"/>
-      <c r="BP49" s="78"/>
-      <c r="BQ49" s="78"/>
-      <c r="BR49" s="78"/>
-      <c r="BS49" s="78"/>
-      <c r="BT49" s="78"/>
-      <c r="BU49" s="78"/>
-      <c r="BV49" s="78"/>
-      <c r="BW49" s="78"/>
-      <c r="BX49" s="78"/>
-      <c r="BY49" s="78"/>
-      <c r="BZ49" s="78"/>
-      <c r="CA49" s="78"/>
-      <c r="CB49" s="78"/>
-      <c r="CC49" s="78"/>
-      <c r="CD49" s="78"/>
-      <c r="CE49" s="78"/>
-      <c r="CF49" s="78"/>
-      <c r="CG49" s="78"/>
-      <c r="CH49" s="78"/>
-      <c r="CI49" s="78"/>
-      <c r="CJ49" s="78"/>
-      <c r="CK49" s="78"/>
-      <c r="CL49" s="78"/>
-      <c r="CM49" s="78"/>
-      <c r="CN49" s="78"/>
-      <c r="CO49" s="78"/>
-      <c r="CP49" s="78"/>
-      <c r="CQ49" s="78"/>
-      <c r="CR49" s="78"/>
-      <c r="CS49" s="78"/>
-      <c r="CT49" s="78"/>
-      <c r="CU49" s="78"/>
-      <c r="CV49" s="78"/>
-      <c r="CW49" s="78"/>
-      <c r="CX49" s="78"/>
-      <c r="CY49" s="78"/>
-      <c r="CZ49" s="78"/>
-      <c r="DA49" s="78"/>
-      <c r="DB49" s="78"/>
-      <c r="DC49" s="78"/>
-      <c r="DD49" s="78"/>
-      <c r="DE49" s="78"/>
-      <c r="DF49" s="78"/>
-      <c r="DG49" s="78"/>
-      <c r="DH49" s="78"/>
-      <c r="DI49" s="78"/>
-      <c r="DJ49" s="78"/>
-      <c r="DK49" s="78"/>
-      <c r="DL49" s="78"/>
-      <c r="DM49" s="78"/>
-      <c r="DN49" s="78"/>
-      <c r="DO49" s="78"/>
-      <c r="DP49" s="78"/>
-      <c r="DQ49" s="78"/>
-      <c r="DR49" s="78"/>
-      <c r="DS49" s="78"/>
-      <c r="DT49" s="78"/>
-      <c r="DU49" s="78"/>
-      <c r="DV49" s="78"/>
-      <c r="DW49" s="78"/>
-      <c r="DX49" s="78"/>
-      <c r="DY49" s="78"/>
-      <c r="DZ49" s="78"/>
-      <c r="EA49" s="78"/>
-      <c r="EB49" s="78"/>
-      <c r="EC49" s="78"/>
-      <c r="ED49" s="78"/>
-      <c r="EE49" s="78"/>
-      <c r="EF49" s="78"/>
-      <c r="EG49" s="78"/>
-      <c r="EH49" s="78"/>
-      <c r="EI49" s="78"/>
-      <c r="EJ49" s="78"/>
-      <c r="EK49" s="78"/>
-      <c r="EL49" s="78"/>
-      <c r="EM49" s="78"/>
-      <c r="EN49" s="78"/>
-      <c r="EO49" s="78"/>
-      <c r="EP49" s="78"/>
-      <c r="EQ49" s="78"/>
-      <c r="ER49" s="78"/>
-      <c r="ES49" s="78"/>
-      <c r="ET49" s="78"/>
-      <c r="EU49" s="78"/>
-      <c r="EV49" s="78"/>
-      <c r="EW49" s="78"/>
-      <c r="EX49" s="78"/>
-      <c r="EY49" s="78"/>
-      <c r="EZ49" s="78"/>
-      <c r="FA49" s="78"/>
-      <c r="FB49" s="78"/>
-      <c r="FC49" s="78"/>
-      <c r="FD49" s="78"/>
-      <c r="FE49" s="78"/>
-      <c r="FF49" s="78"/>
-      <c r="FG49" s="78"/>
-      <c r="FH49" s="78"/>
-      <c r="FI49" s="78"/>
-      <c r="FJ49" s="78"/>
-      <c r="FK49" s="78"/>
-      <c r="FL49" s="78"/>
-      <c r="FM49" s="78"/>
-      <c r="FN49" s="78"/>
-      <c r="FO49" s="78"/>
-      <c r="FP49" s="78"/>
-      <c r="FQ49" s="78"/>
-      <c r="FR49" s="78"/>
-      <c r="FS49" s="78"/>
-      <c r="FT49" s="78"/>
-      <c r="FU49" s="78"/>
-      <c r="FV49" s="78"/>
-      <c r="FW49" s="78"/>
-      <c r="FX49" s="78"/>
-      <c r="FY49" s="78"/>
-      <c r="FZ49" s="78"/>
-      <c r="GA49" s="78"/>
-      <c r="GB49" s="78"/>
-      <c r="GC49" s="78"/>
-      <c r="GD49" s="78"/>
-      <c r="GE49" s="78"/>
-      <c r="GF49" s="78"/>
-      <c r="GG49" s="78"/>
-      <c r="GH49" s="78"/>
-      <c r="GI49" s="78"/>
-      <c r="GJ49" s="78"/>
-      <c r="GK49" s="78"/>
-      <c r="GL49" s="78"/>
-      <c r="GM49" s="78"/>
-      <c r="GN49" s="78"/>
-      <c r="GO49" s="78"/>
-      <c r="GP49" s="78"/>
-      <c r="GQ49" s="78"/>
-      <c r="GR49" s="78"/>
-      <c r="GS49" s="78"/>
-      <c r="GT49" s="78"/>
-      <c r="GU49" s="78"/>
-      <c r="GV49" s="78"/>
-      <c r="GW49" s="78"/>
-      <c r="GX49" s="78"/>
-      <c r="GY49" s="78"/>
-      <c r="GZ49" s="78"/>
-      <c r="HA49" s="78"/>
-      <c r="HB49" s="78"/>
-      <c r="HC49" s="78"/>
-      <c r="HD49" s="78"/>
-      <c r="HE49" s="78"/>
-      <c r="HF49" s="78"/>
-      <c r="HG49" s="78"/>
-      <c r="HH49" s="78"/>
-      <c r="HI49" s="78"/>
-      <c r="HJ49" s="78"/>
-      <c r="HK49" s="78"/>
-      <c r="HL49" s="78"/>
-      <c r="HM49" s="78"/>
-      <c r="HN49" s="78"/>
-      <c r="HO49" s="78"/>
-      <c r="HP49" s="78"/>
-      <c r="HQ49" s="78"/>
-      <c r="HR49" s="78"/>
-      <c r="HS49" s="78"/>
-      <c r="HT49" s="78"/>
-      <c r="HU49" s="78"/>
-      <c r="HV49" s="78"/>
-      <c r="HW49" s="78"/>
-      <c r="HX49" s="78"/>
-      <c r="HY49" s="78"/>
-      <c r="HZ49" s="78"/>
-      <c r="IA49" s="78"/>
-      <c r="IB49" s="78"/>
-      <c r="IC49" s="78"/>
-      <c r="ID49" s="78"/>
-      <c r="IE49" s="78"/>
-      <c r="IF49" s="78"/>
-      <c r="IG49" s="78"/>
-      <c r="IH49" s="78"/>
-      <c r="II49" s="78"/>
-      <c r="IJ49" s="78"/>
-      <c r="IK49" s="78"/>
-      <c r="IL49" s="78"/>
-      <c r="IM49" s="78"/>
-      <c r="IN49" s="78"/>
-      <c r="IO49" s="78"/>
-      <c r="IP49" s="78"/>
-      <c r="IQ49" s="78"/>
-      <c r="IR49" s="78"/>
-      <c r="IS49" s="78"/>
-      <c r="IT49" s="78"/>
-      <c r="IU49" s="79"/>
+      <c r="N49" s="84"/>
+      <c r="O49" s="32"/>
+      <c r="P49" s="32"/>
+      <c r="Q49" s="32"/>
+      <c r="R49" s="32"/>
+      <c r="S49" s="32"/>
+      <c r="T49" s="32"/>
+      <c r="U49" s="32"/>
+      <c r="V49" s="32"/>
+      <c r="W49" s="32"/>
+      <c r="X49" s="32"/>
+      <c r="Y49" s="32"/>
+      <c r="Z49" s="32"/>
+      <c r="AA49" s="32"/>
+      <c r="AB49" s="32"/>
+      <c r="AC49" s="32"/>
+      <c r="AD49" s="32"/>
+      <c r="AE49" s="32"/>
+      <c r="AF49" s="32"/>
+      <c r="AG49" s="32"/>
+      <c r="AH49" s="32"/>
+      <c r="AI49" s="32"/>
+      <c r="AJ49" s="32"/>
+      <c r="AK49" s="32"/>
+      <c r="AL49" s="32"/>
+      <c r="AM49" s="32"/>
+      <c r="AN49" s="32"/>
+      <c r="AO49" s="32"/>
+      <c r="AP49" s="32"/>
+      <c r="AQ49" s="32"/>
+      <c r="AR49" s="32"/>
+      <c r="AS49" s="32"/>
+      <c r="AT49" s="32"/>
+      <c r="AU49" s="32"/>
+      <c r="AV49" s="32"/>
+      <c r="AW49" s="32"/>
+      <c r="AX49" s="32"/>
+      <c r="AY49" s="32"/>
+      <c r="AZ49" s="32"/>
+      <c r="BA49" s="32"/>
+      <c r="BB49" s="32"/>
+      <c r="BC49" s="32"/>
+      <c r="BD49" s="32"/>
+      <c r="BE49" s="32"/>
+      <c r="BF49" s="32"/>
+      <c r="BG49" s="32"/>
+      <c r="BH49" s="32"/>
+      <c r="BI49" s="32"/>
+      <c r="BJ49" s="32"/>
+      <c r="BK49" s="32"/>
+      <c r="BL49" s="32"/>
+      <c r="BM49" s="32"/>
+      <c r="BN49" s="32"/>
+      <c r="BO49" s="32"/>
+      <c r="BP49" s="32"/>
+      <c r="BQ49" s="32"/>
+      <c r="BR49" s="32"/>
+      <c r="BS49" s="32"/>
+      <c r="BT49" s="32"/>
+      <c r="BU49" s="32"/>
+      <c r="BV49" s="32"/>
+      <c r="BW49" s="32"/>
+      <c r="BX49" s="32"/>
+      <c r="BY49" s="32"/>
+      <c r="BZ49" s="32"/>
+      <c r="CA49" s="32"/>
+      <c r="CB49" s="32"/>
+      <c r="CC49" s="32"/>
+      <c r="CD49" s="32"/>
+      <c r="CE49" s="32"/>
+      <c r="CF49" s="32"/>
+      <c r="CG49" s="32"/>
+      <c r="CH49" s="32"/>
+      <c r="CI49" s="32"/>
+      <c r="CJ49" s="32"/>
+      <c r="CK49" s="32"/>
+      <c r="CL49" s="32"/>
+      <c r="CM49" s="32"/>
+      <c r="CN49" s="32"/>
+      <c r="CO49" s="32"/>
+      <c r="CP49" s="32"/>
+      <c r="CQ49" s="32"/>
+      <c r="CR49" s="32"/>
+      <c r="CS49" s="32"/>
+      <c r="CT49" s="32"/>
+      <c r="CU49" s="32"/>
+      <c r="CV49" s="32"/>
+      <c r="CW49" s="32"/>
+      <c r="CX49" s="32"/>
+      <c r="CY49" s="32"/>
+      <c r="CZ49" s="32"/>
+      <c r="DA49" s="32"/>
+      <c r="DB49" s="32"/>
+      <c r="DC49" s="32"/>
+      <c r="DD49" s="32"/>
+      <c r="DE49" s="32"/>
+      <c r="DF49" s="32"/>
+      <c r="DG49" s="32"/>
+      <c r="DH49" s="32"/>
+      <c r="DI49" s="32"/>
+      <c r="DJ49" s="32"/>
+      <c r="DK49" s="32"/>
+      <c r="DL49" s="32"/>
+      <c r="DM49" s="32"/>
+      <c r="DN49" s="32"/>
+      <c r="DO49" s="32"/>
+      <c r="DP49" s="32"/>
+      <c r="DQ49" s="32"/>
+      <c r="DR49" s="32"/>
+      <c r="DS49" s="32"/>
+      <c r="DT49" s="32"/>
+      <c r="DU49" s="32"/>
+      <c r="DV49" s="32"/>
+      <c r="DW49" s="32"/>
+      <c r="DX49" s="32"/>
+      <c r="DY49" s="32"/>
+      <c r="DZ49" s="32"/>
+      <c r="EA49" s="32"/>
+      <c r="EB49" s="32"/>
+      <c r="EC49" s="32"/>
+      <c r="ED49" s="32"/>
+      <c r="EE49" s="32"/>
+      <c r="EF49" s="32"/>
+      <c r="EG49" s="32"/>
+      <c r="EH49" s="32"/>
+      <c r="EI49" s="32"/>
+      <c r="EJ49" s="32"/>
+      <c r="EK49" s="32"/>
+      <c r="EL49" s="32"/>
+      <c r="EM49" s="32"/>
+      <c r="EN49" s="32"/>
+      <c r="EO49" s="32"/>
+      <c r="EP49" s="32"/>
+      <c r="EQ49" s="32"/>
+      <c r="ER49" s="32"/>
+      <c r="ES49" s="32"/>
+      <c r="ET49" s="32"/>
+      <c r="EU49" s="32"/>
+      <c r="EV49" s="32"/>
+      <c r="EW49" s="32"/>
+      <c r="EX49" s="32"/>
+      <c r="EY49" s="32"/>
+      <c r="EZ49" s="32"/>
+      <c r="FA49" s="32"/>
+      <c r="FB49" s="32"/>
+      <c r="FC49" s="32"/>
+      <c r="FD49" s="32"/>
+      <c r="FE49" s="32"/>
+      <c r="FF49" s="32"/>
+      <c r="FG49" s="32"/>
+      <c r="FH49" s="32"/>
+      <c r="FI49" s="32"/>
+      <c r="FJ49" s="32"/>
+      <c r="FK49" s="32"/>
+      <c r="FL49" s="32"/>
+      <c r="FM49" s="32"/>
+      <c r="FN49" s="32"/>
+      <c r="FO49" s="32"/>
+      <c r="FP49" s="32"/>
+      <c r="FQ49" s="32"/>
+      <c r="FR49" s="32"/>
+      <c r="FS49" s="32"/>
+      <c r="FT49" s="32"/>
+      <c r="FU49" s="32"/>
+      <c r="FV49" s="32"/>
+      <c r="FW49" s="32"/>
+      <c r="FX49" s="32"/>
+      <c r="FY49" s="32"/>
+      <c r="FZ49" s="32"/>
+      <c r="GA49" s="32"/>
+      <c r="GB49" s="32"/>
+      <c r="GC49" s="32"/>
+      <c r="GD49" s="32"/>
+      <c r="GE49" s="32"/>
+      <c r="GF49" s="32"/>
+      <c r="GG49" s="32"/>
+      <c r="GH49" s="32"/>
+      <c r="GI49" s="32"/>
+      <c r="GJ49" s="32"/>
+      <c r="GK49" s="32"/>
+      <c r="GL49" s="32"/>
+      <c r="GM49" s="32"/>
+      <c r="GN49" s="32"/>
+      <c r="GO49" s="32"/>
+      <c r="GP49" s="32"/>
+      <c r="GQ49" s="32"/>
+      <c r="GR49" s="32"/>
+      <c r="GS49" s="32"/>
+      <c r="GT49" s="32"/>
+      <c r="GU49" s="32"/>
+      <c r="GV49" s="32"/>
+      <c r="GW49" s="32"/>
+      <c r="GX49" s="32"/>
+      <c r="GY49" s="32"/>
+      <c r="GZ49" s="32"/>
+      <c r="HA49" s="32"/>
+      <c r="HB49" s="32"/>
+      <c r="HC49" s="32"/>
+      <c r="HD49" s="32"/>
+      <c r="HE49" s="32"/>
+      <c r="HF49" s="32"/>
+      <c r="HG49" s="32"/>
+      <c r="HH49" s="32"/>
+      <c r="HI49" s="32"/>
+      <c r="HJ49" s="32"/>
+      <c r="HK49" s="32"/>
+      <c r="HL49" s="32"/>
+      <c r="HM49" s="32"/>
+      <c r="HN49" s="32"/>
+      <c r="HO49" s="32"/>
+      <c r="HP49" s="32"/>
+      <c r="HQ49" s="32"/>
+      <c r="HR49" s="32"/>
+      <c r="HS49" s="32"/>
+      <c r="HT49" s="32"/>
+      <c r="HU49" s="32"/>
+      <c r="HV49" s="32"/>
+      <c r="HW49" s="32"/>
+      <c r="HX49" s="32"/>
+      <c r="HY49" s="32"/>
+      <c r="HZ49" s="32"/>
+      <c r="IA49" s="32"/>
+      <c r="IB49" s="32"/>
+      <c r="IC49" s="32"/>
+      <c r="ID49" s="32"/>
+      <c r="IE49" s="32"/>
+      <c r="IF49" s="32"/>
+      <c r="IG49" s="32"/>
+      <c r="IH49" s="32"/>
+      <c r="II49" s="32"/>
+      <c r="IJ49" s="32"/>
+      <c r="IK49" s="32"/>
+      <c r="IL49" s="32"/>
+      <c r="IM49" s="32"/>
+      <c r="IN49" s="32"/>
+      <c r="IO49" s="32"/>
+      <c r="IP49" s="32"/>
+      <c r="IQ49" s="32"/>
+      <c r="IR49" s="32"/>
+      <c r="IS49" s="32"/>
+      <c r="IT49" s="32"/>
+      <c r="IU49" s="81"/>
     </row>
     <row r="50" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="29" t="n">
@@ -15849,14 +15846,14 @@
         <v>82</v>
       </c>
       <c r="D50" s="34" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="E50" s="34" t="s">
         <v>61</v>
       </c>
       <c r="F50" s="3"/>
       <c r="G50" s="34" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="H50" s="3"/>
       <c r="I50" s="3"/>
@@ -15866,518 +15863,250 @@
       </c>
       <c r="L50" s="3"/>
       <c r="M50" s="3"/>
-      <c r="N50" s="84"/>
-      <c r="O50" s="32"/>
-      <c r="P50" s="32"/>
-      <c r="Q50" s="32"/>
-      <c r="R50" s="32"/>
-      <c r="S50" s="32"/>
-      <c r="T50" s="32"/>
-      <c r="U50" s="32"/>
-      <c r="V50" s="32"/>
-      <c r="W50" s="32"/>
-      <c r="X50" s="32"/>
-      <c r="Y50" s="32"/>
-      <c r="Z50" s="32"/>
-      <c r="AA50" s="32"/>
-      <c r="AB50" s="32"/>
-      <c r="AC50" s="32"/>
-      <c r="AD50" s="32"/>
-      <c r="AE50" s="32"/>
-      <c r="AF50" s="32"/>
-      <c r="AG50" s="32"/>
-      <c r="AH50" s="32"/>
-      <c r="AI50" s="32"/>
-      <c r="AJ50" s="32"/>
-      <c r="AK50" s="32"/>
-      <c r="AL50" s="32"/>
-      <c r="AM50" s="32"/>
-      <c r="AN50" s="32"/>
-      <c r="AO50" s="32"/>
-      <c r="AP50" s="32"/>
-      <c r="AQ50" s="32"/>
-      <c r="AR50" s="32"/>
-      <c r="AS50" s="32"/>
-      <c r="AT50" s="32"/>
-      <c r="AU50" s="32"/>
-      <c r="AV50" s="32"/>
-      <c r="AW50" s="32"/>
-      <c r="AX50" s="32"/>
-      <c r="AY50" s="32"/>
-      <c r="AZ50" s="32"/>
-      <c r="BA50" s="32"/>
-      <c r="BB50" s="32"/>
-      <c r="BC50" s="32"/>
-      <c r="BD50" s="32"/>
-      <c r="BE50" s="32"/>
-      <c r="BF50" s="32"/>
-      <c r="BG50" s="32"/>
-      <c r="BH50" s="32"/>
-      <c r="BI50" s="32"/>
-      <c r="BJ50" s="32"/>
-      <c r="BK50" s="32"/>
-      <c r="BL50" s="32"/>
-      <c r="BM50" s="32"/>
-      <c r="BN50" s="32"/>
-      <c r="BO50" s="32"/>
-      <c r="BP50" s="32"/>
-      <c r="BQ50" s="32"/>
-      <c r="BR50" s="32"/>
-      <c r="BS50" s="32"/>
-      <c r="BT50" s="32"/>
-      <c r="BU50" s="32"/>
-      <c r="BV50" s="32"/>
-      <c r="BW50" s="32"/>
-      <c r="BX50" s="32"/>
-      <c r="BY50" s="32"/>
-      <c r="BZ50" s="32"/>
-      <c r="CA50" s="32"/>
-      <c r="CB50" s="32"/>
-      <c r="CC50" s="32"/>
-      <c r="CD50" s="32"/>
-      <c r="CE50" s="32"/>
-      <c r="CF50" s="32"/>
-      <c r="CG50" s="32"/>
-      <c r="CH50" s="32"/>
-      <c r="CI50" s="32"/>
-      <c r="CJ50" s="32"/>
-      <c r="CK50" s="32"/>
-      <c r="CL50" s="32"/>
-      <c r="CM50" s="32"/>
-      <c r="CN50" s="32"/>
-      <c r="CO50" s="32"/>
-      <c r="CP50" s="32"/>
-      <c r="CQ50" s="32"/>
-      <c r="CR50" s="32"/>
-      <c r="CS50" s="32"/>
-      <c r="CT50" s="32"/>
-      <c r="CU50" s="32"/>
-      <c r="CV50" s="32"/>
-      <c r="CW50" s="32"/>
-      <c r="CX50" s="32"/>
-      <c r="CY50" s="32"/>
-      <c r="CZ50" s="32"/>
-      <c r="DA50" s="32"/>
-      <c r="DB50" s="32"/>
-      <c r="DC50" s="32"/>
-      <c r="DD50" s="32"/>
-      <c r="DE50" s="32"/>
-      <c r="DF50" s="32"/>
-      <c r="DG50" s="32"/>
-      <c r="DH50" s="32"/>
-      <c r="DI50" s="32"/>
-      <c r="DJ50" s="32"/>
-      <c r="DK50" s="32"/>
-      <c r="DL50" s="32"/>
-      <c r="DM50" s="32"/>
-      <c r="DN50" s="32"/>
-      <c r="DO50" s="32"/>
-      <c r="DP50" s="32"/>
-      <c r="DQ50" s="32"/>
-      <c r="DR50" s="32"/>
-      <c r="DS50" s="32"/>
-      <c r="DT50" s="32"/>
-      <c r="DU50" s="32"/>
-      <c r="DV50" s="32"/>
-      <c r="DW50" s="32"/>
-      <c r="DX50" s="32"/>
-      <c r="DY50" s="32"/>
-      <c r="DZ50" s="32"/>
-      <c r="EA50" s="32"/>
-      <c r="EB50" s="32"/>
-      <c r="EC50" s="32"/>
-      <c r="ED50" s="32"/>
-      <c r="EE50" s="32"/>
-      <c r="EF50" s="32"/>
-      <c r="EG50" s="32"/>
-      <c r="EH50" s="32"/>
-      <c r="EI50" s="32"/>
-      <c r="EJ50" s="32"/>
-      <c r="EK50" s="32"/>
-      <c r="EL50" s="32"/>
-      <c r="EM50" s="32"/>
-      <c r="EN50" s="32"/>
-      <c r="EO50" s="32"/>
-      <c r="EP50" s="32"/>
-      <c r="EQ50" s="32"/>
-      <c r="ER50" s="32"/>
-      <c r="ES50" s="32"/>
-      <c r="ET50" s="32"/>
-      <c r="EU50" s="32"/>
-      <c r="EV50" s="32"/>
-      <c r="EW50" s="32"/>
-      <c r="EX50" s="32"/>
-      <c r="EY50" s="32"/>
-      <c r="EZ50" s="32"/>
-      <c r="FA50" s="32"/>
-      <c r="FB50" s="32"/>
-      <c r="FC50" s="32"/>
-      <c r="FD50" s="32"/>
-      <c r="FE50" s="32"/>
-      <c r="FF50" s="32"/>
-      <c r="FG50" s="32"/>
-      <c r="FH50" s="32"/>
-      <c r="FI50" s="32"/>
-      <c r="FJ50" s="32"/>
-      <c r="FK50" s="32"/>
-      <c r="FL50" s="32"/>
-      <c r="FM50" s="32"/>
-      <c r="FN50" s="32"/>
-      <c r="FO50" s="32"/>
-      <c r="FP50" s="32"/>
-      <c r="FQ50" s="32"/>
-      <c r="FR50" s="32"/>
-      <c r="FS50" s="32"/>
-      <c r="FT50" s="32"/>
-      <c r="FU50" s="32"/>
-      <c r="FV50" s="32"/>
-      <c r="FW50" s="32"/>
-      <c r="FX50" s="32"/>
-      <c r="FY50" s="32"/>
-      <c r="FZ50" s="32"/>
-      <c r="GA50" s="32"/>
-      <c r="GB50" s="32"/>
-      <c r="GC50" s="32"/>
-      <c r="GD50" s="32"/>
-      <c r="GE50" s="32"/>
-      <c r="GF50" s="32"/>
-      <c r="GG50" s="32"/>
-      <c r="GH50" s="32"/>
-      <c r="GI50" s="32"/>
-      <c r="GJ50" s="32"/>
-      <c r="GK50" s="32"/>
-      <c r="GL50" s="32"/>
-      <c r="GM50" s="32"/>
-      <c r="GN50" s="32"/>
-      <c r="GO50" s="32"/>
-      <c r="GP50" s="32"/>
-      <c r="GQ50" s="32"/>
-      <c r="GR50" s="32"/>
-      <c r="GS50" s="32"/>
-      <c r="GT50" s="32"/>
-      <c r="GU50" s="32"/>
-      <c r="GV50" s="32"/>
-      <c r="GW50" s="32"/>
-      <c r="GX50" s="32"/>
-      <c r="GY50" s="32"/>
-      <c r="GZ50" s="32"/>
-      <c r="HA50" s="32"/>
-      <c r="HB50" s="32"/>
-      <c r="HC50" s="32"/>
-      <c r="HD50" s="32"/>
-      <c r="HE50" s="32"/>
-      <c r="HF50" s="32"/>
-      <c r="HG50" s="32"/>
-      <c r="HH50" s="32"/>
-      <c r="HI50" s="32"/>
-      <c r="HJ50" s="32"/>
-      <c r="HK50" s="32"/>
-      <c r="HL50" s="32"/>
-      <c r="HM50" s="32"/>
-      <c r="HN50" s="32"/>
-      <c r="HO50" s="32"/>
-      <c r="HP50" s="32"/>
-      <c r="HQ50" s="32"/>
-      <c r="HR50" s="32"/>
-      <c r="HS50" s="32"/>
-      <c r="HT50" s="32"/>
-      <c r="HU50" s="32"/>
-      <c r="HV50" s="32"/>
-      <c r="HW50" s="32"/>
-      <c r="HX50" s="32"/>
-      <c r="HY50" s="32"/>
-      <c r="HZ50" s="32"/>
-      <c r="IA50" s="32"/>
-      <c r="IB50" s="32"/>
-      <c r="IC50" s="32"/>
-      <c r="ID50" s="32"/>
-      <c r="IE50" s="32"/>
-      <c r="IF50" s="32"/>
-      <c r="IG50" s="32"/>
-      <c r="IH50" s="32"/>
-      <c r="II50" s="32"/>
-      <c r="IJ50" s="32"/>
-      <c r="IK50" s="32"/>
-      <c r="IL50" s="32"/>
-      <c r="IM50" s="32"/>
-      <c r="IN50" s="32"/>
-      <c r="IO50" s="32"/>
-      <c r="IP50" s="32"/>
-      <c r="IQ50" s="32"/>
-      <c r="IR50" s="32"/>
-      <c r="IS50" s="32"/>
-      <c r="IT50" s="32"/>
-      <c r="IU50" s="81"/>
+      <c r="N50" s="90"/>
+      <c r="O50" s="91"/>
+      <c r="P50" s="91"/>
+      <c r="Q50" s="91"/>
+      <c r="R50" s="91"/>
+      <c r="S50" s="91"/>
+      <c r="T50" s="91"/>
+      <c r="U50" s="91"/>
+      <c r="V50" s="91"/>
+      <c r="W50" s="91"/>
+      <c r="X50" s="91"/>
+      <c r="Y50" s="91"/>
+      <c r="Z50" s="91"/>
+      <c r="AA50" s="91"/>
+      <c r="AB50" s="91"/>
+      <c r="AC50" s="91"/>
+      <c r="AD50" s="91"/>
+      <c r="AE50" s="91"/>
+      <c r="AF50" s="91"/>
+      <c r="AG50" s="91"/>
+      <c r="AH50" s="91"/>
+      <c r="AI50" s="91"/>
+      <c r="AJ50" s="91"/>
+      <c r="AK50" s="91"/>
+      <c r="AL50" s="91"/>
+      <c r="AM50" s="91"/>
+      <c r="AN50" s="91"/>
+      <c r="AO50" s="91"/>
+      <c r="AP50" s="91"/>
+      <c r="AQ50" s="91"/>
+      <c r="AR50" s="91"/>
+      <c r="AS50" s="91"/>
+      <c r="AT50" s="91"/>
+      <c r="AU50" s="91"/>
+      <c r="AV50" s="91"/>
+      <c r="AW50" s="91"/>
+      <c r="AX50" s="91"/>
+      <c r="AY50" s="91"/>
+      <c r="AZ50" s="91"/>
+      <c r="BA50" s="91"/>
+      <c r="BB50" s="91"/>
+      <c r="BC50" s="91"/>
+      <c r="BD50" s="91"/>
+      <c r="BE50" s="91"/>
+      <c r="BF50" s="91"/>
+      <c r="BG50" s="91"/>
+      <c r="BH50" s="91"/>
+      <c r="BI50" s="91"/>
+      <c r="BJ50" s="91"/>
+      <c r="BK50" s="91"/>
+      <c r="BL50" s="91"/>
+      <c r="BM50" s="91"/>
+      <c r="BN50" s="91"/>
+      <c r="BO50" s="91"/>
+      <c r="BP50" s="91"/>
+      <c r="BQ50" s="91"/>
+      <c r="BR50" s="91"/>
+      <c r="BS50" s="91"/>
+      <c r="BT50" s="91"/>
+      <c r="BU50" s="91"/>
+      <c r="BV50" s="91"/>
+      <c r="BW50" s="91"/>
+      <c r="BX50" s="91"/>
+      <c r="BY50" s="91"/>
+      <c r="BZ50" s="91"/>
+      <c r="CA50" s="91"/>
+      <c r="CB50" s="91"/>
+      <c r="CC50" s="91"/>
+      <c r="CD50" s="91"/>
+      <c r="CE50" s="91"/>
+      <c r="CF50" s="91"/>
+      <c r="CG50" s="91"/>
+      <c r="CH50" s="91"/>
+      <c r="CI50" s="91"/>
+      <c r="CJ50" s="91"/>
+      <c r="CK50" s="91"/>
+      <c r="CL50" s="91"/>
+      <c r="CM50" s="91"/>
+      <c r="CN50" s="91"/>
+      <c r="CO50" s="91"/>
+      <c r="CP50" s="91"/>
+      <c r="CQ50" s="91"/>
+      <c r="CR50" s="91"/>
+      <c r="CS50" s="91"/>
+      <c r="CT50" s="91"/>
+      <c r="CU50" s="91"/>
+      <c r="CV50" s="91"/>
+      <c r="CW50" s="91"/>
+      <c r="CX50" s="91"/>
+      <c r="CY50" s="91"/>
+      <c r="CZ50" s="91"/>
+      <c r="DA50" s="91"/>
+      <c r="DB50" s="91"/>
+      <c r="DC50" s="91"/>
+      <c r="DD50" s="91"/>
+      <c r="DE50" s="91"/>
+      <c r="DF50" s="91"/>
+      <c r="DG50" s="91"/>
+      <c r="DH50" s="91"/>
+      <c r="DI50" s="91"/>
+      <c r="DJ50" s="91"/>
+      <c r="DK50" s="91"/>
+      <c r="DL50" s="91"/>
+      <c r="DM50" s="91"/>
+      <c r="DN50" s="91"/>
+      <c r="DO50" s="91"/>
+      <c r="DP50" s="91"/>
+      <c r="DQ50" s="91"/>
+      <c r="DR50" s="91"/>
+      <c r="DS50" s="91"/>
+      <c r="DT50" s="91"/>
+      <c r="DU50" s="91"/>
+      <c r="DV50" s="91"/>
+      <c r="DW50" s="91"/>
+      <c r="DX50" s="91"/>
+      <c r="DY50" s="91"/>
+      <c r="DZ50" s="91"/>
+      <c r="EA50" s="91"/>
+      <c r="EB50" s="91"/>
+      <c r="EC50" s="91"/>
+      <c r="ED50" s="91"/>
+      <c r="EE50" s="91"/>
+      <c r="EF50" s="91"/>
+      <c r="EG50" s="91"/>
+      <c r="EH50" s="91"/>
+      <c r="EI50" s="91"/>
+      <c r="EJ50" s="91"/>
+      <c r="EK50" s="91"/>
+      <c r="EL50" s="91"/>
+      <c r="EM50" s="91"/>
+      <c r="EN50" s="91"/>
+      <c r="EO50" s="91"/>
+      <c r="EP50" s="91"/>
+      <c r="EQ50" s="91"/>
+      <c r="ER50" s="91"/>
+      <c r="ES50" s="91"/>
+      <c r="ET50" s="91"/>
+      <c r="EU50" s="91"/>
+      <c r="EV50" s="91"/>
+      <c r="EW50" s="91"/>
+      <c r="EX50" s="91"/>
+      <c r="EY50" s="91"/>
+      <c r="EZ50" s="91"/>
+      <c r="FA50" s="91"/>
+      <c r="FB50" s="91"/>
+      <c r="FC50" s="91"/>
+      <c r="FD50" s="91"/>
+      <c r="FE50" s="91"/>
+      <c r="FF50" s="91"/>
+      <c r="FG50" s="91"/>
+      <c r="FH50" s="91"/>
+      <c r="FI50" s="91"/>
+      <c r="FJ50" s="91"/>
+      <c r="FK50" s="91"/>
+      <c r="FL50" s="91"/>
+      <c r="FM50" s="91"/>
+      <c r="FN50" s="91"/>
+      <c r="FO50" s="91"/>
+      <c r="FP50" s="91"/>
+      <c r="FQ50" s="91"/>
+      <c r="FR50" s="91"/>
+      <c r="FS50" s="91"/>
+      <c r="FT50" s="91"/>
+      <c r="FU50" s="91"/>
+      <c r="FV50" s="91"/>
+      <c r="FW50" s="91"/>
+      <c r="FX50" s="91"/>
+      <c r="FY50" s="91"/>
+      <c r="FZ50" s="91"/>
+      <c r="GA50" s="91"/>
+      <c r="GB50" s="91"/>
+      <c r="GC50" s="91"/>
+      <c r="GD50" s="91"/>
+      <c r="GE50" s="91"/>
+      <c r="GF50" s="91"/>
+      <c r="GG50" s="91"/>
+      <c r="GH50" s="91"/>
+      <c r="GI50" s="91"/>
+      <c r="GJ50" s="91"/>
+      <c r="GK50" s="91"/>
+      <c r="GL50" s="91"/>
+      <c r="GM50" s="91"/>
+      <c r="GN50" s="91"/>
+      <c r="GO50" s="91"/>
+      <c r="GP50" s="91"/>
+      <c r="GQ50" s="91"/>
+      <c r="GR50" s="91"/>
+      <c r="GS50" s="91"/>
+      <c r="GT50" s="91"/>
+      <c r="GU50" s="91"/>
+      <c r="GV50" s="91"/>
+      <c r="GW50" s="91"/>
+      <c r="GX50" s="91"/>
+      <c r="GY50" s="91"/>
+      <c r="GZ50" s="91"/>
+      <c r="HA50" s="91"/>
+      <c r="HB50" s="91"/>
+      <c r="HC50" s="91"/>
+      <c r="HD50" s="91"/>
+      <c r="HE50" s="91"/>
+      <c r="HF50" s="91"/>
+      <c r="HG50" s="91"/>
+      <c r="HH50" s="91"/>
+      <c r="HI50" s="91"/>
+      <c r="HJ50" s="91"/>
+      <c r="HK50" s="91"/>
+      <c r="HL50" s="91"/>
+      <c r="HM50" s="91"/>
+      <c r="HN50" s="91"/>
+      <c r="HO50" s="91"/>
+      <c r="HP50" s="91"/>
+      <c r="HQ50" s="91"/>
+      <c r="HR50" s="91"/>
+      <c r="HS50" s="91"/>
+      <c r="HT50" s="91"/>
+      <c r="HU50" s="91"/>
+      <c r="HV50" s="91"/>
+      <c r="HW50" s="91"/>
+      <c r="HX50" s="91"/>
+      <c r="HY50" s="91"/>
+      <c r="HZ50" s="91"/>
+      <c r="IA50" s="91"/>
+      <c r="IB50" s="91"/>
+      <c r="IC50" s="91"/>
+      <c r="ID50" s="91"/>
+      <c r="IE50" s="91"/>
+      <c r="IF50" s="91"/>
+      <c r="IG50" s="91"/>
+      <c r="IH50" s="91"/>
+      <c r="II50" s="91"/>
+      <c r="IJ50" s="91"/>
+      <c r="IK50" s="91"/>
+      <c r="IL50" s="91"/>
+      <c r="IM50" s="91"/>
+      <c r="IN50" s="91"/>
+      <c r="IO50" s="91"/>
+      <c r="IP50" s="91"/>
+      <c r="IQ50" s="91"/>
+      <c r="IR50" s="91"/>
+      <c r="IS50" s="91"/>
+      <c r="IT50" s="91"/>
+      <c r="IU50" s="92"/>
     </row>
-    <row r="51" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A51" s="29" t="n">
-        <v>42736</v>
-      </c>
-      <c r="B51" s="3"/>
-      <c r="C51" s="34" t="s">
-        <v>82</v>
-      </c>
-      <c r="D51" s="34" t="s">
-        <v>378</v>
-      </c>
-      <c r="E51" s="34" t="s">
-        <v>61</v>
-      </c>
-      <c r="F51" s="3"/>
-      <c r="G51" s="34" t="s">
-        <v>379</v>
-      </c>
-      <c r="H51" s="3"/>
-      <c r="I51" s="3"/>
-      <c r="J51" s="3"/>
-      <c r="K51" s="34" t="s">
-        <v>40</v>
-      </c>
-      <c r="L51" s="3"/>
-      <c r="M51" s="3"/>
-      <c r="N51" s="90"/>
-      <c r="O51" s="91"/>
-      <c r="P51" s="91"/>
-      <c r="Q51" s="91"/>
-      <c r="R51" s="91"/>
-      <c r="S51" s="91"/>
-      <c r="T51" s="91"/>
-      <c r="U51" s="91"/>
-      <c r="V51" s="91"/>
-      <c r="W51" s="91"/>
-      <c r="X51" s="91"/>
-      <c r="Y51" s="91"/>
-      <c r="Z51" s="91"/>
-      <c r="AA51" s="91"/>
-      <c r="AB51" s="91"/>
-      <c r="AC51" s="91"/>
-      <c r="AD51" s="91"/>
-      <c r="AE51" s="91"/>
-      <c r="AF51" s="91"/>
-      <c r="AG51" s="91"/>
-      <c r="AH51" s="91"/>
-      <c r="AI51" s="91"/>
-      <c r="AJ51" s="91"/>
-      <c r="AK51" s="91"/>
-      <c r="AL51" s="91"/>
-      <c r="AM51" s="91"/>
-      <c r="AN51" s="91"/>
-      <c r="AO51" s="91"/>
-      <c r="AP51" s="91"/>
-      <c r="AQ51" s="91"/>
-      <c r="AR51" s="91"/>
-      <c r="AS51" s="91"/>
-      <c r="AT51" s="91"/>
-      <c r="AU51" s="91"/>
-      <c r="AV51" s="91"/>
-      <c r="AW51" s="91"/>
-      <c r="AX51" s="91"/>
-      <c r="AY51" s="91"/>
-      <c r="AZ51" s="91"/>
-      <c r="BA51" s="91"/>
-      <c r="BB51" s="91"/>
-      <c r="BC51" s="91"/>
-      <c r="BD51" s="91"/>
-      <c r="BE51" s="91"/>
-      <c r="BF51" s="91"/>
-      <c r="BG51" s="91"/>
-      <c r="BH51" s="91"/>
-      <c r="BI51" s="91"/>
-      <c r="BJ51" s="91"/>
-      <c r="BK51" s="91"/>
-      <c r="BL51" s="91"/>
-      <c r="BM51" s="91"/>
-      <c r="BN51" s="91"/>
-      <c r="BO51" s="91"/>
-      <c r="BP51" s="91"/>
-      <c r="BQ51" s="91"/>
-      <c r="BR51" s="91"/>
-      <c r="BS51" s="91"/>
-      <c r="BT51" s="91"/>
-      <c r="BU51" s="91"/>
-      <c r="BV51" s="91"/>
-      <c r="BW51" s="91"/>
-      <c r="BX51" s="91"/>
-      <c r="BY51" s="91"/>
-      <c r="BZ51" s="91"/>
-      <c r="CA51" s="91"/>
-      <c r="CB51" s="91"/>
-      <c r="CC51" s="91"/>
-      <c r="CD51" s="91"/>
-      <c r="CE51" s="91"/>
-      <c r="CF51" s="91"/>
-      <c r="CG51" s="91"/>
-      <c r="CH51" s="91"/>
-      <c r="CI51" s="91"/>
-      <c r="CJ51" s="91"/>
-      <c r="CK51" s="91"/>
-      <c r="CL51" s="91"/>
-      <c r="CM51" s="91"/>
-      <c r="CN51" s="91"/>
-      <c r="CO51" s="91"/>
-      <c r="CP51" s="91"/>
-      <c r="CQ51" s="91"/>
-      <c r="CR51" s="91"/>
-      <c r="CS51" s="91"/>
-      <c r="CT51" s="91"/>
-      <c r="CU51" s="91"/>
-      <c r="CV51" s="91"/>
-      <c r="CW51" s="91"/>
-      <c r="CX51" s="91"/>
-      <c r="CY51" s="91"/>
-      <c r="CZ51" s="91"/>
-      <c r="DA51" s="91"/>
-      <c r="DB51" s="91"/>
-      <c r="DC51" s="91"/>
-      <c r="DD51" s="91"/>
-      <c r="DE51" s="91"/>
-      <c r="DF51" s="91"/>
-      <c r="DG51" s="91"/>
-      <c r="DH51" s="91"/>
-      <c r="DI51" s="91"/>
-      <c r="DJ51" s="91"/>
-      <c r="DK51" s="91"/>
-      <c r="DL51" s="91"/>
-      <c r="DM51" s="91"/>
-      <c r="DN51" s="91"/>
-      <c r="DO51" s="91"/>
-      <c r="DP51" s="91"/>
-      <c r="DQ51" s="91"/>
-      <c r="DR51" s="91"/>
-      <c r="DS51" s="91"/>
-      <c r="DT51" s="91"/>
-      <c r="DU51" s="91"/>
-      <c r="DV51" s="91"/>
-      <c r="DW51" s="91"/>
-      <c r="DX51" s="91"/>
-      <c r="DY51" s="91"/>
-      <c r="DZ51" s="91"/>
-      <c r="EA51" s="91"/>
-      <c r="EB51" s="91"/>
-      <c r="EC51" s="91"/>
-      <c r="ED51" s="91"/>
-      <c r="EE51" s="91"/>
-      <c r="EF51" s="91"/>
-      <c r="EG51" s="91"/>
-      <c r="EH51" s="91"/>
-      <c r="EI51" s="91"/>
-      <c r="EJ51" s="91"/>
-      <c r="EK51" s="91"/>
-      <c r="EL51" s="91"/>
-      <c r="EM51" s="91"/>
-      <c r="EN51" s="91"/>
-      <c r="EO51" s="91"/>
-      <c r="EP51" s="91"/>
-      <c r="EQ51" s="91"/>
-      <c r="ER51" s="91"/>
-      <c r="ES51" s="91"/>
-      <c r="ET51" s="91"/>
-      <c r="EU51" s="91"/>
-      <c r="EV51" s="91"/>
-      <c r="EW51" s="91"/>
-      <c r="EX51" s="91"/>
-      <c r="EY51" s="91"/>
-      <c r="EZ51" s="91"/>
-      <c r="FA51" s="91"/>
-      <c r="FB51" s="91"/>
-      <c r="FC51" s="91"/>
-      <c r="FD51" s="91"/>
-      <c r="FE51" s="91"/>
-      <c r="FF51" s="91"/>
-      <c r="FG51" s="91"/>
-      <c r="FH51" s="91"/>
-      <c r="FI51" s="91"/>
-      <c r="FJ51" s="91"/>
-      <c r="FK51" s="91"/>
-      <c r="FL51" s="91"/>
-      <c r="FM51" s="91"/>
-      <c r="FN51" s="91"/>
-      <c r="FO51" s="91"/>
-      <c r="FP51" s="91"/>
-      <c r="FQ51" s="91"/>
-      <c r="FR51" s="91"/>
-      <c r="FS51" s="91"/>
-      <c r="FT51" s="91"/>
-      <c r="FU51" s="91"/>
-      <c r="FV51" s="91"/>
-      <c r="FW51" s="91"/>
-      <c r="FX51" s="91"/>
-      <c r="FY51" s="91"/>
-      <c r="FZ51" s="91"/>
-      <c r="GA51" s="91"/>
-      <c r="GB51" s="91"/>
-      <c r="GC51" s="91"/>
-      <c r="GD51" s="91"/>
-      <c r="GE51" s="91"/>
-      <c r="GF51" s="91"/>
-      <c r="GG51" s="91"/>
-      <c r="GH51" s="91"/>
-      <c r="GI51" s="91"/>
-      <c r="GJ51" s="91"/>
-      <c r="GK51" s="91"/>
-      <c r="GL51" s="91"/>
-      <c r="GM51" s="91"/>
-      <c r="GN51" s="91"/>
-      <c r="GO51" s="91"/>
-      <c r="GP51" s="91"/>
-      <c r="GQ51" s="91"/>
-      <c r="GR51" s="91"/>
-      <c r="GS51" s="91"/>
-      <c r="GT51" s="91"/>
-      <c r="GU51" s="91"/>
-      <c r="GV51" s="91"/>
-      <c r="GW51" s="91"/>
-      <c r="GX51" s="91"/>
-      <c r="GY51" s="91"/>
-      <c r="GZ51" s="91"/>
-      <c r="HA51" s="91"/>
-      <c r="HB51" s="91"/>
-      <c r="HC51" s="91"/>
-      <c r="HD51" s="91"/>
-      <c r="HE51" s="91"/>
-      <c r="HF51" s="91"/>
-      <c r="HG51" s="91"/>
-      <c r="HH51" s="91"/>
-      <c r="HI51" s="91"/>
-      <c r="HJ51" s="91"/>
-      <c r="HK51" s="91"/>
-      <c r="HL51" s="91"/>
-      <c r="HM51" s="91"/>
-      <c r="HN51" s="91"/>
-      <c r="HO51" s="91"/>
-      <c r="HP51" s="91"/>
-      <c r="HQ51" s="91"/>
-      <c r="HR51" s="91"/>
-      <c r="HS51" s="91"/>
-      <c r="HT51" s="91"/>
-      <c r="HU51" s="91"/>
-      <c r="HV51" s="91"/>
-      <c r="HW51" s="91"/>
-      <c r="HX51" s="91"/>
-      <c r="HY51" s="91"/>
-      <c r="HZ51" s="91"/>
-      <c r="IA51" s="91"/>
-      <c r="IB51" s="91"/>
-      <c r="IC51" s="91"/>
-      <c r="ID51" s="91"/>
-      <c r="IE51" s="91"/>
-      <c r="IF51" s="91"/>
-      <c r="IG51" s="91"/>
-      <c r="IH51" s="91"/>
-      <c r="II51" s="91"/>
-      <c r="IJ51" s="91"/>
-      <c r="IK51" s="91"/>
-      <c r="IL51" s="91"/>
-      <c r="IM51" s="91"/>
-      <c r="IN51" s="91"/>
-      <c r="IO51" s="91"/>
-      <c r="IP51" s="91"/>
-      <c r="IQ51" s="91"/>
-      <c r="IR51" s="91"/>
-      <c r="IS51" s="91"/>
-      <c r="IT51" s="91"/>
-      <c r="IU51" s="92"/>
-    </row>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -16413,7 +16142,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="10" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B1" s="108" t="s">
         <v>11</v>
@@ -16442,13 +16171,13 @@
         <v>42</v>
       </c>
       <c r="D2" s="14" t="s">
+        <v>380</v>
+      </c>
+      <c r="E2" s="14" t="s">
         <v>381</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="F2" s="14" t="s">
         <v>382</v>
-      </c>
-      <c r="F2" s="14" t="s">
-        <v>383</v>
       </c>
       <c r="G2" s="111"/>
       <c r="H2" s="112"/>
@@ -16491,7 +16220,7 @@
         <v>59</v>
       </c>
       <c r="E4" s="117" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="F4" s="67" t="n">
         <v>1</v>
@@ -16513,7 +16242,7 @@
         <v>62</v>
       </c>
       <c r="E5" s="35" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="F5" s="4" t="n">
         <v>2</v>
@@ -16535,7 +16264,7 @@
         <v>64</v>
       </c>
       <c r="E6" s="35" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="F6" s="4" t="n">
         <v>3</v>
@@ -16634,7 +16363,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="10" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>11</v>
@@ -16669,13 +16398,13 @@
         <v>42</v>
       </c>
       <c r="D2" s="14" t="s">
+        <v>387</v>
+      </c>
+      <c r="E2" s="14" t="s">
         <v>388</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="F2" s="14" t="s">
         <v>389</v>
-      </c>
-      <c r="F2" s="14" t="s">
-        <v>390</v>
       </c>
       <c r="G2" s="111"/>
       <c r="H2" s="112"/>
@@ -16730,7 +16459,7 @@
         <v>59</v>
       </c>
       <c r="E4" s="117" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="F4" s="67" t="n">
         <v>1</v>
@@ -16758,7 +16487,7 @@
         <v>62</v>
       </c>
       <c r="E5" s="35" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="F5" s="4" t="n">
         <v>2</v>
@@ -16786,7 +16515,7 @@
         <v>64</v>
       </c>
       <c r="E6" s="35" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="F6" s="4" t="n">
         <v>3</v>
@@ -16915,7 +16644,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="10" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>11</v>
@@ -16950,13 +16679,13 @@
         <v>42</v>
       </c>
       <c r="D2" s="14" t="s">
+        <v>387</v>
+      </c>
+      <c r="E2" s="14" t="s">
         <v>388</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="F2" s="14" t="s">
         <v>389</v>
-      </c>
-      <c r="F2" s="14" t="s">
-        <v>390</v>
       </c>
       <c r="G2" s="121"/>
       <c r="H2" s="122"/>
@@ -17011,7 +16740,7 @@
         <v>59</v>
       </c>
       <c r="E4" s="117" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="F4" s="67" t="n">
         <v>1</v>
@@ -17039,7 +16768,7 @@
         <v>62</v>
       </c>
       <c r="E5" s="35" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="F5" s="4" t="n">
         <v>2</v>
@@ -17067,7 +16796,7 @@
         <v>64</v>
       </c>
       <c r="E6" s="35" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="F6" s="4" t="n">
         <v>3</v>
@@ -17196,7 +16925,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="19" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="10" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B1" s="108" t="s">
         <v>11</v>
@@ -17225,13 +16954,13 @@
         <v>42</v>
       </c>
       <c r="D2" s="14" t="s">
+        <v>380</v>
+      </c>
+      <c r="E2" s="14" t="s">
         <v>381</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="F2" s="14" t="s">
         <v>382</v>
-      </c>
-      <c r="F2" s="14" t="s">
-        <v>383</v>
       </c>
       <c r="G2" s="111"/>
       <c r="H2" s="112"/>
@@ -17274,7 +17003,7 @@
         <v>59</v>
       </c>
       <c r="E4" s="117" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="F4" s="67" t="n">
         <v>1</v>
@@ -17296,7 +17025,7 @@
         <v>62</v>
       </c>
       <c r="E5" s="35" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="F5" s="4" t="n">
         <v>2</v>
@@ -17318,7 +17047,7 @@
         <v>64</v>
       </c>
       <c r="E6" s="35" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="F6" s="4" t="n">
         <v>3</v>
@@ -17419,7 +17148,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="10" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>11</v>
@@ -17452,13 +17181,13 @@
       </c>
       <c r="C2" s="123"/>
       <c r="D2" s="14" t="s">
+        <v>393</v>
+      </c>
+      <c r="E2" s="14" t="s">
         <v>394</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="F2" s="14" t="s">
         <v>395</v>
-      </c>
-      <c r="F2" s="14" t="s">
-        <v>396</v>
       </c>
       <c r="G2" s="13"/>
       <c r="H2" s="3"/>
@@ -17479,16 +17208,16 @@
         <v>20</v>
       </c>
       <c r="C3" s="6" t="s">
+        <v>396</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>397</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="E3" s="6" t="s">
         <v>398</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="F3" s="6" t="s">
         <v>399</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>400</v>
       </c>
       <c r="G3" s="124"/>
       <c r="H3" s="125"/>
@@ -17507,7 +17236,7 @@
       </c>
       <c r="B4" s="97"/>
       <c r="C4" s="126" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D4" s="126" t="s">
         <v>24</v>
@@ -17535,7 +17264,7 @@
       </c>
       <c r="B5" s="75"/>
       <c r="C5" s="127" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="D5" s="127" t="s">
         <v>24</v>
@@ -17563,7 +17292,7 @@
       </c>
       <c r="B6" s="75"/>
       <c r="C6" s="127" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="D6" s="127" t="s">
         <v>24</v>
@@ -17591,7 +17320,7 @@
       </c>
       <c r="B7" s="100"/>
       <c r="C7" s="128" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="D7" s="128" t="s">
         <v>24</v>
@@ -17619,7 +17348,7 @@
       </c>
       <c r="B8" s="129"/>
       <c r="C8" s="11" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="D8" s="11" t="s">
         <v>24</v>
@@ -17708,7 +17437,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="10" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>11</v>
@@ -17739,13 +17468,13 @@
         <v>15</v>
       </c>
       <c r="C2" s="14" t="s">
+        <v>406</v>
+      </c>
+      <c r="D2" s="14" t="s">
         <v>407</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="E2" s="14" t="s">
         <v>408</v>
-      </c>
-      <c r="E2" s="14" t="s">
-        <v>409</v>
       </c>
       <c r="F2" s="121"/>
       <c r="G2" s="122"/>
@@ -17769,10 +17498,10 @@
         <v>51</v>
       </c>
       <c r="D3" s="6" t="s">
+        <v>409</v>
+      </c>
+      <c r="E3" s="6" t="s">
         <v>410</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>411</v>
       </c>
       <c r="F3" s="13"/>
       <c r="G3" s="3"/>
@@ -17794,10 +17523,10 @@
         <v>37</v>
       </c>
       <c r="D4" s="52" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="E4" s="130" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="F4" s="13"/>
       <c r="G4" s="3"/>
@@ -17946,7 +17675,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="10" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>11</v>
@@ -18217,16 +17946,16 @@
         <v>15</v>
       </c>
       <c r="C2" s="14" t="s">
+        <v>413</v>
+      </c>
+      <c r="D2" s="14" t="s">
         <v>414</v>
       </c>
-      <c r="D2" s="14" t="s">
-        <v>415</v>
-      </c>
       <c r="E2" s="14" t="s">
+        <v>407</v>
+      </c>
+      <c r="F2" s="14" t="s">
         <v>408</v>
-      </c>
-      <c r="F2" s="14" t="s">
-        <v>409</v>
       </c>
       <c r="G2" s="15"/>
       <c r="H2" s="16"/>
@@ -18492,10 +18221,10 @@
         <v>107</v>
       </c>
       <c r="E3" s="6" t="s">
+        <v>409</v>
+      </c>
+      <c r="F3" s="6" t="s">
         <v>410</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>411</v>
       </c>
       <c r="G3" s="17"/>
       <c r="H3" s="16"/>
@@ -18759,10 +18488,10 @@
         <v>59</v>
       </c>
       <c r="E4" s="132" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="F4" s="130" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="G4" s="13"/>
       <c r="H4" s="3"/>
@@ -19026,10 +18755,10 @@
         <v>62</v>
       </c>
       <c r="E5" s="134" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="F5" s="130" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="G5" s="13"/>
       <c r="H5" s="3"/>
@@ -19293,10 +19022,10 @@
         <v>64</v>
       </c>
       <c r="E6" s="134" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="F6" s="130" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="G6" s="13"/>
       <c r="H6" s="3"/>
@@ -19560,10 +19289,10 @@
         <v>66</v>
       </c>
       <c r="E7" s="134" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="F7" s="130" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="G7" s="13"/>
       <c r="H7" s="3"/>
@@ -19827,10 +19556,10 @@
         <v>68</v>
       </c>
       <c r="E8" s="134" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="F8" s="130" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="G8" s="13"/>
       <c r="H8" s="3"/>
@@ -20094,10 +19823,10 @@
         <v>71</v>
       </c>
       <c r="E9" s="134" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="F9" s="130" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="G9" s="13"/>
       <c r="H9" s="3"/>
@@ -20361,10 +20090,10 @@
         <v>75</v>
       </c>
       <c r="E10" s="134" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="F10" s="130" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="G10" s="13"/>
       <c r="H10" s="3"/>
@@ -20628,10 +20357,10 @@
         <v>80</v>
       </c>
       <c r="E11" s="134" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="F11" s="130" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="G11" s="13"/>
       <c r="H11" s="3"/>
@@ -20895,10 +20624,10 @@
         <v>83</v>
       </c>
       <c r="E12" s="136" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="F12" s="130" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="G12" s="13"/>
       <c r="H12" s="3"/>
@@ -21162,10 +20891,10 @@
         <v>84</v>
       </c>
       <c r="E13" s="132" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="F13" s="130" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="G13" s="13"/>
       <c r="H13" s="3"/>
@@ -21429,10 +21158,10 @@
         <v>86</v>
       </c>
       <c r="E14" s="134" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="F14" s="130" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="G14" s="13"/>
       <c r="H14" s="3"/>
@@ -21696,10 +21425,10 @@
         <v>88</v>
       </c>
       <c r="E15" s="134" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="F15" s="130" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="G15" s="13"/>
       <c r="H15" s="3"/>
@@ -21963,10 +21692,10 @@
         <v>90</v>
       </c>
       <c r="E16" s="134" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="F16" s="130" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="G16" s="13"/>
       <c r="H16" s="3"/>
@@ -22230,10 +21959,10 @@
         <v>92</v>
       </c>
       <c r="E17" s="134" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="F17" s="130" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="G17" s="13"/>
       <c r="H17" s="3"/>
@@ -22516,7 +22245,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="10" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>11</v>
@@ -22547,16 +22276,16 @@
         <v>15</v>
       </c>
       <c r="C2" s="14" t="s">
+        <v>406</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>416</v>
+      </c>
+      <c r="E2" s="14" t="s">
         <v>407</v>
       </c>
-      <c r="D2" s="14" t="s">
-        <v>417</v>
-      </c>
-      <c r="E2" s="14" t="s">
+      <c r="F2" s="14" t="s">
         <v>408</v>
-      </c>
-      <c r="F2" s="14" t="s">
-        <v>409</v>
       </c>
       <c r="G2" s="21"/>
       <c r="H2" s="22"/>
@@ -22582,10 +22311,10 @@
         <v>201</v>
       </c>
       <c r="E3" s="94" t="s">
+        <v>409</v>
+      </c>
+      <c r="F3" s="94" t="s">
         <v>410</v>
-      </c>
-      <c r="F3" s="94" t="s">
-        <v>411</v>
       </c>
       <c r="G3" s="95"/>
       <c r="H3" s="22"/>
@@ -22609,10 +22338,10 @@
         <v>154</v>
       </c>
       <c r="E4" s="139" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="F4" s="130" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="G4" s="13"/>
       <c r="H4" s="3"/>
@@ -22636,10 +22365,10 @@
         <v>158</v>
       </c>
       <c r="E5" s="141" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="F5" s="130" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="G5" s="13"/>
       <c r="H5" s="3"/>
@@ -22663,10 +22392,10 @@
         <v>162</v>
       </c>
       <c r="E6" s="141" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="F6" s="130" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="G6" s="13"/>
       <c r="H6" s="3"/>
@@ -22690,10 +22419,10 @@
         <v>166</v>
       </c>
       <c r="E7" s="141" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="F7" s="130" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="G7" s="13"/>
       <c r="H7" s="3"/>
@@ -22717,10 +22446,10 @@
         <v>173</v>
       </c>
       <c r="E8" s="141" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="F8" s="130" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="G8" s="13"/>
       <c r="H8" s="3"/>
@@ -22744,10 +22473,10 @@
         <v>169</v>
       </c>
       <c r="E9" s="141" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="F9" s="130" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="G9" s="13"/>
       <c r="H9" s="3"/>
@@ -22771,10 +22500,10 @@
         <v>177</v>
       </c>
       <c r="E10" s="141" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="F10" s="130" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="G10" s="13"/>
       <c r="H10" s="3"/>
@@ -22798,10 +22527,10 @@
         <v>184</v>
       </c>
       <c r="E11" s="141" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="F11" s="130" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="G11" s="13"/>
       <c r="H11" s="3"/>
@@ -22825,10 +22554,10 @@
         <v>187</v>
       </c>
       <c r="E12" s="141" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="F12" s="130" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="G12" s="13"/>
       <c r="H12" s="3"/>
@@ -22905,7 +22634,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="10" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>11</v>
@@ -22937,16 +22666,16 @@
         <v>15</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="E2" s="14" t="s">
+        <v>407</v>
+      </c>
+      <c r="F2" s="14" t="s">
         <v>408</v>
-      </c>
-      <c r="F2" s="14" t="s">
-        <v>409</v>
       </c>
       <c r="G2" s="21"/>
       <c r="H2" s="22"/>
@@ -22970,13 +22699,13 @@
         <v>51</v>
       </c>
       <c r="D3" s="94" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="E3" s="94" t="s">
+        <v>409</v>
+      </c>
+      <c r="F3" s="94" t="s">
         <v>410</v>
-      </c>
-      <c r="F3" s="94" t="s">
-        <v>411</v>
       </c>
       <c r="G3" s="95"/>
       <c r="H3" s="96"/>
@@ -23001,10 +22730,10 @@
         <v>126</v>
       </c>
       <c r="E4" s="52" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="F4" s="130" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="G4" s="13"/>
       <c r="H4" s="3"/>
@@ -23397,7 +23126,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="10" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>11</v>
@@ -23664,19 +23393,19 @@
       <c r="A2" s="123"/>
       <c r="B2" s="123"/>
       <c r="C2" s="14" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="D2" s="14" t="s">
+        <v>421</v>
+      </c>
+      <c r="E2" s="14" t="s">
         <v>422</v>
       </c>
-      <c r="E2" s="14" t="s">
-        <v>423</v>
-      </c>
       <c r="F2" s="14" t="s">
+        <v>407</v>
+      </c>
+      <c r="G2" s="14" t="s">
         <v>408</v>
-      </c>
-      <c r="G2" s="14" t="s">
-        <v>409</v>
       </c>
       <c r="H2" s="80"/>
       <c r="I2" s="32"/>
@@ -23944,10 +23673,10 @@
         <v>224</v>
       </c>
       <c r="F3" s="94" t="s">
+        <v>409</v>
+      </c>
+      <c r="G3" s="94" t="s">
         <v>410</v>
-      </c>
-      <c r="G3" s="94" t="s">
-        <v>411</v>
       </c>
       <c r="H3" s="80"/>
       <c r="I3" s="32"/>
@@ -24210,13 +23939,13 @@
         <v>75</v>
       </c>
       <c r="E4" s="126" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="F4" s="52" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="G4" s="130" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="H4" s="80"/>
       <c r="I4" s="32"/>
@@ -24479,13 +24208,13 @@
         <v>75</v>
       </c>
       <c r="E5" s="127" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="F5" s="52" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="G5" s="130" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="H5" s="80"/>
       <c r="I5" s="32"/>
@@ -24751,10 +24480,10 @@
         <v>306</v>
       </c>
       <c r="F6" s="52" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="G6" s="130" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="H6" s="80"/>
       <c r="I6" s="32"/>
@@ -25017,13 +24746,13 @@
         <v>75</v>
       </c>
       <c r="E7" s="127" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="F7" s="52" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="G7" s="130" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="H7" s="80"/>
       <c r="I7" s="32"/>
@@ -25286,13 +25015,13 @@
         <v>75</v>
       </c>
       <c r="E8" s="127" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="F8" s="52" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="G8" s="130" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="H8" s="80"/>
       <c r="I8" s="32"/>
@@ -25558,10 +25287,10 @@
         <v>312</v>
       </c>
       <c r="F9" s="52" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="G9" s="130" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="H9" s="80"/>
       <c r="I9" s="32"/>
@@ -25827,10 +25556,10 @@
         <v>315</v>
       </c>
       <c r="F10" s="52" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="G10" s="130" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="H10" s="80"/>
       <c r="I10" s="32"/>
@@ -26093,13 +25822,13 @@
         <v>75</v>
       </c>
       <c r="E11" s="127" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="F11" s="52" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="G11" s="130" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="H11" s="80"/>
       <c r="I11" s="32"/>
@@ -26362,13 +26091,13 @@
         <v>75</v>
       </c>
       <c r="E12" s="127" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="F12" s="52" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="G12" s="130" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="H12" s="80"/>
       <c r="I12" s="32"/>
@@ -26631,13 +26360,13 @@
         <v>75</v>
       </c>
       <c r="E13" s="127" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="F13" s="52" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="G13" s="130" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="H13" s="80"/>
       <c r="I13" s="32"/>
@@ -26900,13 +26629,13 @@
         <v>75</v>
       </c>
       <c r="E14" s="127" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="F14" s="52" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="G14" s="130" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="H14" s="80"/>
       <c r="I14" s="32"/>
@@ -27169,13 +26898,13 @@
         <v>75</v>
       </c>
       <c r="E15" s="127" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="F15" s="52" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="G15" s="130" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="H15" s="80"/>
       <c r="I15" s="32"/>
@@ -27441,10 +27170,10 @@
         <v>268</v>
       </c>
       <c r="F16" s="52" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="G16" s="130" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="H16" s="80"/>
       <c r="I16" s="32"/>
@@ -27710,10 +27439,10 @@
         <v>263</v>
       </c>
       <c r="F17" s="52" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="G17" s="130" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="H17" s="80"/>
       <c r="I17" s="32"/>
@@ -27976,13 +27705,13 @@
         <v>75</v>
       </c>
       <c r="E18" s="127" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="F18" s="52" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="G18" s="130" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="H18" s="80"/>
       <c r="I18" s="32"/>
@@ -28245,13 +27974,13 @@
         <v>75</v>
       </c>
       <c r="E19" s="127" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="F19" s="52" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="G19" s="130" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="H19" s="80"/>
       <c r="I19" s="32"/>
@@ -28514,13 +28243,13 @@
         <v>75</v>
       </c>
       <c r="E20" s="127" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="F20" s="52" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="G20" s="130" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="H20" s="80"/>
       <c r="I20" s="32"/>
@@ -28783,13 +28512,13 @@
         <v>75</v>
       </c>
       <c r="E21" s="127" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="F21" s="52" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="G21" s="130" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="H21" s="80"/>
       <c r="I21" s="32"/>
@@ -29052,13 +28781,13 @@
         <v>75</v>
       </c>
       <c r="E22" s="128" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="F22" s="52" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="G22" s="130" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="H22" s="80"/>
       <c r="I22" s="32"/>
@@ -29321,13 +29050,13 @@
         <v>80</v>
       </c>
       <c r="E23" s="126" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="F23" s="52" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="G23" s="130" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="H23" s="80"/>
       <c r="I23" s="32"/>
@@ -29590,13 +29319,13 @@
         <v>80</v>
       </c>
       <c r="E24" s="127" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="F24" s="52" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="G24" s="130" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="H24" s="80"/>
       <c r="I24" s="32"/>
@@ -29859,13 +29588,13 @@
         <v>80</v>
       </c>
       <c r="E25" s="127" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="F25" s="52" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="G25" s="130" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="H25" s="80"/>
       <c r="I25" s="32"/>
@@ -30128,13 +29857,13 @@
         <v>80</v>
       </c>
       <c r="E26" s="127" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="F26" s="52" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="G26" s="130" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="H26" s="80"/>
       <c r="I26" s="32"/>
@@ -30397,13 +30126,13 @@
         <v>80</v>
       </c>
       <c r="E27" s="127" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="F27" s="52" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="G27" s="130" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="H27" s="80"/>
       <c r="I27" s="32"/>
@@ -30666,13 +30395,13 @@
         <v>80</v>
       </c>
       <c r="E28" s="127" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="F28" s="52" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="G28" s="130" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="H28" s="80"/>
       <c r="I28" s="32"/>
@@ -30935,13 +30664,13 @@
         <v>80</v>
       </c>
       <c r="E29" s="127" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="F29" s="52" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="G29" s="130" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="H29" s="80"/>
       <c r="I29" s="32"/>
@@ -31204,13 +30933,13 @@
         <v>80</v>
       </c>
       <c r="E30" s="127" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="F30" s="52" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="G30" s="130" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="H30" s="145"/>
       <c r="I30" s="91"/>

</xml_diff>

<commit_message>
EM-1800: Alter headings for watermark image fields so that they are more intuitive
</commit_message>
<xml_diff>
--- a/src/aat/resources/adv_bundling_functional_tests_ccd_def.xlsx
+++ b/src/aat/resources/adv_bundling_functional_tests_ccd_def.xlsx
@@ -974,13 +974,13 @@
     <t>opaque</t>
   </si>
   <si>
-    <t>Opaque( e.g. HMCTS logo)</t>
+    <t>Opaque</t>
   </si>
   <si>
     <t>translucent</t>
   </si>
   <si>
-    <t>Translucent(e.g. watermark, court seal etc.)</t>
+    <t>Translucent</t>
   </si>
   <si>
     <t>imageRenderingLocation</t>
@@ -989,13 +989,13 @@
     <t>allPages</t>
   </si>
   <si>
-    <t>Image at all Pages</t>
+    <t>Image on all pages of the Document</t>
   </si>
   <si>
     <t>firstPage</t>
   </si>
   <si>
-    <t>Image at First Page of each document</t>
+    <t>Image on the First Page of each document</t>
   </si>
   <si>
     <t>ComplexTypes</t>
@@ -1097,7 +1097,7 @@
     <t>docmosisAssetId</t>
   </si>
   <si>
-    <t>Enter the image location</t>
+    <t>The filename of the Image you wish to embed</t>
   </si>
   <si>
     <t>coordinateX</t>
@@ -38164,7 +38164,7 @@
     </row>
     <row r="4" ht="14" customHeight="1">
       <c r="A4" s="18">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B4" s="24"/>
       <c r="C4" t="s" s="62">

</xml_diff>

<commit_message>
EM-2625: Make changes to spreadsheet and remove logging
</commit_message>
<xml_diff>
--- a/src/aat/resources/adv_bundling_functional_tests_ccd_def.xlsx
+++ b/src/aat/resources/adv_bundling_functional_tests_ccd_def.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="426">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="427">
   <si>
     <t>Change History</t>
   </si>
@@ -1185,6 +1185,9 @@
   </si>
   <si>
     <t>Name of the PDF</t>
+  </si>
+  <si>
+    <t>fileNameIdentifier</t>
   </si>
   <si>
     <t>Pagination Style</t>
@@ -3768,7 +3771,7 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:IU50"/>
+  <dimension ref="A1:IU51"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -13512,27 +13515,27 @@
       <c r="IU36" s="84"/>
     </row>
     <row r="37" ht="13.75" customHeight="1">
-      <c r="A37" s="107">
+      <c r="A37" s="106">
         <v>42736</v>
       </c>
-      <c r="B37" s="5"/>
-      <c r="C37" t="s" s="41">
+      <c r="B37" s="3"/>
+      <c r="C37" t="s" s="35">
         <v>79</v>
       </c>
-      <c r="D37" t="s" s="41">
+      <c r="D37" t="s" s="35">
         <v>356</v>
       </c>
-      <c r="E37" t="s" s="41">
+      <c r="E37" t="s" s="35">
         <v>61</v>
       </c>
-      <c r="F37" s="5"/>
-      <c r="G37" t="s" s="41">
+      <c r="F37" s="3"/>
+      <c r="G37" t="s" s="35">
         <v>357</v>
       </c>
-      <c r="H37" s="5"/>
-      <c r="I37" s="5"/>
-      <c r="J37" s="5"/>
-      <c r="K37" t="s" s="104">
+      <c r="H37" s="3"/>
+      <c r="I37" s="3"/>
+      <c r="J37" s="3"/>
+      <c r="K37" t="s" s="71">
         <v>40</v>
       </c>
       <c r="L37" s="14"/>
@@ -13781,29 +13784,27 @@
       <c r="IU37" s="84"/>
     </row>
     <row r="38" ht="13.75" customHeight="1">
-      <c r="A38" s="108">
+      <c r="A38" s="107">
         <v>42736</v>
       </c>
-      <c r="B38" s="47"/>
-      <c r="C38" t="s" s="48">
+      <c r="B38" s="5"/>
+      <c r="C38" t="s" s="41">
         <v>79</v>
       </c>
-      <c r="D38" t="s" s="48">
-        <v>272</v>
-      </c>
-      <c r="E38" t="s" s="48">
-        <v>73</v>
-      </c>
-      <c r="F38" t="s" s="48">
-        <v>272</v>
-      </c>
-      <c r="G38" t="s" s="48">
+      <c r="D38" t="s" s="41">
         <v>358</v>
       </c>
-      <c r="H38" s="47"/>
-      <c r="I38" s="47"/>
-      <c r="J38" s="47"/>
-      <c r="K38" t="s" s="109">
+      <c r="E38" t="s" s="41">
+        <v>61</v>
+      </c>
+      <c r="F38" s="5"/>
+      <c r="G38" t="s" s="41">
+        <v>357</v>
+      </c>
+      <c r="H38" s="5"/>
+      <c r="I38" s="5"/>
+      <c r="J38" s="5"/>
+      <c r="K38" t="s" s="104">
         <v>40</v>
       </c>
       <c r="L38" s="14"/>
@@ -14060,14 +14061,16 @@
         <v>79</v>
       </c>
       <c r="D39" t="s" s="48">
+        <v>272</v>
+      </c>
+      <c r="E39" t="s" s="48">
+        <v>73</v>
+      </c>
+      <c r="F39" t="s" s="48">
+        <v>272</v>
+      </c>
+      <c r="G39" t="s" s="48">
         <v>359</v>
-      </c>
-      <c r="E39" t="s" s="48">
-        <v>61</v>
-      </c>
-      <c r="F39" s="48"/>
-      <c r="G39" t="s" s="48">
-        <v>360</v>
       </c>
       <c r="H39" s="47"/>
       <c r="I39" s="47"/>
@@ -14329,14 +14332,12 @@
         <v>79</v>
       </c>
       <c r="D40" t="s" s="48">
-        <v>267</v>
+        <v>360</v>
       </c>
       <c r="E40" t="s" s="48">
-        <v>73</v>
-      </c>
-      <c r="F40" t="s" s="48">
-        <v>267</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="F40" s="48"/>
       <c r="G40" t="s" s="48">
         <v>361</v>
       </c>
@@ -14600,14 +14601,16 @@
         <v>79</v>
       </c>
       <c r="D41" t="s" s="48">
+        <v>267</v>
+      </c>
+      <c r="E41" t="s" s="48">
+        <v>73</v>
+      </c>
+      <c r="F41" t="s" s="48">
+        <v>267</v>
+      </c>
+      <c r="G41" t="s" s="48">
         <v>362</v>
-      </c>
-      <c r="E41" t="s" s="48">
-        <v>338</v>
-      </c>
-      <c r="F41" s="48"/>
-      <c r="G41" t="s" s="48">
-        <v>363</v>
       </c>
       <c r="H41" s="47"/>
       <c r="I41" s="47"/>
@@ -14869,16 +14872,14 @@
         <v>79</v>
       </c>
       <c r="D42" t="s" s="48">
+        <v>363</v>
+      </c>
+      <c r="E42" t="s" s="48">
+        <v>338</v>
+      </c>
+      <c r="F42" s="48"/>
+      <c r="G42" t="s" s="48">
         <v>364</v>
-      </c>
-      <c r="E42" t="s" s="48">
-        <v>323</v>
-      </c>
-      <c r="F42" t="s" s="48">
-        <v>323</v>
-      </c>
-      <c r="G42" t="s" s="48">
-        <v>365</v>
       </c>
       <c r="H42" s="47"/>
       <c r="I42" s="47"/>
@@ -15132,27 +15133,29 @@
       <c r="IU42" s="84"/>
     </row>
     <row r="43" ht="13.75" customHeight="1">
-      <c r="A43" s="105">
+      <c r="A43" s="108">
         <v>42736</v>
       </c>
-      <c r="B43" s="24"/>
-      <c r="C43" t="s" s="8">
-        <v>82</v>
-      </c>
-      <c r="D43" t="s" s="8">
+      <c r="B43" s="47"/>
+      <c r="C43" t="s" s="48">
+        <v>79</v>
+      </c>
+      <c r="D43" t="s" s="48">
+        <v>365</v>
+      </c>
+      <c r="E43" t="s" s="48">
+        <v>323</v>
+      </c>
+      <c r="F43" t="s" s="48">
+        <v>323</v>
+      </c>
+      <c r="G43" t="s" s="48">
         <v>366</v>
       </c>
-      <c r="E43" t="s" s="8">
-        <v>61</v>
-      </c>
-      <c r="F43" s="24"/>
-      <c r="G43" t="s" s="8">
-        <v>367</v>
-      </c>
-      <c r="H43" s="24"/>
-      <c r="I43" s="24"/>
-      <c r="J43" s="24"/>
-      <c r="K43" t="s" s="62">
+      <c r="H43" s="47"/>
+      <c r="I43" s="47"/>
+      <c r="J43" s="47"/>
+      <c r="K43" t="s" s="109">
         <v>40</v>
       </c>
       <c r="L43" s="14"/>
@@ -15401,27 +15404,27 @@
       <c r="IU43" s="84"/>
     </row>
     <row r="44" ht="13.75" customHeight="1">
-      <c r="A44" s="106">
+      <c r="A44" s="105">
         <v>42736</v>
       </c>
-      <c r="B44" s="3"/>
-      <c r="C44" t="s" s="35">
+      <c r="B44" s="24"/>
+      <c r="C44" t="s" s="8">
         <v>82</v>
       </c>
-      <c r="D44" t="s" s="35">
+      <c r="D44" t="s" s="8">
+        <v>367</v>
+      </c>
+      <c r="E44" t="s" s="8">
+        <v>61</v>
+      </c>
+      <c r="F44" s="24"/>
+      <c r="G44" t="s" s="8">
         <v>368</v>
       </c>
-      <c r="E44" t="s" s="35">
-        <v>61</v>
-      </c>
-      <c r="F44" s="3"/>
-      <c r="G44" t="s" s="35">
-        <v>369</v>
-      </c>
-      <c r="H44" s="3"/>
-      <c r="I44" s="3"/>
-      <c r="J44" s="3"/>
-      <c r="K44" t="s" s="71">
+      <c r="H44" s="24"/>
+      <c r="I44" s="24"/>
+      <c r="J44" s="24"/>
+      <c r="K44" t="s" s="62">
         <v>40</v>
       </c>
       <c r="L44" s="14"/>
@@ -15678,14 +15681,14 @@
         <v>82</v>
       </c>
       <c r="D45" t="s" s="35">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="E45" t="s" s="35">
-        <v>312</v>
+        <v>61</v>
       </c>
       <c r="F45" s="3"/>
       <c r="G45" t="s" s="35">
-        <v>312</v>
+        <v>370</v>
       </c>
       <c r="H45" s="3"/>
       <c r="I45" s="3"/>
@@ -15950,11 +15953,11 @@
         <v>371</v>
       </c>
       <c r="E46" t="s" s="35">
-        <v>372</v>
+        <v>312</v>
       </c>
       <c r="F46" s="3"/>
       <c r="G46" t="s" s="35">
-        <v>373</v>
+        <v>312</v>
       </c>
       <c r="H46" s="3"/>
       <c r="I46" s="3"/>
@@ -16216,14 +16219,14 @@
         <v>82</v>
       </c>
       <c r="D47" t="s" s="35">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="E47" t="s" s="35">
-        <v>61</v>
+        <v>373</v>
       </c>
       <c r="F47" s="3"/>
       <c r="G47" t="s" s="35">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="H47" s="3"/>
       <c r="I47" s="3"/>
@@ -16233,251 +16236,251 @@
       </c>
       <c r="L47" s="14"/>
       <c r="M47" s="3"/>
-      <c r="N47" s="93"/>
-      <c r="O47" s="94"/>
-      <c r="P47" s="94"/>
-      <c r="Q47" s="94"/>
-      <c r="R47" s="94"/>
-      <c r="S47" s="94"/>
-      <c r="T47" s="94"/>
-      <c r="U47" s="94"/>
-      <c r="V47" s="94"/>
-      <c r="W47" s="94"/>
-      <c r="X47" s="94"/>
-      <c r="Y47" s="94"/>
-      <c r="Z47" s="94"/>
-      <c r="AA47" s="94"/>
-      <c r="AB47" s="94"/>
-      <c r="AC47" s="94"/>
-      <c r="AD47" s="94"/>
-      <c r="AE47" s="94"/>
-      <c r="AF47" s="94"/>
-      <c r="AG47" s="94"/>
-      <c r="AH47" s="94"/>
-      <c r="AI47" s="94"/>
-      <c r="AJ47" s="94"/>
-      <c r="AK47" s="94"/>
-      <c r="AL47" s="94"/>
-      <c r="AM47" s="94"/>
-      <c r="AN47" s="94"/>
-      <c r="AO47" s="94"/>
-      <c r="AP47" s="94"/>
-      <c r="AQ47" s="94"/>
-      <c r="AR47" s="94"/>
-      <c r="AS47" s="94"/>
-      <c r="AT47" s="94"/>
-      <c r="AU47" s="94"/>
-      <c r="AV47" s="94"/>
-      <c r="AW47" s="94"/>
-      <c r="AX47" s="94"/>
-      <c r="AY47" s="94"/>
-      <c r="AZ47" s="94"/>
-      <c r="BA47" s="94"/>
-      <c r="BB47" s="94"/>
-      <c r="BC47" s="94"/>
-      <c r="BD47" s="94"/>
-      <c r="BE47" s="94"/>
-      <c r="BF47" s="94"/>
-      <c r="BG47" s="94"/>
-      <c r="BH47" s="94"/>
-      <c r="BI47" s="94"/>
-      <c r="BJ47" s="94"/>
-      <c r="BK47" s="94"/>
-      <c r="BL47" s="94"/>
-      <c r="BM47" s="94"/>
-      <c r="BN47" s="94"/>
-      <c r="BO47" s="94"/>
-      <c r="BP47" s="94"/>
-      <c r="BQ47" s="94"/>
-      <c r="BR47" s="94"/>
-      <c r="BS47" s="94"/>
-      <c r="BT47" s="94"/>
-      <c r="BU47" s="94"/>
-      <c r="BV47" s="94"/>
-      <c r="BW47" s="94"/>
-      <c r="BX47" s="94"/>
-      <c r="BY47" s="94"/>
-      <c r="BZ47" s="94"/>
-      <c r="CA47" s="94"/>
-      <c r="CB47" s="94"/>
-      <c r="CC47" s="94"/>
-      <c r="CD47" s="94"/>
-      <c r="CE47" s="94"/>
-      <c r="CF47" s="94"/>
-      <c r="CG47" s="94"/>
-      <c r="CH47" s="94"/>
-      <c r="CI47" s="94"/>
-      <c r="CJ47" s="94"/>
-      <c r="CK47" s="94"/>
-      <c r="CL47" s="94"/>
-      <c r="CM47" s="94"/>
-      <c r="CN47" s="94"/>
-      <c r="CO47" s="94"/>
-      <c r="CP47" s="94"/>
-      <c r="CQ47" s="94"/>
-      <c r="CR47" s="94"/>
-      <c r="CS47" s="94"/>
-      <c r="CT47" s="94"/>
-      <c r="CU47" s="94"/>
-      <c r="CV47" s="94"/>
-      <c r="CW47" s="94"/>
-      <c r="CX47" s="94"/>
-      <c r="CY47" s="94"/>
-      <c r="CZ47" s="94"/>
-      <c r="DA47" s="94"/>
-      <c r="DB47" s="94"/>
-      <c r="DC47" s="94"/>
-      <c r="DD47" s="94"/>
-      <c r="DE47" s="94"/>
-      <c r="DF47" s="94"/>
-      <c r="DG47" s="94"/>
-      <c r="DH47" s="94"/>
-      <c r="DI47" s="94"/>
-      <c r="DJ47" s="94"/>
-      <c r="DK47" s="94"/>
-      <c r="DL47" s="94"/>
-      <c r="DM47" s="94"/>
-      <c r="DN47" s="94"/>
-      <c r="DO47" s="94"/>
-      <c r="DP47" s="94"/>
-      <c r="DQ47" s="94"/>
-      <c r="DR47" s="94"/>
-      <c r="DS47" s="94"/>
-      <c r="DT47" s="94"/>
-      <c r="DU47" s="94"/>
-      <c r="DV47" s="94"/>
-      <c r="DW47" s="94"/>
-      <c r="DX47" s="94"/>
-      <c r="DY47" s="94"/>
-      <c r="DZ47" s="94"/>
-      <c r="EA47" s="94"/>
-      <c r="EB47" s="94"/>
-      <c r="EC47" s="94"/>
-      <c r="ED47" s="94"/>
-      <c r="EE47" s="94"/>
-      <c r="EF47" s="94"/>
-      <c r="EG47" s="94"/>
-      <c r="EH47" s="94"/>
-      <c r="EI47" s="94"/>
-      <c r="EJ47" s="94"/>
-      <c r="EK47" s="94"/>
-      <c r="EL47" s="94"/>
-      <c r="EM47" s="94"/>
-      <c r="EN47" s="94"/>
-      <c r="EO47" s="94"/>
-      <c r="EP47" s="94"/>
-      <c r="EQ47" s="94"/>
-      <c r="ER47" s="94"/>
-      <c r="ES47" s="94"/>
-      <c r="ET47" s="94"/>
-      <c r="EU47" s="94"/>
-      <c r="EV47" s="94"/>
-      <c r="EW47" s="94"/>
-      <c r="EX47" s="94"/>
-      <c r="EY47" s="94"/>
-      <c r="EZ47" s="94"/>
-      <c r="FA47" s="94"/>
-      <c r="FB47" s="94"/>
-      <c r="FC47" s="94"/>
-      <c r="FD47" s="94"/>
-      <c r="FE47" s="94"/>
-      <c r="FF47" s="94"/>
-      <c r="FG47" s="94"/>
-      <c r="FH47" s="94"/>
-      <c r="FI47" s="94"/>
-      <c r="FJ47" s="94"/>
-      <c r="FK47" s="94"/>
-      <c r="FL47" s="94"/>
-      <c r="FM47" s="94"/>
-      <c r="FN47" s="94"/>
-      <c r="FO47" s="94"/>
-      <c r="FP47" s="94"/>
-      <c r="FQ47" s="94"/>
-      <c r="FR47" s="94"/>
-      <c r="FS47" s="94"/>
-      <c r="FT47" s="94"/>
-      <c r="FU47" s="94"/>
-      <c r="FV47" s="94"/>
-      <c r="FW47" s="94"/>
-      <c r="FX47" s="94"/>
-      <c r="FY47" s="94"/>
-      <c r="FZ47" s="94"/>
-      <c r="GA47" s="94"/>
-      <c r="GB47" s="94"/>
-      <c r="GC47" s="94"/>
-      <c r="GD47" s="94"/>
-      <c r="GE47" s="94"/>
-      <c r="GF47" s="94"/>
-      <c r="GG47" s="94"/>
-      <c r="GH47" s="94"/>
-      <c r="GI47" s="94"/>
-      <c r="GJ47" s="94"/>
-      <c r="GK47" s="94"/>
-      <c r="GL47" s="94"/>
-      <c r="GM47" s="94"/>
-      <c r="GN47" s="94"/>
-      <c r="GO47" s="94"/>
-      <c r="GP47" s="94"/>
-      <c r="GQ47" s="94"/>
-      <c r="GR47" s="94"/>
-      <c r="GS47" s="94"/>
-      <c r="GT47" s="94"/>
-      <c r="GU47" s="94"/>
-      <c r="GV47" s="94"/>
-      <c r="GW47" s="94"/>
-      <c r="GX47" s="94"/>
-      <c r="GY47" s="94"/>
-      <c r="GZ47" s="94"/>
-      <c r="HA47" s="94"/>
-      <c r="HB47" s="94"/>
-      <c r="HC47" s="94"/>
-      <c r="HD47" s="94"/>
-      <c r="HE47" s="94"/>
-      <c r="HF47" s="94"/>
-      <c r="HG47" s="94"/>
-      <c r="HH47" s="94"/>
-      <c r="HI47" s="94"/>
-      <c r="HJ47" s="94"/>
-      <c r="HK47" s="94"/>
-      <c r="HL47" s="94"/>
-      <c r="HM47" s="94"/>
-      <c r="HN47" s="94"/>
-      <c r="HO47" s="94"/>
-      <c r="HP47" s="94"/>
-      <c r="HQ47" s="94"/>
-      <c r="HR47" s="94"/>
-      <c r="HS47" s="94"/>
-      <c r="HT47" s="94"/>
-      <c r="HU47" s="94"/>
-      <c r="HV47" s="94"/>
-      <c r="HW47" s="94"/>
-      <c r="HX47" s="94"/>
-      <c r="HY47" s="94"/>
-      <c r="HZ47" s="94"/>
-      <c r="IA47" s="94"/>
-      <c r="IB47" s="94"/>
-      <c r="IC47" s="94"/>
-      <c r="ID47" s="94"/>
-      <c r="IE47" s="94"/>
-      <c r="IF47" s="94"/>
-      <c r="IG47" s="94"/>
-      <c r="IH47" s="94"/>
-      <c r="II47" s="94"/>
-      <c r="IJ47" s="94"/>
-      <c r="IK47" s="94"/>
-      <c r="IL47" s="94"/>
-      <c r="IM47" s="94"/>
-      <c r="IN47" s="94"/>
-      <c r="IO47" s="94"/>
-      <c r="IP47" s="94"/>
-      <c r="IQ47" s="94"/>
-      <c r="IR47" s="94"/>
-      <c r="IS47" s="94"/>
-      <c r="IT47" s="94"/>
-      <c r="IU47" s="95"/>
+      <c r="N47" s="87"/>
+      <c r="O47" s="33"/>
+      <c r="P47" s="33"/>
+      <c r="Q47" s="33"/>
+      <c r="R47" s="33"/>
+      <c r="S47" s="33"/>
+      <c r="T47" s="33"/>
+      <c r="U47" s="33"/>
+      <c r="V47" s="33"/>
+      <c r="W47" s="33"/>
+      <c r="X47" s="33"/>
+      <c r="Y47" s="33"/>
+      <c r="Z47" s="33"/>
+      <c r="AA47" s="33"/>
+      <c r="AB47" s="33"/>
+      <c r="AC47" s="33"/>
+      <c r="AD47" s="33"/>
+      <c r="AE47" s="33"/>
+      <c r="AF47" s="33"/>
+      <c r="AG47" s="33"/>
+      <c r="AH47" s="33"/>
+      <c r="AI47" s="33"/>
+      <c r="AJ47" s="33"/>
+      <c r="AK47" s="33"/>
+      <c r="AL47" s="33"/>
+      <c r="AM47" s="33"/>
+      <c r="AN47" s="33"/>
+      <c r="AO47" s="33"/>
+      <c r="AP47" s="33"/>
+      <c r="AQ47" s="33"/>
+      <c r="AR47" s="33"/>
+      <c r="AS47" s="33"/>
+      <c r="AT47" s="33"/>
+      <c r="AU47" s="33"/>
+      <c r="AV47" s="33"/>
+      <c r="AW47" s="33"/>
+      <c r="AX47" s="33"/>
+      <c r="AY47" s="33"/>
+      <c r="AZ47" s="33"/>
+      <c r="BA47" s="33"/>
+      <c r="BB47" s="33"/>
+      <c r="BC47" s="33"/>
+      <c r="BD47" s="33"/>
+      <c r="BE47" s="33"/>
+      <c r="BF47" s="33"/>
+      <c r="BG47" s="33"/>
+      <c r="BH47" s="33"/>
+      <c r="BI47" s="33"/>
+      <c r="BJ47" s="33"/>
+      <c r="BK47" s="33"/>
+      <c r="BL47" s="33"/>
+      <c r="BM47" s="33"/>
+      <c r="BN47" s="33"/>
+      <c r="BO47" s="33"/>
+      <c r="BP47" s="33"/>
+      <c r="BQ47" s="33"/>
+      <c r="BR47" s="33"/>
+      <c r="BS47" s="33"/>
+      <c r="BT47" s="33"/>
+      <c r="BU47" s="33"/>
+      <c r="BV47" s="33"/>
+      <c r="BW47" s="33"/>
+      <c r="BX47" s="33"/>
+      <c r="BY47" s="33"/>
+      <c r="BZ47" s="33"/>
+      <c r="CA47" s="33"/>
+      <c r="CB47" s="33"/>
+      <c r="CC47" s="33"/>
+      <c r="CD47" s="33"/>
+      <c r="CE47" s="33"/>
+      <c r="CF47" s="33"/>
+      <c r="CG47" s="33"/>
+      <c r="CH47" s="33"/>
+      <c r="CI47" s="33"/>
+      <c r="CJ47" s="33"/>
+      <c r="CK47" s="33"/>
+      <c r="CL47" s="33"/>
+      <c r="CM47" s="33"/>
+      <c r="CN47" s="33"/>
+      <c r="CO47" s="33"/>
+      <c r="CP47" s="33"/>
+      <c r="CQ47" s="33"/>
+      <c r="CR47" s="33"/>
+      <c r="CS47" s="33"/>
+      <c r="CT47" s="33"/>
+      <c r="CU47" s="33"/>
+      <c r="CV47" s="33"/>
+      <c r="CW47" s="33"/>
+      <c r="CX47" s="33"/>
+      <c r="CY47" s="33"/>
+      <c r="CZ47" s="33"/>
+      <c r="DA47" s="33"/>
+      <c r="DB47" s="33"/>
+      <c r="DC47" s="33"/>
+      <c r="DD47" s="33"/>
+      <c r="DE47" s="33"/>
+      <c r="DF47" s="33"/>
+      <c r="DG47" s="33"/>
+      <c r="DH47" s="33"/>
+      <c r="DI47" s="33"/>
+      <c r="DJ47" s="33"/>
+      <c r="DK47" s="33"/>
+      <c r="DL47" s="33"/>
+      <c r="DM47" s="33"/>
+      <c r="DN47" s="33"/>
+      <c r="DO47" s="33"/>
+      <c r="DP47" s="33"/>
+      <c r="DQ47" s="33"/>
+      <c r="DR47" s="33"/>
+      <c r="DS47" s="33"/>
+      <c r="DT47" s="33"/>
+      <c r="DU47" s="33"/>
+      <c r="DV47" s="33"/>
+      <c r="DW47" s="33"/>
+      <c r="DX47" s="33"/>
+      <c r="DY47" s="33"/>
+      <c r="DZ47" s="33"/>
+      <c r="EA47" s="33"/>
+      <c r="EB47" s="33"/>
+      <c r="EC47" s="33"/>
+      <c r="ED47" s="33"/>
+      <c r="EE47" s="33"/>
+      <c r="EF47" s="33"/>
+      <c r="EG47" s="33"/>
+      <c r="EH47" s="33"/>
+      <c r="EI47" s="33"/>
+      <c r="EJ47" s="33"/>
+      <c r="EK47" s="33"/>
+      <c r="EL47" s="33"/>
+      <c r="EM47" s="33"/>
+      <c r="EN47" s="33"/>
+      <c r="EO47" s="33"/>
+      <c r="EP47" s="33"/>
+      <c r="EQ47" s="33"/>
+      <c r="ER47" s="33"/>
+      <c r="ES47" s="33"/>
+      <c r="ET47" s="33"/>
+      <c r="EU47" s="33"/>
+      <c r="EV47" s="33"/>
+      <c r="EW47" s="33"/>
+      <c r="EX47" s="33"/>
+      <c r="EY47" s="33"/>
+      <c r="EZ47" s="33"/>
+      <c r="FA47" s="33"/>
+      <c r="FB47" s="33"/>
+      <c r="FC47" s="33"/>
+      <c r="FD47" s="33"/>
+      <c r="FE47" s="33"/>
+      <c r="FF47" s="33"/>
+      <c r="FG47" s="33"/>
+      <c r="FH47" s="33"/>
+      <c r="FI47" s="33"/>
+      <c r="FJ47" s="33"/>
+      <c r="FK47" s="33"/>
+      <c r="FL47" s="33"/>
+      <c r="FM47" s="33"/>
+      <c r="FN47" s="33"/>
+      <c r="FO47" s="33"/>
+      <c r="FP47" s="33"/>
+      <c r="FQ47" s="33"/>
+      <c r="FR47" s="33"/>
+      <c r="FS47" s="33"/>
+      <c r="FT47" s="33"/>
+      <c r="FU47" s="33"/>
+      <c r="FV47" s="33"/>
+      <c r="FW47" s="33"/>
+      <c r="FX47" s="33"/>
+      <c r="FY47" s="33"/>
+      <c r="FZ47" s="33"/>
+      <c r="GA47" s="33"/>
+      <c r="GB47" s="33"/>
+      <c r="GC47" s="33"/>
+      <c r="GD47" s="33"/>
+      <c r="GE47" s="33"/>
+      <c r="GF47" s="33"/>
+      <c r="GG47" s="33"/>
+      <c r="GH47" s="33"/>
+      <c r="GI47" s="33"/>
+      <c r="GJ47" s="33"/>
+      <c r="GK47" s="33"/>
+      <c r="GL47" s="33"/>
+      <c r="GM47" s="33"/>
+      <c r="GN47" s="33"/>
+      <c r="GO47" s="33"/>
+      <c r="GP47" s="33"/>
+      <c r="GQ47" s="33"/>
+      <c r="GR47" s="33"/>
+      <c r="GS47" s="33"/>
+      <c r="GT47" s="33"/>
+      <c r="GU47" s="33"/>
+      <c r="GV47" s="33"/>
+      <c r="GW47" s="33"/>
+      <c r="GX47" s="33"/>
+      <c r="GY47" s="33"/>
+      <c r="GZ47" s="33"/>
+      <c r="HA47" s="33"/>
+      <c r="HB47" s="33"/>
+      <c r="HC47" s="33"/>
+      <c r="HD47" s="33"/>
+      <c r="HE47" s="33"/>
+      <c r="HF47" s="33"/>
+      <c r="HG47" s="33"/>
+      <c r="HH47" s="33"/>
+      <c r="HI47" s="33"/>
+      <c r="HJ47" s="33"/>
+      <c r="HK47" s="33"/>
+      <c r="HL47" s="33"/>
+      <c r="HM47" s="33"/>
+      <c r="HN47" s="33"/>
+      <c r="HO47" s="33"/>
+      <c r="HP47" s="33"/>
+      <c r="HQ47" s="33"/>
+      <c r="HR47" s="33"/>
+      <c r="HS47" s="33"/>
+      <c r="HT47" s="33"/>
+      <c r="HU47" s="33"/>
+      <c r="HV47" s="33"/>
+      <c r="HW47" s="33"/>
+      <c r="HX47" s="33"/>
+      <c r="HY47" s="33"/>
+      <c r="HZ47" s="33"/>
+      <c r="IA47" s="33"/>
+      <c r="IB47" s="33"/>
+      <c r="IC47" s="33"/>
+      <c r="ID47" s="33"/>
+      <c r="IE47" s="33"/>
+      <c r="IF47" s="33"/>
+      <c r="IG47" s="33"/>
+      <c r="IH47" s="33"/>
+      <c r="II47" s="33"/>
+      <c r="IJ47" s="33"/>
+      <c r="IK47" s="33"/>
+      <c r="IL47" s="33"/>
+      <c r="IM47" s="33"/>
+      <c r="IN47" s="33"/>
+      <c r="IO47" s="33"/>
+      <c r="IP47" s="33"/>
+      <c r="IQ47" s="33"/>
+      <c r="IR47" s="33"/>
+      <c r="IS47" s="33"/>
+      <c r="IT47" s="33"/>
+      <c r="IU47" s="84"/>
     </row>
     <row r="48" ht="13.75" customHeight="1">
-      <c r="A48" s="30">
+      <c r="A48" s="106">
         <v>42736</v>
       </c>
       <c r="B48" s="3"/>
@@ -16485,265 +16488,265 @@
         <v>82</v>
       </c>
       <c r="D48" t="s" s="35">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E48" t="s" s="35">
-        <v>372</v>
+        <v>61</v>
       </c>
       <c r="F48" s="3"/>
       <c r="G48" t="s" s="35">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H48" s="3"/>
       <c r="I48" s="3"/>
       <c r="J48" s="3"/>
-      <c r="K48" t="s" s="35">
+      <c r="K48" t="s" s="71">
         <v>40</v>
       </c>
-      <c r="L48" s="3"/>
+      <c r="L48" s="14"/>
       <c r="M48" s="3"/>
-      <c r="N48" s="97"/>
-      <c r="O48" s="81"/>
-      <c r="P48" s="81"/>
-      <c r="Q48" s="81"/>
-      <c r="R48" s="81"/>
-      <c r="S48" s="81"/>
-      <c r="T48" s="81"/>
-      <c r="U48" s="81"/>
-      <c r="V48" s="81"/>
-      <c r="W48" s="81"/>
-      <c r="X48" s="81"/>
-      <c r="Y48" s="81"/>
-      <c r="Z48" s="81"/>
-      <c r="AA48" s="81"/>
-      <c r="AB48" s="81"/>
-      <c r="AC48" s="81"/>
-      <c r="AD48" s="81"/>
-      <c r="AE48" s="81"/>
-      <c r="AF48" s="81"/>
-      <c r="AG48" s="81"/>
-      <c r="AH48" s="81"/>
-      <c r="AI48" s="81"/>
-      <c r="AJ48" s="81"/>
-      <c r="AK48" s="81"/>
-      <c r="AL48" s="81"/>
-      <c r="AM48" s="81"/>
-      <c r="AN48" s="81"/>
-      <c r="AO48" s="81"/>
-      <c r="AP48" s="81"/>
-      <c r="AQ48" s="81"/>
-      <c r="AR48" s="81"/>
-      <c r="AS48" s="81"/>
-      <c r="AT48" s="81"/>
-      <c r="AU48" s="81"/>
-      <c r="AV48" s="81"/>
-      <c r="AW48" s="81"/>
-      <c r="AX48" s="81"/>
-      <c r="AY48" s="81"/>
-      <c r="AZ48" s="81"/>
-      <c r="BA48" s="81"/>
-      <c r="BB48" s="81"/>
-      <c r="BC48" s="81"/>
-      <c r="BD48" s="81"/>
-      <c r="BE48" s="81"/>
-      <c r="BF48" s="81"/>
-      <c r="BG48" s="81"/>
-      <c r="BH48" s="81"/>
-      <c r="BI48" s="81"/>
-      <c r="BJ48" s="81"/>
-      <c r="BK48" s="81"/>
-      <c r="BL48" s="81"/>
-      <c r="BM48" s="81"/>
-      <c r="BN48" s="81"/>
-      <c r="BO48" s="81"/>
-      <c r="BP48" s="81"/>
-      <c r="BQ48" s="81"/>
-      <c r="BR48" s="81"/>
-      <c r="BS48" s="81"/>
-      <c r="BT48" s="81"/>
-      <c r="BU48" s="81"/>
-      <c r="BV48" s="81"/>
-      <c r="BW48" s="81"/>
-      <c r="BX48" s="81"/>
-      <c r="BY48" s="81"/>
-      <c r="BZ48" s="81"/>
-      <c r="CA48" s="81"/>
-      <c r="CB48" s="81"/>
-      <c r="CC48" s="81"/>
-      <c r="CD48" s="81"/>
-      <c r="CE48" s="81"/>
-      <c r="CF48" s="81"/>
-      <c r="CG48" s="81"/>
-      <c r="CH48" s="81"/>
-      <c r="CI48" s="81"/>
-      <c r="CJ48" s="81"/>
-      <c r="CK48" s="81"/>
-      <c r="CL48" s="81"/>
-      <c r="CM48" s="81"/>
-      <c r="CN48" s="81"/>
-      <c r="CO48" s="81"/>
-      <c r="CP48" s="81"/>
-      <c r="CQ48" s="81"/>
-      <c r="CR48" s="81"/>
-      <c r="CS48" s="81"/>
-      <c r="CT48" s="81"/>
-      <c r="CU48" s="81"/>
-      <c r="CV48" s="81"/>
-      <c r="CW48" s="81"/>
-      <c r="CX48" s="81"/>
-      <c r="CY48" s="81"/>
-      <c r="CZ48" s="81"/>
-      <c r="DA48" s="81"/>
-      <c r="DB48" s="81"/>
-      <c r="DC48" s="81"/>
-      <c r="DD48" s="81"/>
-      <c r="DE48" s="81"/>
-      <c r="DF48" s="81"/>
-      <c r="DG48" s="81"/>
-      <c r="DH48" s="81"/>
-      <c r="DI48" s="81"/>
-      <c r="DJ48" s="81"/>
-      <c r="DK48" s="81"/>
-      <c r="DL48" s="81"/>
-      <c r="DM48" s="81"/>
-      <c r="DN48" s="81"/>
-      <c r="DO48" s="81"/>
-      <c r="DP48" s="81"/>
-      <c r="DQ48" s="81"/>
-      <c r="DR48" s="81"/>
-      <c r="DS48" s="81"/>
-      <c r="DT48" s="81"/>
-      <c r="DU48" s="81"/>
-      <c r="DV48" s="81"/>
-      <c r="DW48" s="81"/>
-      <c r="DX48" s="81"/>
-      <c r="DY48" s="81"/>
-      <c r="DZ48" s="81"/>
-      <c r="EA48" s="81"/>
-      <c r="EB48" s="81"/>
-      <c r="EC48" s="81"/>
-      <c r="ED48" s="81"/>
-      <c r="EE48" s="81"/>
-      <c r="EF48" s="81"/>
-      <c r="EG48" s="81"/>
-      <c r="EH48" s="81"/>
-      <c r="EI48" s="81"/>
-      <c r="EJ48" s="81"/>
-      <c r="EK48" s="81"/>
-      <c r="EL48" s="81"/>
-      <c r="EM48" s="81"/>
-      <c r="EN48" s="81"/>
-      <c r="EO48" s="81"/>
-      <c r="EP48" s="81"/>
-      <c r="EQ48" s="81"/>
-      <c r="ER48" s="81"/>
-      <c r="ES48" s="81"/>
-      <c r="ET48" s="81"/>
-      <c r="EU48" s="81"/>
-      <c r="EV48" s="81"/>
-      <c r="EW48" s="81"/>
-      <c r="EX48" s="81"/>
-      <c r="EY48" s="81"/>
-      <c r="EZ48" s="81"/>
-      <c r="FA48" s="81"/>
-      <c r="FB48" s="81"/>
-      <c r="FC48" s="81"/>
-      <c r="FD48" s="81"/>
-      <c r="FE48" s="81"/>
-      <c r="FF48" s="81"/>
-      <c r="FG48" s="81"/>
-      <c r="FH48" s="81"/>
-      <c r="FI48" s="81"/>
-      <c r="FJ48" s="81"/>
-      <c r="FK48" s="81"/>
-      <c r="FL48" s="81"/>
-      <c r="FM48" s="81"/>
-      <c r="FN48" s="81"/>
-      <c r="FO48" s="81"/>
-      <c r="FP48" s="81"/>
-      <c r="FQ48" s="81"/>
-      <c r="FR48" s="81"/>
-      <c r="FS48" s="81"/>
-      <c r="FT48" s="81"/>
-      <c r="FU48" s="81"/>
-      <c r="FV48" s="81"/>
-      <c r="FW48" s="81"/>
-      <c r="FX48" s="81"/>
-      <c r="FY48" s="81"/>
-      <c r="FZ48" s="81"/>
-      <c r="GA48" s="81"/>
-      <c r="GB48" s="81"/>
-      <c r="GC48" s="81"/>
-      <c r="GD48" s="81"/>
-      <c r="GE48" s="81"/>
-      <c r="GF48" s="81"/>
-      <c r="GG48" s="81"/>
-      <c r="GH48" s="81"/>
-      <c r="GI48" s="81"/>
-      <c r="GJ48" s="81"/>
-      <c r="GK48" s="81"/>
-      <c r="GL48" s="81"/>
-      <c r="GM48" s="81"/>
-      <c r="GN48" s="81"/>
-      <c r="GO48" s="81"/>
-      <c r="GP48" s="81"/>
-      <c r="GQ48" s="81"/>
-      <c r="GR48" s="81"/>
-      <c r="GS48" s="81"/>
-      <c r="GT48" s="81"/>
-      <c r="GU48" s="81"/>
-      <c r="GV48" s="81"/>
-      <c r="GW48" s="81"/>
-      <c r="GX48" s="81"/>
-      <c r="GY48" s="81"/>
-      <c r="GZ48" s="81"/>
-      <c r="HA48" s="81"/>
-      <c r="HB48" s="81"/>
-      <c r="HC48" s="81"/>
-      <c r="HD48" s="81"/>
-      <c r="HE48" s="81"/>
-      <c r="HF48" s="81"/>
-      <c r="HG48" s="81"/>
-      <c r="HH48" s="81"/>
-      <c r="HI48" s="81"/>
-      <c r="HJ48" s="81"/>
-      <c r="HK48" s="81"/>
-      <c r="HL48" s="81"/>
-      <c r="HM48" s="81"/>
-      <c r="HN48" s="81"/>
-      <c r="HO48" s="81"/>
-      <c r="HP48" s="81"/>
-      <c r="HQ48" s="81"/>
-      <c r="HR48" s="81"/>
-      <c r="HS48" s="81"/>
-      <c r="HT48" s="81"/>
-      <c r="HU48" s="81"/>
-      <c r="HV48" s="81"/>
-      <c r="HW48" s="81"/>
-      <c r="HX48" s="81"/>
-      <c r="HY48" s="81"/>
-      <c r="HZ48" s="81"/>
-      <c r="IA48" s="81"/>
-      <c r="IB48" s="81"/>
-      <c r="IC48" s="81"/>
-      <c r="ID48" s="81"/>
-      <c r="IE48" s="81"/>
-      <c r="IF48" s="81"/>
-      <c r="IG48" s="81"/>
-      <c r="IH48" s="81"/>
-      <c r="II48" s="81"/>
-      <c r="IJ48" s="81"/>
-      <c r="IK48" s="81"/>
-      <c r="IL48" s="81"/>
-      <c r="IM48" s="81"/>
-      <c r="IN48" s="81"/>
-      <c r="IO48" s="81"/>
-      <c r="IP48" s="81"/>
-      <c r="IQ48" s="81"/>
-      <c r="IR48" s="81"/>
-      <c r="IS48" s="81"/>
-      <c r="IT48" s="81"/>
-      <c r="IU48" s="82"/>
+      <c r="N48" s="93"/>
+      <c r="O48" s="94"/>
+      <c r="P48" s="94"/>
+      <c r="Q48" s="94"/>
+      <c r="R48" s="94"/>
+      <c r="S48" s="94"/>
+      <c r="T48" s="94"/>
+      <c r="U48" s="94"/>
+      <c r="V48" s="94"/>
+      <c r="W48" s="94"/>
+      <c r="X48" s="94"/>
+      <c r="Y48" s="94"/>
+      <c r="Z48" s="94"/>
+      <c r="AA48" s="94"/>
+      <c r="AB48" s="94"/>
+      <c r="AC48" s="94"/>
+      <c r="AD48" s="94"/>
+      <c r="AE48" s="94"/>
+      <c r="AF48" s="94"/>
+      <c r="AG48" s="94"/>
+      <c r="AH48" s="94"/>
+      <c r="AI48" s="94"/>
+      <c r="AJ48" s="94"/>
+      <c r="AK48" s="94"/>
+      <c r="AL48" s="94"/>
+      <c r="AM48" s="94"/>
+      <c r="AN48" s="94"/>
+      <c r="AO48" s="94"/>
+      <c r="AP48" s="94"/>
+      <c r="AQ48" s="94"/>
+      <c r="AR48" s="94"/>
+      <c r="AS48" s="94"/>
+      <c r="AT48" s="94"/>
+      <c r="AU48" s="94"/>
+      <c r="AV48" s="94"/>
+      <c r="AW48" s="94"/>
+      <c r="AX48" s="94"/>
+      <c r="AY48" s="94"/>
+      <c r="AZ48" s="94"/>
+      <c r="BA48" s="94"/>
+      <c r="BB48" s="94"/>
+      <c r="BC48" s="94"/>
+      <c r="BD48" s="94"/>
+      <c r="BE48" s="94"/>
+      <c r="BF48" s="94"/>
+      <c r="BG48" s="94"/>
+      <c r="BH48" s="94"/>
+      <c r="BI48" s="94"/>
+      <c r="BJ48" s="94"/>
+      <c r="BK48" s="94"/>
+      <c r="BL48" s="94"/>
+      <c r="BM48" s="94"/>
+      <c r="BN48" s="94"/>
+      <c r="BO48" s="94"/>
+      <c r="BP48" s="94"/>
+      <c r="BQ48" s="94"/>
+      <c r="BR48" s="94"/>
+      <c r="BS48" s="94"/>
+      <c r="BT48" s="94"/>
+      <c r="BU48" s="94"/>
+      <c r="BV48" s="94"/>
+      <c r="BW48" s="94"/>
+      <c r="BX48" s="94"/>
+      <c r="BY48" s="94"/>
+      <c r="BZ48" s="94"/>
+      <c r="CA48" s="94"/>
+      <c r="CB48" s="94"/>
+      <c r="CC48" s="94"/>
+      <c r="CD48" s="94"/>
+      <c r="CE48" s="94"/>
+      <c r="CF48" s="94"/>
+      <c r="CG48" s="94"/>
+      <c r="CH48" s="94"/>
+      <c r="CI48" s="94"/>
+      <c r="CJ48" s="94"/>
+      <c r="CK48" s="94"/>
+      <c r="CL48" s="94"/>
+      <c r="CM48" s="94"/>
+      <c r="CN48" s="94"/>
+      <c r="CO48" s="94"/>
+      <c r="CP48" s="94"/>
+      <c r="CQ48" s="94"/>
+      <c r="CR48" s="94"/>
+      <c r="CS48" s="94"/>
+      <c r="CT48" s="94"/>
+      <c r="CU48" s="94"/>
+      <c r="CV48" s="94"/>
+      <c r="CW48" s="94"/>
+      <c r="CX48" s="94"/>
+      <c r="CY48" s="94"/>
+      <c r="CZ48" s="94"/>
+      <c r="DA48" s="94"/>
+      <c r="DB48" s="94"/>
+      <c r="DC48" s="94"/>
+      <c r="DD48" s="94"/>
+      <c r="DE48" s="94"/>
+      <c r="DF48" s="94"/>
+      <c r="DG48" s="94"/>
+      <c r="DH48" s="94"/>
+      <c r="DI48" s="94"/>
+      <c r="DJ48" s="94"/>
+      <c r="DK48" s="94"/>
+      <c r="DL48" s="94"/>
+      <c r="DM48" s="94"/>
+      <c r="DN48" s="94"/>
+      <c r="DO48" s="94"/>
+      <c r="DP48" s="94"/>
+      <c r="DQ48" s="94"/>
+      <c r="DR48" s="94"/>
+      <c r="DS48" s="94"/>
+      <c r="DT48" s="94"/>
+      <c r="DU48" s="94"/>
+      <c r="DV48" s="94"/>
+      <c r="DW48" s="94"/>
+      <c r="DX48" s="94"/>
+      <c r="DY48" s="94"/>
+      <c r="DZ48" s="94"/>
+      <c r="EA48" s="94"/>
+      <c r="EB48" s="94"/>
+      <c r="EC48" s="94"/>
+      <c r="ED48" s="94"/>
+      <c r="EE48" s="94"/>
+      <c r="EF48" s="94"/>
+      <c r="EG48" s="94"/>
+      <c r="EH48" s="94"/>
+      <c r="EI48" s="94"/>
+      <c r="EJ48" s="94"/>
+      <c r="EK48" s="94"/>
+      <c r="EL48" s="94"/>
+      <c r="EM48" s="94"/>
+      <c r="EN48" s="94"/>
+      <c r="EO48" s="94"/>
+      <c r="EP48" s="94"/>
+      <c r="EQ48" s="94"/>
+      <c r="ER48" s="94"/>
+      <c r="ES48" s="94"/>
+      <c r="ET48" s="94"/>
+      <c r="EU48" s="94"/>
+      <c r="EV48" s="94"/>
+      <c r="EW48" s="94"/>
+      <c r="EX48" s="94"/>
+      <c r="EY48" s="94"/>
+      <c r="EZ48" s="94"/>
+      <c r="FA48" s="94"/>
+      <c r="FB48" s="94"/>
+      <c r="FC48" s="94"/>
+      <c r="FD48" s="94"/>
+      <c r="FE48" s="94"/>
+      <c r="FF48" s="94"/>
+      <c r="FG48" s="94"/>
+      <c r="FH48" s="94"/>
+      <c r="FI48" s="94"/>
+      <c r="FJ48" s="94"/>
+      <c r="FK48" s="94"/>
+      <c r="FL48" s="94"/>
+      <c r="FM48" s="94"/>
+      <c r="FN48" s="94"/>
+      <c r="FO48" s="94"/>
+      <c r="FP48" s="94"/>
+      <c r="FQ48" s="94"/>
+      <c r="FR48" s="94"/>
+      <c r="FS48" s="94"/>
+      <c r="FT48" s="94"/>
+      <c r="FU48" s="94"/>
+      <c r="FV48" s="94"/>
+      <c r="FW48" s="94"/>
+      <c r="FX48" s="94"/>
+      <c r="FY48" s="94"/>
+      <c r="FZ48" s="94"/>
+      <c r="GA48" s="94"/>
+      <c r="GB48" s="94"/>
+      <c r="GC48" s="94"/>
+      <c r="GD48" s="94"/>
+      <c r="GE48" s="94"/>
+      <c r="GF48" s="94"/>
+      <c r="GG48" s="94"/>
+      <c r="GH48" s="94"/>
+      <c r="GI48" s="94"/>
+      <c r="GJ48" s="94"/>
+      <c r="GK48" s="94"/>
+      <c r="GL48" s="94"/>
+      <c r="GM48" s="94"/>
+      <c r="GN48" s="94"/>
+      <c r="GO48" s="94"/>
+      <c r="GP48" s="94"/>
+      <c r="GQ48" s="94"/>
+      <c r="GR48" s="94"/>
+      <c r="GS48" s="94"/>
+      <c r="GT48" s="94"/>
+      <c r="GU48" s="94"/>
+      <c r="GV48" s="94"/>
+      <c r="GW48" s="94"/>
+      <c r="GX48" s="94"/>
+      <c r="GY48" s="94"/>
+      <c r="GZ48" s="94"/>
+      <c r="HA48" s="94"/>
+      <c r="HB48" s="94"/>
+      <c r="HC48" s="94"/>
+      <c r="HD48" s="94"/>
+      <c r="HE48" s="94"/>
+      <c r="HF48" s="94"/>
+      <c r="HG48" s="94"/>
+      <c r="HH48" s="94"/>
+      <c r="HI48" s="94"/>
+      <c r="HJ48" s="94"/>
+      <c r="HK48" s="94"/>
+      <c r="HL48" s="94"/>
+      <c r="HM48" s="94"/>
+      <c r="HN48" s="94"/>
+      <c r="HO48" s="94"/>
+      <c r="HP48" s="94"/>
+      <c r="HQ48" s="94"/>
+      <c r="HR48" s="94"/>
+      <c r="HS48" s="94"/>
+      <c r="HT48" s="94"/>
+      <c r="HU48" s="94"/>
+      <c r="HV48" s="94"/>
+      <c r="HW48" s="94"/>
+      <c r="HX48" s="94"/>
+      <c r="HY48" s="94"/>
+      <c r="HZ48" s="94"/>
+      <c r="IA48" s="94"/>
+      <c r="IB48" s="94"/>
+      <c r="IC48" s="94"/>
+      <c r="ID48" s="94"/>
+      <c r="IE48" s="94"/>
+      <c r="IF48" s="94"/>
+      <c r="IG48" s="94"/>
+      <c r="IH48" s="94"/>
+      <c r="II48" s="94"/>
+      <c r="IJ48" s="94"/>
+      <c r="IK48" s="94"/>
+      <c r="IL48" s="94"/>
+      <c r="IM48" s="94"/>
+      <c r="IN48" s="94"/>
+      <c r="IO48" s="94"/>
+      <c r="IP48" s="94"/>
+      <c r="IQ48" s="94"/>
+      <c r="IR48" s="94"/>
+      <c r="IS48" s="94"/>
+      <c r="IT48" s="94"/>
+      <c r="IU48" s="95"/>
     </row>
     <row r="49" ht="13.75" customHeight="1">
       <c r="A49" s="30">
@@ -16754,14 +16757,14 @@
         <v>82</v>
       </c>
       <c r="D49" t="s" s="35">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="E49" t="s" s="35">
-        <v>61</v>
+        <v>373</v>
       </c>
       <c r="F49" s="3"/>
       <c r="G49" t="s" s="35">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="H49" s="3"/>
       <c r="I49" s="3"/>
@@ -16771,248 +16774,248 @@
       </c>
       <c r="L49" s="3"/>
       <c r="M49" s="3"/>
-      <c r="N49" s="87"/>
-      <c r="O49" s="33"/>
-      <c r="P49" s="33"/>
-      <c r="Q49" s="33"/>
-      <c r="R49" s="33"/>
-      <c r="S49" s="33"/>
-      <c r="T49" s="33"/>
-      <c r="U49" s="33"/>
-      <c r="V49" s="33"/>
-      <c r="W49" s="33"/>
-      <c r="X49" s="33"/>
-      <c r="Y49" s="33"/>
-      <c r="Z49" s="33"/>
-      <c r="AA49" s="33"/>
-      <c r="AB49" s="33"/>
-      <c r="AC49" s="33"/>
-      <c r="AD49" s="33"/>
-      <c r="AE49" s="33"/>
-      <c r="AF49" s="33"/>
-      <c r="AG49" s="33"/>
-      <c r="AH49" s="33"/>
-      <c r="AI49" s="33"/>
-      <c r="AJ49" s="33"/>
-      <c r="AK49" s="33"/>
-      <c r="AL49" s="33"/>
-      <c r="AM49" s="33"/>
-      <c r="AN49" s="33"/>
-      <c r="AO49" s="33"/>
-      <c r="AP49" s="33"/>
-      <c r="AQ49" s="33"/>
-      <c r="AR49" s="33"/>
-      <c r="AS49" s="33"/>
-      <c r="AT49" s="33"/>
-      <c r="AU49" s="33"/>
-      <c r="AV49" s="33"/>
-      <c r="AW49" s="33"/>
-      <c r="AX49" s="33"/>
-      <c r="AY49" s="33"/>
-      <c r="AZ49" s="33"/>
-      <c r="BA49" s="33"/>
-      <c r="BB49" s="33"/>
-      <c r="BC49" s="33"/>
-      <c r="BD49" s="33"/>
-      <c r="BE49" s="33"/>
-      <c r="BF49" s="33"/>
-      <c r="BG49" s="33"/>
-      <c r="BH49" s="33"/>
-      <c r="BI49" s="33"/>
-      <c r="BJ49" s="33"/>
-      <c r="BK49" s="33"/>
-      <c r="BL49" s="33"/>
-      <c r="BM49" s="33"/>
-      <c r="BN49" s="33"/>
-      <c r="BO49" s="33"/>
-      <c r="BP49" s="33"/>
-      <c r="BQ49" s="33"/>
-      <c r="BR49" s="33"/>
-      <c r="BS49" s="33"/>
-      <c r="BT49" s="33"/>
-      <c r="BU49" s="33"/>
-      <c r="BV49" s="33"/>
-      <c r="BW49" s="33"/>
-      <c r="BX49" s="33"/>
-      <c r="BY49" s="33"/>
-      <c r="BZ49" s="33"/>
-      <c r="CA49" s="33"/>
-      <c r="CB49" s="33"/>
-      <c r="CC49" s="33"/>
-      <c r="CD49" s="33"/>
-      <c r="CE49" s="33"/>
-      <c r="CF49" s="33"/>
-      <c r="CG49" s="33"/>
-      <c r="CH49" s="33"/>
-      <c r="CI49" s="33"/>
-      <c r="CJ49" s="33"/>
-      <c r="CK49" s="33"/>
-      <c r="CL49" s="33"/>
-      <c r="CM49" s="33"/>
-      <c r="CN49" s="33"/>
-      <c r="CO49" s="33"/>
-      <c r="CP49" s="33"/>
-      <c r="CQ49" s="33"/>
-      <c r="CR49" s="33"/>
-      <c r="CS49" s="33"/>
-      <c r="CT49" s="33"/>
-      <c r="CU49" s="33"/>
-      <c r="CV49" s="33"/>
-      <c r="CW49" s="33"/>
-      <c r="CX49" s="33"/>
-      <c r="CY49" s="33"/>
-      <c r="CZ49" s="33"/>
-      <c r="DA49" s="33"/>
-      <c r="DB49" s="33"/>
-      <c r="DC49" s="33"/>
-      <c r="DD49" s="33"/>
-      <c r="DE49" s="33"/>
-      <c r="DF49" s="33"/>
-      <c r="DG49" s="33"/>
-      <c r="DH49" s="33"/>
-      <c r="DI49" s="33"/>
-      <c r="DJ49" s="33"/>
-      <c r="DK49" s="33"/>
-      <c r="DL49" s="33"/>
-      <c r="DM49" s="33"/>
-      <c r="DN49" s="33"/>
-      <c r="DO49" s="33"/>
-      <c r="DP49" s="33"/>
-      <c r="DQ49" s="33"/>
-      <c r="DR49" s="33"/>
-      <c r="DS49" s="33"/>
-      <c r="DT49" s="33"/>
-      <c r="DU49" s="33"/>
-      <c r="DV49" s="33"/>
-      <c r="DW49" s="33"/>
-      <c r="DX49" s="33"/>
-      <c r="DY49" s="33"/>
-      <c r="DZ49" s="33"/>
-      <c r="EA49" s="33"/>
-      <c r="EB49" s="33"/>
-      <c r="EC49" s="33"/>
-      <c r="ED49" s="33"/>
-      <c r="EE49" s="33"/>
-      <c r="EF49" s="33"/>
-      <c r="EG49" s="33"/>
-      <c r="EH49" s="33"/>
-      <c r="EI49" s="33"/>
-      <c r="EJ49" s="33"/>
-      <c r="EK49" s="33"/>
-      <c r="EL49" s="33"/>
-      <c r="EM49" s="33"/>
-      <c r="EN49" s="33"/>
-      <c r="EO49" s="33"/>
-      <c r="EP49" s="33"/>
-      <c r="EQ49" s="33"/>
-      <c r="ER49" s="33"/>
-      <c r="ES49" s="33"/>
-      <c r="ET49" s="33"/>
-      <c r="EU49" s="33"/>
-      <c r="EV49" s="33"/>
-      <c r="EW49" s="33"/>
-      <c r="EX49" s="33"/>
-      <c r="EY49" s="33"/>
-      <c r="EZ49" s="33"/>
-      <c r="FA49" s="33"/>
-      <c r="FB49" s="33"/>
-      <c r="FC49" s="33"/>
-      <c r="FD49" s="33"/>
-      <c r="FE49" s="33"/>
-      <c r="FF49" s="33"/>
-      <c r="FG49" s="33"/>
-      <c r="FH49" s="33"/>
-      <c r="FI49" s="33"/>
-      <c r="FJ49" s="33"/>
-      <c r="FK49" s="33"/>
-      <c r="FL49" s="33"/>
-      <c r="FM49" s="33"/>
-      <c r="FN49" s="33"/>
-      <c r="FO49" s="33"/>
-      <c r="FP49" s="33"/>
-      <c r="FQ49" s="33"/>
-      <c r="FR49" s="33"/>
-      <c r="FS49" s="33"/>
-      <c r="FT49" s="33"/>
-      <c r="FU49" s="33"/>
-      <c r="FV49" s="33"/>
-      <c r="FW49" s="33"/>
-      <c r="FX49" s="33"/>
-      <c r="FY49" s="33"/>
-      <c r="FZ49" s="33"/>
-      <c r="GA49" s="33"/>
-      <c r="GB49" s="33"/>
-      <c r="GC49" s="33"/>
-      <c r="GD49" s="33"/>
-      <c r="GE49" s="33"/>
-      <c r="GF49" s="33"/>
-      <c r="GG49" s="33"/>
-      <c r="GH49" s="33"/>
-      <c r="GI49" s="33"/>
-      <c r="GJ49" s="33"/>
-      <c r="GK49" s="33"/>
-      <c r="GL49" s="33"/>
-      <c r="GM49" s="33"/>
-      <c r="GN49" s="33"/>
-      <c r="GO49" s="33"/>
-      <c r="GP49" s="33"/>
-      <c r="GQ49" s="33"/>
-      <c r="GR49" s="33"/>
-      <c r="GS49" s="33"/>
-      <c r="GT49" s="33"/>
-      <c r="GU49" s="33"/>
-      <c r="GV49" s="33"/>
-      <c r="GW49" s="33"/>
-      <c r="GX49" s="33"/>
-      <c r="GY49" s="33"/>
-      <c r="GZ49" s="33"/>
-      <c r="HA49" s="33"/>
-      <c r="HB49" s="33"/>
-      <c r="HC49" s="33"/>
-      <c r="HD49" s="33"/>
-      <c r="HE49" s="33"/>
-      <c r="HF49" s="33"/>
-      <c r="HG49" s="33"/>
-      <c r="HH49" s="33"/>
-      <c r="HI49" s="33"/>
-      <c r="HJ49" s="33"/>
-      <c r="HK49" s="33"/>
-      <c r="HL49" s="33"/>
-      <c r="HM49" s="33"/>
-      <c r="HN49" s="33"/>
-      <c r="HO49" s="33"/>
-      <c r="HP49" s="33"/>
-      <c r="HQ49" s="33"/>
-      <c r="HR49" s="33"/>
-      <c r="HS49" s="33"/>
-      <c r="HT49" s="33"/>
-      <c r="HU49" s="33"/>
-      <c r="HV49" s="33"/>
-      <c r="HW49" s="33"/>
-      <c r="HX49" s="33"/>
-      <c r="HY49" s="33"/>
-      <c r="HZ49" s="33"/>
-      <c r="IA49" s="33"/>
-      <c r="IB49" s="33"/>
-      <c r="IC49" s="33"/>
-      <c r="ID49" s="33"/>
-      <c r="IE49" s="33"/>
-      <c r="IF49" s="33"/>
-      <c r="IG49" s="33"/>
-      <c r="IH49" s="33"/>
-      <c r="II49" s="33"/>
-      <c r="IJ49" s="33"/>
-      <c r="IK49" s="33"/>
-      <c r="IL49" s="33"/>
-      <c r="IM49" s="33"/>
-      <c r="IN49" s="33"/>
-      <c r="IO49" s="33"/>
-      <c r="IP49" s="33"/>
-      <c r="IQ49" s="33"/>
-      <c r="IR49" s="33"/>
-      <c r="IS49" s="33"/>
-      <c r="IT49" s="33"/>
-      <c r="IU49" s="84"/>
+      <c r="N49" s="97"/>
+      <c r="O49" s="81"/>
+      <c r="P49" s="81"/>
+      <c r="Q49" s="81"/>
+      <c r="R49" s="81"/>
+      <c r="S49" s="81"/>
+      <c r="T49" s="81"/>
+      <c r="U49" s="81"/>
+      <c r="V49" s="81"/>
+      <c r="W49" s="81"/>
+      <c r="X49" s="81"/>
+      <c r="Y49" s="81"/>
+      <c r="Z49" s="81"/>
+      <c r="AA49" s="81"/>
+      <c r="AB49" s="81"/>
+      <c r="AC49" s="81"/>
+      <c r="AD49" s="81"/>
+      <c r="AE49" s="81"/>
+      <c r="AF49" s="81"/>
+      <c r="AG49" s="81"/>
+      <c r="AH49" s="81"/>
+      <c r="AI49" s="81"/>
+      <c r="AJ49" s="81"/>
+      <c r="AK49" s="81"/>
+      <c r="AL49" s="81"/>
+      <c r="AM49" s="81"/>
+      <c r="AN49" s="81"/>
+      <c r="AO49" s="81"/>
+      <c r="AP49" s="81"/>
+      <c r="AQ49" s="81"/>
+      <c r="AR49" s="81"/>
+      <c r="AS49" s="81"/>
+      <c r="AT49" s="81"/>
+      <c r="AU49" s="81"/>
+      <c r="AV49" s="81"/>
+      <c r="AW49" s="81"/>
+      <c r="AX49" s="81"/>
+      <c r="AY49" s="81"/>
+      <c r="AZ49" s="81"/>
+      <c r="BA49" s="81"/>
+      <c r="BB49" s="81"/>
+      <c r="BC49" s="81"/>
+      <c r="BD49" s="81"/>
+      <c r="BE49" s="81"/>
+      <c r="BF49" s="81"/>
+      <c r="BG49" s="81"/>
+      <c r="BH49" s="81"/>
+      <c r="BI49" s="81"/>
+      <c r="BJ49" s="81"/>
+      <c r="BK49" s="81"/>
+      <c r="BL49" s="81"/>
+      <c r="BM49" s="81"/>
+      <c r="BN49" s="81"/>
+      <c r="BO49" s="81"/>
+      <c r="BP49" s="81"/>
+      <c r="BQ49" s="81"/>
+      <c r="BR49" s="81"/>
+      <c r="BS49" s="81"/>
+      <c r="BT49" s="81"/>
+      <c r="BU49" s="81"/>
+      <c r="BV49" s="81"/>
+      <c r="BW49" s="81"/>
+      <c r="BX49" s="81"/>
+      <c r="BY49" s="81"/>
+      <c r="BZ49" s="81"/>
+      <c r="CA49" s="81"/>
+      <c r="CB49" s="81"/>
+      <c r="CC49" s="81"/>
+      <c r="CD49" s="81"/>
+      <c r="CE49" s="81"/>
+      <c r="CF49" s="81"/>
+      <c r="CG49" s="81"/>
+      <c r="CH49" s="81"/>
+      <c r="CI49" s="81"/>
+      <c r="CJ49" s="81"/>
+      <c r="CK49" s="81"/>
+      <c r="CL49" s="81"/>
+      <c r="CM49" s="81"/>
+      <c r="CN49" s="81"/>
+      <c r="CO49" s="81"/>
+      <c r="CP49" s="81"/>
+      <c r="CQ49" s="81"/>
+      <c r="CR49" s="81"/>
+      <c r="CS49" s="81"/>
+      <c r="CT49" s="81"/>
+      <c r="CU49" s="81"/>
+      <c r="CV49" s="81"/>
+      <c r="CW49" s="81"/>
+      <c r="CX49" s="81"/>
+      <c r="CY49" s="81"/>
+      <c r="CZ49" s="81"/>
+      <c r="DA49" s="81"/>
+      <c r="DB49" s="81"/>
+      <c r="DC49" s="81"/>
+      <c r="DD49" s="81"/>
+      <c r="DE49" s="81"/>
+      <c r="DF49" s="81"/>
+      <c r="DG49" s="81"/>
+      <c r="DH49" s="81"/>
+      <c r="DI49" s="81"/>
+      <c r="DJ49" s="81"/>
+      <c r="DK49" s="81"/>
+      <c r="DL49" s="81"/>
+      <c r="DM49" s="81"/>
+      <c r="DN49" s="81"/>
+      <c r="DO49" s="81"/>
+      <c r="DP49" s="81"/>
+      <c r="DQ49" s="81"/>
+      <c r="DR49" s="81"/>
+      <c r="DS49" s="81"/>
+      <c r="DT49" s="81"/>
+      <c r="DU49" s="81"/>
+      <c r="DV49" s="81"/>
+      <c r="DW49" s="81"/>
+      <c r="DX49" s="81"/>
+      <c r="DY49" s="81"/>
+      <c r="DZ49" s="81"/>
+      <c r="EA49" s="81"/>
+      <c r="EB49" s="81"/>
+      <c r="EC49" s="81"/>
+      <c r="ED49" s="81"/>
+      <c r="EE49" s="81"/>
+      <c r="EF49" s="81"/>
+      <c r="EG49" s="81"/>
+      <c r="EH49" s="81"/>
+      <c r="EI49" s="81"/>
+      <c r="EJ49" s="81"/>
+      <c r="EK49" s="81"/>
+      <c r="EL49" s="81"/>
+      <c r="EM49" s="81"/>
+      <c r="EN49" s="81"/>
+      <c r="EO49" s="81"/>
+      <c r="EP49" s="81"/>
+      <c r="EQ49" s="81"/>
+      <c r="ER49" s="81"/>
+      <c r="ES49" s="81"/>
+      <c r="ET49" s="81"/>
+      <c r="EU49" s="81"/>
+      <c r="EV49" s="81"/>
+      <c r="EW49" s="81"/>
+      <c r="EX49" s="81"/>
+      <c r="EY49" s="81"/>
+      <c r="EZ49" s="81"/>
+      <c r="FA49" s="81"/>
+      <c r="FB49" s="81"/>
+      <c r="FC49" s="81"/>
+      <c r="FD49" s="81"/>
+      <c r="FE49" s="81"/>
+      <c r="FF49" s="81"/>
+      <c r="FG49" s="81"/>
+      <c r="FH49" s="81"/>
+      <c r="FI49" s="81"/>
+      <c r="FJ49" s="81"/>
+      <c r="FK49" s="81"/>
+      <c r="FL49" s="81"/>
+      <c r="FM49" s="81"/>
+      <c r="FN49" s="81"/>
+      <c r="FO49" s="81"/>
+      <c r="FP49" s="81"/>
+      <c r="FQ49" s="81"/>
+      <c r="FR49" s="81"/>
+      <c r="FS49" s="81"/>
+      <c r="FT49" s="81"/>
+      <c r="FU49" s="81"/>
+      <c r="FV49" s="81"/>
+      <c r="FW49" s="81"/>
+      <c r="FX49" s="81"/>
+      <c r="FY49" s="81"/>
+      <c r="FZ49" s="81"/>
+      <c r="GA49" s="81"/>
+      <c r="GB49" s="81"/>
+      <c r="GC49" s="81"/>
+      <c r="GD49" s="81"/>
+      <c r="GE49" s="81"/>
+      <c r="GF49" s="81"/>
+      <c r="GG49" s="81"/>
+      <c r="GH49" s="81"/>
+      <c r="GI49" s="81"/>
+      <c r="GJ49" s="81"/>
+      <c r="GK49" s="81"/>
+      <c r="GL49" s="81"/>
+      <c r="GM49" s="81"/>
+      <c r="GN49" s="81"/>
+      <c r="GO49" s="81"/>
+      <c r="GP49" s="81"/>
+      <c r="GQ49" s="81"/>
+      <c r="GR49" s="81"/>
+      <c r="GS49" s="81"/>
+      <c r="GT49" s="81"/>
+      <c r="GU49" s="81"/>
+      <c r="GV49" s="81"/>
+      <c r="GW49" s="81"/>
+      <c r="GX49" s="81"/>
+      <c r="GY49" s="81"/>
+      <c r="GZ49" s="81"/>
+      <c r="HA49" s="81"/>
+      <c r="HB49" s="81"/>
+      <c r="HC49" s="81"/>
+      <c r="HD49" s="81"/>
+      <c r="HE49" s="81"/>
+      <c r="HF49" s="81"/>
+      <c r="HG49" s="81"/>
+      <c r="HH49" s="81"/>
+      <c r="HI49" s="81"/>
+      <c r="HJ49" s="81"/>
+      <c r="HK49" s="81"/>
+      <c r="HL49" s="81"/>
+      <c r="HM49" s="81"/>
+      <c r="HN49" s="81"/>
+      <c r="HO49" s="81"/>
+      <c r="HP49" s="81"/>
+      <c r="HQ49" s="81"/>
+      <c r="HR49" s="81"/>
+      <c r="HS49" s="81"/>
+      <c r="HT49" s="81"/>
+      <c r="HU49" s="81"/>
+      <c r="HV49" s="81"/>
+      <c r="HW49" s="81"/>
+      <c r="HX49" s="81"/>
+      <c r="HY49" s="81"/>
+      <c r="HZ49" s="81"/>
+      <c r="IA49" s="81"/>
+      <c r="IB49" s="81"/>
+      <c r="IC49" s="81"/>
+      <c r="ID49" s="81"/>
+      <c r="IE49" s="81"/>
+      <c r="IF49" s="81"/>
+      <c r="IG49" s="81"/>
+      <c r="IH49" s="81"/>
+      <c r="II49" s="81"/>
+      <c r="IJ49" s="81"/>
+      <c r="IK49" s="81"/>
+      <c r="IL49" s="81"/>
+      <c r="IM49" s="81"/>
+      <c r="IN49" s="81"/>
+      <c r="IO49" s="81"/>
+      <c r="IP49" s="81"/>
+      <c r="IQ49" s="81"/>
+      <c r="IR49" s="81"/>
+      <c r="IS49" s="81"/>
+      <c r="IT49" s="81"/>
+      <c r="IU49" s="82"/>
     </row>
     <row r="50" ht="13.75" customHeight="1">
       <c r="A50" s="30">
@@ -17023,14 +17026,14 @@
         <v>82</v>
       </c>
       <c r="D50" t="s" s="35">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="E50" t="s" s="35">
         <v>61</v>
       </c>
       <c r="F50" s="3"/>
       <c r="G50" t="s" s="35">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="H50" s="3"/>
       <c r="I50" s="3"/>
@@ -17040,248 +17043,517 @@
       </c>
       <c r="L50" s="3"/>
       <c r="M50" s="3"/>
-      <c r="N50" s="93"/>
-      <c r="O50" s="94"/>
-      <c r="P50" s="94"/>
-      <c r="Q50" s="94"/>
-      <c r="R50" s="94"/>
-      <c r="S50" s="94"/>
-      <c r="T50" s="94"/>
-      <c r="U50" s="94"/>
-      <c r="V50" s="94"/>
-      <c r="W50" s="94"/>
-      <c r="X50" s="94"/>
-      <c r="Y50" s="94"/>
-      <c r="Z50" s="94"/>
-      <c r="AA50" s="94"/>
-      <c r="AB50" s="94"/>
-      <c r="AC50" s="94"/>
-      <c r="AD50" s="94"/>
-      <c r="AE50" s="94"/>
-      <c r="AF50" s="94"/>
-      <c r="AG50" s="94"/>
-      <c r="AH50" s="94"/>
-      <c r="AI50" s="94"/>
-      <c r="AJ50" s="94"/>
-      <c r="AK50" s="94"/>
-      <c r="AL50" s="94"/>
-      <c r="AM50" s="94"/>
-      <c r="AN50" s="94"/>
-      <c r="AO50" s="94"/>
-      <c r="AP50" s="94"/>
-      <c r="AQ50" s="94"/>
-      <c r="AR50" s="94"/>
-      <c r="AS50" s="94"/>
-      <c r="AT50" s="94"/>
-      <c r="AU50" s="94"/>
-      <c r="AV50" s="94"/>
-      <c r="AW50" s="94"/>
-      <c r="AX50" s="94"/>
-      <c r="AY50" s="94"/>
-      <c r="AZ50" s="94"/>
-      <c r="BA50" s="94"/>
-      <c r="BB50" s="94"/>
-      <c r="BC50" s="94"/>
-      <c r="BD50" s="94"/>
-      <c r="BE50" s="94"/>
-      <c r="BF50" s="94"/>
-      <c r="BG50" s="94"/>
-      <c r="BH50" s="94"/>
-      <c r="BI50" s="94"/>
-      <c r="BJ50" s="94"/>
-      <c r="BK50" s="94"/>
-      <c r="BL50" s="94"/>
-      <c r="BM50" s="94"/>
-      <c r="BN50" s="94"/>
-      <c r="BO50" s="94"/>
-      <c r="BP50" s="94"/>
-      <c r="BQ50" s="94"/>
-      <c r="BR50" s="94"/>
-      <c r="BS50" s="94"/>
-      <c r="BT50" s="94"/>
-      <c r="BU50" s="94"/>
-      <c r="BV50" s="94"/>
-      <c r="BW50" s="94"/>
-      <c r="BX50" s="94"/>
-      <c r="BY50" s="94"/>
-      <c r="BZ50" s="94"/>
-      <c r="CA50" s="94"/>
-      <c r="CB50" s="94"/>
-      <c r="CC50" s="94"/>
-      <c r="CD50" s="94"/>
-      <c r="CE50" s="94"/>
-      <c r="CF50" s="94"/>
-      <c r="CG50" s="94"/>
-      <c r="CH50" s="94"/>
-      <c r="CI50" s="94"/>
-      <c r="CJ50" s="94"/>
-      <c r="CK50" s="94"/>
-      <c r="CL50" s="94"/>
-      <c r="CM50" s="94"/>
-      <c r="CN50" s="94"/>
-      <c r="CO50" s="94"/>
-      <c r="CP50" s="94"/>
-      <c r="CQ50" s="94"/>
-      <c r="CR50" s="94"/>
-      <c r="CS50" s="94"/>
-      <c r="CT50" s="94"/>
-      <c r="CU50" s="94"/>
-      <c r="CV50" s="94"/>
-      <c r="CW50" s="94"/>
-      <c r="CX50" s="94"/>
-      <c r="CY50" s="94"/>
-      <c r="CZ50" s="94"/>
-      <c r="DA50" s="94"/>
-      <c r="DB50" s="94"/>
-      <c r="DC50" s="94"/>
-      <c r="DD50" s="94"/>
-      <c r="DE50" s="94"/>
-      <c r="DF50" s="94"/>
-      <c r="DG50" s="94"/>
-      <c r="DH50" s="94"/>
-      <c r="DI50" s="94"/>
-      <c r="DJ50" s="94"/>
-      <c r="DK50" s="94"/>
-      <c r="DL50" s="94"/>
-      <c r="DM50" s="94"/>
-      <c r="DN50" s="94"/>
-      <c r="DO50" s="94"/>
-      <c r="DP50" s="94"/>
-      <c r="DQ50" s="94"/>
-      <c r="DR50" s="94"/>
-      <c r="DS50" s="94"/>
-      <c r="DT50" s="94"/>
-      <c r="DU50" s="94"/>
-      <c r="DV50" s="94"/>
-      <c r="DW50" s="94"/>
-      <c r="DX50" s="94"/>
-      <c r="DY50" s="94"/>
-      <c r="DZ50" s="94"/>
-      <c r="EA50" s="94"/>
-      <c r="EB50" s="94"/>
-      <c r="EC50" s="94"/>
-      <c r="ED50" s="94"/>
-      <c r="EE50" s="94"/>
-      <c r="EF50" s="94"/>
-      <c r="EG50" s="94"/>
-      <c r="EH50" s="94"/>
-      <c r="EI50" s="94"/>
-      <c r="EJ50" s="94"/>
-      <c r="EK50" s="94"/>
-      <c r="EL50" s="94"/>
-      <c r="EM50" s="94"/>
-      <c r="EN50" s="94"/>
-      <c r="EO50" s="94"/>
-      <c r="EP50" s="94"/>
-      <c r="EQ50" s="94"/>
-      <c r="ER50" s="94"/>
-      <c r="ES50" s="94"/>
-      <c r="ET50" s="94"/>
-      <c r="EU50" s="94"/>
-      <c r="EV50" s="94"/>
-      <c r="EW50" s="94"/>
-      <c r="EX50" s="94"/>
-      <c r="EY50" s="94"/>
-      <c r="EZ50" s="94"/>
-      <c r="FA50" s="94"/>
-      <c r="FB50" s="94"/>
-      <c r="FC50" s="94"/>
-      <c r="FD50" s="94"/>
-      <c r="FE50" s="94"/>
-      <c r="FF50" s="94"/>
-      <c r="FG50" s="94"/>
-      <c r="FH50" s="94"/>
-      <c r="FI50" s="94"/>
-      <c r="FJ50" s="94"/>
-      <c r="FK50" s="94"/>
-      <c r="FL50" s="94"/>
-      <c r="FM50" s="94"/>
-      <c r="FN50" s="94"/>
-      <c r="FO50" s="94"/>
-      <c r="FP50" s="94"/>
-      <c r="FQ50" s="94"/>
-      <c r="FR50" s="94"/>
-      <c r="FS50" s="94"/>
-      <c r="FT50" s="94"/>
-      <c r="FU50" s="94"/>
-      <c r="FV50" s="94"/>
-      <c r="FW50" s="94"/>
-      <c r="FX50" s="94"/>
-      <c r="FY50" s="94"/>
-      <c r="FZ50" s="94"/>
-      <c r="GA50" s="94"/>
-      <c r="GB50" s="94"/>
-      <c r="GC50" s="94"/>
-      <c r="GD50" s="94"/>
-      <c r="GE50" s="94"/>
-      <c r="GF50" s="94"/>
-      <c r="GG50" s="94"/>
-      <c r="GH50" s="94"/>
-      <c r="GI50" s="94"/>
-      <c r="GJ50" s="94"/>
-      <c r="GK50" s="94"/>
-      <c r="GL50" s="94"/>
-      <c r="GM50" s="94"/>
-      <c r="GN50" s="94"/>
-      <c r="GO50" s="94"/>
-      <c r="GP50" s="94"/>
-      <c r="GQ50" s="94"/>
-      <c r="GR50" s="94"/>
-      <c r="GS50" s="94"/>
-      <c r="GT50" s="94"/>
-      <c r="GU50" s="94"/>
-      <c r="GV50" s="94"/>
-      <c r="GW50" s="94"/>
-      <c r="GX50" s="94"/>
-      <c r="GY50" s="94"/>
-      <c r="GZ50" s="94"/>
-      <c r="HA50" s="94"/>
-      <c r="HB50" s="94"/>
-      <c r="HC50" s="94"/>
-      <c r="HD50" s="94"/>
-      <c r="HE50" s="94"/>
-      <c r="HF50" s="94"/>
-      <c r="HG50" s="94"/>
-      <c r="HH50" s="94"/>
-      <c r="HI50" s="94"/>
-      <c r="HJ50" s="94"/>
-      <c r="HK50" s="94"/>
-      <c r="HL50" s="94"/>
-      <c r="HM50" s="94"/>
-      <c r="HN50" s="94"/>
-      <c r="HO50" s="94"/>
-      <c r="HP50" s="94"/>
-      <c r="HQ50" s="94"/>
-      <c r="HR50" s="94"/>
-      <c r="HS50" s="94"/>
-      <c r="HT50" s="94"/>
-      <c r="HU50" s="94"/>
-      <c r="HV50" s="94"/>
-      <c r="HW50" s="94"/>
-      <c r="HX50" s="94"/>
-      <c r="HY50" s="94"/>
-      <c r="HZ50" s="94"/>
-      <c r="IA50" s="94"/>
-      <c r="IB50" s="94"/>
-      <c r="IC50" s="94"/>
-      <c r="ID50" s="94"/>
-      <c r="IE50" s="94"/>
-      <c r="IF50" s="94"/>
-      <c r="IG50" s="94"/>
-      <c r="IH50" s="94"/>
-      <c r="II50" s="94"/>
-      <c r="IJ50" s="94"/>
-      <c r="IK50" s="94"/>
-      <c r="IL50" s="94"/>
-      <c r="IM50" s="94"/>
-      <c r="IN50" s="94"/>
-      <c r="IO50" s="94"/>
-      <c r="IP50" s="94"/>
-      <c r="IQ50" s="94"/>
-      <c r="IR50" s="94"/>
-      <c r="IS50" s="94"/>
-      <c r="IT50" s="94"/>
-      <c r="IU50" s="95"/>
+      <c r="N50" s="87"/>
+      <c r="O50" s="33"/>
+      <c r="P50" s="33"/>
+      <c r="Q50" s="33"/>
+      <c r="R50" s="33"/>
+      <c r="S50" s="33"/>
+      <c r="T50" s="33"/>
+      <c r="U50" s="33"/>
+      <c r="V50" s="33"/>
+      <c r="W50" s="33"/>
+      <c r="X50" s="33"/>
+      <c r="Y50" s="33"/>
+      <c r="Z50" s="33"/>
+      <c r="AA50" s="33"/>
+      <c r="AB50" s="33"/>
+      <c r="AC50" s="33"/>
+      <c r="AD50" s="33"/>
+      <c r="AE50" s="33"/>
+      <c r="AF50" s="33"/>
+      <c r="AG50" s="33"/>
+      <c r="AH50" s="33"/>
+      <c r="AI50" s="33"/>
+      <c r="AJ50" s="33"/>
+      <c r="AK50" s="33"/>
+      <c r="AL50" s="33"/>
+      <c r="AM50" s="33"/>
+      <c r="AN50" s="33"/>
+      <c r="AO50" s="33"/>
+      <c r="AP50" s="33"/>
+      <c r="AQ50" s="33"/>
+      <c r="AR50" s="33"/>
+      <c r="AS50" s="33"/>
+      <c r="AT50" s="33"/>
+      <c r="AU50" s="33"/>
+      <c r="AV50" s="33"/>
+      <c r="AW50" s="33"/>
+      <c r="AX50" s="33"/>
+      <c r="AY50" s="33"/>
+      <c r="AZ50" s="33"/>
+      <c r="BA50" s="33"/>
+      <c r="BB50" s="33"/>
+      <c r="BC50" s="33"/>
+      <c r="BD50" s="33"/>
+      <c r="BE50" s="33"/>
+      <c r="BF50" s="33"/>
+      <c r="BG50" s="33"/>
+      <c r="BH50" s="33"/>
+      <c r="BI50" s="33"/>
+      <c r="BJ50" s="33"/>
+      <c r="BK50" s="33"/>
+      <c r="BL50" s="33"/>
+      <c r="BM50" s="33"/>
+      <c r="BN50" s="33"/>
+      <c r="BO50" s="33"/>
+      <c r="BP50" s="33"/>
+      <c r="BQ50" s="33"/>
+      <c r="BR50" s="33"/>
+      <c r="BS50" s="33"/>
+      <c r="BT50" s="33"/>
+      <c r="BU50" s="33"/>
+      <c r="BV50" s="33"/>
+      <c r="BW50" s="33"/>
+      <c r="BX50" s="33"/>
+      <c r="BY50" s="33"/>
+      <c r="BZ50" s="33"/>
+      <c r="CA50" s="33"/>
+      <c r="CB50" s="33"/>
+      <c r="CC50" s="33"/>
+      <c r="CD50" s="33"/>
+      <c r="CE50" s="33"/>
+      <c r="CF50" s="33"/>
+      <c r="CG50" s="33"/>
+      <c r="CH50" s="33"/>
+      <c r="CI50" s="33"/>
+      <c r="CJ50" s="33"/>
+      <c r="CK50" s="33"/>
+      <c r="CL50" s="33"/>
+      <c r="CM50" s="33"/>
+      <c r="CN50" s="33"/>
+      <c r="CO50" s="33"/>
+      <c r="CP50" s="33"/>
+      <c r="CQ50" s="33"/>
+      <c r="CR50" s="33"/>
+      <c r="CS50" s="33"/>
+      <c r="CT50" s="33"/>
+      <c r="CU50" s="33"/>
+      <c r="CV50" s="33"/>
+      <c r="CW50" s="33"/>
+      <c r="CX50" s="33"/>
+      <c r="CY50" s="33"/>
+      <c r="CZ50" s="33"/>
+      <c r="DA50" s="33"/>
+      <c r="DB50" s="33"/>
+      <c r="DC50" s="33"/>
+      <c r="DD50" s="33"/>
+      <c r="DE50" s="33"/>
+      <c r="DF50" s="33"/>
+      <c r="DG50" s="33"/>
+      <c r="DH50" s="33"/>
+      <c r="DI50" s="33"/>
+      <c r="DJ50" s="33"/>
+      <c r="DK50" s="33"/>
+      <c r="DL50" s="33"/>
+      <c r="DM50" s="33"/>
+      <c r="DN50" s="33"/>
+      <c r="DO50" s="33"/>
+      <c r="DP50" s="33"/>
+      <c r="DQ50" s="33"/>
+      <c r="DR50" s="33"/>
+      <c r="DS50" s="33"/>
+      <c r="DT50" s="33"/>
+      <c r="DU50" s="33"/>
+      <c r="DV50" s="33"/>
+      <c r="DW50" s="33"/>
+      <c r="DX50" s="33"/>
+      <c r="DY50" s="33"/>
+      <c r="DZ50" s="33"/>
+      <c r="EA50" s="33"/>
+      <c r="EB50" s="33"/>
+      <c r="EC50" s="33"/>
+      <c r="ED50" s="33"/>
+      <c r="EE50" s="33"/>
+      <c r="EF50" s="33"/>
+      <c r="EG50" s="33"/>
+      <c r="EH50" s="33"/>
+      <c r="EI50" s="33"/>
+      <c r="EJ50" s="33"/>
+      <c r="EK50" s="33"/>
+      <c r="EL50" s="33"/>
+      <c r="EM50" s="33"/>
+      <c r="EN50" s="33"/>
+      <c r="EO50" s="33"/>
+      <c r="EP50" s="33"/>
+      <c r="EQ50" s="33"/>
+      <c r="ER50" s="33"/>
+      <c r="ES50" s="33"/>
+      <c r="ET50" s="33"/>
+      <c r="EU50" s="33"/>
+      <c r="EV50" s="33"/>
+      <c r="EW50" s="33"/>
+      <c r="EX50" s="33"/>
+      <c r="EY50" s="33"/>
+      <c r="EZ50" s="33"/>
+      <c r="FA50" s="33"/>
+      <c r="FB50" s="33"/>
+      <c r="FC50" s="33"/>
+      <c r="FD50" s="33"/>
+      <c r="FE50" s="33"/>
+      <c r="FF50" s="33"/>
+      <c r="FG50" s="33"/>
+      <c r="FH50" s="33"/>
+      <c r="FI50" s="33"/>
+      <c r="FJ50" s="33"/>
+      <c r="FK50" s="33"/>
+      <c r="FL50" s="33"/>
+      <c r="FM50" s="33"/>
+      <c r="FN50" s="33"/>
+      <c r="FO50" s="33"/>
+      <c r="FP50" s="33"/>
+      <c r="FQ50" s="33"/>
+      <c r="FR50" s="33"/>
+      <c r="FS50" s="33"/>
+      <c r="FT50" s="33"/>
+      <c r="FU50" s="33"/>
+      <c r="FV50" s="33"/>
+      <c r="FW50" s="33"/>
+      <c r="FX50" s="33"/>
+      <c r="FY50" s="33"/>
+      <c r="FZ50" s="33"/>
+      <c r="GA50" s="33"/>
+      <c r="GB50" s="33"/>
+      <c r="GC50" s="33"/>
+      <c r="GD50" s="33"/>
+      <c r="GE50" s="33"/>
+      <c r="GF50" s="33"/>
+      <c r="GG50" s="33"/>
+      <c r="GH50" s="33"/>
+      <c r="GI50" s="33"/>
+      <c r="GJ50" s="33"/>
+      <c r="GK50" s="33"/>
+      <c r="GL50" s="33"/>
+      <c r="GM50" s="33"/>
+      <c r="GN50" s="33"/>
+      <c r="GO50" s="33"/>
+      <c r="GP50" s="33"/>
+      <c r="GQ50" s="33"/>
+      <c r="GR50" s="33"/>
+      <c r="GS50" s="33"/>
+      <c r="GT50" s="33"/>
+      <c r="GU50" s="33"/>
+      <c r="GV50" s="33"/>
+      <c r="GW50" s="33"/>
+      <c r="GX50" s="33"/>
+      <c r="GY50" s="33"/>
+      <c r="GZ50" s="33"/>
+      <c r="HA50" s="33"/>
+      <c r="HB50" s="33"/>
+      <c r="HC50" s="33"/>
+      <c r="HD50" s="33"/>
+      <c r="HE50" s="33"/>
+      <c r="HF50" s="33"/>
+      <c r="HG50" s="33"/>
+      <c r="HH50" s="33"/>
+      <c r="HI50" s="33"/>
+      <c r="HJ50" s="33"/>
+      <c r="HK50" s="33"/>
+      <c r="HL50" s="33"/>
+      <c r="HM50" s="33"/>
+      <c r="HN50" s="33"/>
+      <c r="HO50" s="33"/>
+      <c r="HP50" s="33"/>
+      <c r="HQ50" s="33"/>
+      <c r="HR50" s="33"/>
+      <c r="HS50" s="33"/>
+      <c r="HT50" s="33"/>
+      <c r="HU50" s="33"/>
+      <c r="HV50" s="33"/>
+      <c r="HW50" s="33"/>
+      <c r="HX50" s="33"/>
+      <c r="HY50" s="33"/>
+      <c r="HZ50" s="33"/>
+      <c r="IA50" s="33"/>
+      <c r="IB50" s="33"/>
+      <c r="IC50" s="33"/>
+      <c r="ID50" s="33"/>
+      <c r="IE50" s="33"/>
+      <c r="IF50" s="33"/>
+      <c r="IG50" s="33"/>
+      <c r="IH50" s="33"/>
+      <c r="II50" s="33"/>
+      <c r="IJ50" s="33"/>
+      <c r="IK50" s="33"/>
+      <c r="IL50" s="33"/>
+      <c r="IM50" s="33"/>
+      <c r="IN50" s="33"/>
+      <c r="IO50" s="33"/>
+      <c r="IP50" s="33"/>
+      <c r="IQ50" s="33"/>
+      <c r="IR50" s="33"/>
+      <c r="IS50" s="33"/>
+      <c r="IT50" s="33"/>
+      <c r="IU50" s="84"/>
+    </row>
+    <row r="51" ht="13.75" customHeight="1">
+      <c r="A51" s="30">
+        <v>42736</v>
+      </c>
+      <c r="B51" s="3"/>
+      <c r="C51" t="s" s="35">
+        <v>82</v>
+      </c>
+      <c r="D51" t="s" s="35">
+        <v>381</v>
+      </c>
+      <c r="E51" t="s" s="35">
+        <v>61</v>
+      </c>
+      <c r="F51" s="3"/>
+      <c r="G51" t="s" s="35">
+        <v>382</v>
+      </c>
+      <c r="H51" s="3"/>
+      <c r="I51" s="3"/>
+      <c r="J51" s="3"/>
+      <c r="K51" t="s" s="35">
+        <v>40</v>
+      </c>
+      <c r="L51" s="3"/>
+      <c r="M51" s="3"/>
+      <c r="N51" s="93"/>
+      <c r="O51" s="94"/>
+      <c r="P51" s="94"/>
+      <c r="Q51" s="94"/>
+      <c r="R51" s="94"/>
+      <c r="S51" s="94"/>
+      <c r="T51" s="94"/>
+      <c r="U51" s="94"/>
+      <c r="V51" s="94"/>
+      <c r="W51" s="94"/>
+      <c r="X51" s="94"/>
+      <c r="Y51" s="94"/>
+      <c r="Z51" s="94"/>
+      <c r="AA51" s="94"/>
+      <c r="AB51" s="94"/>
+      <c r="AC51" s="94"/>
+      <c r="AD51" s="94"/>
+      <c r="AE51" s="94"/>
+      <c r="AF51" s="94"/>
+      <c r="AG51" s="94"/>
+      <c r="AH51" s="94"/>
+      <c r="AI51" s="94"/>
+      <c r="AJ51" s="94"/>
+      <c r="AK51" s="94"/>
+      <c r="AL51" s="94"/>
+      <c r="AM51" s="94"/>
+      <c r="AN51" s="94"/>
+      <c r="AO51" s="94"/>
+      <c r="AP51" s="94"/>
+      <c r="AQ51" s="94"/>
+      <c r="AR51" s="94"/>
+      <c r="AS51" s="94"/>
+      <c r="AT51" s="94"/>
+      <c r="AU51" s="94"/>
+      <c r="AV51" s="94"/>
+      <c r="AW51" s="94"/>
+      <c r="AX51" s="94"/>
+      <c r="AY51" s="94"/>
+      <c r="AZ51" s="94"/>
+      <c r="BA51" s="94"/>
+      <c r="BB51" s="94"/>
+      <c r="BC51" s="94"/>
+      <c r="BD51" s="94"/>
+      <c r="BE51" s="94"/>
+      <c r="BF51" s="94"/>
+      <c r="BG51" s="94"/>
+      <c r="BH51" s="94"/>
+      <c r="BI51" s="94"/>
+      <c r="BJ51" s="94"/>
+      <c r="BK51" s="94"/>
+      <c r="BL51" s="94"/>
+      <c r="BM51" s="94"/>
+      <c r="BN51" s="94"/>
+      <c r="BO51" s="94"/>
+      <c r="BP51" s="94"/>
+      <c r="BQ51" s="94"/>
+      <c r="BR51" s="94"/>
+      <c r="BS51" s="94"/>
+      <c r="BT51" s="94"/>
+      <c r="BU51" s="94"/>
+      <c r="BV51" s="94"/>
+      <c r="BW51" s="94"/>
+      <c r="BX51" s="94"/>
+      <c r="BY51" s="94"/>
+      <c r="BZ51" s="94"/>
+      <c r="CA51" s="94"/>
+      <c r="CB51" s="94"/>
+      <c r="CC51" s="94"/>
+      <c r="CD51" s="94"/>
+      <c r="CE51" s="94"/>
+      <c r="CF51" s="94"/>
+      <c r="CG51" s="94"/>
+      <c r="CH51" s="94"/>
+      <c r="CI51" s="94"/>
+      <c r="CJ51" s="94"/>
+      <c r="CK51" s="94"/>
+      <c r="CL51" s="94"/>
+      <c r="CM51" s="94"/>
+      <c r="CN51" s="94"/>
+      <c r="CO51" s="94"/>
+      <c r="CP51" s="94"/>
+      <c r="CQ51" s="94"/>
+      <c r="CR51" s="94"/>
+      <c r="CS51" s="94"/>
+      <c r="CT51" s="94"/>
+      <c r="CU51" s="94"/>
+      <c r="CV51" s="94"/>
+      <c r="CW51" s="94"/>
+      <c r="CX51" s="94"/>
+      <c r="CY51" s="94"/>
+      <c r="CZ51" s="94"/>
+      <c r="DA51" s="94"/>
+      <c r="DB51" s="94"/>
+      <c r="DC51" s="94"/>
+      <c r="DD51" s="94"/>
+      <c r="DE51" s="94"/>
+      <c r="DF51" s="94"/>
+      <c r="DG51" s="94"/>
+      <c r="DH51" s="94"/>
+      <c r="DI51" s="94"/>
+      <c r="DJ51" s="94"/>
+      <c r="DK51" s="94"/>
+      <c r="DL51" s="94"/>
+      <c r="DM51" s="94"/>
+      <c r="DN51" s="94"/>
+      <c r="DO51" s="94"/>
+      <c r="DP51" s="94"/>
+      <c r="DQ51" s="94"/>
+      <c r="DR51" s="94"/>
+      <c r="DS51" s="94"/>
+      <c r="DT51" s="94"/>
+      <c r="DU51" s="94"/>
+      <c r="DV51" s="94"/>
+      <c r="DW51" s="94"/>
+      <c r="DX51" s="94"/>
+      <c r="DY51" s="94"/>
+      <c r="DZ51" s="94"/>
+      <c r="EA51" s="94"/>
+      <c r="EB51" s="94"/>
+      <c r="EC51" s="94"/>
+      <c r="ED51" s="94"/>
+      <c r="EE51" s="94"/>
+      <c r="EF51" s="94"/>
+      <c r="EG51" s="94"/>
+      <c r="EH51" s="94"/>
+      <c r="EI51" s="94"/>
+      <c r="EJ51" s="94"/>
+      <c r="EK51" s="94"/>
+      <c r="EL51" s="94"/>
+      <c r="EM51" s="94"/>
+      <c r="EN51" s="94"/>
+      <c r="EO51" s="94"/>
+      <c r="EP51" s="94"/>
+      <c r="EQ51" s="94"/>
+      <c r="ER51" s="94"/>
+      <c r="ES51" s="94"/>
+      <c r="ET51" s="94"/>
+      <c r="EU51" s="94"/>
+      <c r="EV51" s="94"/>
+      <c r="EW51" s="94"/>
+      <c r="EX51" s="94"/>
+      <c r="EY51" s="94"/>
+      <c r="EZ51" s="94"/>
+      <c r="FA51" s="94"/>
+      <c r="FB51" s="94"/>
+      <c r="FC51" s="94"/>
+      <c r="FD51" s="94"/>
+      <c r="FE51" s="94"/>
+      <c r="FF51" s="94"/>
+      <c r="FG51" s="94"/>
+      <c r="FH51" s="94"/>
+      <c r="FI51" s="94"/>
+      <c r="FJ51" s="94"/>
+      <c r="FK51" s="94"/>
+      <c r="FL51" s="94"/>
+      <c r="FM51" s="94"/>
+      <c r="FN51" s="94"/>
+      <c r="FO51" s="94"/>
+      <c r="FP51" s="94"/>
+      <c r="FQ51" s="94"/>
+      <c r="FR51" s="94"/>
+      <c r="FS51" s="94"/>
+      <c r="FT51" s="94"/>
+      <c r="FU51" s="94"/>
+      <c r="FV51" s="94"/>
+      <c r="FW51" s="94"/>
+      <c r="FX51" s="94"/>
+      <c r="FY51" s="94"/>
+      <c r="FZ51" s="94"/>
+      <c r="GA51" s="94"/>
+      <c r="GB51" s="94"/>
+      <c r="GC51" s="94"/>
+      <c r="GD51" s="94"/>
+      <c r="GE51" s="94"/>
+      <c r="GF51" s="94"/>
+      <c r="GG51" s="94"/>
+      <c r="GH51" s="94"/>
+      <c r="GI51" s="94"/>
+      <c r="GJ51" s="94"/>
+      <c r="GK51" s="94"/>
+      <c r="GL51" s="94"/>
+      <c r="GM51" s="94"/>
+      <c r="GN51" s="94"/>
+      <c r="GO51" s="94"/>
+      <c r="GP51" s="94"/>
+      <c r="GQ51" s="94"/>
+      <c r="GR51" s="94"/>
+      <c r="GS51" s="94"/>
+      <c r="GT51" s="94"/>
+      <c r="GU51" s="94"/>
+      <c r="GV51" s="94"/>
+      <c r="GW51" s="94"/>
+      <c r="GX51" s="94"/>
+      <c r="GY51" s="94"/>
+      <c r="GZ51" s="94"/>
+      <c r="HA51" s="94"/>
+      <c r="HB51" s="94"/>
+      <c r="HC51" s="94"/>
+      <c r="HD51" s="94"/>
+      <c r="HE51" s="94"/>
+      <c r="HF51" s="94"/>
+      <c r="HG51" s="94"/>
+      <c r="HH51" s="94"/>
+      <c r="HI51" s="94"/>
+      <c r="HJ51" s="94"/>
+      <c r="HK51" s="94"/>
+      <c r="HL51" s="94"/>
+      <c r="HM51" s="94"/>
+      <c r="HN51" s="94"/>
+      <c r="HO51" s="94"/>
+      <c r="HP51" s="94"/>
+      <c r="HQ51" s="94"/>
+      <c r="HR51" s="94"/>
+      <c r="HS51" s="94"/>
+      <c r="HT51" s="94"/>
+      <c r="HU51" s="94"/>
+      <c r="HV51" s="94"/>
+      <c r="HW51" s="94"/>
+      <c r="HX51" s="94"/>
+      <c r="HY51" s="94"/>
+      <c r="HZ51" s="94"/>
+      <c r="IA51" s="94"/>
+      <c r="IB51" s="94"/>
+      <c r="IC51" s="94"/>
+      <c r="ID51" s="94"/>
+      <c r="IE51" s="94"/>
+      <c r="IF51" s="94"/>
+      <c r="IG51" s="94"/>
+      <c r="IH51" s="94"/>
+      <c r="II51" s="94"/>
+      <c r="IJ51" s="94"/>
+      <c r="IK51" s="94"/>
+      <c r="IL51" s="94"/>
+      <c r="IM51" s="94"/>
+      <c r="IN51" s="94"/>
+      <c r="IO51" s="94"/>
+      <c r="IP51" s="94"/>
+      <c r="IQ51" s="94"/>
+      <c r="IR51" s="94"/>
+      <c r="IS51" s="94"/>
+      <c r="IT51" s="94"/>
+      <c r="IU51" s="95"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511806" footer="0.511806"/>
@@ -17309,7 +17581,7 @@
   <sheetData>
     <row r="1" ht="18" customHeight="1">
       <c r="A1" t="s" s="11">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="B1" t="s" s="111">
         <v>11</v>
@@ -17338,13 +17610,13 @@
         <v>42</v>
       </c>
       <c r="D2" t="s" s="15">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="E2" t="s" s="15">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="F2" t="s" s="15">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="G2" s="114"/>
       <c r="H2" s="115"/>
@@ -17387,7 +17659,7 @@
         <v>59</v>
       </c>
       <c r="E4" t="s" s="120">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="F4" s="69">
         <v>1</v>
@@ -17409,7 +17681,7 @@
         <v>62</v>
       </c>
       <c r="E5" t="s" s="36">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="F5" s="4">
         <v>2</v>
@@ -17431,7 +17703,7 @@
         <v>64</v>
       </c>
       <c r="E6" t="s" s="36">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="F6" s="4">
         <v>3</v>
@@ -17522,7 +17794,7 @@
   <sheetData>
     <row r="1" ht="18" customHeight="1">
       <c r="A1" t="s" s="11">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="B1" t="s" s="12">
         <v>11</v>
@@ -17557,13 +17829,13 @@
         <v>42</v>
       </c>
       <c r="D2" t="s" s="15">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="E2" t="s" s="15">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="F2" t="s" s="15">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="G2" s="114"/>
       <c r="H2" s="115"/>
@@ -17618,7 +17890,7 @@
         <v>59</v>
       </c>
       <c r="E4" t="s" s="120">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="F4" s="69">
         <v>1</v>
@@ -17646,7 +17918,7 @@
         <v>62</v>
       </c>
       <c r="E5" t="s" s="36">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="F5" s="4">
         <v>2</v>
@@ -17674,7 +17946,7 @@
         <v>64</v>
       </c>
       <c r="E6" t="s" s="36">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="F6" s="4">
         <v>3</v>
@@ -17795,7 +18067,7 @@
   <sheetData>
     <row r="1" ht="18" customHeight="1">
       <c r="A1" t="s" s="11">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="B1" t="s" s="12">
         <v>11</v>
@@ -17830,13 +18102,13 @@
         <v>42</v>
       </c>
       <c r="D2" t="s" s="15">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="E2" t="s" s="15">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="F2" t="s" s="15">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="G2" s="21"/>
       <c r="H2" s="22"/>
@@ -17891,7 +18163,7 @@
         <v>59</v>
       </c>
       <c r="E4" t="s" s="120">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="F4" s="69">
         <v>1</v>
@@ -17919,7 +18191,7 @@
         <v>62</v>
       </c>
       <c r="E5" t="s" s="36">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="F5" s="4">
         <v>2</v>
@@ -17947,7 +18219,7 @@
         <v>64</v>
       </c>
       <c r="E6" t="s" s="36">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="F6" s="4">
         <v>3</v>
@@ -18068,7 +18340,7 @@
   <sheetData>
     <row r="1" ht="19" customHeight="1">
       <c r="A1" t="s" s="11">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B1" t="s" s="111">
         <v>11</v>
@@ -18097,13 +18369,13 @@
         <v>42</v>
       </c>
       <c r="D2" t="s" s="15">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="E2" t="s" s="15">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="F2" t="s" s="15">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="G2" s="114"/>
       <c r="H2" s="115"/>
@@ -18146,7 +18418,7 @@
         <v>59</v>
       </c>
       <c r="E4" t="s" s="120">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="F4" s="69">
         <v>1</v>
@@ -18168,7 +18440,7 @@
         <v>62</v>
       </c>
       <c r="E5" t="s" s="36">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="F5" s="4">
         <v>2</v>
@@ -18190,7 +18462,7 @@
         <v>64</v>
       </c>
       <c r="E6" t="s" s="36">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="F6" s="4">
         <v>3</v>
@@ -18283,7 +18555,7 @@
   <sheetData>
     <row r="1" ht="18" customHeight="1">
       <c r="A1" t="s" s="11">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B1" t="s" s="12">
         <v>11</v>
@@ -18316,13 +18588,13 @@
       </c>
       <c r="C2" s="66"/>
       <c r="D2" t="s" s="15">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="E2" t="s" s="15">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="F2" t="s" s="15">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="G2" s="14"/>
       <c r="H2" s="3"/>
@@ -18343,16 +18615,16 @@
         <v>20</v>
       </c>
       <c r="C3" t="s" s="6">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="D3" t="s" s="6">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="E3" t="s" s="6">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="F3" t="s" s="6">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="G3" s="16"/>
       <c r="H3" s="17"/>
@@ -18371,7 +18643,7 @@
       </c>
       <c r="B4" s="98"/>
       <c r="C4" t="s" s="128">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="D4" t="s" s="128">
         <v>24</v>
@@ -18399,7 +18671,7 @@
       </c>
       <c r="B5" s="77"/>
       <c r="C5" t="s" s="129">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="D5" t="s" s="129">
         <v>24</v>
@@ -18427,7 +18699,7 @@
       </c>
       <c r="B6" s="77"/>
       <c r="C6" t="s" s="129">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="D6" t="s" s="129">
         <v>24</v>
@@ -18455,7 +18727,7 @@
       </c>
       <c r="B7" s="102"/>
       <c r="C7" t="s" s="130">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="D7" t="s" s="130">
         <v>24</v>
@@ -18483,7 +18755,7 @@
       </c>
       <c r="B8" s="131"/>
       <c r="C8" t="s" s="12">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="D8" t="s" s="12">
         <v>24</v>
@@ -18564,7 +18836,7 @@
   <sheetData>
     <row r="1" ht="18" customHeight="1">
       <c r="A1" t="s" s="11">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="B1" t="s" s="12">
         <v>11</v>
@@ -18595,13 +18867,13 @@
         <v>15</v>
       </c>
       <c r="C2" t="s" s="15">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="D2" t="s" s="15">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="E2" t="s" s="15">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="F2" s="21"/>
       <c r="G2" s="22"/>
@@ -18625,10 +18897,10 @@
         <v>51</v>
       </c>
       <c r="D3" t="s" s="6">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="E3" t="s" s="6">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="F3" s="14"/>
       <c r="G3" s="3"/>
@@ -18650,10 +18922,10 @@
         <v>37</v>
       </c>
       <c r="D4" t="s" s="15">
+        <v>415</v>
+      </c>
+      <c r="E4" t="s" s="133">
         <v>414</v>
-      </c>
-      <c r="E4" t="s" s="133">
-        <v>413</v>
       </c>
       <c r="F4" s="14"/>
       <c r="G4" s="3"/>
@@ -18794,7 +19066,7 @@
   <sheetData>
     <row r="1" ht="18" customHeight="1">
       <c r="A1" t="s" s="11">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="B1" t="s" s="12">
         <v>11</v>
@@ -19065,16 +19337,16 @@
         <v>15</v>
       </c>
       <c r="C2" t="s" s="15">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="D2" t="s" s="15">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="E2" t="s" s="15">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="F2" t="s" s="15">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="G2" s="14"/>
       <c r="H2" s="3"/>
@@ -19340,10 +19612,10 @@
         <v>107</v>
       </c>
       <c r="E3" t="s" s="6">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="F3" t="s" s="6">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="G3" s="16"/>
       <c r="H3" s="3"/>
@@ -19607,10 +19879,10 @@
         <v>59</v>
       </c>
       <c r="E4" t="s" s="136">
+        <v>415</v>
+      </c>
+      <c r="F4" t="s" s="133">
         <v>414</v>
-      </c>
-      <c r="F4" t="s" s="133">
-        <v>413</v>
       </c>
       <c r="G4" s="14"/>
       <c r="H4" s="3"/>
@@ -19874,10 +20146,10 @@
         <v>62</v>
       </c>
       <c r="E5" t="s" s="138">
+        <v>415</v>
+      </c>
+      <c r="F5" t="s" s="133">
         <v>414</v>
-      </c>
-      <c r="F5" t="s" s="133">
-        <v>413</v>
       </c>
       <c r="G5" s="14"/>
       <c r="H5" s="3"/>
@@ -20141,10 +20413,10 @@
         <v>64</v>
       </c>
       <c r="E6" t="s" s="138">
+        <v>415</v>
+      </c>
+      <c r="F6" t="s" s="133">
         <v>414</v>
-      </c>
-      <c r="F6" t="s" s="133">
-        <v>413</v>
       </c>
       <c r="G6" s="14"/>
       <c r="H6" s="3"/>
@@ -20408,10 +20680,10 @@
         <v>66</v>
       </c>
       <c r="E7" t="s" s="138">
+        <v>415</v>
+      </c>
+      <c r="F7" t="s" s="133">
         <v>414</v>
-      </c>
-      <c r="F7" t="s" s="133">
-        <v>413</v>
       </c>
       <c r="G7" s="14"/>
       <c r="H7" s="3"/>
@@ -20675,10 +20947,10 @@
         <v>68</v>
       </c>
       <c r="E8" t="s" s="138">
+        <v>415</v>
+      </c>
+      <c r="F8" t="s" s="133">
         <v>414</v>
-      </c>
-      <c r="F8" t="s" s="133">
-        <v>413</v>
       </c>
       <c r="G8" s="14"/>
       <c r="H8" s="3"/>
@@ -20942,10 +21214,10 @@
         <v>71</v>
       </c>
       <c r="E9" t="s" s="138">
+        <v>415</v>
+      </c>
+      <c r="F9" t="s" s="133">
         <v>414</v>
-      </c>
-      <c r="F9" t="s" s="133">
-        <v>413</v>
       </c>
       <c r="G9" s="14"/>
       <c r="H9" s="3"/>
@@ -21209,10 +21481,10 @@
         <v>75</v>
       </c>
       <c r="E10" t="s" s="138">
+        <v>415</v>
+      </c>
+      <c r="F10" t="s" s="133">
         <v>414</v>
-      </c>
-      <c r="F10" t="s" s="133">
-        <v>413</v>
       </c>
       <c r="G10" s="14"/>
       <c r="H10" s="3"/>
@@ -21476,10 +21748,10 @@
         <v>80</v>
       </c>
       <c r="E11" t="s" s="138">
+        <v>415</v>
+      </c>
+      <c r="F11" t="s" s="133">
         <v>414</v>
-      </c>
-      <c r="F11" t="s" s="133">
-        <v>413</v>
       </c>
       <c r="G11" s="14"/>
       <c r="H11" s="3"/>
@@ -21743,10 +22015,10 @@
         <v>83</v>
       </c>
       <c r="E12" t="s" s="140">
+        <v>415</v>
+      </c>
+      <c r="F12" t="s" s="133">
         <v>414</v>
-      </c>
-      <c r="F12" t="s" s="133">
-        <v>413</v>
       </c>
       <c r="G12" s="14"/>
       <c r="H12" s="3"/>
@@ -22010,10 +22282,10 @@
         <v>84</v>
       </c>
       <c r="E13" t="s" s="136">
+        <v>415</v>
+      </c>
+      <c r="F13" t="s" s="133">
         <v>414</v>
-      </c>
-      <c r="F13" t="s" s="133">
-        <v>413</v>
       </c>
       <c r="G13" s="14"/>
       <c r="H13" s="3"/>
@@ -22277,10 +22549,10 @@
         <v>86</v>
       </c>
       <c r="E14" t="s" s="138">
+        <v>415</v>
+      </c>
+      <c r="F14" t="s" s="133">
         <v>414</v>
-      </c>
-      <c r="F14" t="s" s="133">
-        <v>413</v>
       </c>
       <c r="G14" s="14"/>
       <c r="H14" s="3"/>
@@ -22544,10 +22816,10 @@
         <v>88</v>
       </c>
       <c r="E15" t="s" s="138">
+        <v>415</v>
+      </c>
+      <c r="F15" t="s" s="133">
         <v>414</v>
-      </c>
-      <c r="F15" t="s" s="133">
-        <v>413</v>
       </c>
       <c r="G15" s="14"/>
       <c r="H15" s="3"/>
@@ -22811,10 +23083,10 @@
         <v>90</v>
       </c>
       <c r="E16" t="s" s="138">
+        <v>415</v>
+      </c>
+      <c r="F16" t="s" s="133">
         <v>414</v>
-      </c>
-      <c r="F16" t="s" s="133">
-        <v>413</v>
       </c>
       <c r="G16" s="14"/>
       <c r="H16" s="3"/>
@@ -23078,10 +23350,10 @@
         <v>92</v>
       </c>
       <c r="E17" t="s" s="138">
+        <v>415</v>
+      </c>
+      <c r="F17" t="s" s="133">
         <v>414</v>
-      </c>
-      <c r="F17" t="s" s="133">
-        <v>413</v>
       </c>
       <c r="G17" s="14"/>
       <c r="H17" s="3"/>
@@ -23356,7 +23628,7 @@
   <sheetData>
     <row r="1" ht="18" customHeight="1">
       <c r="A1" t="s" s="11">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="B1" t="s" s="12">
         <v>11</v>
@@ -23387,16 +23659,16 @@
         <v>15</v>
       </c>
       <c r="C2" t="s" s="15">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="D2" t="s" s="15">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="E2" t="s" s="15">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="F2" t="s" s="15">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="G2" s="21"/>
       <c r="H2" s="22"/>
@@ -23422,10 +23694,10 @@
         <v>201</v>
       </c>
       <c r="E3" t="s" s="12">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="F3" t="s" s="12">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="G3" s="14"/>
       <c r="H3" s="22"/>
@@ -23449,10 +23721,10 @@
         <v>154</v>
       </c>
       <c r="E4" t="s" s="144">
+        <v>415</v>
+      </c>
+      <c r="F4" t="s" s="133">
         <v>414</v>
-      </c>
-      <c r="F4" t="s" s="133">
-        <v>413</v>
       </c>
       <c r="G4" s="14"/>
       <c r="H4" s="3"/>
@@ -23476,10 +23748,10 @@
         <v>158</v>
       </c>
       <c r="E5" t="s" s="146">
+        <v>415</v>
+      </c>
+      <c r="F5" t="s" s="133">
         <v>414</v>
-      </c>
-      <c r="F5" t="s" s="133">
-        <v>413</v>
       </c>
       <c r="G5" s="14"/>
       <c r="H5" s="3"/>
@@ -23503,10 +23775,10 @@
         <v>162</v>
       </c>
       <c r="E6" t="s" s="146">
+        <v>415</v>
+      </c>
+      <c r="F6" t="s" s="133">
         <v>414</v>
-      </c>
-      <c r="F6" t="s" s="133">
-        <v>413</v>
       </c>
       <c r="G6" s="14"/>
       <c r="H6" s="3"/>
@@ -23530,10 +23802,10 @@
         <v>166</v>
       </c>
       <c r="E7" t="s" s="146">
+        <v>415</v>
+      </c>
+      <c r="F7" t="s" s="133">
         <v>414</v>
-      </c>
-      <c r="F7" t="s" s="133">
-        <v>413</v>
       </c>
       <c r="G7" s="14"/>
       <c r="H7" s="3"/>
@@ -23557,10 +23829,10 @@
         <v>173</v>
       </c>
       <c r="E8" t="s" s="146">
+        <v>415</v>
+      </c>
+      <c r="F8" t="s" s="133">
         <v>414</v>
-      </c>
-      <c r="F8" t="s" s="133">
-        <v>413</v>
       </c>
       <c r="G8" s="14"/>
       <c r="H8" s="3"/>
@@ -23584,10 +23856,10 @@
         <v>169</v>
       </c>
       <c r="E9" t="s" s="146">
+        <v>415</v>
+      </c>
+      <c r="F9" t="s" s="133">
         <v>414</v>
-      </c>
-      <c r="F9" t="s" s="133">
-        <v>413</v>
       </c>
       <c r="G9" s="14"/>
       <c r="H9" s="3"/>
@@ -23611,10 +23883,10 @@
         <v>177</v>
       </c>
       <c r="E10" t="s" s="146">
+        <v>415</v>
+      </c>
+      <c r="F10" t="s" s="133">
         <v>414</v>
-      </c>
-      <c r="F10" t="s" s="133">
-        <v>413</v>
       </c>
       <c r="G10" s="14"/>
       <c r="H10" s="3"/>
@@ -23638,10 +23910,10 @@
         <v>184</v>
       </c>
       <c r="E11" t="s" s="146">
+        <v>415</v>
+      </c>
+      <c r="F11" t="s" s="133">
         <v>414</v>
-      </c>
-      <c r="F11" t="s" s="133">
-        <v>413</v>
       </c>
       <c r="G11" s="14"/>
       <c r="H11" s="3"/>
@@ -23665,10 +23937,10 @@
         <v>187</v>
       </c>
       <c r="E12" t="s" s="146">
+        <v>415</v>
+      </c>
+      <c r="F12" t="s" s="133">
         <v>414</v>
-      </c>
-      <c r="F12" t="s" s="133">
-        <v>413</v>
       </c>
       <c r="G12" s="14"/>
       <c r="H12" s="3"/>
@@ -23737,7 +24009,7 @@
   <sheetData>
     <row r="1" ht="18" customHeight="1">
       <c r="A1" t="s" s="11">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="B1" t="s" s="12">
         <v>11</v>
@@ -23769,16 +24041,16 @@
         <v>15</v>
       </c>
       <c r="C2" t="s" s="15">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="D2" t="s" s="15">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="E2" t="s" s="15">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="F2" t="s" s="15">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="G2" s="21"/>
       <c r="H2" s="22"/>
@@ -23802,13 +24074,13 @@
         <v>51</v>
       </c>
       <c r="D3" t="s" s="12">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="E3" t="s" s="12">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="F3" t="s" s="12">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="G3" s="14"/>
       <c r="H3" s="3"/>
@@ -23833,10 +24105,10 @@
         <v>126</v>
       </c>
       <c r="E4" t="s" s="15">
+        <v>415</v>
+      </c>
+      <c r="F4" t="s" s="133">
         <v>414</v>
-      </c>
-      <c r="F4" t="s" s="133">
-        <v>413</v>
       </c>
       <c r="G4" s="14"/>
       <c r="H4" s="3"/>
@@ -24213,7 +24485,7 @@
   <sheetData>
     <row r="1" ht="18" customHeight="1">
       <c r="A1" t="s" s="11">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="B1" t="s" s="12">
         <v>11</v>
@@ -24480,19 +24752,19 @@
       <c r="A2" s="66"/>
       <c r="B2" s="66"/>
       <c r="C2" t="s" s="15">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="D2" t="s" s="15">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="E2" t="s" s="15">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="F2" t="s" s="15">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="G2" t="s" s="15">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="H2" s="83"/>
       <c r="I2" s="33"/>
@@ -24760,10 +25032,10 @@
         <v>224</v>
       </c>
       <c r="F3" t="s" s="12">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="G3" t="s" s="12">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="H3" s="83"/>
       <c r="I3" s="33"/>
@@ -25029,10 +25301,10 @@
         <v>333</v>
       </c>
       <c r="F4" t="s" s="15">
+        <v>415</v>
+      </c>
+      <c r="G4" t="s" s="133">
         <v>414</v>
-      </c>
-      <c r="G4" t="s" s="133">
-        <v>413</v>
       </c>
       <c r="H4" s="83"/>
       <c r="I4" s="33"/>
@@ -25298,10 +25570,10 @@
         <v>335</v>
       </c>
       <c r="F5" t="s" s="15">
+        <v>415</v>
+      </c>
+      <c r="G5" t="s" s="133">
         <v>414</v>
-      </c>
-      <c r="G5" t="s" s="133">
-        <v>413</v>
       </c>
       <c r="H5" s="83"/>
       <c r="I5" s="33"/>
@@ -25567,10 +25839,10 @@
         <v>310</v>
       </c>
       <c r="F6" t="s" s="15">
+        <v>415</v>
+      </c>
+      <c r="G6" t="s" s="133">
         <v>414</v>
-      </c>
-      <c r="G6" t="s" s="133">
-        <v>413</v>
       </c>
       <c r="H6" s="83"/>
       <c r="I6" s="33"/>
@@ -25836,10 +26108,10 @@
         <v>337</v>
       </c>
       <c r="F7" t="s" s="15">
+        <v>415</v>
+      </c>
+      <c r="G7" t="s" s="133">
         <v>414</v>
-      </c>
-      <c r="G7" t="s" s="133">
-        <v>413</v>
       </c>
       <c r="H7" s="83"/>
       <c r="I7" s="33"/>
@@ -26105,10 +26377,10 @@
         <v>340</v>
       </c>
       <c r="F8" t="s" s="15">
+        <v>415</v>
+      </c>
+      <c r="G8" t="s" s="133">
         <v>414</v>
-      </c>
-      <c r="G8" t="s" s="133">
-        <v>413</v>
       </c>
       <c r="H8" s="83"/>
       <c r="I8" s="33"/>
@@ -26374,10 +26646,10 @@
         <v>316</v>
       </c>
       <c r="F9" t="s" s="15">
+        <v>415</v>
+      </c>
+      <c r="G9" t="s" s="133">
         <v>414</v>
-      </c>
-      <c r="G9" t="s" s="133">
-        <v>413</v>
       </c>
       <c r="H9" s="83"/>
       <c r="I9" s="33"/>
@@ -26643,10 +26915,10 @@
         <v>319</v>
       </c>
       <c r="F10" t="s" s="15">
+        <v>415</v>
+      </c>
+      <c r="G10" t="s" s="133">
         <v>414</v>
-      </c>
-      <c r="G10" t="s" s="133">
-        <v>413</v>
       </c>
       <c r="H10" s="83"/>
       <c r="I10" s="33"/>
@@ -26912,10 +27184,10 @@
         <v>344</v>
       </c>
       <c r="F11" t="s" s="15">
+        <v>415</v>
+      </c>
+      <c r="G11" t="s" s="133">
         <v>414</v>
-      </c>
-      <c r="G11" t="s" s="133">
-        <v>413</v>
       </c>
       <c r="H11" s="83"/>
       <c r="I11" s="33"/>
@@ -27181,10 +27453,10 @@
         <v>346</v>
       </c>
       <c r="F12" t="s" s="15">
+        <v>415</v>
+      </c>
+      <c r="G12" t="s" s="133">
         <v>414</v>
-      </c>
-      <c r="G12" t="s" s="133">
-        <v>413</v>
       </c>
       <c r="H12" s="83"/>
       <c r="I12" s="33"/>
@@ -27450,10 +27722,10 @@
         <v>348</v>
       </c>
       <c r="F13" t="s" s="15">
+        <v>415</v>
+      </c>
+      <c r="G13" t="s" s="133">
         <v>414</v>
-      </c>
-      <c r="G13" t="s" s="133">
-        <v>413</v>
       </c>
       <c r="H13" s="83"/>
       <c r="I13" s="33"/>
@@ -27719,10 +27991,10 @@
         <v>352</v>
       </c>
       <c r="F14" t="s" s="15">
+        <v>415</v>
+      </c>
+      <c r="G14" t="s" s="133">
         <v>414</v>
-      </c>
-      <c r="G14" t="s" s="133">
-        <v>413</v>
       </c>
       <c r="H14" s="83"/>
       <c r="I14" s="33"/>
@@ -27988,10 +28260,10 @@
         <v>350</v>
       </c>
       <c r="F15" t="s" s="15">
+        <v>415</v>
+      </c>
+      <c r="G15" t="s" s="133">
         <v>414</v>
-      </c>
-      <c r="G15" t="s" s="133">
-        <v>413</v>
       </c>
       <c r="H15" s="83"/>
       <c r="I15" s="33"/>
@@ -28257,10 +28529,10 @@
         <v>272</v>
       </c>
       <c r="F16" t="s" s="15">
+        <v>415</v>
+      </c>
+      <c r="G16" t="s" s="133">
         <v>414</v>
-      </c>
-      <c r="G16" t="s" s="133">
-        <v>413</v>
       </c>
       <c r="H16" s="83"/>
       <c r="I16" s="33"/>
@@ -28526,10 +28798,10 @@
         <v>267</v>
       </c>
       <c r="F17" t="s" s="15">
+        <v>415</v>
+      </c>
+      <c r="G17" t="s" s="133">
         <v>414</v>
-      </c>
-      <c r="G17" t="s" s="133">
-        <v>413</v>
       </c>
       <c r="H17" s="83"/>
       <c r="I17" s="33"/>
@@ -28795,10 +29067,10 @@
         <v>354</v>
       </c>
       <c r="F18" t="s" s="15">
+        <v>415</v>
+      </c>
+      <c r="G18" t="s" s="133">
         <v>414</v>
-      </c>
-      <c r="G18" t="s" s="133">
-        <v>413</v>
       </c>
       <c r="H18" s="83"/>
       <c r="I18" s="33"/>
@@ -29061,13 +29333,13 @@
         <v>75</v>
       </c>
       <c r="E19" t="s" s="129">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="F19" t="s" s="15">
+        <v>415</v>
+      </c>
+      <c r="G19" t="s" s="133">
         <v>414</v>
-      </c>
-      <c r="G19" t="s" s="133">
-        <v>413</v>
       </c>
       <c r="H19" s="83"/>
       <c r="I19" s="33"/>
@@ -29330,13 +29602,13 @@
         <v>75</v>
       </c>
       <c r="E20" t="s" s="129">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="F20" t="s" s="15">
+        <v>415</v>
+      </c>
+      <c r="G20" t="s" s="133">
         <v>414</v>
-      </c>
-      <c r="G20" t="s" s="133">
-        <v>413</v>
       </c>
       <c r="H20" s="83"/>
       <c r="I20" s="33"/>
@@ -29599,13 +29871,13 @@
         <v>75</v>
       </c>
       <c r="E21" t="s" s="129">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="F21" t="s" s="15">
+        <v>415</v>
+      </c>
+      <c r="G21" t="s" s="133">
         <v>414</v>
-      </c>
-      <c r="G21" t="s" s="133">
-        <v>413</v>
       </c>
       <c r="H21" s="83"/>
       <c r="I21" s="33"/>
@@ -29871,10 +30143,10 @@
         <v>356</v>
       </c>
       <c r="F22" t="s" s="15">
+        <v>415</v>
+      </c>
+      <c r="G22" t="s" s="133">
         <v>414</v>
-      </c>
-      <c r="G22" t="s" s="133">
-        <v>413</v>
       </c>
       <c r="H22" s="83"/>
       <c r="I22" s="33"/>
@@ -30137,13 +30409,13 @@
         <v>80</v>
       </c>
       <c r="E23" t="s" s="128">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="F23" t="s" s="15">
+        <v>415</v>
+      </c>
+      <c r="G23" t="s" s="133">
         <v>414</v>
-      </c>
-      <c r="G23" t="s" s="133">
-        <v>413</v>
       </c>
       <c r="H23" s="83"/>
       <c r="I23" s="33"/>
@@ -30406,13 +30678,13 @@
         <v>80</v>
       </c>
       <c r="E24" t="s" s="129">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="F24" t="s" s="15">
+        <v>415</v>
+      </c>
+      <c r="G24" t="s" s="133">
         <v>414</v>
-      </c>
-      <c r="G24" t="s" s="133">
-        <v>413</v>
       </c>
       <c r="H24" s="83"/>
       <c r="I24" s="33"/>
@@ -30675,13 +30947,13 @@
         <v>80</v>
       </c>
       <c r="E25" t="s" s="129">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="F25" t="s" s="15">
+        <v>415</v>
+      </c>
+      <c r="G25" t="s" s="133">
         <v>414</v>
-      </c>
-      <c r="G25" t="s" s="133">
-        <v>413</v>
       </c>
       <c r="H25" s="83"/>
       <c r="I25" s="33"/>
@@ -30944,13 +31216,13 @@
         <v>80</v>
       </c>
       <c r="E26" t="s" s="129">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="F26" t="s" s="15">
+        <v>415</v>
+      </c>
+      <c r="G26" t="s" s="133">
         <v>414</v>
-      </c>
-      <c r="G26" t="s" s="133">
-        <v>413</v>
       </c>
       <c r="H26" s="83"/>
       <c r="I26" s="33"/>
@@ -31213,13 +31485,13 @@
         <v>80</v>
       </c>
       <c r="E27" t="s" s="129">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="F27" t="s" s="15">
+        <v>415</v>
+      </c>
+      <c r="G27" t="s" s="133">
         <v>414</v>
-      </c>
-      <c r="G27" t="s" s="133">
-        <v>413</v>
       </c>
       <c r="H27" s="83"/>
       <c r="I27" s="33"/>
@@ -31482,13 +31754,13 @@
         <v>80</v>
       </c>
       <c r="E28" t="s" s="129">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="F28" t="s" s="15">
+        <v>415</v>
+      </c>
+      <c r="G28" t="s" s="133">
         <v>414</v>
-      </c>
-      <c r="G28" t="s" s="133">
-        <v>413</v>
       </c>
       <c r="H28" s="83"/>
       <c r="I28" s="33"/>
@@ -31751,13 +32023,13 @@
         <v>80</v>
       </c>
       <c r="E29" t="s" s="129">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="F29" t="s" s="15">
+        <v>415</v>
+      </c>
+      <c r="G29" t="s" s="133">
         <v>414</v>
-      </c>
-      <c r="G29" t="s" s="133">
-        <v>413</v>
       </c>
       <c r="H29" s="83"/>
       <c r="I29" s="33"/>
@@ -32020,13 +32292,13 @@
         <v>80</v>
       </c>
       <c r="E30" t="s" s="129">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="F30" t="s" s="15">
+        <v>415</v>
+      </c>
+      <c r="G30" t="s" s="133">
         <v>414</v>
-      </c>
-      <c r="G30" t="s" s="133">
-        <v>413</v>
       </c>
       <c r="H30" s="152"/>
       <c r="I30" s="94"/>
@@ -38164,7 +38436,7 @@
     </row>
     <row r="4" ht="14" customHeight="1">
       <c r="A4" s="18">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B4" s="24"/>
       <c r="C4" t="s" s="62">

</xml_diff>

<commit_message>
EM-2625: Update element details in spreadsheet for filename identifier
</commit_message>
<xml_diff>
--- a/src/aat/resources/adv_bundling_functional_tests_ccd_def.xlsx
+++ b/src/aat/resources/adv_bundling_functional_tests_ccd_def.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="427">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="428">
   <si>
     <t>Change History</t>
   </si>
@@ -1188,6 +1188,9 @@
   </si>
   <si>
     <t>fileNameIdentifier</t>
+  </si>
+  <si>
+    <t>Unique filename identifier</t>
   </si>
   <si>
     <t>Pagination Style</t>
@@ -13799,7 +13802,7 @@
       </c>
       <c r="F38" s="5"/>
       <c r="G38" t="s" s="41">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="H38" s="5"/>
       <c r="I38" s="5"/>
@@ -14070,7 +14073,7 @@
         <v>272</v>
       </c>
       <c r="G39" t="s" s="48">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="H39" s="47"/>
       <c r="I39" s="47"/>
@@ -14332,14 +14335,14 @@
         <v>79</v>
       </c>
       <c r="D40" t="s" s="48">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="E40" t="s" s="48">
         <v>61</v>
       </c>
       <c r="F40" s="48"/>
       <c r="G40" t="s" s="48">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="H40" s="47"/>
       <c r="I40" s="47"/>
@@ -14610,7 +14613,7 @@
         <v>267</v>
       </c>
       <c r="G41" t="s" s="48">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="H41" s="47"/>
       <c r="I41" s="47"/>
@@ -14872,14 +14875,14 @@
         <v>79</v>
       </c>
       <c r="D42" t="s" s="48">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="E42" t="s" s="48">
         <v>338</v>
       </c>
       <c r="F42" s="48"/>
       <c r="G42" t="s" s="48">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="H42" s="47"/>
       <c r="I42" s="47"/>
@@ -15141,7 +15144,7 @@
         <v>79</v>
       </c>
       <c r="D43" t="s" s="48">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="E43" t="s" s="48">
         <v>323</v>
@@ -15150,7 +15153,7 @@
         <v>323</v>
       </c>
       <c r="G43" t="s" s="48">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="H43" s="47"/>
       <c r="I43" s="47"/>
@@ -15412,14 +15415,14 @@
         <v>82</v>
       </c>
       <c r="D44" t="s" s="8">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="E44" t="s" s="8">
         <v>61</v>
       </c>
       <c r="F44" s="24"/>
       <c r="G44" t="s" s="8">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="H44" s="24"/>
       <c r="I44" s="24"/>
@@ -15681,14 +15684,14 @@
         <v>82</v>
       </c>
       <c r="D45" t="s" s="35">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="E45" t="s" s="35">
         <v>61</v>
       </c>
       <c r="F45" s="3"/>
       <c r="G45" t="s" s="35">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="H45" s="3"/>
       <c r="I45" s="3"/>
@@ -15950,7 +15953,7 @@
         <v>82</v>
       </c>
       <c r="D46" t="s" s="35">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="E46" t="s" s="35">
         <v>312</v>
@@ -16219,14 +16222,14 @@
         <v>82</v>
       </c>
       <c r="D47" t="s" s="35">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="E47" t="s" s="35">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="F47" s="3"/>
       <c r="G47" t="s" s="35">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="H47" s="3"/>
       <c r="I47" s="3"/>
@@ -16488,14 +16491,14 @@
         <v>82</v>
       </c>
       <c r="D48" t="s" s="35">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="E48" t="s" s="35">
         <v>61</v>
       </c>
       <c r="F48" s="3"/>
       <c r="G48" t="s" s="35">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="H48" s="3"/>
       <c r="I48" s="3"/>
@@ -16757,14 +16760,14 @@
         <v>82</v>
       </c>
       <c r="D49" t="s" s="35">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="E49" t="s" s="35">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="F49" s="3"/>
       <c r="G49" t="s" s="35">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="H49" s="3"/>
       <c r="I49" s="3"/>
@@ -17026,14 +17029,14 @@
         <v>82</v>
       </c>
       <c r="D50" t="s" s="35">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="E50" t="s" s="35">
         <v>61</v>
       </c>
       <c r="F50" s="3"/>
       <c r="G50" t="s" s="35">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="H50" s="3"/>
       <c r="I50" s="3"/>
@@ -17295,14 +17298,14 @@
         <v>82</v>
       </c>
       <c r="D51" t="s" s="35">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="E51" t="s" s="35">
         <v>61</v>
       </c>
       <c r="F51" s="3"/>
       <c r="G51" t="s" s="35">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="H51" s="3"/>
       <c r="I51" s="3"/>
@@ -17581,7 +17584,7 @@
   <sheetData>
     <row r="1" ht="18" customHeight="1">
       <c r="A1" t="s" s="11">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="B1" t="s" s="111">
         <v>11</v>
@@ -17610,13 +17613,13 @@
         <v>42</v>
       </c>
       <c r="D2" t="s" s="15">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="E2" t="s" s="15">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="F2" t="s" s="15">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="G2" s="114"/>
       <c r="H2" s="115"/>
@@ -17659,7 +17662,7 @@
         <v>59</v>
       </c>
       <c r="E4" t="s" s="120">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="F4" s="69">
         <v>1</v>
@@ -17681,7 +17684,7 @@
         <v>62</v>
       </c>
       <c r="E5" t="s" s="36">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="F5" s="4">
         <v>2</v>
@@ -17703,7 +17706,7 @@
         <v>64</v>
       </c>
       <c r="E6" t="s" s="36">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="F6" s="4">
         <v>3</v>
@@ -17794,7 +17797,7 @@
   <sheetData>
     <row r="1" ht="18" customHeight="1">
       <c r="A1" t="s" s="11">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="B1" t="s" s="12">
         <v>11</v>
@@ -17829,13 +17832,13 @@
         <v>42</v>
       </c>
       <c r="D2" t="s" s="15">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="E2" t="s" s="15">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="F2" t="s" s="15">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="G2" s="114"/>
       <c r="H2" s="115"/>
@@ -17890,7 +17893,7 @@
         <v>59</v>
       </c>
       <c r="E4" t="s" s="120">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="F4" s="69">
         <v>1</v>
@@ -17918,7 +17921,7 @@
         <v>62</v>
       </c>
       <c r="E5" t="s" s="36">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="F5" s="4">
         <v>2</v>
@@ -17946,7 +17949,7 @@
         <v>64</v>
       </c>
       <c r="E6" t="s" s="36">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="F6" s="4">
         <v>3</v>
@@ -18067,7 +18070,7 @@
   <sheetData>
     <row r="1" ht="18" customHeight="1">
       <c r="A1" t="s" s="11">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B1" t="s" s="12">
         <v>11</v>
@@ -18102,13 +18105,13 @@
         <v>42</v>
       </c>
       <c r="D2" t="s" s="15">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="E2" t="s" s="15">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="F2" t="s" s="15">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="G2" s="21"/>
       <c r="H2" s="22"/>
@@ -18163,7 +18166,7 @@
         <v>59</v>
       </c>
       <c r="E4" t="s" s="120">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="F4" s="69">
         <v>1</v>
@@ -18191,7 +18194,7 @@
         <v>62</v>
       </c>
       <c r="E5" t="s" s="36">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="F5" s="4">
         <v>2</v>
@@ -18219,7 +18222,7 @@
         <v>64</v>
       </c>
       <c r="E6" t="s" s="36">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="F6" s="4">
         <v>3</v>
@@ -18340,7 +18343,7 @@
   <sheetData>
     <row r="1" ht="19" customHeight="1">
       <c r="A1" t="s" s="11">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B1" t="s" s="111">
         <v>11</v>
@@ -18369,13 +18372,13 @@
         <v>42</v>
       </c>
       <c r="D2" t="s" s="15">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="E2" t="s" s="15">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="F2" t="s" s="15">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="G2" s="114"/>
       <c r="H2" s="115"/>
@@ -18418,7 +18421,7 @@
         <v>59</v>
       </c>
       <c r="E4" t="s" s="120">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="F4" s="69">
         <v>1</v>
@@ -18440,7 +18443,7 @@
         <v>62</v>
       </c>
       <c r="E5" t="s" s="36">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="F5" s="4">
         <v>2</v>
@@ -18462,7 +18465,7 @@
         <v>64</v>
       </c>
       <c r="E6" t="s" s="36">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="F6" s="4">
         <v>3</v>
@@ -18555,7 +18558,7 @@
   <sheetData>
     <row r="1" ht="18" customHeight="1">
       <c r="A1" t="s" s="11">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B1" t="s" s="12">
         <v>11</v>
@@ -18588,13 +18591,13 @@
       </c>
       <c r="C2" s="66"/>
       <c r="D2" t="s" s="15">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="E2" t="s" s="15">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="F2" t="s" s="15">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="G2" s="14"/>
       <c r="H2" s="3"/>
@@ -18615,16 +18618,16 @@
         <v>20</v>
       </c>
       <c r="C3" t="s" s="6">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="D3" t="s" s="6">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="E3" t="s" s="6">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="F3" t="s" s="6">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="G3" s="16"/>
       <c r="H3" s="17"/>
@@ -18643,7 +18646,7 @@
       </c>
       <c r="B4" s="98"/>
       <c r="C4" t="s" s="128">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="D4" t="s" s="128">
         <v>24</v>
@@ -18671,7 +18674,7 @@
       </c>
       <c r="B5" s="77"/>
       <c r="C5" t="s" s="129">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="D5" t="s" s="129">
         <v>24</v>
@@ -18699,7 +18702,7 @@
       </c>
       <c r="B6" s="77"/>
       <c r="C6" t="s" s="129">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="D6" t="s" s="129">
         <v>24</v>
@@ -18727,7 +18730,7 @@
       </c>
       <c r="B7" s="102"/>
       <c r="C7" t="s" s="130">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="D7" t="s" s="130">
         <v>24</v>
@@ -18755,7 +18758,7 @@
       </c>
       <c r="B8" s="131"/>
       <c r="C8" t="s" s="12">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="D8" t="s" s="12">
         <v>24</v>
@@ -18836,7 +18839,7 @@
   <sheetData>
     <row r="1" ht="18" customHeight="1">
       <c r="A1" t="s" s="11">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="B1" t="s" s="12">
         <v>11</v>
@@ -18867,13 +18870,13 @@
         <v>15</v>
       </c>
       <c r="C2" t="s" s="15">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="D2" t="s" s="15">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="E2" t="s" s="15">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="F2" s="21"/>
       <c r="G2" s="22"/>
@@ -18897,10 +18900,10 @@
         <v>51</v>
       </c>
       <c r="D3" t="s" s="6">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="E3" t="s" s="6">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="F3" s="14"/>
       <c r="G3" s="3"/>
@@ -18922,10 +18925,10 @@
         <v>37</v>
       </c>
       <c r="D4" t="s" s="15">
+        <v>416</v>
+      </c>
+      <c r="E4" t="s" s="133">
         <v>415</v>
-      </c>
-      <c r="E4" t="s" s="133">
-        <v>414</v>
       </c>
       <c r="F4" s="14"/>
       <c r="G4" s="3"/>
@@ -19066,7 +19069,7 @@
   <sheetData>
     <row r="1" ht="18" customHeight="1">
       <c r="A1" t="s" s="11">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="B1" t="s" s="12">
         <v>11</v>
@@ -19337,16 +19340,16 @@
         <v>15</v>
       </c>
       <c r="C2" t="s" s="15">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="D2" t="s" s="15">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="E2" t="s" s="15">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="F2" t="s" s="15">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="G2" s="14"/>
       <c r="H2" s="3"/>
@@ -19612,10 +19615,10 @@
         <v>107</v>
       </c>
       <c r="E3" t="s" s="6">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="F3" t="s" s="6">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="G3" s="16"/>
       <c r="H3" s="3"/>
@@ -19879,10 +19882,10 @@
         <v>59</v>
       </c>
       <c r="E4" t="s" s="136">
+        <v>416</v>
+      </c>
+      <c r="F4" t="s" s="133">
         <v>415</v>
-      </c>
-      <c r="F4" t="s" s="133">
-        <v>414</v>
       </c>
       <c r="G4" s="14"/>
       <c r="H4" s="3"/>
@@ -20146,10 +20149,10 @@
         <v>62</v>
       </c>
       <c r="E5" t="s" s="138">
+        <v>416</v>
+      </c>
+      <c r="F5" t="s" s="133">
         <v>415</v>
-      </c>
-      <c r="F5" t="s" s="133">
-        <v>414</v>
       </c>
       <c r="G5" s="14"/>
       <c r="H5" s="3"/>
@@ -20413,10 +20416,10 @@
         <v>64</v>
       </c>
       <c r="E6" t="s" s="138">
+        <v>416</v>
+      </c>
+      <c r="F6" t="s" s="133">
         <v>415</v>
-      </c>
-      <c r="F6" t="s" s="133">
-        <v>414</v>
       </c>
       <c r="G6" s="14"/>
       <c r="H6" s="3"/>
@@ -20680,10 +20683,10 @@
         <v>66</v>
       </c>
       <c r="E7" t="s" s="138">
+        <v>416</v>
+      </c>
+      <c r="F7" t="s" s="133">
         <v>415</v>
-      </c>
-      <c r="F7" t="s" s="133">
-        <v>414</v>
       </c>
       <c r="G7" s="14"/>
       <c r="H7" s="3"/>
@@ -20947,10 +20950,10 @@
         <v>68</v>
       </c>
       <c r="E8" t="s" s="138">
+        <v>416</v>
+      </c>
+      <c r="F8" t="s" s="133">
         <v>415</v>
-      </c>
-      <c r="F8" t="s" s="133">
-        <v>414</v>
       </c>
       <c r="G8" s="14"/>
       <c r="H8" s="3"/>
@@ -21214,10 +21217,10 @@
         <v>71</v>
       </c>
       <c r="E9" t="s" s="138">
+        <v>416</v>
+      </c>
+      <c r="F9" t="s" s="133">
         <v>415</v>
-      </c>
-      <c r="F9" t="s" s="133">
-        <v>414</v>
       </c>
       <c r="G9" s="14"/>
       <c r="H9" s="3"/>
@@ -21481,10 +21484,10 @@
         <v>75</v>
       </c>
       <c r="E10" t="s" s="138">
+        <v>416</v>
+      </c>
+      <c r="F10" t="s" s="133">
         <v>415</v>
-      </c>
-      <c r="F10" t="s" s="133">
-        <v>414</v>
       </c>
       <c r="G10" s="14"/>
       <c r="H10" s="3"/>
@@ -21748,10 +21751,10 @@
         <v>80</v>
       </c>
       <c r="E11" t="s" s="138">
+        <v>416</v>
+      </c>
+      <c r="F11" t="s" s="133">
         <v>415</v>
-      </c>
-      <c r="F11" t="s" s="133">
-        <v>414</v>
       </c>
       <c r="G11" s="14"/>
       <c r="H11" s="3"/>
@@ -22015,10 +22018,10 @@
         <v>83</v>
       </c>
       <c r="E12" t="s" s="140">
+        <v>416</v>
+      </c>
+      <c r="F12" t="s" s="133">
         <v>415</v>
-      </c>
-      <c r="F12" t="s" s="133">
-        <v>414</v>
       </c>
       <c r="G12" s="14"/>
       <c r="H12" s="3"/>
@@ -22282,10 +22285,10 @@
         <v>84</v>
       </c>
       <c r="E13" t="s" s="136">
+        <v>416</v>
+      </c>
+      <c r="F13" t="s" s="133">
         <v>415</v>
-      </c>
-      <c r="F13" t="s" s="133">
-        <v>414</v>
       </c>
       <c r="G13" s="14"/>
       <c r="H13" s="3"/>
@@ -22549,10 +22552,10 @@
         <v>86</v>
       </c>
       <c r="E14" t="s" s="138">
+        <v>416</v>
+      </c>
+      <c r="F14" t="s" s="133">
         <v>415</v>
-      </c>
-      <c r="F14" t="s" s="133">
-        <v>414</v>
       </c>
       <c r="G14" s="14"/>
       <c r="H14" s="3"/>
@@ -22816,10 +22819,10 @@
         <v>88</v>
       </c>
       <c r="E15" t="s" s="138">
+        <v>416</v>
+      </c>
+      <c r="F15" t="s" s="133">
         <v>415</v>
-      </c>
-      <c r="F15" t="s" s="133">
-        <v>414</v>
       </c>
       <c r="G15" s="14"/>
       <c r="H15" s="3"/>
@@ -23083,10 +23086,10 @@
         <v>90</v>
       </c>
       <c r="E16" t="s" s="138">
+        <v>416</v>
+      </c>
+      <c r="F16" t="s" s="133">
         <v>415</v>
-      </c>
-      <c r="F16" t="s" s="133">
-        <v>414</v>
       </c>
       <c r="G16" s="14"/>
       <c r="H16" s="3"/>
@@ -23350,10 +23353,10 @@
         <v>92</v>
       </c>
       <c r="E17" t="s" s="138">
+        <v>416</v>
+      </c>
+      <c r="F17" t="s" s="133">
         <v>415</v>
-      </c>
-      <c r="F17" t="s" s="133">
-        <v>414</v>
       </c>
       <c r="G17" s="14"/>
       <c r="H17" s="3"/>
@@ -23628,7 +23631,7 @@
   <sheetData>
     <row r="1" ht="18" customHeight="1">
       <c r="A1" t="s" s="11">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="B1" t="s" s="12">
         <v>11</v>
@@ -23659,16 +23662,16 @@
         <v>15</v>
       </c>
       <c r="C2" t="s" s="15">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="D2" t="s" s="15">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="E2" t="s" s="15">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="F2" t="s" s="15">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="G2" s="21"/>
       <c r="H2" s="22"/>
@@ -23694,10 +23697,10 @@
         <v>201</v>
       </c>
       <c r="E3" t="s" s="12">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="F3" t="s" s="12">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="G3" s="14"/>
       <c r="H3" s="22"/>
@@ -23721,10 +23724,10 @@
         <v>154</v>
       </c>
       <c r="E4" t="s" s="144">
+        <v>416</v>
+      </c>
+      <c r="F4" t="s" s="133">
         <v>415</v>
-      </c>
-      <c r="F4" t="s" s="133">
-        <v>414</v>
       </c>
       <c r="G4" s="14"/>
       <c r="H4" s="3"/>
@@ -23748,10 +23751,10 @@
         <v>158</v>
       </c>
       <c r="E5" t="s" s="146">
+        <v>416</v>
+      </c>
+      <c r="F5" t="s" s="133">
         <v>415</v>
-      </c>
-      <c r="F5" t="s" s="133">
-        <v>414</v>
       </c>
       <c r="G5" s="14"/>
       <c r="H5" s="3"/>
@@ -23775,10 +23778,10 @@
         <v>162</v>
       </c>
       <c r="E6" t="s" s="146">
+        <v>416</v>
+      </c>
+      <c r="F6" t="s" s="133">
         <v>415</v>
-      </c>
-      <c r="F6" t="s" s="133">
-        <v>414</v>
       </c>
       <c r="G6" s="14"/>
       <c r="H6" s="3"/>
@@ -23802,10 +23805,10 @@
         <v>166</v>
       </c>
       <c r="E7" t="s" s="146">
+        <v>416</v>
+      </c>
+      <c r="F7" t="s" s="133">
         <v>415</v>
-      </c>
-      <c r="F7" t="s" s="133">
-        <v>414</v>
       </c>
       <c r="G7" s="14"/>
       <c r="H7" s="3"/>
@@ -23829,10 +23832,10 @@
         <v>173</v>
       </c>
       <c r="E8" t="s" s="146">
+        <v>416</v>
+      </c>
+      <c r="F8" t="s" s="133">
         <v>415</v>
-      </c>
-      <c r="F8" t="s" s="133">
-        <v>414</v>
       </c>
       <c r="G8" s="14"/>
       <c r="H8" s="3"/>
@@ -23856,10 +23859,10 @@
         <v>169</v>
       </c>
       <c r="E9" t="s" s="146">
+        <v>416</v>
+      </c>
+      <c r="F9" t="s" s="133">
         <v>415</v>
-      </c>
-      <c r="F9" t="s" s="133">
-        <v>414</v>
       </c>
       <c r="G9" s="14"/>
       <c r="H9" s="3"/>
@@ -23883,10 +23886,10 @@
         <v>177</v>
       </c>
       <c r="E10" t="s" s="146">
+        <v>416</v>
+      </c>
+      <c r="F10" t="s" s="133">
         <v>415</v>
-      </c>
-      <c r="F10" t="s" s="133">
-        <v>414</v>
       </c>
       <c r="G10" s="14"/>
       <c r="H10" s="3"/>
@@ -23910,10 +23913,10 @@
         <v>184</v>
       </c>
       <c r="E11" t="s" s="146">
+        <v>416</v>
+      </c>
+      <c r="F11" t="s" s="133">
         <v>415</v>
-      </c>
-      <c r="F11" t="s" s="133">
-        <v>414</v>
       </c>
       <c r="G11" s="14"/>
       <c r="H11" s="3"/>
@@ -23937,10 +23940,10 @@
         <v>187</v>
       </c>
       <c r="E12" t="s" s="146">
+        <v>416</v>
+      </c>
+      <c r="F12" t="s" s="133">
         <v>415</v>
-      </c>
-      <c r="F12" t="s" s="133">
-        <v>414</v>
       </c>
       <c r="G12" s="14"/>
       <c r="H12" s="3"/>
@@ -24009,7 +24012,7 @@
   <sheetData>
     <row r="1" ht="18" customHeight="1">
       <c r="A1" t="s" s="11">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="B1" t="s" s="12">
         <v>11</v>
@@ -24041,16 +24044,16 @@
         <v>15</v>
       </c>
       <c r="C2" t="s" s="15">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="D2" t="s" s="15">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="E2" t="s" s="15">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="F2" t="s" s="15">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="G2" s="21"/>
       <c r="H2" s="22"/>
@@ -24074,13 +24077,13 @@
         <v>51</v>
       </c>
       <c r="D3" t="s" s="12">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="E3" t="s" s="12">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="F3" t="s" s="12">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="G3" s="14"/>
       <c r="H3" s="3"/>
@@ -24105,10 +24108,10 @@
         <v>126</v>
       </c>
       <c r="E4" t="s" s="15">
+        <v>416</v>
+      </c>
+      <c r="F4" t="s" s="133">
         <v>415</v>
-      </c>
-      <c r="F4" t="s" s="133">
-        <v>414</v>
       </c>
       <c r="G4" s="14"/>
       <c r="H4" s="3"/>
@@ -24485,7 +24488,7 @@
   <sheetData>
     <row r="1" ht="18" customHeight="1">
       <c r="A1" t="s" s="11">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="B1" t="s" s="12">
         <v>11</v>
@@ -24752,19 +24755,19 @@
       <c r="A2" s="66"/>
       <c r="B2" s="66"/>
       <c r="C2" t="s" s="15">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="D2" t="s" s="15">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="E2" t="s" s="15">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="F2" t="s" s="15">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="G2" t="s" s="15">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="H2" s="83"/>
       <c r="I2" s="33"/>
@@ -25032,10 +25035,10 @@
         <v>224</v>
       </c>
       <c r="F3" t="s" s="12">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="G3" t="s" s="12">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="H3" s="83"/>
       <c r="I3" s="33"/>
@@ -25301,10 +25304,10 @@
         <v>333</v>
       </c>
       <c r="F4" t="s" s="15">
+        <v>416</v>
+      </c>
+      <c r="G4" t="s" s="133">
         <v>415</v>
-      </c>
-      <c r="G4" t="s" s="133">
-        <v>414</v>
       </c>
       <c r="H4" s="83"/>
       <c r="I4" s="33"/>
@@ -25570,10 +25573,10 @@
         <v>335</v>
       </c>
       <c r="F5" t="s" s="15">
+        <v>416</v>
+      </c>
+      <c r="G5" t="s" s="133">
         <v>415</v>
-      </c>
-      <c r="G5" t="s" s="133">
-        <v>414</v>
       </c>
       <c r="H5" s="83"/>
       <c r="I5" s="33"/>
@@ -25839,10 +25842,10 @@
         <v>310</v>
       </c>
       <c r="F6" t="s" s="15">
+        <v>416</v>
+      </c>
+      <c r="G6" t="s" s="133">
         <v>415</v>
-      </c>
-      <c r="G6" t="s" s="133">
-        <v>414</v>
       </c>
       <c r="H6" s="83"/>
       <c r="I6" s="33"/>
@@ -26108,10 +26111,10 @@
         <v>337</v>
       </c>
       <c r="F7" t="s" s="15">
+        <v>416</v>
+      </c>
+      <c r="G7" t="s" s="133">
         <v>415</v>
-      </c>
-      <c r="G7" t="s" s="133">
-        <v>414</v>
       </c>
       <c r="H7" s="83"/>
       <c r="I7" s="33"/>
@@ -26377,10 +26380,10 @@
         <v>340</v>
       </c>
       <c r="F8" t="s" s="15">
+        <v>416</v>
+      </c>
+      <c r="G8" t="s" s="133">
         <v>415</v>
-      </c>
-      <c r="G8" t="s" s="133">
-        <v>414</v>
       </c>
       <c r="H8" s="83"/>
       <c r="I8" s="33"/>
@@ -26646,10 +26649,10 @@
         <v>316</v>
       </c>
       <c r="F9" t="s" s="15">
+        <v>416</v>
+      </c>
+      <c r="G9" t="s" s="133">
         <v>415</v>
-      </c>
-      <c r="G9" t="s" s="133">
-        <v>414</v>
       </c>
       <c r="H9" s="83"/>
       <c r="I9" s="33"/>
@@ -26915,10 +26918,10 @@
         <v>319</v>
       </c>
       <c r="F10" t="s" s="15">
+        <v>416</v>
+      </c>
+      <c r="G10" t="s" s="133">
         <v>415</v>
-      </c>
-      <c r="G10" t="s" s="133">
-        <v>414</v>
       </c>
       <c r="H10" s="83"/>
       <c r="I10" s="33"/>
@@ -27184,10 +27187,10 @@
         <v>344</v>
       </c>
       <c r="F11" t="s" s="15">
+        <v>416</v>
+      </c>
+      <c r="G11" t="s" s="133">
         <v>415</v>
-      </c>
-      <c r="G11" t="s" s="133">
-        <v>414</v>
       </c>
       <c r="H11" s="83"/>
       <c r="I11" s="33"/>
@@ -27453,10 +27456,10 @@
         <v>346</v>
       </c>
       <c r="F12" t="s" s="15">
+        <v>416</v>
+      </c>
+      <c r="G12" t="s" s="133">
         <v>415</v>
-      </c>
-      <c r="G12" t="s" s="133">
-        <v>414</v>
       </c>
       <c r="H12" s="83"/>
       <c r="I12" s="33"/>
@@ -27722,10 +27725,10 @@
         <v>348</v>
       </c>
       <c r="F13" t="s" s="15">
+        <v>416</v>
+      </c>
+      <c r="G13" t="s" s="133">
         <v>415</v>
-      </c>
-      <c r="G13" t="s" s="133">
-        <v>414</v>
       </c>
       <c r="H13" s="83"/>
       <c r="I13" s="33"/>
@@ -27991,10 +27994,10 @@
         <v>352</v>
       </c>
       <c r="F14" t="s" s="15">
+        <v>416</v>
+      </c>
+      <c r="G14" t="s" s="133">
         <v>415</v>
-      </c>
-      <c r="G14" t="s" s="133">
-        <v>414</v>
       </c>
       <c r="H14" s="83"/>
       <c r="I14" s="33"/>
@@ -28260,10 +28263,10 @@
         <v>350</v>
       </c>
       <c r="F15" t="s" s="15">
+        <v>416</v>
+      </c>
+      <c r="G15" t="s" s="133">
         <v>415</v>
-      </c>
-      <c r="G15" t="s" s="133">
-        <v>414</v>
       </c>
       <c r="H15" s="83"/>
       <c r="I15" s="33"/>
@@ -28529,10 +28532,10 @@
         <v>272</v>
       </c>
       <c r="F16" t="s" s="15">
+        <v>416</v>
+      </c>
+      <c r="G16" t="s" s="133">
         <v>415</v>
-      </c>
-      <c r="G16" t="s" s="133">
-        <v>414</v>
       </c>
       <c r="H16" s="83"/>
       <c r="I16" s="33"/>
@@ -28798,10 +28801,10 @@
         <v>267</v>
       </c>
       <c r="F17" t="s" s="15">
+        <v>416</v>
+      </c>
+      <c r="G17" t="s" s="133">
         <v>415</v>
-      </c>
-      <c r="G17" t="s" s="133">
-        <v>414</v>
       </c>
       <c r="H17" s="83"/>
       <c r="I17" s="33"/>
@@ -29067,10 +29070,10 @@
         <v>354</v>
       </c>
       <c r="F18" t="s" s="15">
+        <v>416</v>
+      </c>
+      <c r="G18" t="s" s="133">
         <v>415</v>
-      </c>
-      <c r="G18" t="s" s="133">
-        <v>414</v>
       </c>
       <c r="H18" s="83"/>
       <c r="I18" s="33"/>
@@ -29333,13 +29336,13 @@
         <v>75</v>
       </c>
       <c r="E19" t="s" s="129">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="F19" t="s" s="15">
+        <v>416</v>
+      </c>
+      <c r="G19" t="s" s="133">
         <v>415</v>
-      </c>
-      <c r="G19" t="s" s="133">
-        <v>414</v>
       </c>
       <c r="H19" s="83"/>
       <c r="I19" s="33"/>
@@ -29602,13 +29605,13 @@
         <v>75</v>
       </c>
       <c r="E20" t="s" s="129">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="F20" t="s" s="15">
+        <v>416</v>
+      </c>
+      <c r="G20" t="s" s="133">
         <v>415</v>
-      </c>
-      <c r="G20" t="s" s="133">
-        <v>414</v>
       </c>
       <c r="H20" s="83"/>
       <c r="I20" s="33"/>
@@ -29871,13 +29874,13 @@
         <v>75</v>
       </c>
       <c r="E21" t="s" s="129">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="F21" t="s" s="15">
+        <v>416</v>
+      </c>
+      <c r="G21" t="s" s="133">
         <v>415</v>
-      </c>
-      <c r="G21" t="s" s="133">
-        <v>414</v>
       </c>
       <c r="H21" s="83"/>
       <c r="I21" s="33"/>
@@ -30143,10 +30146,10 @@
         <v>356</v>
       </c>
       <c r="F22" t="s" s="15">
+        <v>416</v>
+      </c>
+      <c r="G22" t="s" s="133">
         <v>415</v>
-      </c>
-      <c r="G22" t="s" s="133">
-        <v>414</v>
       </c>
       <c r="H22" s="83"/>
       <c r="I22" s="33"/>
@@ -30409,13 +30412,13 @@
         <v>80</v>
       </c>
       <c r="E23" t="s" s="128">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="F23" t="s" s="15">
+        <v>416</v>
+      </c>
+      <c r="G23" t="s" s="133">
         <v>415</v>
-      </c>
-      <c r="G23" t="s" s="133">
-        <v>414</v>
       </c>
       <c r="H23" s="83"/>
       <c r="I23" s="33"/>
@@ -30678,13 +30681,13 @@
         <v>80</v>
       </c>
       <c r="E24" t="s" s="129">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="F24" t="s" s="15">
+        <v>416</v>
+      </c>
+      <c r="G24" t="s" s="133">
         <v>415</v>
-      </c>
-      <c r="G24" t="s" s="133">
-        <v>414</v>
       </c>
       <c r="H24" s="83"/>
       <c r="I24" s="33"/>
@@ -30947,13 +30950,13 @@
         <v>80</v>
       </c>
       <c r="E25" t="s" s="129">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="F25" t="s" s="15">
+        <v>416</v>
+      </c>
+      <c r="G25" t="s" s="133">
         <v>415</v>
-      </c>
-      <c r="G25" t="s" s="133">
-        <v>414</v>
       </c>
       <c r="H25" s="83"/>
       <c r="I25" s="33"/>
@@ -31216,13 +31219,13 @@
         <v>80</v>
       </c>
       <c r="E26" t="s" s="129">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="F26" t="s" s="15">
+        <v>416</v>
+      </c>
+      <c r="G26" t="s" s="133">
         <v>415</v>
-      </c>
-      <c r="G26" t="s" s="133">
-        <v>414</v>
       </c>
       <c r="H26" s="83"/>
       <c r="I26" s="33"/>
@@ -31485,13 +31488,13 @@
         <v>80</v>
       </c>
       <c r="E27" t="s" s="129">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="F27" t="s" s="15">
+        <v>416</v>
+      </c>
+      <c r="G27" t="s" s="133">
         <v>415</v>
-      </c>
-      <c r="G27" t="s" s="133">
-        <v>414</v>
       </c>
       <c r="H27" s="83"/>
       <c r="I27" s="33"/>
@@ -31754,13 +31757,13 @@
         <v>80</v>
       </c>
       <c r="E28" t="s" s="129">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="F28" t="s" s="15">
+        <v>416</v>
+      </c>
+      <c r="G28" t="s" s="133">
         <v>415</v>
-      </c>
-      <c r="G28" t="s" s="133">
-        <v>414</v>
       </c>
       <c r="H28" s="83"/>
       <c r="I28" s="33"/>
@@ -32023,13 +32026,13 @@
         <v>80</v>
       </c>
       <c r="E29" t="s" s="129">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="F29" t="s" s="15">
+        <v>416</v>
+      </c>
+      <c r="G29" t="s" s="133">
         <v>415</v>
-      </c>
-      <c r="G29" t="s" s="133">
-        <v>414</v>
       </c>
       <c r="H29" s="83"/>
       <c r="I29" s="33"/>
@@ -32292,13 +32295,13 @@
         <v>80</v>
       </c>
       <c r="E30" t="s" s="129">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="F30" t="s" s="15">
+        <v>416</v>
+      </c>
+      <c r="G30" t="s" s="133">
         <v>415</v>
-      </c>
-      <c r="G30" t="s" s="133">
-        <v>414</v>
       </c>
       <c r="H30" s="152"/>
       <c r="I30" s="94"/>
@@ -38436,7 +38439,7 @@
     </row>
     <row r="4" ht="14" customHeight="1">
       <c r="A4" s="18">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B4" s="24"/>
       <c r="C4" t="s" s="62">

</xml_diff>

<commit_message>
EM-2625: Alter spreadsheet to add new field in the authorisation complex type table
</commit_message>
<xml_diff>
--- a/src/aat/resources/adv_bundling_functional_tests_ccd_def.xlsx
+++ b/src/aat/resources/adv_bundling_functional_tests_ccd_def.xlsx
@@ -24470,7 +24470,7 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:IU30"/>
+  <dimension ref="A1:IU31"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -30142,7 +30142,7 @@
       <c r="D22" t="s" s="12">
         <v>75</v>
       </c>
-      <c r="E22" t="s" s="130">
+      <c r="E22" t="s" s="129">
         <v>356</v>
       </c>
       <c r="F22" t="s" s="15">
@@ -30409,10 +30409,10 @@
         <v>37</v>
       </c>
       <c r="D23" t="s" s="12">
-        <v>80</v>
-      </c>
-      <c r="E23" t="s" s="128">
-        <v>368</v>
+        <v>75</v>
+      </c>
+      <c r="E23" t="s" s="130">
+        <v>358</v>
       </c>
       <c r="F23" t="s" s="15">
         <v>416</v>
@@ -30680,8 +30680,8 @@
       <c r="D24" t="s" s="12">
         <v>80</v>
       </c>
-      <c r="E24" t="s" s="129">
-        <v>370</v>
+      <c r="E24" t="s" s="128">
+        <v>368</v>
       </c>
       <c r="F24" t="s" s="15">
         <v>416</v>
@@ -30950,7 +30950,7 @@
         <v>80</v>
       </c>
       <c r="E25" t="s" s="129">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="F25" t="s" s="15">
         <v>416</v>
@@ -31219,7 +31219,7 @@
         <v>80</v>
       </c>
       <c r="E26" t="s" s="129">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="F26" t="s" s="15">
         <v>416</v>
@@ -31488,7 +31488,7 @@
         <v>80</v>
       </c>
       <c r="E27" t="s" s="129">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="F27" t="s" s="15">
         <v>416</v>
@@ -31745,7 +31745,7 @@
       <c r="IT27" s="33"/>
       <c r="IU27" s="84"/>
     </row>
-    <row r="28" ht="18.75" customHeight="1">
+    <row r="28" ht="28" customHeight="1">
       <c r="A28" s="108">
         <v>42736</v>
       </c>
@@ -31757,7 +31757,7 @@
         <v>80</v>
       </c>
       <c r="E28" t="s" s="129">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="F28" t="s" s="15">
         <v>416</v>
@@ -32026,7 +32026,7 @@
         <v>80</v>
       </c>
       <c r="E29" t="s" s="129">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="F29" t="s" s="15">
         <v>416</v>
@@ -32295,7 +32295,7 @@
         <v>80</v>
       </c>
       <c r="E30" t="s" s="129">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="F30" t="s" s="15">
         <v>416</v>
@@ -32303,254 +32303,523 @@
       <c r="G30" t="s" s="133">
         <v>415</v>
       </c>
-      <c r="H30" s="152"/>
-      <c r="I30" s="94"/>
-      <c r="J30" s="94"/>
-      <c r="K30" s="94"/>
-      <c r="L30" s="94"/>
-      <c r="M30" s="94"/>
-      <c r="N30" s="94"/>
-      <c r="O30" s="94"/>
-      <c r="P30" s="94"/>
-      <c r="Q30" s="94"/>
-      <c r="R30" s="94"/>
-      <c r="S30" s="94"/>
-      <c r="T30" s="94"/>
-      <c r="U30" s="94"/>
-      <c r="V30" s="94"/>
-      <c r="W30" s="94"/>
-      <c r="X30" s="94"/>
-      <c r="Y30" s="94"/>
-      <c r="Z30" s="94"/>
-      <c r="AA30" s="94"/>
-      <c r="AB30" s="94"/>
-      <c r="AC30" s="94"/>
-      <c r="AD30" s="94"/>
-      <c r="AE30" s="94"/>
-      <c r="AF30" s="94"/>
-      <c r="AG30" s="94"/>
-      <c r="AH30" s="94"/>
-      <c r="AI30" s="94"/>
-      <c r="AJ30" s="94"/>
-      <c r="AK30" s="94"/>
-      <c r="AL30" s="94"/>
-      <c r="AM30" s="94"/>
-      <c r="AN30" s="94"/>
-      <c r="AO30" s="94"/>
-      <c r="AP30" s="94"/>
-      <c r="AQ30" s="94"/>
-      <c r="AR30" s="94"/>
-      <c r="AS30" s="94"/>
-      <c r="AT30" s="94"/>
-      <c r="AU30" s="94"/>
-      <c r="AV30" s="94"/>
-      <c r="AW30" s="94"/>
-      <c r="AX30" s="94"/>
-      <c r="AY30" s="94"/>
-      <c r="AZ30" s="94"/>
-      <c r="BA30" s="94"/>
-      <c r="BB30" s="94"/>
-      <c r="BC30" s="94"/>
-      <c r="BD30" s="94"/>
-      <c r="BE30" s="94"/>
-      <c r="BF30" s="94"/>
-      <c r="BG30" s="94"/>
-      <c r="BH30" s="94"/>
-      <c r="BI30" s="94"/>
-      <c r="BJ30" s="94"/>
-      <c r="BK30" s="94"/>
-      <c r="BL30" s="94"/>
-      <c r="BM30" s="94"/>
-      <c r="BN30" s="94"/>
-      <c r="BO30" s="94"/>
-      <c r="BP30" s="94"/>
-      <c r="BQ30" s="94"/>
-      <c r="BR30" s="94"/>
-      <c r="BS30" s="94"/>
-      <c r="BT30" s="94"/>
-      <c r="BU30" s="94"/>
-      <c r="BV30" s="94"/>
-      <c r="BW30" s="94"/>
-      <c r="BX30" s="94"/>
-      <c r="BY30" s="94"/>
-      <c r="BZ30" s="94"/>
-      <c r="CA30" s="94"/>
-      <c r="CB30" s="94"/>
-      <c r="CC30" s="94"/>
-      <c r="CD30" s="94"/>
-      <c r="CE30" s="94"/>
-      <c r="CF30" s="94"/>
-      <c r="CG30" s="94"/>
-      <c r="CH30" s="94"/>
-      <c r="CI30" s="94"/>
-      <c r="CJ30" s="94"/>
-      <c r="CK30" s="94"/>
-      <c r="CL30" s="94"/>
-      <c r="CM30" s="94"/>
-      <c r="CN30" s="94"/>
-      <c r="CO30" s="94"/>
-      <c r="CP30" s="94"/>
-      <c r="CQ30" s="94"/>
-      <c r="CR30" s="94"/>
-      <c r="CS30" s="94"/>
-      <c r="CT30" s="94"/>
-      <c r="CU30" s="94"/>
-      <c r="CV30" s="94"/>
-      <c r="CW30" s="94"/>
-      <c r="CX30" s="94"/>
-      <c r="CY30" s="94"/>
-      <c r="CZ30" s="94"/>
-      <c r="DA30" s="94"/>
-      <c r="DB30" s="94"/>
-      <c r="DC30" s="94"/>
-      <c r="DD30" s="94"/>
-      <c r="DE30" s="94"/>
-      <c r="DF30" s="94"/>
-      <c r="DG30" s="94"/>
-      <c r="DH30" s="94"/>
-      <c r="DI30" s="94"/>
-      <c r="DJ30" s="94"/>
-      <c r="DK30" s="94"/>
-      <c r="DL30" s="94"/>
-      <c r="DM30" s="94"/>
-      <c r="DN30" s="94"/>
-      <c r="DO30" s="94"/>
-      <c r="DP30" s="94"/>
-      <c r="DQ30" s="94"/>
-      <c r="DR30" s="94"/>
-      <c r="DS30" s="94"/>
-      <c r="DT30" s="94"/>
-      <c r="DU30" s="94"/>
-      <c r="DV30" s="94"/>
-      <c r="DW30" s="94"/>
-      <c r="DX30" s="94"/>
-      <c r="DY30" s="94"/>
-      <c r="DZ30" s="94"/>
-      <c r="EA30" s="94"/>
-      <c r="EB30" s="94"/>
-      <c r="EC30" s="94"/>
-      <c r="ED30" s="94"/>
-      <c r="EE30" s="94"/>
-      <c r="EF30" s="94"/>
-      <c r="EG30" s="94"/>
-      <c r="EH30" s="94"/>
-      <c r="EI30" s="94"/>
-      <c r="EJ30" s="94"/>
-      <c r="EK30" s="94"/>
-      <c r="EL30" s="94"/>
-      <c r="EM30" s="94"/>
-      <c r="EN30" s="94"/>
-      <c r="EO30" s="94"/>
-      <c r="EP30" s="94"/>
-      <c r="EQ30" s="94"/>
-      <c r="ER30" s="94"/>
-      <c r="ES30" s="94"/>
-      <c r="ET30" s="94"/>
-      <c r="EU30" s="94"/>
-      <c r="EV30" s="94"/>
-      <c r="EW30" s="94"/>
-      <c r="EX30" s="94"/>
-      <c r="EY30" s="94"/>
-      <c r="EZ30" s="94"/>
-      <c r="FA30" s="94"/>
-      <c r="FB30" s="94"/>
-      <c r="FC30" s="94"/>
-      <c r="FD30" s="94"/>
-      <c r="FE30" s="94"/>
-      <c r="FF30" s="94"/>
-      <c r="FG30" s="94"/>
-      <c r="FH30" s="94"/>
-      <c r="FI30" s="94"/>
-      <c r="FJ30" s="94"/>
-      <c r="FK30" s="94"/>
-      <c r="FL30" s="94"/>
-      <c r="FM30" s="94"/>
-      <c r="FN30" s="94"/>
-      <c r="FO30" s="94"/>
-      <c r="FP30" s="94"/>
-      <c r="FQ30" s="94"/>
-      <c r="FR30" s="94"/>
-      <c r="FS30" s="94"/>
-      <c r="FT30" s="94"/>
-      <c r="FU30" s="94"/>
-      <c r="FV30" s="94"/>
-      <c r="FW30" s="94"/>
-      <c r="FX30" s="94"/>
-      <c r="FY30" s="94"/>
-      <c r="FZ30" s="94"/>
-      <c r="GA30" s="94"/>
-      <c r="GB30" s="94"/>
-      <c r="GC30" s="94"/>
-      <c r="GD30" s="94"/>
-      <c r="GE30" s="94"/>
-      <c r="GF30" s="94"/>
-      <c r="GG30" s="94"/>
-      <c r="GH30" s="94"/>
-      <c r="GI30" s="94"/>
-      <c r="GJ30" s="94"/>
-      <c r="GK30" s="94"/>
-      <c r="GL30" s="94"/>
-      <c r="GM30" s="94"/>
-      <c r="GN30" s="94"/>
-      <c r="GO30" s="94"/>
-      <c r="GP30" s="94"/>
-      <c r="GQ30" s="94"/>
-      <c r="GR30" s="94"/>
-      <c r="GS30" s="94"/>
-      <c r="GT30" s="94"/>
-      <c r="GU30" s="94"/>
-      <c r="GV30" s="94"/>
-      <c r="GW30" s="94"/>
-      <c r="GX30" s="94"/>
-      <c r="GY30" s="94"/>
-      <c r="GZ30" s="94"/>
-      <c r="HA30" s="94"/>
-      <c r="HB30" s="94"/>
-      <c r="HC30" s="94"/>
-      <c r="HD30" s="94"/>
-      <c r="HE30" s="94"/>
-      <c r="HF30" s="94"/>
-      <c r="HG30" s="94"/>
-      <c r="HH30" s="94"/>
-      <c r="HI30" s="94"/>
-      <c r="HJ30" s="94"/>
-      <c r="HK30" s="94"/>
-      <c r="HL30" s="94"/>
-      <c r="HM30" s="94"/>
-      <c r="HN30" s="94"/>
-      <c r="HO30" s="94"/>
-      <c r="HP30" s="94"/>
-      <c r="HQ30" s="94"/>
-      <c r="HR30" s="94"/>
-      <c r="HS30" s="94"/>
-      <c r="HT30" s="94"/>
-      <c r="HU30" s="94"/>
-      <c r="HV30" s="94"/>
-      <c r="HW30" s="94"/>
-      <c r="HX30" s="94"/>
-      <c r="HY30" s="94"/>
-      <c r="HZ30" s="94"/>
-      <c r="IA30" s="94"/>
-      <c r="IB30" s="94"/>
-      <c r="IC30" s="94"/>
-      <c r="ID30" s="94"/>
-      <c r="IE30" s="94"/>
-      <c r="IF30" s="94"/>
-      <c r="IG30" s="94"/>
-      <c r="IH30" s="94"/>
-      <c r="II30" s="94"/>
-      <c r="IJ30" s="94"/>
-      <c r="IK30" s="94"/>
-      <c r="IL30" s="94"/>
-      <c r="IM30" s="94"/>
-      <c r="IN30" s="94"/>
-      <c r="IO30" s="94"/>
-      <c r="IP30" s="94"/>
-      <c r="IQ30" s="94"/>
-      <c r="IR30" s="94"/>
-      <c r="IS30" s="94"/>
-      <c r="IT30" s="94"/>
-      <c r="IU30" s="95"/>
+      <c r="H30" s="83"/>
+      <c r="I30" s="33"/>
+      <c r="J30" s="33"/>
+      <c r="K30" s="33"/>
+      <c r="L30" s="33"/>
+      <c r="M30" s="33"/>
+      <c r="N30" s="33"/>
+      <c r="O30" s="33"/>
+      <c r="P30" s="33"/>
+      <c r="Q30" s="33"/>
+      <c r="R30" s="33"/>
+      <c r="S30" s="33"/>
+      <c r="T30" s="33"/>
+      <c r="U30" s="33"/>
+      <c r="V30" s="33"/>
+      <c r="W30" s="33"/>
+      <c r="X30" s="33"/>
+      <c r="Y30" s="33"/>
+      <c r="Z30" s="33"/>
+      <c r="AA30" s="33"/>
+      <c r="AB30" s="33"/>
+      <c r="AC30" s="33"/>
+      <c r="AD30" s="33"/>
+      <c r="AE30" s="33"/>
+      <c r="AF30" s="33"/>
+      <c r="AG30" s="33"/>
+      <c r="AH30" s="33"/>
+      <c r="AI30" s="33"/>
+      <c r="AJ30" s="33"/>
+      <c r="AK30" s="33"/>
+      <c r="AL30" s="33"/>
+      <c r="AM30" s="33"/>
+      <c r="AN30" s="33"/>
+      <c r="AO30" s="33"/>
+      <c r="AP30" s="33"/>
+      <c r="AQ30" s="33"/>
+      <c r="AR30" s="33"/>
+      <c r="AS30" s="33"/>
+      <c r="AT30" s="33"/>
+      <c r="AU30" s="33"/>
+      <c r="AV30" s="33"/>
+      <c r="AW30" s="33"/>
+      <c r="AX30" s="33"/>
+      <c r="AY30" s="33"/>
+      <c r="AZ30" s="33"/>
+      <c r="BA30" s="33"/>
+      <c r="BB30" s="33"/>
+      <c r="BC30" s="33"/>
+      <c r="BD30" s="33"/>
+      <c r="BE30" s="33"/>
+      <c r="BF30" s="33"/>
+      <c r="BG30" s="33"/>
+      <c r="BH30" s="33"/>
+      <c r="BI30" s="33"/>
+      <c r="BJ30" s="33"/>
+      <c r="BK30" s="33"/>
+      <c r="BL30" s="33"/>
+      <c r="BM30" s="33"/>
+      <c r="BN30" s="33"/>
+      <c r="BO30" s="33"/>
+      <c r="BP30" s="33"/>
+      <c r="BQ30" s="33"/>
+      <c r="BR30" s="33"/>
+      <c r="BS30" s="33"/>
+      <c r="BT30" s="33"/>
+      <c r="BU30" s="33"/>
+      <c r="BV30" s="33"/>
+      <c r="BW30" s="33"/>
+      <c r="BX30" s="33"/>
+      <c r="BY30" s="33"/>
+      <c r="BZ30" s="33"/>
+      <c r="CA30" s="33"/>
+      <c r="CB30" s="33"/>
+      <c r="CC30" s="33"/>
+      <c r="CD30" s="33"/>
+      <c r="CE30" s="33"/>
+      <c r="CF30" s="33"/>
+      <c r="CG30" s="33"/>
+      <c r="CH30" s="33"/>
+      <c r="CI30" s="33"/>
+      <c r="CJ30" s="33"/>
+      <c r="CK30" s="33"/>
+      <c r="CL30" s="33"/>
+      <c r="CM30" s="33"/>
+      <c r="CN30" s="33"/>
+      <c r="CO30" s="33"/>
+      <c r="CP30" s="33"/>
+      <c r="CQ30" s="33"/>
+      <c r="CR30" s="33"/>
+      <c r="CS30" s="33"/>
+      <c r="CT30" s="33"/>
+      <c r="CU30" s="33"/>
+      <c r="CV30" s="33"/>
+      <c r="CW30" s="33"/>
+      <c r="CX30" s="33"/>
+      <c r="CY30" s="33"/>
+      <c r="CZ30" s="33"/>
+      <c r="DA30" s="33"/>
+      <c r="DB30" s="33"/>
+      <c r="DC30" s="33"/>
+      <c r="DD30" s="33"/>
+      <c r="DE30" s="33"/>
+      <c r="DF30" s="33"/>
+      <c r="DG30" s="33"/>
+      <c r="DH30" s="33"/>
+      <c r="DI30" s="33"/>
+      <c r="DJ30" s="33"/>
+      <c r="DK30" s="33"/>
+      <c r="DL30" s="33"/>
+      <c r="DM30" s="33"/>
+      <c r="DN30" s="33"/>
+      <c r="DO30" s="33"/>
+      <c r="DP30" s="33"/>
+      <c r="DQ30" s="33"/>
+      <c r="DR30" s="33"/>
+      <c r="DS30" s="33"/>
+      <c r="DT30" s="33"/>
+      <c r="DU30" s="33"/>
+      <c r="DV30" s="33"/>
+      <c r="DW30" s="33"/>
+      <c r="DX30" s="33"/>
+      <c r="DY30" s="33"/>
+      <c r="DZ30" s="33"/>
+      <c r="EA30" s="33"/>
+      <c r="EB30" s="33"/>
+      <c r="EC30" s="33"/>
+      <c r="ED30" s="33"/>
+      <c r="EE30" s="33"/>
+      <c r="EF30" s="33"/>
+      <c r="EG30" s="33"/>
+      <c r="EH30" s="33"/>
+      <c r="EI30" s="33"/>
+      <c r="EJ30" s="33"/>
+      <c r="EK30" s="33"/>
+      <c r="EL30" s="33"/>
+      <c r="EM30" s="33"/>
+      <c r="EN30" s="33"/>
+      <c r="EO30" s="33"/>
+      <c r="EP30" s="33"/>
+      <c r="EQ30" s="33"/>
+      <c r="ER30" s="33"/>
+      <c r="ES30" s="33"/>
+      <c r="ET30" s="33"/>
+      <c r="EU30" s="33"/>
+      <c r="EV30" s="33"/>
+      <c r="EW30" s="33"/>
+      <c r="EX30" s="33"/>
+      <c r="EY30" s="33"/>
+      <c r="EZ30" s="33"/>
+      <c r="FA30" s="33"/>
+      <c r="FB30" s="33"/>
+      <c r="FC30" s="33"/>
+      <c r="FD30" s="33"/>
+      <c r="FE30" s="33"/>
+      <c r="FF30" s="33"/>
+      <c r="FG30" s="33"/>
+      <c r="FH30" s="33"/>
+      <c r="FI30" s="33"/>
+      <c r="FJ30" s="33"/>
+      <c r="FK30" s="33"/>
+      <c r="FL30" s="33"/>
+      <c r="FM30" s="33"/>
+      <c r="FN30" s="33"/>
+      <c r="FO30" s="33"/>
+      <c r="FP30" s="33"/>
+      <c r="FQ30" s="33"/>
+      <c r="FR30" s="33"/>
+      <c r="FS30" s="33"/>
+      <c r="FT30" s="33"/>
+      <c r="FU30" s="33"/>
+      <c r="FV30" s="33"/>
+      <c r="FW30" s="33"/>
+      <c r="FX30" s="33"/>
+      <c r="FY30" s="33"/>
+      <c r="FZ30" s="33"/>
+      <c r="GA30" s="33"/>
+      <c r="GB30" s="33"/>
+      <c r="GC30" s="33"/>
+      <c r="GD30" s="33"/>
+      <c r="GE30" s="33"/>
+      <c r="GF30" s="33"/>
+      <c r="GG30" s="33"/>
+      <c r="GH30" s="33"/>
+      <c r="GI30" s="33"/>
+      <c r="GJ30" s="33"/>
+      <c r="GK30" s="33"/>
+      <c r="GL30" s="33"/>
+      <c r="GM30" s="33"/>
+      <c r="GN30" s="33"/>
+      <c r="GO30" s="33"/>
+      <c r="GP30" s="33"/>
+      <c r="GQ30" s="33"/>
+      <c r="GR30" s="33"/>
+      <c r="GS30" s="33"/>
+      <c r="GT30" s="33"/>
+      <c r="GU30" s="33"/>
+      <c r="GV30" s="33"/>
+      <c r="GW30" s="33"/>
+      <c r="GX30" s="33"/>
+      <c r="GY30" s="33"/>
+      <c r="GZ30" s="33"/>
+      <c r="HA30" s="33"/>
+      <c r="HB30" s="33"/>
+      <c r="HC30" s="33"/>
+      <c r="HD30" s="33"/>
+      <c r="HE30" s="33"/>
+      <c r="HF30" s="33"/>
+      <c r="HG30" s="33"/>
+      <c r="HH30" s="33"/>
+      <c r="HI30" s="33"/>
+      <c r="HJ30" s="33"/>
+      <c r="HK30" s="33"/>
+      <c r="HL30" s="33"/>
+      <c r="HM30" s="33"/>
+      <c r="HN30" s="33"/>
+      <c r="HO30" s="33"/>
+      <c r="HP30" s="33"/>
+      <c r="HQ30" s="33"/>
+      <c r="HR30" s="33"/>
+      <c r="HS30" s="33"/>
+      <c r="HT30" s="33"/>
+      <c r="HU30" s="33"/>
+      <c r="HV30" s="33"/>
+      <c r="HW30" s="33"/>
+      <c r="HX30" s="33"/>
+      <c r="HY30" s="33"/>
+      <c r="HZ30" s="33"/>
+      <c r="IA30" s="33"/>
+      <c r="IB30" s="33"/>
+      <c r="IC30" s="33"/>
+      <c r="ID30" s="33"/>
+      <c r="IE30" s="33"/>
+      <c r="IF30" s="33"/>
+      <c r="IG30" s="33"/>
+      <c r="IH30" s="33"/>
+      <c r="II30" s="33"/>
+      <c r="IJ30" s="33"/>
+      <c r="IK30" s="33"/>
+      <c r="IL30" s="33"/>
+      <c r="IM30" s="33"/>
+      <c r="IN30" s="33"/>
+      <c r="IO30" s="33"/>
+      <c r="IP30" s="33"/>
+      <c r="IQ30" s="33"/>
+      <c r="IR30" s="33"/>
+      <c r="IS30" s="33"/>
+      <c r="IT30" s="33"/>
+      <c r="IU30" s="84"/>
+    </row>
+    <row r="31" ht="18.75" customHeight="1">
+      <c r="A31" s="108">
+        <v>42736</v>
+      </c>
+      <c r="B31" s="131"/>
+      <c r="C31" t="s" s="12">
+        <v>37</v>
+      </c>
+      <c r="D31" t="s" s="12">
+        <v>80</v>
+      </c>
+      <c r="E31" t="s" s="129">
+        <v>382</v>
+      </c>
+      <c r="F31" t="s" s="15">
+        <v>416</v>
+      </c>
+      <c r="G31" t="s" s="133">
+        <v>415</v>
+      </c>
+      <c r="H31" s="152"/>
+      <c r="I31" s="94"/>
+      <c r="J31" s="94"/>
+      <c r="K31" s="94"/>
+      <c r="L31" s="94"/>
+      <c r="M31" s="94"/>
+      <c r="N31" s="94"/>
+      <c r="O31" s="94"/>
+      <c r="P31" s="94"/>
+      <c r="Q31" s="94"/>
+      <c r="R31" s="94"/>
+      <c r="S31" s="94"/>
+      <c r="T31" s="94"/>
+      <c r="U31" s="94"/>
+      <c r="V31" s="94"/>
+      <c r="W31" s="94"/>
+      <c r="X31" s="94"/>
+      <c r="Y31" s="94"/>
+      <c r="Z31" s="94"/>
+      <c r="AA31" s="94"/>
+      <c r="AB31" s="94"/>
+      <c r="AC31" s="94"/>
+      <c r="AD31" s="94"/>
+      <c r="AE31" s="94"/>
+      <c r="AF31" s="94"/>
+      <c r="AG31" s="94"/>
+      <c r="AH31" s="94"/>
+      <c r="AI31" s="94"/>
+      <c r="AJ31" s="94"/>
+      <c r="AK31" s="94"/>
+      <c r="AL31" s="94"/>
+      <c r="AM31" s="94"/>
+      <c r="AN31" s="94"/>
+      <c r="AO31" s="94"/>
+      <c r="AP31" s="94"/>
+      <c r="AQ31" s="94"/>
+      <c r="AR31" s="94"/>
+      <c r="AS31" s="94"/>
+      <c r="AT31" s="94"/>
+      <c r="AU31" s="94"/>
+      <c r="AV31" s="94"/>
+      <c r="AW31" s="94"/>
+      <c r="AX31" s="94"/>
+      <c r="AY31" s="94"/>
+      <c r="AZ31" s="94"/>
+      <c r="BA31" s="94"/>
+      <c r="BB31" s="94"/>
+      <c r="BC31" s="94"/>
+      <c r="BD31" s="94"/>
+      <c r="BE31" s="94"/>
+      <c r="BF31" s="94"/>
+      <c r="BG31" s="94"/>
+      <c r="BH31" s="94"/>
+      <c r="BI31" s="94"/>
+      <c r="BJ31" s="94"/>
+      <c r="BK31" s="94"/>
+      <c r="BL31" s="94"/>
+      <c r="BM31" s="94"/>
+      <c r="BN31" s="94"/>
+      <c r="BO31" s="94"/>
+      <c r="BP31" s="94"/>
+      <c r="BQ31" s="94"/>
+      <c r="BR31" s="94"/>
+      <c r="BS31" s="94"/>
+      <c r="BT31" s="94"/>
+      <c r="BU31" s="94"/>
+      <c r="BV31" s="94"/>
+      <c r="BW31" s="94"/>
+      <c r="BX31" s="94"/>
+      <c r="BY31" s="94"/>
+      <c r="BZ31" s="94"/>
+      <c r="CA31" s="94"/>
+      <c r="CB31" s="94"/>
+      <c r="CC31" s="94"/>
+      <c r="CD31" s="94"/>
+      <c r="CE31" s="94"/>
+      <c r="CF31" s="94"/>
+      <c r="CG31" s="94"/>
+      <c r="CH31" s="94"/>
+      <c r="CI31" s="94"/>
+      <c r="CJ31" s="94"/>
+      <c r="CK31" s="94"/>
+      <c r="CL31" s="94"/>
+      <c r="CM31" s="94"/>
+      <c r="CN31" s="94"/>
+      <c r="CO31" s="94"/>
+      <c r="CP31" s="94"/>
+      <c r="CQ31" s="94"/>
+      <c r="CR31" s="94"/>
+      <c r="CS31" s="94"/>
+      <c r="CT31" s="94"/>
+      <c r="CU31" s="94"/>
+      <c r="CV31" s="94"/>
+      <c r="CW31" s="94"/>
+      <c r="CX31" s="94"/>
+      <c r="CY31" s="94"/>
+      <c r="CZ31" s="94"/>
+      <c r="DA31" s="94"/>
+      <c r="DB31" s="94"/>
+      <c r="DC31" s="94"/>
+      <c r="DD31" s="94"/>
+      <c r="DE31" s="94"/>
+      <c r="DF31" s="94"/>
+      <c r="DG31" s="94"/>
+      <c r="DH31" s="94"/>
+      <c r="DI31" s="94"/>
+      <c r="DJ31" s="94"/>
+      <c r="DK31" s="94"/>
+      <c r="DL31" s="94"/>
+      <c r="DM31" s="94"/>
+      <c r="DN31" s="94"/>
+      <c r="DO31" s="94"/>
+      <c r="DP31" s="94"/>
+      <c r="DQ31" s="94"/>
+      <c r="DR31" s="94"/>
+      <c r="DS31" s="94"/>
+      <c r="DT31" s="94"/>
+      <c r="DU31" s="94"/>
+      <c r="DV31" s="94"/>
+      <c r="DW31" s="94"/>
+      <c r="DX31" s="94"/>
+      <c r="DY31" s="94"/>
+      <c r="DZ31" s="94"/>
+      <c r="EA31" s="94"/>
+      <c r="EB31" s="94"/>
+      <c r="EC31" s="94"/>
+      <c r="ED31" s="94"/>
+      <c r="EE31" s="94"/>
+      <c r="EF31" s="94"/>
+      <c r="EG31" s="94"/>
+      <c r="EH31" s="94"/>
+      <c r="EI31" s="94"/>
+      <c r="EJ31" s="94"/>
+      <c r="EK31" s="94"/>
+      <c r="EL31" s="94"/>
+      <c r="EM31" s="94"/>
+      <c r="EN31" s="94"/>
+      <c r="EO31" s="94"/>
+      <c r="EP31" s="94"/>
+      <c r="EQ31" s="94"/>
+      <c r="ER31" s="94"/>
+      <c r="ES31" s="94"/>
+      <c r="ET31" s="94"/>
+      <c r="EU31" s="94"/>
+      <c r="EV31" s="94"/>
+      <c r="EW31" s="94"/>
+      <c r="EX31" s="94"/>
+      <c r="EY31" s="94"/>
+      <c r="EZ31" s="94"/>
+      <c r="FA31" s="94"/>
+      <c r="FB31" s="94"/>
+      <c r="FC31" s="94"/>
+      <c r="FD31" s="94"/>
+      <c r="FE31" s="94"/>
+      <c r="FF31" s="94"/>
+      <c r="FG31" s="94"/>
+      <c r="FH31" s="94"/>
+      <c r="FI31" s="94"/>
+      <c r="FJ31" s="94"/>
+      <c r="FK31" s="94"/>
+      <c r="FL31" s="94"/>
+      <c r="FM31" s="94"/>
+      <c r="FN31" s="94"/>
+      <c r="FO31" s="94"/>
+      <c r="FP31" s="94"/>
+      <c r="FQ31" s="94"/>
+      <c r="FR31" s="94"/>
+      <c r="FS31" s="94"/>
+      <c r="FT31" s="94"/>
+      <c r="FU31" s="94"/>
+      <c r="FV31" s="94"/>
+      <c r="FW31" s="94"/>
+      <c r="FX31" s="94"/>
+      <c r="FY31" s="94"/>
+      <c r="FZ31" s="94"/>
+      <c r="GA31" s="94"/>
+      <c r="GB31" s="94"/>
+      <c r="GC31" s="94"/>
+      <c r="GD31" s="94"/>
+      <c r="GE31" s="94"/>
+      <c r="GF31" s="94"/>
+      <c r="GG31" s="94"/>
+      <c r="GH31" s="94"/>
+      <c r="GI31" s="94"/>
+      <c r="GJ31" s="94"/>
+      <c r="GK31" s="94"/>
+      <c r="GL31" s="94"/>
+      <c r="GM31" s="94"/>
+      <c r="GN31" s="94"/>
+      <c r="GO31" s="94"/>
+      <c r="GP31" s="94"/>
+      <c r="GQ31" s="94"/>
+      <c r="GR31" s="94"/>
+      <c r="GS31" s="94"/>
+      <c r="GT31" s="94"/>
+      <c r="GU31" s="94"/>
+      <c r="GV31" s="94"/>
+      <c r="GW31" s="94"/>
+      <c r="GX31" s="94"/>
+      <c r="GY31" s="94"/>
+      <c r="GZ31" s="94"/>
+      <c r="HA31" s="94"/>
+      <c r="HB31" s="94"/>
+      <c r="HC31" s="94"/>
+      <c r="HD31" s="94"/>
+      <c r="HE31" s="94"/>
+      <c r="HF31" s="94"/>
+      <c r="HG31" s="94"/>
+      <c r="HH31" s="94"/>
+      <c r="HI31" s="94"/>
+      <c r="HJ31" s="94"/>
+      <c r="HK31" s="94"/>
+      <c r="HL31" s="94"/>
+      <c r="HM31" s="94"/>
+      <c r="HN31" s="94"/>
+      <c r="HO31" s="94"/>
+      <c r="HP31" s="94"/>
+      <c r="HQ31" s="94"/>
+      <c r="HR31" s="94"/>
+      <c r="HS31" s="94"/>
+      <c r="HT31" s="94"/>
+      <c r="HU31" s="94"/>
+      <c r="HV31" s="94"/>
+      <c r="HW31" s="94"/>
+      <c r="HX31" s="94"/>
+      <c r="HY31" s="94"/>
+      <c r="HZ31" s="94"/>
+      <c r="IA31" s="94"/>
+      <c r="IB31" s="94"/>
+      <c r="IC31" s="94"/>
+      <c r="ID31" s="94"/>
+      <c r="IE31" s="94"/>
+      <c r="IF31" s="94"/>
+      <c r="IG31" s="94"/>
+      <c r="IH31" s="94"/>
+      <c r="II31" s="94"/>
+      <c r="IJ31" s="94"/>
+      <c r="IK31" s="94"/>
+      <c r="IL31" s="94"/>
+      <c r="IM31" s="94"/>
+      <c r="IN31" s="94"/>
+      <c r="IO31" s="94"/>
+      <c r="IP31" s="94"/>
+      <c r="IQ31" s="94"/>
+      <c r="IR31" s="94"/>
+      <c r="IS31" s="94"/>
+      <c r="IT31" s="94"/>
+      <c r="IU31" s="95"/>
     </row>
   </sheetData>
   <pageMargins left="0.7875" right="0.7875" top="1.05278" bottom="1.05278" header="0.7875" footer="0.7875"/>
@@ -38439,7 +38708,7 @@
     </row>
     <row r="4" ht="14" customHeight="1">
       <c r="A4" s="18">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B4" s="24"/>
       <c r="C4" t="s" s="62">

</xml_diff>